<commit_message>
Update tt to v1.4
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -425,7 +425,7 @@
     <t>Lab-1</t>
   </si>
   <si>
-    <t>COAL Lab-E              Sumayya</t>
+    <t xml:space="preserve">COAL Lab-E              Sumayya  </t>
   </si>
   <si>
     <t>Wp-GR2                              Dr. Farooque</t>
@@ -437,33 +437,33 @@
     <t>Lab-3</t>
   </si>
   <si>
+    <t>DB-Lab E              Mahrukh</t>
+  </si>
+  <si>
+    <t>OS Lab- Gr3                  Ali shah</t>
+  </si>
+  <si>
+    <t>Lab-4</t>
+  </si>
+  <si>
+    <t>OOAD-Lab B      Majid</t>
+  </si>
+  <si>
+    <t>EE Lab-8</t>
+  </si>
+  <si>
+    <t>OOAD-Lab F      Awais</t>
+  </si>
+  <si>
+    <t>DB-Lab D             Ammara</t>
+  </si>
+  <si>
+    <t>EE Lab 9</t>
+  </si>
+  <si>
     <t>COAL Lab-F                  Sehrish</t>
   </si>
   <si>
-    <t>OS Lab- Gr3                  Ali shah</t>
-  </si>
-  <si>
-    <t>Lab-4</t>
-  </si>
-  <si>
-    <t>OOAD-Lab F      Awais</t>
-  </si>
-  <si>
-    <t>EE Lab-8</t>
-  </si>
-  <si>
-    <t>OOAD-Lab B      Majid</t>
-  </si>
-  <si>
-    <t>DB-Lab D             Ammara</t>
-  </si>
-  <si>
-    <t>EE Lab 9</t>
-  </si>
-  <si>
-    <t>DB-Lab E              Mahrukh</t>
-  </si>
-  <si>
     <t>EE MPI Lab</t>
   </si>
   <si>
@@ -521,6 +521,9 @@
     <t xml:space="preserve">ITC-D                                  Javeria                                              </t>
   </si>
   <si>
+    <t>COAL-D                Mahwish</t>
+  </si>
+  <si>
     <t>DLD-Gr1                      Bahraj</t>
   </si>
   <si>
@@ -533,429 +536,426 @@
     <t>SE-GR1                 Abdul rehman</t>
   </si>
   <si>
+    <t>SE-GR2                                 Abdul rehman</t>
+  </si>
+  <si>
+    <t>Discrete-H                              Shoaib</t>
+  </si>
+  <si>
+    <t>Discrete-G                              Shoaib</t>
+  </si>
+  <si>
+    <t>Discrete-A                                  Shoaib</t>
+  </si>
+  <si>
+    <t>NS-GR1                                       Dr. Sufian</t>
+  </si>
+  <si>
+    <t>NS-GR1                                          Dr. Sufian</t>
+  </si>
+  <si>
+    <t>BD-GR1                                 Dr. Jawwad</t>
+  </si>
+  <si>
+    <t>DB-B     Tania</t>
+  </si>
+  <si>
+    <t>Wp-GR2                        Dr. Farooque</t>
+  </si>
+  <si>
+    <t>Wp-GR1                              Dr. Farooque</t>
+  </si>
+  <si>
+    <t>BioInfo-GR1                 M. Shahzad</t>
+  </si>
+  <si>
+    <t>Wp-GR2                                       Dr. Farooque</t>
+  </si>
+  <si>
+    <t>NP-GR1                 Shahbaz</t>
+  </si>
+  <si>
+    <t>IPM-GR1                                       Ubaid</t>
+  </si>
+  <si>
+    <t>IPM-GR1                 Ubaid</t>
+  </si>
+  <si>
+    <t>BE-C                                     Adeel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COAL-F                                Nadeem Kafi            </t>
+  </si>
+  <si>
+    <t>COAL-C                Nadeem Kafi</t>
+  </si>
+  <si>
+    <t>BE-G                                     Ahsan sunny</t>
+  </si>
+  <si>
+    <t>COAL-A                                 Nadeem Kafi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COAL-H                              Danish     </t>
+  </si>
+  <si>
+    <t>LA-C                                                                         Dr. Fahad Riaz</t>
+  </si>
+  <si>
+    <t>LA-A                                                                                  Dr. Fahad Riaz</t>
+  </si>
+  <si>
+    <t>LA-E                                                                                           Dr. Fahad Riaz</t>
+  </si>
+  <si>
+    <t>OOAD-E                           Faiza Sattar</t>
+  </si>
+  <si>
+    <t>Algo-B                           Subash</t>
+  </si>
+  <si>
+    <t>Algo-D                           Subash</t>
+  </si>
+  <si>
+    <t>Algo-E                           Subash</t>
+  </si>
+  <si>
+    <t>OOAD-F                           Faiza Sattar</t>
+  </si>
+  <si>
+    <t>ENG-B2                                                 Sameera</t>
+  </si>
+  <si>
+    <t>CAL I-A                         Dr. Sadaqat</t>
+  </si>
+  <si>
+    <t>CAL I-B                                       Dr. Sadaqat</t>
+  </si>
+  <si>
+    <t>DB-F                                        Ahsan</t>
+  </si>
+  <si>
+    <t>CAL I-G                  Abdul Basit</t>
+  </si>
+  <si>
+    <t>ENG-G2                                                    Faiza Mumtaz</t>
+  </si>
+  <si>
+    <t>COAL Lab-A                Zain</t>
+  </si>
+  <si>
+    <t>OOAD-Lab C      Nadeem</t>
+  </si>
+  <si>
+    <t>OS Lab- Gr2                  Ali shah</t>
+  </si>
+  <si>
+    <t>BioInfo-GR1                             M. Shahzad</t>
+  </si>
+  <si>
+    <t>DB-Lab A              Basit ali</t>
+  </si>
+  <si>
+    <t>COAL Lab-B               Sehrish</t>
+  </si>
+  <si>
+    <t>DB-Lab B             Mahrukh</t>
+  </si>
+  <si>
+    <t>DB-Lab F              Ammara</t>
+  </si>
+  <si>
+    <t>COAL Lab-G                Sumayya</t>
+  </si>
+  <si>
+    <t>OOAD-Lab G      Majid</t>
+  </si>
+  <si>
+    <t>CN Lab Gr1     Awais</t>
+  </si>
+  <si>
+    <t>ENG-F2                                                   Nasir</t>
+  </si>
+  <si>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
+    <t>IRTM-GR1                                      M. Rafi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CN-Gr1                                            Dr. Sufian              </t>
+  </si>
+  <si>
+    <t>Discrete-C               Nouman Durrani</t>
+  </si>
+  <si>
+    <t>Discrete-E                           Nouman Durrani</t>
+  </si>
+  <si>
+    <t>Discrete-F                            Nouman Durrani</t>
+  </si>
+  <si>
+    <t>Discrete-A                             Shoaib</t>
+  </si>
+  <si>
+    <t>Discrete-H                                 Shoaib</t>
+  </si>
+  <si>
+    <t>Discrete-D                                    Dr. Fahad Samad</t>
+  </si>
+  <si>
+    <t>Discrete-B                               Dr. Fahad Samad</t>
+  </si>
+  <si>
+    <t>PIT-E                             Shaharbano</t>
+  </si>
+  <si>
+    <t>Dp-GR2                                   Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>Dp-GR1                                    Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>HCI-A                               Behraj</t>
+  </si>
+  <si>
+    <t>HCI-F                                            Behraj</t>
+  </si>
+  <si>
+    <t>Dsci-GR1                                     Dr. Zeeshan</t>
+  </si>
+  <si>
+    <t>Bcomm-I Gr1  Sameera</t>
+  </si>
+  <si>
+    <t>Bcomm-I Gr2  Sameera</t>
+  </si>
+  <si>
+    <t>DB-C                                     Dr. Zeeshan</t>
+  </si>
+  <si>
+    <t>CM Gr1     Tuba</t>
+  </si>
+  <si>
+    <t>CM Gr2     Tuba</t>
+  </si>
+  <si>
+    <t>LA-B                                                                                  Dr. Faqiha</t>
+  </si>
+  <si>
+    <t>MM Gr1                                         Asiya</t>
+  </si>
+  <si>
+    <t>MM Gr2                                                           Asiya</t>
+  </si>
+  <si>
+    <t>LA-G                                                                                    Dr. Faqiha</t>
+  </si>
+  <si>
+    <t>Cal-II-Gr1                    Dr. Khusro</t>
+  </si>
+  <si>
+    <t>Cal-II-Gr2                       Dr. Khusro</t>
+  </si>
+  <si>
+    <t>AIS-Gr1      Ahsan</t>
+  </si>
+  <si>
+    <t>IRS-A                                            Shahzad Sheikh</t>
+  </si>
+  <si>
+    <t>Eng comp-Gr1                                             Tuba</t>
+  </si>
+  <si>
+    <t>AL-Gr1                        Shahzad Sheikh</t>
+  </si>
+  <si>
+    <t>CAL I-F                               Ashhad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME-Gr1   Micheal    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prob &amp; Stats-Gr1   Abdul Basit </t>
+  </si>
+  <si>
+    <t>CAL I-A                                      Dr. Sadaqat</t>
+  </si>
+  <si>
+    <t>OR-Gr1      Abdul Basit</t>
+  </si>
+  <si>
+    <t>Psych-Gr1  Sumaira</t>
+  </si>
+  <si>
+    <t>Psych-Gr2  Sumaira</t>
+  </si>
+  <si>
+    <t>Socio-Gr1      Sumaira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP Lab-C=         Rahemeen &amp; Mahrukh      </t>
+  </si>
+  <si>
+    <t>OS Lab- Gr1                  Ali shah</t>
+  </si>
+  <si>
+    <t>ITC-Lab A        Maham &amp; Muneem</t>
+  </si>
+  <si>
+    <t>OOAD-Lab D      Majid</t>
+  </si>
+  <si>
+    <t>DS-Lab C     Abdul Aziz</t>
+  </si>
+  <si>
+    <t>OOAD-Lab E      Awais</t>
+  </si>
+  <si>
+    <t>DS-Lab E                      Faizan</t>
+  </si>
+  <si>
+    <t>DB-Lab G              Ammara</t>
+  </si>
+  <si>
+    <t>ITC-Lab B        Farah &amp; Mubashra</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t>DB-E                                      Tania</t>
+  </si>
+  <si>
+    <t>DB-B                                      Tania</t>
+  </si>
+  <si>
+    <t>DB-A                                          Tania</t>
+  </si>
+  <si>
+    <t>Algo-A                           Dr. Atif</t>
+  </si>
+  <si>
+    <t>BioInfo-GR1                       M. Shahzad</t>
+  </si>
+  <si>
+    <t>TOA-Gr1                                    M. Shahzad</t>
+  </si>
+  <si>
+    <t>OOAD-F                           Faiza sattar</t>
+  </si>
+  <si>
+    <t>OOAD-E                           Faiza sattar</t>
+  </si>
+  <si>
+    <t>DB-C                                                             Dr. Zeeshan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COAL-B                                                 Mahwish    </t>
+  </si>
+  <si>
+    <t>COAL-D                                                               Mahwish</t>
+  </si>
+  <si>
+    <t>IRTM-GR1                                    M. Rafi</t>
+  </si>
+  <si>
+    <t>SMD-GR1                                      Nauman Atique</t>
+  </si>
+  <si>
+    <t>CM Gr2                   Tuba</t>
+  </si>
+  <si>
+    <t>DB-F    Ahsan</t>
+  </si>
+  <si>
+    <t>IPM-GR1                                    Ubaid</t>
+  </si>
+  <si>
+    <t>CM Gr1                      Tuba</t>
+  </si>
+  <si>
+    <t>BE-B                                    Kanwal</t>
+  </si>
+  <si>
+    <t>BE-D                                     Kanwal</t>
+  </si>
+  <si>
+    <t>LA-B                                                        Dr. Faqiha</t>
+  </si>
+  <si>
+    <t>LA-C                                      Dr. Fahad Riaz</t>
+  </si>
+  <si>
+    <t>LA-E                                               Dr. Fahad Riaz</t>
+  </si>
+  <si>
+    <t>LA-A                                               Dr. Fahad Riaz</t>
+  </si>
+  <si>
+    <t>MM Gr1                       Asiya</t>
+  </si>
+  <si>
+    <t>MM Gr2                                  Asiya</t>
+  </si>
+  <si>
+    <t>Cal-II-Gr1                   Dr. Khusro</t>
+  </si>
+  <si>
+    <t>LA-F                                        Jamil</t>
+  </si>
+  <si>
+    <t>Psych-Gr2                     Sumaira</t>
+  </si>
+  <si>
+    <t>Socio-Gr1         Sumaira</t>
+  </si>
+  <si>
+    <t>LA-D                                          Jamil</t>
+  </si>
+  <si>
+    <t>ITC-Lab C                   Maham&amp; Muneem</t>
+  </si>
+  <si>
+    <t>ITC-Lab D        Farah &amp; Mubashra</t>
+  </si>
+  <si>
+    <t>DS-Lab A           Abdul Aziz</t>
+  </si>
+  <si>
+    <t>BD-GR1                                  Dr. Jawwad</t>
+  </si>
+  <si>
+    <t>ITC-Lab G        Safia &amp; Maham</t>
+  </si>
+  <si>
+    <t>COAL Lab-D    Sehrish</t>
+  </si>
+  <si>
+    <t>DS-Lab D    Faizan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP Lab-A=            Rahemeen &amp; Basit         </t>
+  </si>
+  <si>
+    <t>COAL Lab-H             Sumayya</t>
+  </si>
+  <si>
+    <t>OOAD-Lab A      Nadeem</t>
+  </si>
+  <si>
+    <t>FRIDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CN-Gr1                                             Dr. Sufian                </t>
+  </si>
+  <si>
+    <t>JUMMA PRAYER</t>
+  </si>
+  <si>
     <t>SE-GR1                                  Abdul rehman</t>
   </si>
   <si>
-    <t>Discrete-H                              Shoaib</t>
-  </si>
-  <si>
-    <t>Discrete-G                              Shoaib</t>
-  </si>
-  <si>
-    <t>Discrete-A                                  Shoaib</t>
-  </si>
-  <si>
-    <t>NS-GR1                                       Dr. Sufian</t>
-  </si>
-  <si>
-    <t>NS-GR1                                          Dr. Sufian</t>
-  </si>
-  <si>
-    <t>BD-GR1                                 Dr. Jawwad</t>
-  </si>
-  <si>
-    <t>DB-B     Tania</t>
-  </si>
-  <si>
-    <t>Wp-GR2                        Dr. Farooque</t>
-  </si>
-  <si>
-    <t>Wp-GR1                              Dr. Farooque</t>
-  </si>
-  <si>
-    <t>COAL-D                Mahwish</t>
-  </si>
-  <si>
-    <t>BioInfo-GR1                 M. Shahzad</t>
-  </si>
-  <si>
-    <t>Wp-GR2                                       Dr. Farooque</t>
-  </si>
-  <si>
-    <t>NP-GR1                 Shahbaz</t>
-  </si>
-  <si>
-    <t>IPM-GR1                                       Ubaid</t>
-  </si>
-  <si>
-    <t>IPM-GR1                 Ubaid</t>
-  </si>
-  <si>
-    <t>BE-C                                     Adeel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COAL-F                                Nadeem Kafi            </t>
-  </si>
-  <si>
-    <t>COAL-C                Nadeem Kafi</t>
-  </si>
-  <si>
-    <t>BE-G                                     Ahsan sunny</t>
-  </si>
-  <si>
-    <t>COAL-A                                 Nadeem Kafi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COAL-H                              Danish     </t>
-  </si>
-  <si>
-    <t>LA-C                                                                         Dr. Fahad Riaz</t>
-  </si>
-  <si>
-    <t>LA-A                                                                                  Dr. Fahad Riaz</t>
-  </si>
-  <si>
-    <t>LA-E                                                                                           Dr. Fahad Riaz</t>
-  </si>
-  <si>
-    <t>OOAD-E                           Faiza Sattar</t>
-  </si>
-  <si>
-    <t>Algo-B                           Subash</t>
-  </si>
-  <si>
-    <t>Algo-D                           Subash</t>
-  </si>
-  <si>
-    <t>Algo-E                           Subash</t>
-  </si>
-  <si>
-    <t>OOAD-F                           Faiza Sattar</t>
-  </si>
-  <si>
-    <t>ENG-B2                                                 Sameera</t>
-  </si>
-  <si>
-    <t>CAL I-A                         Dr. Sadaqat</t>
-  </si>
-  <si>
-    <t>IRS-A                                            Shahzad Sheikh</t>
-  </si>
-  <si>
-    <t>CAL I-G                  Abdul Basit</t>
-  </si>
-  <si>
-    <t>CAL I-B                                       Dr. Sadaqat</t>
-  </si>
-  <si>
-    <t>DB-F                                        Ahsan</t>
-  </si>
-  <si>
-    <t>ENG-G2                                                    Faiza Mumtaz</t>
-  </si>
-  <si>
-    <t>COAL Lab-B                                                                                                                 Sehrish</t>
-  </si>
-  <si>
-    <t>COAL Lab-G                                                                                                                     Sumayya</t>
-  </si>
-  <si>
-    <t>COAL Lab-A                                                                                                                  Zain</t>
-  </si>
-  <si>
-    <t>BioInfo-GR1                             M. Shahzad</t>
-  </si>
-  <si>
-    <t>DB-Lab A              Basit ali</t>
-  </si>
-  <si>
-    <t>OS Lab- Gr2                  Ali shah</t>
-  </si>
-  <si>
-    <t>OOAD-Lab C      Nadeem</t>
-  </si>
-  <si>
-    <t>DB-Lab F              Ammara</t>
-  </si>
-  <si>
-    <t>DB-Lab B             Mahrukh</t>
-  </si>
-  <si>
-    <t>OOAD-Lab G      Majid</t>
-  </si>
-  <si>
-    <t>CN Lab Gr1     Awais</t>
-  </si>
-  <si>
-    <t>ENG-F2                                                   Nasir</t>
-  </si>
-  <si>
-    <t>WEDNESDAY</t>
-  </si>
-  <si>
-    <t>IRTM-GR1                                      M. Rafi</t>
-  </si>
-  <si>
-    <t>Discrete-D                                    Dr. Fahad Samad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN-Gr1                                            Dr. Sufian              </t>
-  </si>
-  <si>
-    <t>Discrete-B                               Dr. Fahad Samad</t>
-  </si>
-  <si>
-    <t>Discrete-C               Nouman Durrani</t>
-  </si>
-  <si>
-    <t>Discrete-E                           Nouman Durrani</t>
-  </si>
-  <si>
-    <t>Discrete-F                            Nouman Durrani</t>
-  </si>
-  <si>
-    <t>Discrete-A                             Shoaib</t>
-  </si>
-  <si>
-    <t>Discrete-H                                 Shoaib</t>
-  </si>
-  <si>
-    <t>PIT-E                             Shaharbano</t>
-  </si>
-  <si>
-    <t>Dp-GR2                                   Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>Dp-GR1                                    Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>HCI-A                               Behraj</t>
-  </si>
-  <si>
-    <t>HCI-F                                            Behraj</t>
-  </si>
-  <si>
-    <t>Dsci-GR1                                     Dr. Zeeshan</t>
-  </si>
-  <si>
-    <t>Bcomm-I Gr1  Sameera</t>
-  </si>
-  <si>
-    <t>Bcomm-I Gr2  Sameera</t>
-  </si>
-  <si>
-    <t>DB-C                                     Dr. Zeeshan</t>
-  </si>
-  <si>
-    <t>CM Gr1     Tuba</t>
-  </si>
-  <si>
-    <t>CM Gr2     Tuba</t>
-  </si>
-  <si>
-    <t>LA-B                                                                                  Dr. Faqiha</t>
-  </si>
-  <si>
-    <t>MM Gr1                                         Asiya</t>
-  </si>
-  <si>
-    <t>MM Gr2                                                           Asiya</t>
-  </si>
-  <si>
-    <t>LA-G                                                                                    Dr. Faqiha</t>
-  </si>
-  <si>
-    <t>Cal-II-Gr1                    Dr. Khusro</t>
-  </si>
-  <si>
-    <t>Cal-II-Gr2                       Dr. Khusro</t>
-  </si>
-  <si>
-    <t>AIS-Gr1      Ahsan</t>
-  </si>
-  <si>
-    <t>Eng comp-Gr1                                             Tuba</t>
-  </si>
-  <si>
-    <t>AL-Gr1                        Shahzad Sheikh</t>
-  </si>
-  <si>
-    <t>CAL I-F                               Ashhad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME-Gr1   Micheal    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prob &amp; Stats-Gr1   Abdul Basit </t>
-  </si>
-  <si>
-    <t>CAL I-A                                      Dr. Sadaqat</t>
-  </si>
-  <si>
-    <t>OR-Gr1      Abdul Basit</t>
-  </si>
-  <si>
-    <t>Psych-Gr1  Sumaira</t>
-  </si>
-  <si>
-    <t>Psych-Gr2  Sumaira</t>
-  </si>
-  <si>
-    <t>Socio-Gr1      Sumaira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP Lab-C=         Rahemeen &amp; Mahrukh      </t>
-  </si>
-  <si>
-    <t>OS Lab- Gr1                  Ali shah</t>
-  </si>
-  <si>
-    <t>DS-Lab E                      Faizan</t>
-  </si>
-  <si>
-    <t>OOAD-Lab D      Majid</t>
-  </si>
-  <si>
-    <t>DS-Lab C     Abdul Aziz</t>
-  </si>
-  <si>
-    <t>DB-Lab G              Ammara</t>
-  </si>
-  <si>
-    <t>ITC-Lab A        Maham &amp; Muneem</t>
-  </si>
-  <si>
-    <t>OOAD-Lab E      Awais</t>
-  </si>
-  <si>
-    <t>ITC-Lab B        Farah &amp; Mubashra</t>
-  </si>
-  <si>
-    <t>THURSDAY</t>
-  </si>
-  <si>
-    <t>DB-E                                      Tania</t>
-  </si>
-  <si>
-    <t>DB-B                                      Tania</t>
-  </si>
-  <si>
-    <t>DB-A                                          Tania</t>
-  </si>
-  <si>
-    <t>Algo-A                           Dr. Atif</t>
-  </si>
-  <si>
-    <t>BioInfo-GR1                       M. Shahzad</t>
-  </si>
-  <si>
-    <t>TOA-Gr1                                    M. Shahzad</t>
-  </si>
-  <si>
-    <t>OOAD-F                           Faiza sattar</t>
-  </si>
-  <si>
-    <t>OOAD-E                           Faiza sattar</t>
-  </si>
-  <si>
-    <t>DB-C                                                             Dr. Zeeshan</t>
-  </si>
-  <si>
-    <t>IRTM-GR1                                    M. Rafi</t>
-  </si>
-  <si>
-    <t>SMD-GR1                                      Nauman Atique</t>
-  </si>
-  <si>
-    <t>CM Gr2                   Tuba</t>
-  </si>
-  <si>
-    <t>DB-F    Ahsan</t>
-  </si>
-  <si>
-    <t>IPM-GR1                                    Ubaid</t>
-  </si>
-  <si>
-    <t>CM Gr1                      Tuba</t>
-  </si>
-  <si>
-    <t>BE-B                                    Kanwal</t>
-  </si>
-  <si>
-    <t>BE-D                                     Kanwal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COAL-B                                                 Mahwish    </t>
-  </si>
-  <si>
-    <t>COAL-D                                                               Mahwish</t>
-  </si>
-  <si>
-    <t>LA-B                                                        Dr. Faqiha</t>
-  </si>
-  <si>
-    <t>LA-C                                      Dr. Fahad Riaz</t>
-  </si>
-  <si>
-    <t>LA-E                                               Dr. Fahad Riaz</t>
-  </si>
-  <si>
-    <t>LA-A                                               Dr. Fahad Riaz</t>
-  </si>
-  <si>
-    <t>MM Gr1                       Asiya</t>
-  </si>
-  <si>
-    <t>MM Gr2                                  Asiya</t>
-  </si>
-  <si>
-    <t>Cal-II-Gr1                   Dr. Khusro</t>
-  </si>
-  <si>
-    <t>LA-F                                        Jamil</t>
-  </si>
-  <si>
-    <t>Psych-Gr2                     Sumaira</t>
-  </si>
-  <si>
-    <t>Socio-Gr1         Sumaira</t>
-  </si>
-  <si>
-    <t>LA-D                                          Jamil</t>
-  </si>
-  <si>
-    <t>ITC-Lab C                   Maham&amp; Muneem</t>
-  </si>
-  <si>
-    <t>ITC-Lab D        Farah &amp; Mubashra</t>
-  </si>
-  <si>
-    <t>DS-Lab A           Abdul Aziz</t>
-  </si>
-  <si>
-    <t>BD-GR1                                  Dr. Jawwad</t>
-  </si>
-  <si>
-    <t>ITC-Lab G        Safia &amp; Maham</t>
-  </si>
-  <si>
-    <t>COAL Lab-D    Sehrish</t>
-  </si>
-  <si>
-    <t>COAL Lab-H                                                                                                                                Sumayya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP Lab-A=            Rahemeen &amp; Basit         </t>
-  </si>
-  <si>
-    <t>DS-Lab D    Faizan</t>
-  </si>
-  <si>
-    <t>OOAD-Lab A      Nadeem</t>
-  </si>
-  <si>
-    <t>FRIDAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN-Gr1                                             Dr. Sufian                </t>
-  </si>
-  <si>
-    <t>JUMMA PRAYER</t>
-  </si>
-  <si>
-    <t>SE-GR2                                 Abdul rehman</t>
-  </si>
-  <si>
     <t>COAL-E                                                        Danish</t>
   </si>
   <si>
@@ -965,31 +965,31 @@
     <t>COAL-G                                                 Danish</t>
   </si>
   <si>
+    <t>Discrete-G                                                       Shoaib</t>
+  </si>
+  <si>
+    <t>Discrete-A                                                         Shoaib</t>
+  </si>
+  <si>
+    <t>Discrete-H                                                Shoaib</t>
+  </si>
+  <si>
+    <t>DB-D                                     Ahsan</t>
+  </si>
+  <si>
+    <t>TOA-Gr1                                M. Shahzad</t>
+  </si>
+  <si>
+    <t>TOA-Gr1                                          M. Shahzad</t>
+  </si>
+  <si>
     <t>COAL-A                                                   Nadeem Kafi</t>
   </si>
   <si>
-    <t>Discrete-G                                                       Shoaib</t>
-  </si>
-  <si>
-    <t>Discrete-H                                                Shoaib</t>
-  </si>
-  <si>
     <t>COAL-C                                                               Nadeem Kafi</t>
   </si>
   <si>
     <t>COAL-F                                                           Nadeem Kafi</t>
-  </si>
-  <si>
-    <t>Discrete-A                                                         Shoaib</t>
-  </si>
-  <si>
-    <t>DB-D                                     Ahsan</t>
-  </si>
-  <si>
-    <t>TOA-Gr1                                M. Shahzad</t>
-  </si>
-  <si>
-    <t>TOA-Gr1                                          M. Shahzad</t>
   </si>
   <si>
     <t>OOAD-C                            Faiza sattar</t>
@@ -1395,7 +1395,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="64" zoomScaleNormal="64" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -1404,7 +1404,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1416,9 +1416,8 @@
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
-      <c r="J1"/>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1446,9 +1445,8 @@
       <c r="I2">
         <v>8</v>
       </c>
-      <c r="J2"/>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1476,9 +1474,8 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1490,9 +1487,8 @@
       <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:10">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1516,9 +1512,8 @@
       <c r="I5" t="s">
         <v>18</v>
       </c>
-      <c r="J5"/>
-    </row>
-    <row r="6" spans="1:10">
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1540,9 +1535,8 @@
         <v>23</v>
       </c>
       <c r="I6"/>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:10">
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1568,9 +1562,8 @@
       <c r="I7" t="s">
         <v>31</v>
       </c>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:10">
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1596,9 +1589,8 @@
         <v>39</v>
       </c>
       <c r="I8"/>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="1:10">
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1622,9 +1614,8 @@
         <v>46</v>
       </c>
       <c r="I9"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:10">
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1650,9 +1641,8 @@
       <c r="I10" t="s">
         <v>54</v>
       </c>
-      <c r="J10"/>
-    </row>
-    <row r="11" spans="1:10">
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1672,9 +1662,8 @@
       <c r="I11" t="s">
         <v>59</v>
       </c>
-      <c r="J11"/>
-    </row>
-    <row r="12" spans="1:10">
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1700,9 +1689,8 @@
       <c r="I12" t="s">
         <v>67</v>
       </c>
-      <c r="J12"/>
-    </row>
-    <row r="13" spans="1:10">
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1724,9 +1712,8 @@
       <c r="I13" t="s">
         <v>73</v>
       </c>
-      <c r="J13"/>
-    </row>
-    <row r="14" spans="1:10">
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1750,9 +1737,8 @@
       </c>
       <c r="H14"/>
       <c r="I14"/>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="1:10">
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -1774,9 +1760,8 @@
         <v>86</v>
       </c>
       <c r="I15"/>
-      <c r="J15"/>
-    </row>
-    <row r="16" spans="1:10">
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -1800,9 +1785,8 @@
       <c r="I16" t="s">
         <v>93</v>
       </c>
-      <c r="J16"/>
-    </row>
-    <row r="17" spans="1:10">
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>94</v>
       </c>
@@ -1826,9 +1810,8 @@
         <v>100</v>
       </c>
       <c r="I17"/>
-      <c r="J17"/>
-    </row>
-    <row r="18" spans="1:10">
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -1850,9 +1833,8 @@
       <c r="I18" t="s">
         <v>106</v>
       </c>
-      <c r="J18"/>
-    </row>
-    <row r="19" spans="1:10">
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>107</v>
       </c>
@@ -1878,9 +1860,8 @@
         <v>114</v>
       </c>
       <c r="I19"/>
-      <c r="J19"/>
-    </row>
-    <row r="20" spans="1:10">
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>115</v>
       </c>
@@ -1904,9 +1885,8 @@
       <c r="I20" t="s">
         <v>121</v>
       </c>
-      <c r="J20"/>
-    </row>
-    <row r="21" spans="1:10">
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>122</v>
       </c>
@@ -1926,9 +1906,8 @@
         <v>126</v>
       </c>
       <c r="I21"/>
-      <c r="J21"/>
-    </row>
-    <row r="22" spans="1:10">
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -1948,9 +1927,8 @@
       </c>
       <c r="H22"/>
       <c r="I22"/>
-      <c r="J22"/>
-    </row>
-    <row r="23" spans="1:10">
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>132</v>
       </c>
@@ -1962,9 +1940,8 @@
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
-      <c r="J23"/>
-    </row>
-    <row r="24" spans="1:10">
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -1984,9 +1961,8 @@
       </c>
       <c r="H24"/>
       <c r="I24"/>
-      <c r="J24"/>
-    </row>
-    <row r="25" spans="1:10">
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -2002,9 +1978,8 @@
       </c>
       <c r="H25"/>
       <c r="I25"/>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="1:10">
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>140</v>
       </c>
@@ -2018,9 +1993,8 @@
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="1:10">
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>142</v>
       </c>
@@ -2036,9 +2010,8 @@
       </c>
       <c r="H27"/>
       <c r="I27"/>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="1:10">
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>145</v>
       </c>
@@ -2052,9 +2025,8 @@
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
-      <c r="J28"/>
-    </row>
-    <row r="29" spans="1:10">
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>147</v>
       </c>
@@ -2068,9 +2040,8 @@
       </c>
       <c r="H29"/>
       <c r="I29"/>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="1:10">
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>149</v>
       </c>
@@ -2084,9 +2055,8 @@
       </c>
       <c r="H30"/>
       <c r="I30"/>
-      <c r="J30"/>
-    </row>
-    <row r="31" spans="1:10">
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -2112,7 +2082,6 @@
       <c r="I31" t="s">
         <v>158</v>
       </c>
-      <c r="J31"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -2318,7 +2287,9 @@
         <v>165</v>
       </c>
       <c r="C8"/>
-      <c r="D8"/>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
       <c r="E8" t="s">
         <v>33</v>
       </c>
@@ -2327,7 +2298,9 @@
         <v>34</v>
       </c>
       <c r="H8"/>
-      <c r="I8"/>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
       <c r="J8"/>
       <c r="K8"/>
     </row>
@@ -2336,17 +2309,17 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G9" t="s">
         <v>98</v>
@@ -2363,21 +2336,21 @@
         <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -2394,10 +2367,10 @@
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
@@ -2413,10 +2386,10 @@
         <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -2434,14 +2407,12 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C13" t="s">
-        <v>179</v>
-      </c>
-      <c r="D13" t="s">
         <v>180</v>
       </c>
+      <c r="D13"/>
       <c r="E13" t="s">
         <v>181</v>
       </c>
@@ -2450,9 +2421,7 @@
         <v>182</v>
       </c>
       <c r="H13"/>
-      <c r="I13" t="s">
-        <v>46</v>
-      </c>
+      <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
     </row>
@@ -2604,9 +2573,7 @@
       <c r="H19" t="s">
         <v>114</v>
       </c>
-      <c r="I19" t="s">
-        <v>108</v>
-      </c>
+      <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
     </row>
@@ -2617,21 +2584,15 @@
       <c r="B20" t="s">
         <v>201</v>
       </c>
-      <c r="C20" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" t="s">
-        <v>202</v>
-      </c>
+      <c r="C20"/>
+      <c r="D20"/>
       <c r="E20"/>
       <c r="F20" t="s">
         <v>116</v>
       </c>
-      <c r="G20" t="s">
-        <v>203</v>
-      </c>
+      <c r="G20"/>
       <c r="H20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
@@ -2649,13 +2610,17 @@
         <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F21" t="s">
         <v>71</v>
       </c>
-      <c r="G21"/>
-      <c r="H21"/>
+      <c r="G21" t="s">
+        <v>204</v>
+      </c>
+      <c r="H21" t="s">
+        <v>108</v>
+      </c>
       <c r="I21" t="s">
         <v>73</v>
       </c>
@@ -2677,7 +2642,7 @@
         <v>153</v>
       </c>
       <c r="F22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G22" t="s">
         <v>157</v>
@@ -2711,14 +2676,14 @@
         <v>133</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -2730,16 +2695,16 @@
         <v>137</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25" t="s">
+        <v>209</v>
+      </c>
+      <c r="G25" t="s">
         <v>210</v>
-      </c>
-      <c r="G25" t="s">
-        <v>211</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -2751,14 +2716,14 @@
         <v>140</v>
       </c>
       <c r="B26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -2770,14 +2735,14 @@
         <v>142</v>
       </c>
       <c r="B27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -2789,7 +2754,7 @@
         <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -2811,7 +2776,7 @@
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
@@ -2837,7 +2802,7 @@
         <v>126</v>
       </c>
       <c r="H30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I30" t="s">
         <v>124</v>
@@ -2878,7 +2843,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3055,27 +3020,23 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" t="s">
         <v>220</v>
-      </c>
-      <c r="C7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D7"/>
-      <c r="E7" t="s">
-        <v>221</v>
-      </c>
-      <c r="F7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" t="s">
-        <v>222</v>
       </c>
       <c r="H7" t="s">
         <v>71</v>
       </c>
-      <c r="I7" t="s">
-        <v>223</v>
-      </c>
+      <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -3121,16 +3082,16 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C9" t="s">
         <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
@@ -3154,17 +3115,17 @@
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H10"/>
       <c r="I10" t="s">
@@ -3182,8 +3143,12 @@
       <c r="A11" t="s">
         <v>55</v>
       </c>
-      <c r="B11"/>
-      <c r="C11"/>
+      <c r="B11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" t="s">
+        <v>227</v>
+      </c>
       <c r="D11"/>
       <c r="E11" t="s">
         <v>67</v>
@@ -3194,7 +3159,7 @@
         <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
@@ -3213,15 +3178,15 @@
         <v>62</v>
       </c>
       <c r="D12" t="s">
+        <v>229</v>
+      </c>
+      <c r="E12" t="s">
         <v>230</v>
-      </c>
-      <c r="E12" t="s">
-        <v>231</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -3243,7 +3208,7 @@
         <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E13" t="s">
         <v>70</v>
@@ -3253,10 +3218,10 @@
         <v>89</v>
       </c>
       <c r="H13" t="s">
+        <v>231</v>
+      </c>
+      <c r="I13" t="s">
         <v>232</v>
-      </c>
-      <c r="I13" t="s">
-        <v>233</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -3271,26 +3236,26 @@
         <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
+        <v>234</v>
+      </c>
+      <c r="F14" t="s">
         <v>235</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>236</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>237</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>238</v>
-      </c>
-      <c r="I14" t="s">
-        <v>239</v>
       </c>
       <c r="J14"/>
       <c r="K14"/>
@@ -3305,22 +3270,22 @@
         <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C15" t="s">
         <v>93</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
+        <v>240</v>
+      </c>
+      <c r="F15" t="s">
         <v>241</v>
-      </c>
-      <c r="F15" t="s">
-        <v>242</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
@@ -3338,10 +3303,10 @@
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16" t="s">
+        <v>243</v>
+      </c>
+      <c r="F16" t="s">
         <v>244</v>
-      </c>
-      <c r="F16" t="s">
-        <v>245</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
@@ -3372,7 +3337,7 @@
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J17"/>
       <c r="K17"/>
@@ -3387,12 +3352,14 @@
         <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C18" t="s">
         <v>156</v>
       </c>
-      <c r="D18"/>
+      <c r="D18" t="s">
+        <v>246</v>
+      </c>
       <c r="E18" t="s">
         <v>247</v>
       </c>
@@ -3459,11 +3426,11 @@
         <v>252</v>
       </c>
       <c r="F20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I20" t="s">
         <v>253</v>
@@ -3629,10 +3596,10 @@
         <v>142</v>
       </c>
       <c r="B27"/>
-      <c r="C27" t="s">
+      <c r="C27"/>
+      <c r="D27" t="s">
         <v>262</v>
       </c>
-      <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
@@ -3653,10 +3620,10 @@
         <v>145</v>
       </c>
       <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28" t="s">
+      <c r="C28" t="s">
         <v>264</v>
       </c>
+      <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
@@ -3709,7 +3676,7 @@
       </c>
       <c r="G30"/>
       <c r="H30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I30" t="s">
         <v>155</v>
@@ -3916,7 +3883,9 @@
         <v>58</v>
       </c>
       <c r="E8"/>
-      <c r="F8"/>
+      <c r="F8" t="s">
+        <v>117</v>
+      </c>
       <c r="G8" t="s">
         <v>271</v>
       </c>
@@ -3942,8 +3911,12 @@
       <c r="F9" t="s">
         <v>15</v>
       </c>
-      <c r="G9"/>
-      <c r="H9"/>
+      <c r="G9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H9" t="s">
+        <v>277</v>
+      </c>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9">
@@ -3951,19 +3924,19 @@
         <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C10" t="s">
         <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E10" t="s">
         <v>247</v>
       </c>
       <c r="F10" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
@@ -3997,17 +3970,17 @@
         <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" t="s">
         <v>230</v>
-      </c>
-      <c r="D12" t="s">
-        <v>231</v>
       </c>
       <c r="E12"/>
       <c r="F12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -4027,7 +4000,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -4046,11 +4019,11 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -4058,26 +4031,22 @@
         <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C15" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
+        <v>234</v>
+      </c>
+      <c r="F15" t="s">
         <v>235</v>
       </c>
-      <c r="F15" t="s">
-        <v>236</v>
-      </c>
-      <c r="G15" t="s">
-        <v>284</v>
-      </c>
-      <c r="H15" t="s">
-        <v>285</v>
-      </c>
+      <c r="G15"/>
+      <c r="H15"/>
       <c r="I15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -4156,7 +4125,7 @@
         <v>292</v>
       </c>
       <c r="F19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G19"/>
       <c r="H19"/>
@@ -4212,7 +4181,7 @@
       </c>
       <c r="B22"/>
       <c r="C22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D22" t="s">
         <v>153</v>
@@ -4365,7 +4334,7 @@
         <v>125</v>
       </c>
       <c r="H30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I30" t="s">
         <v>200</v>
@@ -4538,10 +4507,10 @@
         <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>170</v>
+        <v>310</v>
       </c>
       <c r="D7" t="s">
-        <v>310</v>
+        <v>171</v>
       </c>
       <c r="E7" t="s">
         <v>86</v>
@@ -4560,13 +4529,17 @@
       <c r="B8" t="s">
         <v>311</v>
       </c>
-      <c r="C8"/>
-      <c r="D8"/>
+      <c r="C8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
       <c r="E8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F8" t="s">
-        <v>312</v>
+        <v>97</v>
       </c>
       <c r="G8"/>
       <c r="H8" t="s">
@@ -4597,25 +4570,19 @@
       <c r="A10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10"/>
+      <c r="C10" t="s">
         <v>314</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>315</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10"/>
+      <c r="F10" t="s">
         <v>316</v>
       </c>
-      <c r="E10" t="s">
-        <v>317</v>
-      </c>
-      <c r="F10" t="s">
-        <v>318</v>
-      </c>
       <c r="G10"/>
-      <c r="H10" t="s">
-        <v>319</v>
-      </c>
+      <c r="H10"/>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
@@ -4623,21 +4590,21 @@
         <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C11" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
         <v>104</v>
       </c>
       <c r="F11" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="I11"/>
     </row>
@@ -4645,14 +4612,16 @@
       <c r="A12" t="s">
         <v>60</v>
       </c>
-      <c r="B12"/>
+      <c r="B12" t="s">
+        <v>320</v>
+      </c>
       <c r="C12"/>
-      <c r="D12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12"/>
+      <c r="D12"/>
+      <c r="E12" t="s">
+        <v>321</v>
+      </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>322</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -4675,9 +4644,7 @@
       </c>
       <c r="G13"/>
       <c r="H13"/>
-      <c r="I13" t="s">
-        <v>248</v>
-      </c>
+      <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
@@ -4703,21 +4670,21 @@
         <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C15" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
         <v>130</v>
       </c>
       <c r="F15" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="I15"/>
     </row>
@@ -4731,10 +4698,10 @@
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
@@ -4778,7 +4745,7 @@
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I18" t="s">
         <v>329</v>
@@ -4794,7 +4761,7 @@
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F19" t="s">
         <v>333</v>

</xml_diff>

<commit_message>
Remove starting un-necessary sheets itself in fix.php
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -1395,14 +1395,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="64" zoomScaleNormal="64" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="14.42578125" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -2082,6 +2082,17 @@
       <c r="I31" t="s">
         <v>158</v>
       </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Update timetable to V1.5
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -77,6 +77,9 @@
     <t>HCI-A  Behraj</t>
   </si>
   <si>
+    <t xml:space="preserve">ITC-G                                          M. Shahzad                                                                         </t>
+  </si>
+  <si>
     <t>Wp-GR1                             Dr. Farooque</t>
   </si>
   <si>
@@ -197,9 +200,6 @@
     <t>PIT-B  Khalid</t>
   </si>
   <si>
-    <t xml:space="preserve">ITC-G                                          M. Shahzad                                                                         </t>
-  </si>
-  <si>
     <t>PIT-D  Khalid</t>
   </si>
   <si>
@@ -431,51 +431,51 @@
     <t>Wp-GR2                              Dr. Farooque</t>
   </si>
   <si>
+    <t>DB-Lab C              Basit ali</t>
+  </si>
+  <si>
+    <t>Lab-3</t>
+  </si>
+  <si>
+    <t>DB-Lab E              Mahrukh</t>
+  </si>
+  <si>
+    <t>OS Lab- Gr3                  Ali shah</t>
+  </si>
+  <si>
+    <t>Lab-4</t>
+  </si>
+  <si>
+    <t>OOAD-Lab B      Majid</t>
+  </si>
+  <si>
+    <t>DB-Lab D             Ammara</t>
+  </si>
+  <si>
+    <t>EE Lab-8</t>
+  </si>
+  <si>
+    <t>OOAD-Lab F      Awais</t>
+  </si>
+  <si>
+    <t>EE Lab 9</t>
+  </si>
+  <si>
+    <t>COAL Lab-F                  Sehrish</t>
+  </si>
+  <si>
+    <t>EE MPI Lab</t>
+  </si>
+  <si>
+    <t>DLD Lab-Gr1                 Nadeem</t>
+  </si>
+  <si>
+    <t>EE Lab 10</t>
+  </si>
+  <si>
     <t>COAL Lab-C              Zain</t>
   </si>
   <si>
-    <t>Lab-3</t>
-  </si>
-  <si>
-    <t>DB-Lab E              Mahrukh</t>
-  </si>
-  <si>
-    <t>OS Lab- Gr3                  Ali shah</t>
-  </si>
-  <si>
-    <t>Lab-4</t>
-  </si>
-  <si>
-    <t>OOAD-Lab B      Majid</t>
-  </si>
-  <si>
-    <t>EE Lab-8</t>
-  </si>
-  <si>
-    <t>OOAD-Lab F      Awais</t>
-  </si>
-  <si>
-    <t>DB-Lab D             Ammara</t>
-  </si>
-  <si>
-    <t>EE Lab 9</t>
-  </si>
-  <si>
-    <t>COAL Lab-F                  Sehrish</t>
-  </si>
-  <si>
-    <t>EE MPI Lab</t>
-  </si>
-  <si>
-    <t>DLD Lab-Gr1                 Nadeem</t>
-  </si>
-  <si>
-    <t>EE Lab 10</t>
-  </si>
-  <si>
-    <t>DB-Lab C              Basit ali</t>
-  </si>
-  <si>
     <t>LLC</t>
   </si>
   <si>
@@ -503,78 +503,78 @@
     <t>TUESDAY</t>
   </si>
   <si>
+    <t>DB-A                            Tania</t>
+  </si>
+  <si>
+    <t>NP-GR1                 Shahbaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITC-D                                  Javeria                                              </t>
+  </si>
+  <si>
+    <t>COAL-D                Mahwish</t>
+  </si>
+  <si>
+    <t>DLD-Gr1                      Bahraj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discrete-B                              Dr. Fahad Samad     </t>
+  </si>
+  <si>
+    <t>Discrete-D               Dr. Fahad Samad</t>
+  </si>
+  <si>
+    <t>COAL-E                               Danish</t>
+  </si>
+  <si>
+    <t>SE-GR1                 Abdul rehman</t>
+  </si>
+  <si>
+    <t>SE-GR2                                 Abdul rehman</t>
+  </si>
+  <si>
+    <t>Discrete-H                              Shoaib</t>
+  </si>
+  <si>
+    <t>Discrete-G                              Shoaib</t>
+  </si>
+  <si>
+    <t>Discrete-A                                  Shoaib</t>
+  </si>
+  <si>
+    <t>NS-GR1                                       Dr. Sufian</t>
+  </si>
+  <si>
+    <t>NS-GR1                                          Dr. Sufian</t>
+  </si>
+  <si>
+    <t>BD-GR1                                 Dr. Jawwad</t>
+  </si>
+  <si>
+    <t>DB-B     Tania</t>
+  </si>
+  <si>
+    <t>Discrete-C                               Nouman Durrani</t>
+  </si>
+  <si>
+    <t>Wp-GR2                        Dr. Farooque</t>
+  </si>
+  <si>
+    <t>Wp-GR1                              Dr. Farooque</t>
+  </si>
+  <si>
+    <t>BioInfo-GR1                 M. Shahzad</t>
+  </si>
+  <si>
+    <t>Wp-GR2                                       Dr. Farooque</t>
+  </si>
+  <si>
     <t>Discrete-E               Nouman Durrani</t>
   </si>
   <si>
     <t>Discrete-F                         Nouman Durrani</t>
   </si>
   <si>
-    <t>Discrete-C                               Nouman Durrani</t>
-  </si>
-  <si>
-    <t>DB-A                            Tania</t>
-  </si>
-  <si>
-    <t>COAL-E                               Danish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITC-D                                  Javeria                                              </t>
-  </si>
-  <si>
-    <t>COAL-D                Mahwish</t>
-  </si>
-  <si>
-    <t>DLD-Gr1                      Bahraj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discrete-B                              Dr. Fahad Samad     </t>
-  </si>
-  <si>
-    <t>Discrete-D               Dr. Fahad Samad</t>
-  </si>
-  <si>
-    <t>SE-GR1                 Abdul rehman</t>
-  </si>
-  <si>
-    <t>SE-GR2                                 Abdul rehman</t>
-  </si>
-  <si>
-    <t>Discrete-H                              Shoaib</t>
-  </si>
-  <si>
-    <t>Discrete-G                              Shoaib</t>
-  </si>
-  <si>
-    <t>Discrete-A                                  Shoaib</t>
-  </si>
-  <si>
-    <t>NS-GR1                                       Dr. Sufian</t>
-  </si>
-  <si>
-    <t>NS-GR1                                          Dr. Sufian</t>
-  </si>
-  <si>
-    <t>BD-GR1                                 Dr. Jawwad</t>
-  </si>
-  <si>
-    <t>DB-B     Tania</t>
-  </si>
-  <si>
-    <t>Wp-GR2                        Dr. Farooque</t>
-  </si>
-  <si>
-    <t>Wp-GR1                              Dr. Farooque</t>
-  </si>
-  <si>
-    <t>BioInfo-GR1                 M. Shahzad</t>
-  </si>
-  <si>
-    <t>Wp-GR2                                       Dr. Farooque</t>
-  </si>
-  <si>
-    <t>NP-GR1                 Shahbaz</t>
-  </si>
-  <si>
     <t>IPM-GR1                                       Ubaid</t>
   </si>
   <si>
@@ -641,30 +641,30 @@
     <t>ENG-G2                                                    Faiza Mumtaz</t>
   </si>
   <si>
+    <t>DB-Lab F              Ammara</t>
+  </si>
+  <si>
+    <t>OOAD-Lab C      Nadeem</t>
+  </si>
+  <si>
+    <t>OS Lab- Gr2                  Ali shah</t>
+  </si>
+  <si>
+    <t>BioInfo-GR1                             M. Shahzad</t>
+  </si>
+  <si>
+    <t>DB-Lab A              Basit ali</t>
+  </si>
+  <si>
+    <t>COAL Lab-B               Sehrish</t>
+  </si>
+  <si>
+    <t>DB-Lab B             Mahrukh</t>
+  </si>
+  <si>
     <t>COAL Lab-A                Zain</t>
   </si>
   <si>
-    <t>OOAD-Lab C      Nadeem</t>
-  </si>
-  <si>
-    <t>OS Lab- Gr2                  Ali shah</t>
-  </si>
-  <si>
-    <t>BioInfo-GR1                             M. Shahzad</t>
-  </si>
-  <si>
-    <t>DB-Lab A              Basit ali</t>
-  </si>
-  <si>
-    <t>COAL Lab-B               Sehrish</t>
-  </si>
-  <si>
-    <t>DB-Lab B             Mahrukh</t>
-  </si>
-  <si>
-    <t>DB-Lab F              Ammara</t>
-  </si>
-  <si>
     <t>COAL Lab-G                Sumayya</t>
   </si>
   <si>
@@ -794,6 +794,9 @@
     <t>Socio-Gr1      Sumaira</t>
   </si>
   <si>
+    <t>DB-Lab G              Ammara</t>
+  </si>
+  <si>
     <t xml:space="preserve">CP Lab-C=         Rahemeen &amp; Mahrukh      </t>
   </si>
   <si>
@@ -813,9 +816,6 @@
   </si>
   <si>
     <t>DS-Lab E                      Faizan</t>
-  </si>
-  <si>
-    <t>DB-Lab G              Ammara</t>
   </si>
   <si>
     <t>ITC-Lab B        Farah &amp; Mubashra</t>
@@ -1508,157 +1508,157 @@
       <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="H5"/>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" t="s">
         <v>58</v>
       </c>
+      <c r="H11"/>
       <c r="I11" t="s">
         <v>59</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>135</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" t="s">
         <v>136</v>
@@ -1990,24 +1990,24 @@
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
-      <c r="G26"/>
+      <c r="G26" t="s">
+        <v>142</v>
+      </c>
       <c r="H26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
-      <c r="G27" t="s">
-        <v>144</v>
-      </c>
+      <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
     </row>
@@ -2221,19 +2221,13 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>160</v>
-      </c>
+      <c r="B5"/>
       <c r="C5" t="s">
         <v>88</v>
       </c>
-      <c r="D5" t="s">
-        <v>161</v>
-      </c>
+      <c r="D5"/>
       <c r="E5"/>
-      <c r="F5" t="s">
-        <v>162</v>
-      </c>
+      <c r="F5"/>
       <c r="G5" t="s">
         <v>89</v>
       </c>
@@ -2244,18 +2238,18 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
         <v>49</v>
-      </c>
-      <c r="F6" t="s">
-        <v>48</v>
       </c>
       <c r="G6"/>
       <c r="H6" t="s">
@@ -2267,70 +2261,70 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7"/>
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H7"/>
-      <c r="I7" t="s">
-        <v>164</v>
-      </c>
+      <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G9" t="s">
         <v>98</v>
@@ -2338,30 +2332,32 @@
       <c r="H9" t="s">
         <v>97</v>
       </c>
-      <c r="I9"/>
+      <c r="I9" t="s">
+        <v>167</v>
+      </c>
       <c r="J9"/>
       <c r="K9"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" t="s">
         <v>170</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>171</v>
-      </c>
-      <c r="D10" t="s">
-        <v>172</v>
-      </c>
-      <c r="E10" t="s">
-        <v>173</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -2369,7 +2365,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
@@ -2378,10 +2374,10 @@
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
@@ -2391,24 +2387,26 @@
         <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>62</v>
       </c>
       <c r="D12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" t="s">
         <v>177</v>
       </c>
-      <c r="E12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12"/>
       <c r="G12"/>
       <c r="H12" t="s">
         <v>69</v>
       </c>
       <c r="I12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J12"/>
       <c r="K12"/>
@@ -2418,18 +2416,18 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" t="s">
         <v>179</v>
-      </c>
-      <c r="C13" t="s">
-        <v>180</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -2440,7 +2438,9 @@
       <c r="A14" t="s">
         <v>74</v>
       </c>
-      <c r="B14"/>
+      <c r="B14" t="s">
+        <v>182</v>
+      </c>
       <c r="C14"/>
       <c r="D14" t="s">
         <v>183</v>
@@ -2456,7 +2456,7 @@
         <v>186</v>
       </c>
       <c r="I14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J14"/>
       <c r="K14"/>
@@ -2492,17 +2492,17 @@
         <v>191</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
         <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
@@ -2743,7 +2743,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B27" t="s">
         <v>213</v>
@@ -2845,7 +2845,7 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" zoomScale="60" zoomScaleNormal="60" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="62" zoomScaleNormal="62" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -2973,17 +2973,17 @@
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G5"/>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2996,27 +2996,27 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J6"/>
       <c r="K6"/>
@@ -3028,7 +3028,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>219</v>
@@ -3039,7 +3039,7 @@
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G7" t="s">
         <v>220</v>
@@ -3058,20 +3058,20 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E8"/>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
         <v>84</v>
@@ -3090,7 +3090,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
         <v>221</v>
@@ -3106,10 +3106,10 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
         <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>25</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -3122,25 +3122,25 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
         <v>224</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
         <v>225</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H10"/>
       <c r="I10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>226</v>
@@ -3219,7 +3219,7 @@
         <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E13" t="s">
         <v>70</v>
@@ -3324,7 +3324,7 @@
         <v>186</v>
       </c>
       <c r="I16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -3537,12 +3537,14 @@
         <v>133</v>
       </c>
       <c r="B24"/>
-      <c r="C24"/>
+      <c r="C24" t="s">
+        <v>257</v>
+      </c>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -3561,12 +3563,12 @@
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -3585,12 +3587,12 @@
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -3604,17 +3606,17 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -3631,9 +3633,7 @@
         <v>145</v>
       </c>
       <c r="B28"/>
-      <c r="C28" t="s">
-        <v>264</v>
-      </c>
+      <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
@@ -3842,13 +3842,13 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
@@ -3860,12 +3860,12 @@
         <v>59</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>82</v>
@@ -3884,14 +3884,14 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="E8"/>
       <c r="F8" t="s">
@@ -3907,7 +3907,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
         <v>273</v>
@@ -3932,13 +3932,13 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
         <v>278</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
         <v>279</v>
@@ -3951,15 +3951,15 @@
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
@@ -4234,7 +4234,7 @@
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
@@ -4283,7 +4283,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B27" t="s">
         <v>304</v>
@@ -4493,7 +4493,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>196</v>
@@ -4512,7 +4512,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>82</v>
@@ -4521,7 +4521,7 @@
         <v>310</v>
       </c>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E7" t="s">
         <v>86</v>
@@ -4535,7 +4535,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>311</v>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
         <v>72</v>
@@ -4579,7 +4579,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
@@ -4598,7 +4598,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>317</v>
@@ -4914,7 +4914,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B27" t="s">
         <v>344</v>

</xml_diff>

<commit_message>
Update timetable to v1.5 fake :D
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -15,6 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area_0" localSheetId="0">'Monday'!$A$1:$I$31</definedName>
+    <definedName name="_xlnm.Print_Area_0_0" localSheetId="0">'Monday'!$A$1:$I$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Monday'!$A$1:$I$31</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -780,9 +781,6 @@
     <t xml:space="preserve">ME-GR1   Micheal    </t>
   </si>
   <si>
-    <t xml:space="preserve">Prob &amp; Stats-GR1   Abdul Basit </t>
-  </si>
-  <si>
     <t>CAL I-A                                      Dr. Sadaqat</t>
   </si>
   <si>
@@ -796,6 +794,9 @@
   </si>
   <si>
     <t>Socio-GR1      Sumaira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prob &amp; Stats-GR1   Abdul Basit </t>
   </si>
   <si>
     <t>DB Lab-G              Ammara</t>
@@ -1401,9 +1402,9 @@
   </sheetPr>
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="64" zoomScaleNormal="64" showGridLines="true" showRowColHeaders="1">
+      <pane ySplit="21" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33576,7 +33577,7 @@
   </sheetPr>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="64" zoomScaleNormal="64" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -33826,11 +33827,17 @@
         <v>57</v>
       </c>
       <c r="B11"/>
-      <c r="C11"/>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
       <c r="D11"/>
-      <c r="E11"/>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
       <c r="F11"/>
-      <c r="G11"/>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" t="s">
         <v>174</v>
       </c>
@@ -33949,19 +33956,13 @@
       <c r="B16" t="s">
         <v>192</v>
       </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
+      <c r="C16"/>
       <c r="D16" t="s">
         <v>97</v>
       </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
+      <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
+      <c r="G16"/>
       <c r="H16"/>
       <c r="I16" t="s">
         <v>86</v>
@@ -34303,9 +34304,9 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="64" zoomScaleNormal="64" showGridLines="true" showRowColHeaders="1">
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34417,7 +34418,9 @@
       <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="C5"/>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
       <c r="D5" t="s">
         <v>58</v>
       </c>
@@ -34427,7 +34430,9 @@
       <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="G5"/>
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
       <c r="H5" t="s">
         <v>43</v>
       </c>
@@ -34637,9 +34642,7 @@
       <c r="B13" t="s">
         <v>74</v>
       </c>
-      <c r="C13" t="s">
-        <v>89</v>
-      </c>
+      <c r="C13"/>
       <c r="D13" t="s">
         <v>165</v>
       </c>
@@ -34647,9 +34650,7 @@
         <v>71</v>
       </c>
       <c r="F13"/>
-      <c r="G13" t="s">
-        <v>90</v>
-      </c>
+      <c r="G13"/>
       <c r="H13" t="s">
         <v>232</v>
       </c>
@@ -34827,15 +34828,13 @@
       <c r="A20" t="s">
         <v>116</v>
       </c>
-      <c r="B20" t="s">
-        <v>252</v>
-      </c>
+      <c r="B20"/>
       <c r="C20" t="s">
         <v>117</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F20" t="s">
         <v>203</v>
@@ -34845,7 +34844,7 @@
         <v>205</v>
       </c>
       <c r="I20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
@@ -34864,15 +34863,15 @@
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
+        <v>254</v>
+      </c>
+      <c r="F21" t="s">
         <v>255</v>
-      </c>
-      <c r="F21" t="s">
-        <v>256</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
@@ -34925,7 +34924,9 @@
       <c r="A24" t="s">
         <v>134</v>
       </c>
-      <c r="B24"/>
+      <c r="B24" t="s">
+        <v>257</v>
+      </c>
       <c r="C24" t="s">
         <v>258</v>
       </c>
@@ -35092,9 +35093,9 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="64" zoomScaleNormal="64" showGridLines="true" showRowColHeaders="1">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35462,10 +35463,10 @@
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="I17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -35524,7 +35525,7 @@
         <v>132</v>
       </c>
       <c r="E20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F20" t="s">
         <v>295</v>
@@ -35601,9 +35602,7 @@
       </c>
       <c r="C24"/>
       <c r="D24"/>
-      <c r="E24" t="s">
-        <v>162</v>
-      </c>
+      <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="s">
         <v>299</v>
@@ -35641,7 +35640,9 @@
       </c>
       <c r="C26"/>
       <c r="D26"/>
-      <c r="E26"/>
+      <c r="E26" t="s">
+        <v>162</v>
+      </c>
       <c r="F26"/>
       <c r="G26" t="s">
         <v>304</v>
@@ -35743,9 +35744,9 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="17" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="64" zoomScaleNormal="64" showGridLines="true" showRowColHeaders="1">
+      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36163,10 +36164,10 @@
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>

</xml_diff>

<commit_message>
Update TT to v5.0
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="383">
   <si>
     <t>MONDAY</t>
   </si>
@@ -251,132 +251,132 @@
     <t>R109</t>
   </si>
   <si>
+    <t>DS-A                         Zeshan</t>
+  </si>
+  <si>
+    <t>Eng Comp. A2                                                   Faiza</t>
+  </si>
+  <si>
+    <t>DS-C                     Zeshan</t>
+  </si>
+  <si>
+    <t>DS-B                           Zeshan</t>
+  </si>
+  <si>
+    <t>Eng Comp. E2                                                   Faiza</t>
+  </si>
+  <si>
+    <t>HCI-GR1                               Bahraj</t>
+  </si>
+  <si>
+    <t>HCI-GR2                               Bahraj</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>TOA-F                             Subhash</t>
+  </si>
+  <si>
+    <t>OS-B                        Nausheen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-C                               Dr Rauf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-G                               Dr Rauf </t>
+  </si>
+  <si>
+    <t>COAL-GR2            Danish</t>
+  </si>
+  <si>
+    <t>COAL-GR1            Danish</t>
+  </si>
+  <si>
+    <t>AL-GR1            Shahzad Sheikh</t>
+  </si>
+  <si>
+    <t>CR-3 EE</t>
+  </si>
+  <si>
+    <t>CP-B                             Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>CP-D                             Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>BE-GR1                     Javaid Qureshi</t>
+  </si>
+  <si>
+    <t>CP-F                             Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>Eng Comp. C2                                                   Faiza</t>
+  </si>
+  <si>
+    <t>CR-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA-GR2             Ahsan                        </t>
+  </si>
+  <si>
+    <t>CAL II-A                  Fareeha</t>
+  </si>
+  <si>
+    <t>CAL II-C                  Fareeha</t>
+  </si>
+  <si>
+    <t>CAL II-E                  Fareeha</t>
+  </si>
+  <si>
+    <t>IRS-G                                            Shahzad</t>
+  </si>
+  <si>
+    <t>SE-B                            Ahsan</t>
+  </si>
+  <si>
+    <t>CR-7</t>
+  </si>
+  <si>
+    <t>TBW-F                               Nazia</t>
+  </si>
+  <si>
+    <t>TBW-A                               Nazia</t>
+  </si>
+  <si>
+    <t>TBW-C                               Nazia</t>
+  </si>
+  <si>
+    <t>CR-10</t>
+  </si>
+  <si>
+    <t>DLD-G                      Rabia</t>
+  </si>
+  <si>
+    <t>DLD-A                      Rabia</t>
+  </si>
+  <si>
+    <t>TBW-E                               Sameera</t>
+  </si>
+  <si>
+    <t>TBW-B                               Sameera</t>
+  </si>
+  <si>
+    <t>DLD-C                      Rabia</t>
+  </si>
+  <si>
+    <t>CR-16</t>
+  </si>
+  <si>
     <t>Prob-A                    Osama</t>
   </si>
   <si>
-    <t>DS-A                         Zeshan</t>
-  </si>
-  <si>
-    <t>Eng Comp. A2                                                   Faiza</t>
-  </si>
-  <si>
     <t>Prob-C                                      Osama</t>
   </si>
   <si>
     <t>Prob-E                      Osama</t>
   </si>
   <si>
-    <t>Eng Comp. E2                                                   Faiza</t>
-  </si>
-  <si>
-    <t>HCI-GR1                               Bahraj</t>
-  </si>
-  <si>
-    <t>HCI-GR2                               Bahraj</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>TOA-F                             Subhash</t>
-  </si>
-  <si>
-    <t>OS-B                        Nausheen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-C                               Dr Rauf </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-G                               Dr Rauf </t>
-  </si>
-  <si>
-    <t>COAL-GR2            Danish</t>
-  </si>
-  <si>
-    <t>COAL-GR1            Danish</t>
-  </si>
-  <si>
-    <t>AL-GR1            Shahzad Sheikh</t>
-  </si>
-  <si>
-    <t>CR-3 EE</t>
-  </si>
-  <si>
-    <t>CP-B                             Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>CP-D                             Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>BE-GR1                     Javaid Qureshi</t>
-  </si>
-  <si>
-    <t>CP-F                             Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>Eng Comp. C2                                                   Faiza</t>
-  </si>
-  <si>
-    <t>CR-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA-GR2             Ahsan                        </t>
-  </si>
-  <si>
-    <t>DS-C  Zeshan</t>
-  </si>
-  <si>
-    <t>DS-B                           Zeshan</t>
-  </si>
-  <si>
-    <t>IRS-G                                            Shahzad</t>
-  </si>
-  <si>
-    <t>SE-B                            Ahsan</t>
-  </si>
-  <si>
-    <t>CR-7</t>
-  </si>
-  <si>
-    <t>TBW-F                               Nazia</t>
-  </si>
-  <si>
-    <t>DLD-G                      Rabia</t>
-  </si>
-  <si>
-    <t>DLD-A                      Rabia</t>
-  </si>
-  <si>
-    <t>TBW-A                               Nazia</t>
-  </si>
-  <si>
-    <t>TBW-C                               Nazia</t>
-  </si>
-  <si>
-    <t>DLD-C                      Rabia</t>
-  </si>
-  <si>
-    <t>CR-10</t>
-  </si>
-  <si>
-    <t>CAL II-A                  Fareeha</t>
-  </si>
-  <si>
-    <t>CAL II-C                  Fareeha</t>
-  </si>
-  <si>
-    <t>TBW-E                               Sameera</t>
-  </si>
-  <si>
-    <t>TBW-B                               Sameera</t>
-  </si>
-  <si>
-    <t>CR-16</t>
-  </si>
-  <si>
-    <t>CAL II-E                  Fareeha</t>
-  </si>
-  <si>
     <t>TOA-C                                    Shaharbano</t>
   </si>
   <si>
@@ -530,13 +530,16 @@
     <t xml:space="preserve">AI-D                                                             Farrukh </t>
   </si>
   <si>
-    <t xml:space="preserve">AI-E                               Farrukh </t>
+    <t>SE-G                                                            Abdur Rehman</t>
   </si>
   <si>
     <t>DS-D                                   Abdul Aziz</t>
   </si>
   <si>
-    <t xml:space="preserve">AI-F                                                  Farrukh </t>
+    <t xml:space="preserve">AI-E                                                  Farrukh </t>
+  </si>
+  <si>
+    <t>SE-G                                                     Abdur Rehman</t>
   </si>
   <si>
     <t>OS-D                                     Tania</t>
@@ -569,9 +572,6 @@
     <t>TBW-G                                                 Sameera</t>
   </si>
   <si>
-    <t>SE-G                                                     Abdur Rehman</t>
-  </si>
-  <si>
     <t>CN-C                                            Shoaib</t>
   </si>
   <si>
@@ -659,6 +659,9 @@
     <t>LA-GR1                               Dr Fahad</t>
   </si>
   <si>
+    <t>Eng Comp. B1                                                   Hafza Yusra</t>
+  </si>
+  <si>
     <t>Prob-B                                                    Asma</t>
   </si>
   <si>
@@ -689,13 +692,16 @@
     <t>Prob-A                                      Osama</t>
   </si>
   <si>
+    <t>Psych-GR4                           Sumaira</t>
+  </si>
+  <si>
+    <t>Prob-E                                              Osama</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pst. E                                                        Kashif </t>
   </si>
   <si>
-    <t>Psych-GR4                           Sumaira</t>
-  </si>
-  <si>
-    <t>Prob-E                                              Osama</t>
+    <t xml:space="preserve">Pst. E                             Kashif </t>
   </si>
   <si>
     <t>OS-Lab A                                                                                                                        Ms. Summiyah</t>
@@ -734,9 +740,6 @@
     <t>DLD-Lab  D                                                                                                                                              M. Nadeem</t>
   </si>
   <si>
-    <t>Eng Comp. B1                                                   Hafza Yusra</t>
-  </si>
-  <si>
     <t>WEDNESDAY</t>
   </si>
   <si>
@@ -758,6 +761,9 @@
     <t>IPT -GR1                          Murtaza</t>
   </si>
   <si>
+    <t>SE-G                                                              Abdur Rehman</t>
+  </si>
+  <si>
     <t>CP-E                                                             Faiza</t>
   </si>
   <si>
@@ -767,6 +773,9 @@
     <t>Prob-G                                  Amjad</t>
   </si>
   <si>
+    <t>OS-D                                   Tania</t>
+  </si>
+  <si>
     <t>CN-E                                            Faraz</t>
   </si>
   <si>
@@ -776,9 +785,6 @@
     <t>OS-E                          Tania</t>
   </si>
   <si>
-    <t>OS-D                                   Tania</t>
-  </si>
-  <si>
     <t>AI-B                                                                      Ali Naqvi</t>
   </si>
   <si>
@@ -791,97 +797,97 @@
     <t>AI-B                                                        Ali Naqvi</t>
   </si>
   <si>
+    <t>OS-C                                 Nausheen</t>
+  </si>
+  <si>
+    <t>SE-E                                                           Rubab</t>
+  </si>
+  <si>
     <t>SE-A                                                             Rubab</t>
   </si>
   <si>
     <t>SE-C                          Rubab</t>
   </si>
   <si>
+    <t>RM-GR1                                 Shoaib</t>
+  </si>
+  <si>
+    <t>PIT-GR1                                                     Khalid</t>
+  </si>
+  <si>
+    <t>PIT-GR2                 Khalid</t>
+  </si>
+  <si>
+    <t>Dwh-GR1                                   Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>Dwh-GR2                                   Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>TOA-G                                         Shaharbano</t>
+  </si>
+  <si>
+    <t>IOT-GR2                                                                     Dr. Farooque</t>
+  </si>
+  <si>
+    <t>OS-A                                                Dr. Hasina</t>
+  </si>
+  <si>
+    <t>SE-B                                        Ahsan</t>
+  </si>
+  <si>
+    <t>TOA-E                                                 Shahzad</t>
+  </si>
+  <si>
+    <t>Discrete-GR1                                      Dr Jalal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discrete-GR2            Dr Jalal </t>
+  </si>
+  <si>
+    <t>TOA-A                                             Shahzad</t>
+  </si>
+  <si>
+    <t>IS -GR2                                   Abdul Rehman</t>
+  </si>
+  <si>
+    <t>IS-GR1                               Abdul rehman</t>
+  </si>
+  <si>
+    <t>IS -GR2                          Abdul Rehman</t>
+  </si>
+  <si>
+    <t>TOA-B                                               Subhash</t>
+  </si>
+  <si>
+    <t>TOA-D                                             Subhash</t>
+  </si>
+  <si>
+    <t>DS-A                    Zeshan</t>
+  </si>
+  <si>
+    <t>DS-B                                   Zeshan</t>
+  </si>
+  <si>
+    <t>TOA-F                                            Subhash</t>
+  </si>
+  <si>
+    <t>Prob-D                                                     Asma</t>
+  </si>
+  <si>
+    <t>LA-GR1                       Dr Fahad</t>
+  </si>
+  <si>
+    <t>OS-B                             Nausheen</t>
+  </si>
+  <si>
+    <t>Prob-B                                                                 Asma</t>
+  </si>
+  <si>
     <t>CP-B                                                                           Shoaib Rauf</t>
   </si>
   <si>
-    <t>OS-C                                 Nausheen</t>
-  </si>
-  <si>
-    <t>RM-GR1                                 Shoaib</t>
-  </si>
-  <si>
-    <t>PIT-GR1                                                     Khalid</t>
-  </si>
-  <si>
-    <t>PIT-GR2                 Khalid</t>
-  </si>
-  <si>
-    <t>Dwh-GR1                                   Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>Dwh-GR2                                   Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>TOA-G                                         Shaharbano</t>
-  </si>
-  <si>
-    <t>IOT-GR2                                                                     Dr. Farooque</t>
-  </si>
-  <si>
-    <t>OS-A                                                Dr. Hasina</t>
-  </si>
-  <si>
-    <t>SE-B                                        Ahsan</t>
-  </si>
-  <si>
-    <t>Discrete-GR1                                      Dr Jalal</t>
-  </si>
-  <si>
-    <t>IS -GR2                          Abdul Rehman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discrete-GR2            Dr Jalal </t>
-  </si>
-  <si>
-    <t>TOA-A                                             Shahzad</t>
-  </si>
-  <si>
-    <t>IS -GR2                                   Abdul Rehman</t>
-  </si>
-  <si>
-    <t>IS-GR1                               Abdul rehman</t>
-  </si>
-  <si>
-    <t>TOA-E                                                 Shahzad</t>
-  </si>
-  <si>
-    <t>TOA-B                                               Subhash</t>
-  </si>
-  <si>
-    <t>TOA-D                                             Subhash</t>
-  </si>
-  <si>
-    <t>DS-A                    Zeshan</t>
-  </si>
-  <si>
-    <t>DS-C                     Zeshan</t>
-  </si>
-  <si>
-    <t>DS-B                                   Zeshan</t>
-  </si>
-  <si>
-    <t>TOA-F                                            Subhash</t>
-  </si>
-  <si>
-    <t>Prob-D                                                     Asma</t>
-  </si>
-  <si>
-    <t>LA-GR1                       Dr Fahad</t>
-  </si>
-  <si>
-    <t>OS-B                             Nausheen</t>
-  </si>
-  <si>
-    <t>Prob-B                                                                 Asma</t>
-  </si>
-  <si>
-    <t>SE-E                                                           Rubab</t>
+    <t>CP-F                                             Shoaib Rauf</t>
   </si>
   <si>
     <t>Prob-E                                               Osama</t>
@@ -890,22 +896,22 @@
     <t>Prob-A                                                             Osama</t>
   </si>
   <si>
-    <t>SE-G                                                              Abdur Rehman</t>
+    <t>CN-F                                                          Faraz</t>
   </si>
   <si>
     <t>Pst. B                        Michael</t>
   </si>
   <si>
-    <t>CP-F                                             Shoaib Rauf</t>
-  </si>
-  <si>
     <t xml:space="preserve">CA-GR2                                                Ahsan                        </t>
   </si>
   <si>
+    <t xml:space="preserve">Pst. C                                                   Kashif </t>
+  </si>
+  <si>
     <t xml:space="preserve">Pst. A                                                        Kashif </t>
   </si>
   <si>
-    <t xml:space="preserve">Pst. E                             Kashif </t>
+    <t xml:space="preserve">Pst. D                                         Kashif </t>
   </si>
   <si>
     <t xml:space="preserve">Pst. D                                                    Kashif </t>
@@ -992,9 +998,6 @@
     <t>TOA-E                                           Shahzad</t>
   </si>
   <si>
-    <t>CN-F                                                          Faraz</t>
-  </si>
-  <si>
     <t>OS-A                                              Dr. Hasina</t>
   </si>
   <si>
@@ -1034,7 +1037,7 @@
     <t>DLD-A                                         Rabia</t>
   </si>
   <si>
-    <t>Pst. B Michael</t>
+    <t>Pst. B                      Michael</t>
   </si>
   <si>
     <t>Prob-C                                        Osama</t>
@@ -1055,9 +1058,6 @@
     <t>CM-GR1             Jameel</t>
   </si>
   <si>
-    <t xml:space="preserve">Pst. D                                         Kashif </t>
-  </si>
-  <si>
     <t xml:space="preserve">Pst. C                                          Kashif </t>
   </si>
   <si>
@@ -1067,15 +1067,15 @@
     <t>COAL-Lab GR1                                                                                             Zain</t>
   </si>
   <si>
+    <t>CP-Lab C1+C2                                                                                                                            Tooba &amp; Irfan</t>
+  </si>
+  <si>
+    <t>CP-Lab E1+E2                                                                                                       Mahrukh &amp; Maham</t>
+  </si>
+  <si>
     <t>ITC-Lab B B1+B2                                                                                             Rahemeen &amp; Majid</t>
   </si>
   <si>
-    <t>CP-Lab E1+E2                                                                                                       Mahrukh &amp; Maham</t>
-  </si>
-  <si>
-    <t>CP-Lab C1+C2                                                                                                                            Tooba &amp; Irfan</t>
-  </si>
-  <si>
     <t>DB-Lab GR1                                                                                                    Mubashyra</t>
   </si>
   <si>
@@ -1097,7 +1097,7 @@
     <t xml:space="preserve">AI-C                                            Dr Rauf </t>
   </si>
   <si>
-    <t>JUMMA PRAYER</t>
+    <t>J              UMM           A                                                                                                                                                       P                             R                         A                           Y                           E          R</t>
   </si>
   <si>
     <t>CN-F                                            Faraz</t>
@@ -1106,18 +1106,15 @@
     <t xml:space="preserve">AI-E                                               Farrukh </t>
   </si>
   <si>
+    <t>SE-B                                              Ahsan</t>
+  </si>
+  <si>
     <t xml:space="preserve">AI-D                                               Farrukh </t>
   </si>
   <si>
-    <t>SE-B                                              Ahsan</t>
-  </si>
-  <si>
     <t>IS -GR2                          Abdul rehman</t>
   </si>
   <si>
-    <t>SE-G                                                            Abdur Rehman</t>
-  </si>
-  <si>
     <t>SE-C                                          Rubab</t>
   </si>
   <si>
@@ -1130,19 +1127,16 @@
     <t>NM-GR1             Dr Khusro</t>
   </si>
   <si>
+    <t>Pst. B                                            Michael</t>
+  </si>
+  <si>
+    <t>Prob-G                                          Amjad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pst. C                          Kashif </t>
+  </si>
+  <si>
     <t xml:space="preserve">Pst. A                                           Kashif </t>
-  </si>
-  <si>
-    <t>Prob-G                                          Amjad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pst. C                          Kashif </t>
-  </si>
-  <si>
-    <t>Pst. B                                            Michael</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pst. C                                                   Kashif </t>
   </si>
   <si>
     <t xml:space="preserve">Pst. D                                          Kashif </t>
@@ -1898,29 +1892,27 @@
       <c r="A13" t="s">
         <v>75</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13"/>
+      <c r="C13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>77</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>78</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>79</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>80</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>81</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>82</v>
-      </c>
-      <c r="I13" t="s">
-        <v>83</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -1931,29 +1923,29 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
         <v>84</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>85</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>86</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>87</v>
-      </c>
-      <c r="E14" t="s">
-        <v>88</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" t="s">
         <v>89</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>90</v>
-      </c>
-      <c r="I14" t="s">
-        <v>91</v>
       </c>
       <c r="J14"/>
       <c r="K14"/>
@@ -1964,27 +1956,27 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s">
         <v>92</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>93</v>
-      </c>
-      <c r="C15" t="s">
-        <v>94</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" t="s">
         <v>96</v>
       </c>
-      <c r="H15" t="s">
-        <v>97</v>
-      </c>
       <c r="I15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
@@ -1995,16 +1987,18 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" t="s">
         <v>98</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>99</v>
       </c>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16" t="s">
+      <c r="D16" t="s">
         <v>100</v>
       </c>
+      <c r="E16"/>
       <c r="F16" t="s">
         <v>101</v>
       </c>
@@ -2030,22 +2024,16 @@
         <v>105</v>
       </c>
       <c r="C17"/>
-      <c r="D17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" t="s">
-        <v>107</v>
-      </c>
+      <c r="D17"/>
+      <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H17" t="s">
-        <v>109</v>
-      </c>
-      <c r="I17" t="s">
-        <v>110</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
@@ -2055,24 +2043,26 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" t="s">
         <v>111</v>
-      </c>
-      <c r="B18"/>
-      <c r="C18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E18"/>
-      <c r="F18" t="s">
-        <v>114</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>115</v>
-      </c>
-      <c r="I18"/>
+        <v>112</v>
+      </c>
+      <c r="I18" t="s">
+        <v>113</v>
+      </c>
       <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
@@ -2082,12 +2072,16 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19"/>
+        <v>114</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
       <c r="C19"/>
       <c r="D19"/>
-      <c r="E19"/>
+      <c r="E19" t="s">
+        <v>116</v>
+      </c>
       <c r="F19" t="s">
         <v>117</v>
       </c>
@@ -2582,16 +2576,20 @@
         <v>168</v>
       </c>
       <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
         <v>169</v>
       </c>
-      <c r="F6"/>
       <c r="G6" t="s">
         <v>170</v>
       </c>
       <c r="H6" t="s">
         <v>171</v>
       </c>
-      <c r="I6"/>
+      <c r="I6" t="s">
+        <v>172</v>
+      </c>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -2607,22 +2605,20 @@
         <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>172</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="F7"/>
       <c r="G7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -2636,17 +2632,17 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H8" t="s">
         <v>138</v>
@@ -2665,27 +2661,25 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H9" t="s">
-        <v>181</v>
-      </c>
-      <c r="I9" t="s">
         <v>182</v>
       </c>
+      <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
@@ -2733,10 +2727,10 @@
         <v>188</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
         <v>189</v>
@@ -2770,7 +2764,7 @@
         <v>194</v>
       </c>
       <c r="E12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F12" t="s">
         <v>195</v>
@@ -2805,7 +2799,9 @@
       </c>
       <c r="E13"/>
       <c r="F13"/>
-      <c r="G13"/>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
       <c r="H13" t="s">
         <v>201</v>
       </c>
@@ -2820,17 +2816,17 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
         <v>203</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" t="s">
         <v>89</v>
-      </c>
-      <c r="E14" t="s">
-        <v>90</v>
       </c>
       <c r="F14" t="s">
         <v>204</v>
@@ -2848,7 +2844,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
         <v>137</v>
@@ -2876,23 +2872,23 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16"/>
       <c r="C16" t="s">
         <v>209</v>
       </c>
       <c r="D16" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="G16" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="H16" t="s">
         <v>210</v>
@@ -2916,8 +2912,12 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
+      <c r="H17" t="s">
+        <v>212</v>
+      </c>
+      <c r="I17" t="s">
+        <v>34</v>
+      </c>
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
@@ -2926,27 +2926,27 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F18" t="s">
         <v>130</v>
       </c>
       <c r="G18" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H18" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I18" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J18"/>
       <c r="K18"/>
@@ -2956,26 +2956,26 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D19" t="s">
         <v>134</v>
       </c>
       <c r="E19"/>
       <c r="F19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
@@ -2989,21 +2989,19 @@
         <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
         <v>123</v>
       </c>
       <c r="F20" t="s">
-        <v>221</v>
-      </c>
-      <c r="G20" t="s">
         <v>222</v>
       </c>
+      <c r="G20"/>
       <c r="H20" t="s">
         <v>223</v>
       </c>
@@ -3043,8 +3041,12 @@
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
+      <c r="G22" t="s">
+        <v>225</v>
+      </c>
+      <c r="H22" t="s">
+        <v>226</v>
+      </c>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -3075,7 +3077,7 @@
         <v>140</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
@@ -3097,19 +3099,19 @@
         <v>145</v>
       </c>
       <c r="B25" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C25" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D25" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E25" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F25" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G25"/>
       <c r="H25"/>
@@ -3125,7 +3127,7 @@
         <v>147</v>
       </c>
       <c r="B26" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -3145,13 +3147,13 @@
         <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G27"/>
       <c r="H27"/>
@@ -3167,7 +3169,7 @@
         <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -3187,7 +3189,7 @@
         <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -3208,13 +3210,13 @@
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
@@ -3236,9 +3238,7 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31" t="s">
-        <v>237</v>
-      </c>
+      <c r="H31"/>
       <c r="I31" t="s">
         <v>162</v>
       </c>
@@ -3272,7 +3272,7 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" zoomScale="70" zoomScaleNormal="70" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="60" zoomScaleNormal="60" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -3281,7 +3281,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3368,24 +3368,24 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3399,24 +3399,26 @@
         <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H6"/>
-      <c r="I6"/>
+      <c r="I6" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -3428,10 +3430,10 @@
         <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="G7" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="H7" t="s">
         <v>38</v>
@@ -3446,20 +3448,18 @@
         <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="D8" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E8" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F8" t="s">
-        <v>250</v>
-      </c>
-      <c r="G8" t="s">
-        <v>251</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
     </row>
@@ -3468,22 +3468,22 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F9" t="s">
-        <v>256</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -3493,11 +3493,9 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C10" t="s">
-        <v>94</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="C10"/>
       <c r="D10" t="s">
         <v>183</v>
       </c>
@@ -3505,13 +3503,13 @@
         <v>184</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>260</v>
       </c>
       <c r="G10" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="H10" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="I10"/>
     </row>
@@ -3520,23 +3518,23 @@
         <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C11" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D11" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E11" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F11" t="s">
         <v>118</v>
       </c>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="I11"/>
     </row>
@@ -3545,32 +3543,38 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C12" t="s">
         <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E12" t="s">
         <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
+      <c r="H12" t="s">
+        <v>271</v>
+      </c>
+      <c r="I12" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>269</v>
-      </c>
-      <c r="C13"/>
+        <v>272</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
       <c r="D13" t="s">
         <v>70</v>
       </c>
@@ -3578,61 +3582,59 @@
         <v>71</v>
       </c>
       <c r="F13"/>
-      <c r="G13" t="s">
-        <v>270</v>
-      </c>
+      <c r="G13"/>
       <c r="H13" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E14" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14" t="s">
-        <v>275</v>
-      </c>
+      <c r="G14" t="s">
+        <v>277</v>
+      </c>
+      <c r="H14"/>
       <c r="I14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C15" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D15" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E15" t="s">
         <v>129</v>
       </c>
       <c r="F15" t="s">
-        <v>279</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H15" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I15" t="s">
         <v>132</v>
@@ -3640,26 +3642,26 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C16" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D16" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E16" t="s">
         <v>207</v>
       </c>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H16" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I16" t="s">
         <v>120</v>
@@ -3670,58 +3672,56 @@
         <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>286</v>
-      </c>
-      <c r="C17"/>
+        <v>287</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
       <c r="D17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17"/>
+        <v>116</v>
+      </c>
+      <c r="E17" t="s">
+        <v>288</v>
+      </c>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H17" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
-        <v>290</v>
-      </c>
-      <c r="E18" t="s">
-        <v>291</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="E18"/>
       <c r="F18" t="s">
         <v>125</v>
       </c>
-      <c r="G18" t="s">
-        <v>33</v>
-      </c>
+      <c r="G18"/>
       <c r="H18" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" t="s">
-        <v>126</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D19" t="s">
         <v>102</v>
@@ -3733,32 +3733,36 @@
         <v>124</v>
       </c>
       <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
+      <c r="H19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>121</v>
       </c>
       <c r="B20"/>
-      <c r="C20"/>
+      <c r="C20" t="s">
+        <v>294</v>
+      </c>
       <c r="D20" t="s">
-        <v>293</v>
-      </c>
-      <c r="E20" t="s">
-        <v>294</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="E20"/>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="G20" t="s">
-        <v>81</v>
+        <v>296</v>
       </c>
       <c r="H20" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="I20" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -3767,17 +3771,11 @@
       </c>
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21" t="s">
-        <v>203</v>
-      </c>
+      <c r="D21"/>
       <c r="E21"/>
-      <c r="F21" t="s">
-        <v>138</v>
-      </c>
+      <c r="F21"/>
       <c r="G21"/>
-      <c r="H21" t="s">
-        <v>134</v>
-      </c>
+      <c r="H21"/>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
@@ -3811,14 +3809,14 @@
         <v>140</v>
       </c>
       <c r="B24" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -3828,7 +3826,7 @@
         <v>145</v>
       </c>
       <c r="B25" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
@@ -3837,7 +3835,7 @@
         <v>37</v>
       </c>
       <c r="G25" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -3847,14 +3845,14 @@
         <v>147</v>
       </c>
       <c r="B26" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -3864,14 +3862,14 @@
         <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -3881,7 +3879,7 @@
         <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -3896,14 +3894,14 @@
         <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
@@ -3914,12 +3912,12 @@
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
@@ -3932,14 +3930,14 @@
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E31"/>
       <c r="F31" t="s">
         <v>162</v>
       </c>
       <c r="G31" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
@@ -3977,7 +3975,7 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -4084,22 +4082,22 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C5" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D5" t="s">
         <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="F5" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -4114,16 +4112,16 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C6" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D6" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E6" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="F6"/>
       <c r="G6"/>
@@ -4176,22 +4174,22 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
         <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>83</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="F9" t="s">
         <v>204</v>
       </c>
-      <c r="G9"/>
-      <c r="H9" t="s">
+      <c r="G9" t="s">
         <v>62</v>
       </c>
+      <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -4204,19 +4202,19 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C10" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F10" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -4232,23 +4230,21 @@
         <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C11" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D11" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E11" t="s">
         <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>249</v>
-      </c>
-      <c r="G11" t="s">
-        <v>323</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -4262,23 +4258,21 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C12" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D12" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F12" t="s">
-        <v>327</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="G12"/>
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12"/>
@@ -4292,12 +4286,14 @@
         <v>75</v>
       </c>
       <c r="B13"/>
-      <c r="C13"/>
+      <c r="C13" t="s">
+        <v>203</v>
+      </c>
       <c r="D13" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F13"/>
       <c r="G13"/>
@@ -4311,20 +4307,20 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>330</v>
-      </c>
-      <c r="E14" t="s">
-        <v>330</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="E14"/>
       <c r="F14" t="s">
+        <v>332</v>
+      </c>
+      <c r="G14" t="s">
         <v>331</v>
       </c>
-      <c r="G14"/>
       <c r="H14" t="s">
         <v>206</v>
       </c>
@@ -4337,7 +4333,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -4355,25 +4351,23 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16"/>
       <c r="C16" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="F16" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G16"/>
-      <c r="H16" t="s">
-        <v>237</v>
-      </c>
+      <c r="H16"/>
       <c r="I16" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -4386,14 +4380,14 @@
         <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C17" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F17" t="s">
         <v>210</v>
@@ -4402,9 +4396,7 @@
       <c r="H17" t="s">
         <v>209</v>
       </c>
-      <c r="I17" t="s">
-        <v>113</v>
-      </c>
+      <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
@@ -4413,13 +4405,13 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C18" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
@@ -4429,11 +4421,13 @@
         <v>137</v>
       </c>
       <c r="G18" t="s">
-        <v>110</v>
-      </c>
-      <c r="H18"/>
+        <v>113</v>
+      </c>
+      <c r="H18" t="s">
+        <v>207</v>
+      </c>
       <c r="I18" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="J18"/>
       <c r="K18"/>
@@ -4443,20 +4437,20 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
@@ -4476,25 +4470,23 @@
         <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C20" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D20" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E20"/>
       <c r="F20" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>216</v>
-      </c>
-      <c r="I20" t="s">
-        <v>207</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
@@ -4506,7 +4498,7 @@
         <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C21" t="s">
         <v>102</v>
@@ -4514,14 +4506,12 @@
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" t="s">
-        <v>344</v>
-      </c>
+      <c r="G21"/>
       <c r="H21" t="s">
         <v>345</v>
       </c>
       <c r="I21" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
@@ -4658,7 +4648,7 @@
         <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -4678,7 +4668,7 @@
         <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -4725,8 +4715,12 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
+      <c r="H31" t="s">
+        <v>212</v>
+      </c>
+      <c r="I31" t="s">
+        <v>33</v>
+      </c>
       <c r="J31"/>
       <c r="K31"/>
       <c r="L31"/>
@@ -4853,10 +4847,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D5" t="s">
         <v>356</v>
@@ -4878,7 +4872,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -4890,7 +4884,7 @@
       </c>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I6"/>
     </row>
@@ -4898,18 +4892,24 @@
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
       <c r="D7" t="s">
         <v>360</v>
       </c>
       <c r="E7" t="s">
         <v>47</v>
       </c>
-      <c r="F7"/>
+      <c r="F7" t="s">
+        <v>361</v>
+      </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="I7"/>
     </row>
@@ -4917,19 +4917,11 @@
       <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>330</v>
-      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
       <c r="E8"/>
-      <c r="F8" t="s">
-        <v>362</v>
-      </c>
+      <c r="F8"/>
       <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
@@ -4962,7 +4954,7 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="I10"/>
     </row>
@@ -4972,20 +4964,18 @@
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
         <v>363</v>
       </c>
       <c r="F11" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
-      <c r="I11" t="s">
-        <v>364</v>
-      </c>
+      <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
@@ -4997,7 +4987,7 @@
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -5010,43 +5000,45 @@
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13" t="s">
+        <v>365</v>
+      </c>
+      <c r="I13" t="s">
         <v>366</v>
-      </c>
-      <c r="I13" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D14" t="s">
+        <v>331</v>
+      </c>
+      <c r="E14" t="s">
         <v>244</v>
       </c>
-      <c r="D14"/>
-      <c r="E14" t="s">
-        <v>243</v>
-      </c>
       <c r="F14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G14"/>
       <c r="H14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -5061,15 +5053,21 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>96</v>
+      </c>
       <c r="G16"/>
-      <c r="H16"/>
+      <c r="H16" t="s">
+        <v>80</v>
+      </c>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
@@ -5084,10 +5082,12 @@
       </c>
       <c r="D17"/>
       <c r="E17"/>
-      <c r="F17"/>
+      <c r="F17" t="s">
+        <v>107</v>
+      </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="I17" t="s">
         <v>33</v>
@@ -5095,51 +5095,53 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18"/>
-      <c r="D18" t="s">
-        <v>368</v>
-      </c>
+      <c r="C18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18"/>
       <c r="E18" t="s">
         <v>206</v>
       </c>
       <c r="F18" t="s">
-        <v>109</v>
+        <v>367</v>
       </c>
       <c r="G18"/>
-      <c r="H18"/>
+      <c r="H18" t="s">
+        <v>129</v>
+      </c>
       <c r="I18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" t="s">
-        <v>210</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="D19"/>
       <c r="E19" t="s">
         <v>209</v>
       </c>
       <c r="F19" t="s">
-        <v>124</v>
+        <v>210</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>122</v>
-      </c>
-      <c r="I19"/>
+        <v>126</v>
+      </c>
+      <c r="I19" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
@@ -5147,23 +5149,21 @@
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>344</v>
       </c>
       <c r="D20" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
       <c r="E20" t="s">
+        <v>217</v>
+      </c>
+      <c r="F20" t="s">
+        <v>219</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20" t="s">
         <v>216</v>
-      </c>
-      <c r="F20" t="s">
-        <v>218</v>
-      </c>
-      <c r="G20"/>
-      <c r="H20" t="s">
-        <v>129</v>
-      </c>
-      <c r="I20" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -5176,14 +5176,12 @@
       <c r="C21" t="s">
         <v>73</v>
       </c>
-      <c r="D21" t="s">
-        <v>369</v>
-      </c>
+      <c r="D21"/>
       <c r="E21" t="s">
         <v>135</v>
       </c>
       <c r="F21" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
@@ -5196,26 +5194,22 @@
         <v>133</v>
       </c>
       <c r="B22" t="s">
+        <v>370</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22" t="s">
         <v>371</v>
       </c>
-      <c r="C22" t="s">
-        <v>220</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>372</v>
       </c>
-      <c r="E22" t="s">
-        <v>78</v>
-      </c>
       <c r="F22" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22" t="s">
         <v>373</v>
-      </c>
-      <c r="G22"/>
-      <c r="H22" t="s">
-        <v>374</v>
-      </c>
-      <c r="I22" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -5236,7 +5230,7 @@
         <v>140</v>
       </c>
       <c r="B24" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
@@ -5245,7 +5239,7 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H24" t="s">
         <v>153</v>
@@ -5257,15 +5251,15 @@
         <v>145</v>
       </c>
       <c r="B25" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F25" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="G25"/>
       <c r="H25"/>
@@ -5276,7 +5270,7 @@
         <v>147</v>
       </c>
       <c r="B26" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -5291,7 +5285,7 @@
         <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -5310,7 +5304,7 @@
         <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -5344,11 +5338,11 @@
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G30"/>
       <c r="H30" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I30"/>
     </row>
@@ -5359,14 +5353,14 @@
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
-      <c r="E31" t="s">
+      <c r="E31"/>
+      <c r="F31" t="s">
         <v>162</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31"/>
+      <c r="H31" t="s">
         <v>160</v>
       </c>
-      <c r="G31"/>
-      <c r="H31"/>
       <c r="I31"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update TT to v6.0
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -107,6 +107,9 @@
     <t>Discrete-GR2            Dr Jalal</t>
   </si>
   <si>
+    <t>SE-B                            Ahsan</t>
+  </si>
+  <si>
     <t>E3</t>
   </si>
   <si>
@@ -125,540 +128,552 @@
     <t>Eng Comp. D1                                                   Hafza Yusra</t>
   </si>
   <si>
+    <t>Eng Comp. B1                                                   Hafza Yusra</t>
+  </si>
+  <si>
+    <t>SE-A                        Rubab</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>TOA-F                             Subhash</t>
+  </si>
+  <si>
+    <t>OS-B                        Nausheen</t>
+  </si>
+  <si>
+    <t>DLD-E                      Nouman</t>
+  </si>
+  <si>
+    <t>DLD-F                      Nouman</t>
+  </si>
+  <si>
+    <t>TOA-B                               Subhash</t>
+  </si>
+  <si>
+    <t>TOA-D                                            Subhash</t>
+  </si>
+  <si>
+    <t>DLD-B                      Nouman</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>CP-E                             Faiza</t>
+  </si>
+  <si>
+    <t>CP-G                             Faiza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-D                               Farrukh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-F                               Farrukh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-E                              Farrukh </t>
+  </si>
+  <si>
+    <t>OOAD-GR1                  Faiza</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA-GR1             Danish                         </t>
+  </si>
+  <si>
+    <t>CC-GR1                                          M. Shahzad</t>
+  </si>
+  <si>
+    <t>CC-GR2                                          M. Shahzad</t>
+  </si>
+  <si>
+    <t>OS-E               Tania</t>
+  </si>
+  <si>
+    <t>OS-D                     Tania</t>
+  </si>
+  <si>
+    <t>TOA-A                             Shahzad</t>
+  </si>
+  <si>
+    <t>TOA-E                                Shahzad</t>
+  </si>
+  <si>
+    <t>SE-F                           Javeria</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>ITC-A                             Shahbaz</t>
+  </si>
+  <si>
+    <t>ITC-C                            Shahbaz</t>
+  </si>
+  <si>
+    <t>DLD-D                      Bahraj</t>
+  </si>
+  <si>
+    <t>PIT-GR1                           Khalid</t>
+  </si>
+  <si>
+    <t>PIT-GR2                                                  Khalid</t>
+  </si>
+  <si>
+    <t>EP-GR2                                Wamiq</t>
+  </si>
+  <si>
+    <t>EP-GR1                                 Wamiq</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>ITC-B                            Tania</t>
+  </si>
+  <si>
+    <t>OS-A                            Dr. Hasina</t>
+  </si>
+  <si>
+    <t>Dsci.-GR3                                     Dr. Atif</t>
+  </si>
+  <si>
+    <t>Dsci.-GR4                                     Dr. Atif</t>
+  </si>
+  <si>
+    <t>SE-D                         Javeria</t>
+  </si>
+  <si>
+    <t>IHRM-GR2                               M. Zeeshan</t>
+  </si>
+  <si>
+    <t>IHRM-GR1                                 M. Zeeshan</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>DS-A                         Zeshan</t>
+  </si>
+  <si>
+    <t>Eng Comp. A2                                                   Faiza</t>
+  </si>
+  <si>
+    <t>DS-C                     Zeshan</t>
+  </si>
+  <si>
+    <t>DS-B                           Zeshan</t>
+  </si>
+  <si>
+    <t>Eng Comp. E2                                                   Faiza</t>
+  </si>
+  <si>
+    <t>HCI-GR1                               Bahraj</t>
+  </si>
+  <si>
+    <t>HCI-GR2                               Bahraj</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-C                               Dr Rauf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-G                               Dr Rauf </t>
+  </si>
+  <si>
+    <t>COAL-GR2            Danish</t>
+  </si>
+  <si>
+    <t>COAL-GR1            Danish</t>
+  </si>
+  <si>
+    <t>CR-3 EE</t>
+  </si>
+  <si>
+    <t>CP-B                             Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>CP-D                             Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>BE-GR1                     Javaid Qureshi</t>
+  </si>
+  <si>
+    <t>CP-F                             Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>Eng Comp. C2                                                   Faiza</t>
+  </si>
+  <si>
+    <t>CR-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA-GR2             Ahsan                        </t>
+  </si>
+  <si>
+    <t>CAL II-A                  Fareeha</t>
+  </si>
+  <si>
+    <t>CAL II-C                  Fareeha</t>
+  </si>
+  <si>
+    <t>CAL II-E                  Fareeha</t>
+  </si>
+  <si>
+    <t>IRS-G                                            Shahzad</t>
+  </si>
+  <si>
+    <t>AL-GR1            Shahzad Sheikh</t>
+  </si>
+  <si>
+    <t>CR-7</t>
+  </si>
+  <si>
+    <t>TBW-F                               Nazia</t>
+  </si>
+  <si>
+    <t>TBW-A                               Nazia</t>
+  </si>
+  <si>
+    <t>TBW-C                               Nazia</t>
+  </si>
+  <si>
+    <t>CR-10</t>
+  </si>
+  <si>
+    <t>DLD-G                      Rabia</t>
+  </si>
+  <si>
+    <t>DLD-A                      Rabia</t>
+  </si>
+  <si>
+    <t>TBW-E                               Sameera</t>
+  </si>
+  <si>
+    <t>TBW-B                               Sameera</t>
+  </si>
+  <si>
+    <t>DLD-C                      Rabia</t>
+  </si>
+  <si>
+    <t>CR-16</t>
+  </si>
+  <si>
+    <t>Prob-A                    Osama</t>
+  </si>
+  <si>
+    <t>Prob-C                                      Osama</t>
+  </si>
+  <si>
+    <t>Prob-E                      Osama</t>
+  </si>
+  <si>
+    <t>TOA-C                                    Shaharbano</t>
+  </si>
+  <si>
+    <t>TOA-G                       Shaharbano</t>
+  </si>
+  <si>
+    <t>AL-GR2            Hassan Saeed</t>
+  </si>
+  <si>
+    <t>CR-17</t>
+  </si>
+  <si>
+    <t>Eng Comp. G2                                                   Ahmed Bux</t>
+  </si>
+  <si>
+    <t>Psych-GR4 Sumaira</t>
+  </si>
+  <si>
+    <t>Psych-GR1 Sumaira</t>
+  </si>
+  <si>
+    <t>Eng Comp. F2                                                   Ahmed Bux</t>
+  </si>
+  <si>
+    <t>Psych-GR2 Sumaira</t>
+  </si>
+  <si>
+    <t>CR-18</t>
+  </si>
+  <si>
+    <t>Prob-B                     Asma</t>
+  </si>
+  <si>
+    <t>OB-GR2            Asiya</t>
+  </si>
+  <si>
+    <t>Prob-D                                          Asma</t>
+  </si>
+  <si>
+    <t>Prob-F                        Asma</t>
+  </si>
+  <si>
+    <t>OB-GR1            Asiya</t>
+  </si>
+  <si>
+    <t>CR-20</t>
+  </si>
+  <si>
+    <t>Eng Comp. G1                                                   Javed Iqbal</t>
+  </si>
+  <si>
+    <t>Eng Comp. A1                                                   Javed Iqbal</t>
+  </si>
+  <si>
+    <t>CAL II-F                  Nadeem</t>
+  </si>
+  <si>
+    <t>CAL II-B                  Nadeem</t>
+  </si>
+  <si>
+    <t>Eng Comp. C1                                                   Javed Iqbal</t>
+  </si>
+  <si>
+    <t>LABS</t>
+  </si>
+  <si>
+    <t>Lab-1</t>
+  </si>
+  <si>
+    <t>DS-Lab B                                                                                                Aziz + Irfan</t>
+  </si>
+  <si>
+    <t>IOT-GR1                                         Dr. Farooque</t>
+  </si>
+  <si>
+    <t>IOT-GR2                                       Dr. Farooque</t>
+  </si>
+  <si>
+    <t>NP-GR1                                        Shahbaz</t>
+  </si>
+  <si>
+    <t>Lab-3</t>
+  </si>
+  <si>
+    <t>CG-GR1                              Javeria</t>
+  </si>
+  <si>
+    <t>CN-Lab  B                                                                                                                Awais</t>
+  </si>
+  <si>
+    <t>Lab-4</t>
+  </si>
+  <si>
+    <t>OS-Lab C                                                                                                      Ms. Safia</t>
+  </si>
+  <si>
+    <t>EE Lab-8</t>
+  </si>
+  <si>
+    <t>CP-Lab F1+F2                                                                                                 Ammara &amp; Tooba</t>
+  </si>
+  <si>
+    <t>EE Lab 9</t>
+  </si>
+  <si>
+    <t>OS-Lab D                                                                                                                Ms. Summiyah</t>
+  </si>
+  <si>
+    <t>RESERVED  BBA</t>
+  </si>
+  <si>
+    <t>RESERVED  EE</t>
+  </si>
+  <si>
+    <t>EE Lab 10</t>
+  </si>
+  <si>
+    <t>EE MPI Lab</t>
+  </si>
+  <si>
+    <t>DLD-Lab  B                                                                                                        Sehrish</t>
+  </si>
+  <si>
+    <t>LLC</t>
+  </si>
+  <si>
+    <t>Eng Comp. D2                                                   Nasir</t>
+  </si>
+  <si>
+    <t>Eng Comp. E1                                                   Nasir</t>
+  </si>
+  <si>
+    <t>ENG-GR1                                                   Nasir</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>CP-A                                           Abdul Aziz</t>
+  </si>
+  <si>
+    <t>CP-C                                             Abdul Aziz</t>
+  </si>
+  <si>
+    <t>SE-F                                                             Javeria</t>
+  </si>
+  <si>
+    <t>SE-D                                              Javeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-D                                                             Farrukh </t>
+  </si>
+  <si>
+    <t>SE-G                                                            Abdur Rehman</t>
+  </si>
+  <si>
+    <t>DS-D                                   Abdul Aziz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-E                                                  Farrukh </t>
+  </si>
+  <si>
+    <t>SE-G                                                     Abdur Rehman</t>
+  </si>
+  <si>
+    <t>OS-D                                     Tania</t>
+  </si>
+  <si>
+    <t>OS-E                                          Tania</t>
+  </si>
+  <si>
+    <t>IR-GR1                                                       Dr Rafi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-G                                                                   Dr Rauf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-C                                                           Dr Rauf </t>
+  </si>
+  <si>
+    <t>CN-F                                                            Faraz</t>
+  </si>
+  <si>
+    <t>CP-F                                            Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>Dwh-GR1                                                 Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>Dwh-GR2                                                Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>TBW-G                                                 Sameera</t>
+  </si>
+  <si>
+    <t>CN-C                                            Shoaib</t>
+  </si>
+  <si>
+    <t>CN-G                                            Shoaib</t>
+  </si>
+  <si>
+    <t>CP-B                                                  Shoaib Rauf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RM-GR1                                                Shoaib </t>
+  </si>
+  <si>
+    <t>PIT-GR1                                              Khalid</t>
+  </si>
+  <si>
+    <t>PIT-GR2                                               Khalid</t>
+  </si>
+  <si>
+    <t>OS-B                            Nausheen</t>
+  </si>
+  <si>
+    <t>OS-F                                 Nausheen</t>
+  </si>
+  <si>
+    <t>EP-GR1                                                      Wamiq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  EP-GR2                                                      Wamiq</t>
+  </si>
+  <si>
+    <t>DLD-D                                         Bahraj</t>
+  </si>
+  <si>
+    <t>OS-C                          Nausheen</t>
+  </si>
+  <si>
+    <t>CN-B                                            Dr Sufian</t>
+  </si>
+  <si>
+    <t>CN-A                                                                Dr Sufian</t>
+  </si>
+  <si>
+    <t>IHRM-GR1                                                        M. Zeeshan</t>
+  </si>
+  <si>
+    <t>IHRM-GR2                                                     M. Zeeshan</t>
+  </si>
+  <si>
+    <t>CP-E                                                 Faiza</t>
+  </si>
+  <si>
+    <t>CP-G                                             Faiza</t>
+  </si>
+  <si>
+    <t>Eng Comp. B2                                                   Ahmed Bux</t>
+  </si>
+  <si>
+    <t>OOAD-GR1                                    Faiza</t>
+  </si>
+  <si>
+    <t>TBW-D                               Sameera</t>
+  </si>
+  <si>
+    <t>CAL I-GR1                  Imran Shah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA-GR1                                    Danish                         </t>
+  </si>
+  <si>
+    <t>NM-GR2            Dr Khusro</t>
+  </si>
+  <si>
+    <t>CAL II-D                  Nadeem</t>
+  </si>
+  <si>
+    <t>NM-GR1                                       Dr Khusro</t>
+  </si>
+  <si>
+    <t>SM-GR2            Dr Fahad</t>
+  </si>
+  <si>
+    <t>SM-GR1                               Dr Fahad</t>
+  </si>
+  <si>
+    <t>LA-GR1                               Dr Fahad</t>
+  </si>
+  <si>
+    <t>IRS-F                                            Shahzad</t>
+  </si>
+  <si>
+    <t>Prob-A                                      Osama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pst. C                                                   Kashif </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pst. E                             Kashif </t>
+  </si>
+  <si>
+    <t>Prob-E                                              Osama</t>
+  </si>
+  <si>
     <t>Eng Comp. F1                                                   Hafza Yusra</t>
   </si>
   <si>
-    <t>SE-A                        Rubab</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>TOA-F                             Subhash</t>
-  </si>
-  <si>
-    <t>OS-B                        Nausheen</t>
-  </si>
-  <si>
-    <t>DLD-E                      Nouman</t>
-  </si>
-  <si>
-    <t>DLD-F                      Nouman</t>
-  </si>
-  <si>
-    <t>TOA-B                               Subhash</t>
-  </si>
-  <si>
-    <t>TOA-D                                            Subhash</t>
-  </si>
-  <si>
-    <t>DLD-B                      Nouman</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>CP-E                             Faiza</t>
-  </si>
-  <si>
-    <t>CP-G                             Faiza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-D                               Farrukh </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-F                               Farrukh </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-E                              Farrukh </t>
-  </si>
-  <si>
-    <t>OOAD-GR1                  Faiza</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA-GR1             Danish                         </t>
-  </si>
-  <si>
-    <t>CC-GR1                                          M. Shahzad</t>
-  </si>
-  <si>
-    <t>CC-GR2                                          M. Shahzad</t>
-  </si>
-  <si>
-    <t>OS-E               Tania</t>
-  </si>
-  <si>
-    <t>OS-D                     Tania</t>
-  </si>
-  <si>
-    <t>TOA-A                             Shahzad</t>
-  </si>
-  <si>
-    <t>TOA-E                                Shahzad</t>
-  </si>
-  <si>
-    <t>SE-F                           Javeria</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>ITC-A                             Shahbaz</t>
-  </si>
-  <si>
-    <t>ITC-C                            Shahbaz</t>
-  </si>
-  <si>
-    <t>DLD-D                      Bahraj</t>
-  </si>
-  <si>
-    <t>PIT-GR1                           Khalid</t>
-  </si>
-  <si>
-    <t>PIT-GR2                                                  Khalid</t>
-  </si>
-  <si>
-    <t>EP-GR2                                Wamiq</t>
-  </si>
-  <si>
-    <t>EP-GR1                                 Wamiq</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>ITC-B                            Tania</t>
-  </si>
-  <si>
-    <t>OS-A                            Dr. Hasina</t>
-  </si>
-  <si>
-    <t>Dsci.-GR3                                     Dr. Atif</t>
-  </si>
-  <si>
-    <t>Dsci.-GR4                                     Dr. Atif</t>
-  </si>
-  <si>
-    <t>SE-D                         Javeria</t>
-  </si>
-  <si>
-    <t>IHRM-GR2                               M. Zeeshan</t>
-  </si>
-  <si>
-    <t>IHRM-GR1                                 M. Zeeshan</t>
-  </si>
-  <si>
-    <t>R109</t>
-  </si>
-  <si>
-    <t>DS-A                         Zeshan</t>
-  </si>
-  <si>
-    <t>Eng Comp. A2                                                   Faiza</t>
-  </si>
-  <si>
-    <t>DS-C                     Zeshan</t>
-  </si>
-  <si>
-    <t>DS-B                           Zeshan</t>
-  </si>
-  <si>
-    <t>Eng Comp. E2                                                   Faiza</t>
-  </si>
-  <si>
-    <t>HCI-GR1                               Bahraj</t>
-  </si>
-  <si>
-    <t>HCI-GR2                               Bahraj</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-C                               Dr Rauf </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-G                               Dr Rauf </t>
-  </si>
-  <si>
-    <t>COAL-GR2            Danish</t>
-  </si>
-  <si>
-    <t>COAL-GR1            Danish</t>
-  </si>
-  <si>
-    <t>AL-GR1            Shahzad Sheikh</t>
-  </si>
-  <si>
-    <t>CR-3 EE</t>
-  </si>
-  <si>
-    <t>CP-B                             Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>CP-D                             Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>BE-GR1                     Javaid Qureshi</t>
-  </si>
-  <si>
-    <t>CP-F                             Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>Eng Comp. C2                                                   Faiza</t>
-  </si>
-  <si>
-    <t>CR-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA-GR2             Ahsan                        </t>
-  </si>
-  <si>
-    <t>CAL II-A                  Fareeha</t>
-  </si>
-  <si>
-    <t>CAL II-C                  Fareeha</t>
-  </si>
-  <si>
-    <t>CAL II-E                  Fareeha</t>
-  </si>
-  <si>
-    <t>IRS-G                                            Shahzad</t>
-  </si>
-  <si>
-    <t>SE-B                            Ahsan</t>
-  </si>
-  <si>
-    <t>CR-7</t>
-  </si>
-  <si>
-    <t>TBW-F                               Nazia</t>
-  </si>
-  <si>
-    <t>TBW-A                               Nazia</t>
-  </si>
-  <si>
-    <t>TBW-C                               Nazia</t>
-  </si>
-  <si>
-    <t>CR-10</t>
-  </si>
-  <si>
-    <t>DLD-G                      Rabia</t>
-  </si>
-  <si>
-    <t>DLD-A                      Rabia</t>
-  </si>
-  <si>
-    <t>TBW-E                               Sameera</t>
-  </si>
-  <si>
-    <t>TBW-B                               Sameera</t>
-  </si>
-  <si>
-    <t>DLD-C                      Rabia</t>
-  </si>
-  <si>
-    <t>CR-16</t>
-  </si>
-  <si>
-    <t>Prob-A                    Osama</t>
-  </si>
-  <si>
-    <t>Prob-C                                      Osama</t>
-  </si>
-  <si>
-    <t>Prob-E                      Osama</t>
-  </si>
-  <si>
-    <t>TOA-C                                    Shaharbano</t>
-  </si>
-  <si>
-    <t>TOA-G                       Shaharbano</t>
-  </si>
-  <si>
-    <t>AL-GR2            Hassan Saeed</t>
-  </si>
-  <si>
-    <t>CR-17</t>
-  </si>
-  <si>
-    <t>Psych-GR4 Sumaira</t>
-  </si>
-  <si>
-    <t>Psych-GR1 Sumaira</t>
-  </si>
-  <si>
-    <t>Eng Comp. F2                                                   Ahmed Bux</t>
-  </si>
-  <si>
-    <t>Psych-GR2 Sumaira</t>
-  </si>
-  <si>
-    <t>CR-18</t>
-  </si>
-  <si>
-    <t>Prob-B                     Asma</t>
-  </si>
-  <si>
-    <t>OB-GR2            Asiya</t>
-  </si>
-  <si>
-    <t>Prob-D                                          Asma</t>
-  </si>
-  <si>
-    <t>Prob-F                        Asma</t>
-  </si>
-  <si>
-    <t>OB-GR1            Asiya</t>
-  </si>
-  <si>
-    <t>CR-20</t>
-  </si>
-  <si>
-    <t>Eng Comp. G1                                                   Javed Iqbal</t>
-  </si>
-  <si>
-    <t>Eng Comp. A1                                                   Javed Iqbal</t>
-  </si>
-  <si>
-    <t>CAL II-F                  Nadeem</t>
-  </si>
-  <si>
-    <t>CAL II-B                  Nadeem</t>
-  </si>
-  <si>
-    <t>Eng Comp. C1                                                   Javed Iqbal</t>
-  </si>
-  <si>
-    <t>LABS</t>
-  </si>
-  <si>
-    <t>Lab-1</t>
-  </si>
-  <si>
-    <t>DS-Lab B                                                                                                Aziz + Irfan</t>
-  </si>
-  <si>
-    <t>IOT-GR1                                         Dr. Farooque</t>
-  </si>
-  <si>
-    <t>IOT-GR2                                       Dr. Farooque</t>
-  </si>
-  <si>
-    <t>NP-GR1                                        Shahbaz</t>
-  </si>
-  <si>
-    <t>Lab-3</t>
-  </si>
-  <si>
-    <t>CG-GR1                              Javeria</t>
-  </si>
-  <si>
-    <t>CN-Lab  B                                                                                                                Awais</t>
-  </si>
-  <si>
-    <t>Lab-4</t>
-  </si>
-  <si>
-    <t>OS-Lab C                                                                                                      Ms. Safia</t>
-  </si>
-  <si>
-    <t>EE Lab-8</t>
-  </si>
-  <si>
-    <t>CP-Lab F1+F2                                                                                                 Ammara &amp; Tooba</t>
-  </si>
-  <si>
-    <t>EE Lab 9</t>
-  </si>
-  <si>
-    <t>OS-Lab D                                                                                                                Ms. Summiyah</t>
-  </si>
-  <si>
-    <t>RESERVED  BBA</t>
-  </si>
-  <si>
-    <t>RESERVED  EE</t>
-  </si>
-  <si>
-    <t>EE Lab 10</t>
-  </si>
-  <si>
-    <t>EE MPI Lab</t>
-  </si>
-  <si>
-    <t>DLD-Lab  B                                                                                                        Sehrish</t>
-  </si>
-  <si>
-    <t>LLC</t>
-  </si>
-  <si>
-    <t>Eng Comp. G2                                                   Ahmed Bux</t>
-  </si>
-  <si>
-    <t>Eng Comp. D2                                                   Nasir</t>
-  </si>
-  <si>
-    <t>Eng Comp. E1                                                   Nasir</t>
-  </si>
-  <si>
-    <t>ENG-GR1                                                   Nasir</t>
-  </si>
-  <si>
-    <t>TUESDAY</t>
-  </si>
-  <si>
-    <t>CP-A                                           Abdul Aziz</t>
-  </si>
-  <si>
-    <t>CP-C                                             Abdul Aziz</t>
-  </si>
-  <si>
-    <t>SE-F                                                             Javeria</t>
-  </si>
-  <si>
-    <t>SE-D                                              Javeria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-D                                                             Farrukh </t>
-  </si>
-  <si>
-    <t>SE-G                                                            Abdur Rehman</t>
-  </si>
-  <si>
-    <t>DS-D                                   Abdul Aziz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-E                                                  Farrukh </t>
-  </si>
-  <si>
-    <t>SE-G                                                     Abdur Rehman</t>
-  </si>
-  <si>
-    <t>OS-D                                     Tania</t>
-  </si>
-  <si>
-    <t>OS-E                                          Tania</t>
-  </si>
-  <si>
-    <t>IR-GR1                                                       Dr Rafi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-G                                                                   Dr Rauf </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-C                                                           Dr Rauf </t>
-  </si>
-  <si>
-    <t>CN-F                                                            Faraz</t>
-  </si>
-  <si>
-    <t>CP-F                                            Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>Dwh-GR1                                                 Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>Dwh-GR2                                                Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>TBW-G                                                 Sameera</t>
-  </si>
-  <si>
-    <t>CN-C                                            Shoaib</t>
-  </si>
-  <si>
-    <t>CN-G                                            Shoaib</t>
-  </si>
-  <si>
-    <t>CP-B                                                  Shoaib Rauf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RM-GR1                                                Shoaib </t>
-  </si>
-  <si>
-    <t>PIT-GR1                                              Khalid</t>
-  </si>
-  <si>
-    <t>PIT-GR2                                               Khalid</t>
-  </si>
-  <si>
-    <t>OS-B                            Nausheen</t>
-  </si>
-  <si>
-    <t>OS-F                                 Nausheen</t>
-  </si>
-  <si>
-    <t>EP-GR1                                                      Wamiq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  EP-GR2                                                      Wamiq</t>
-  </si>
-  <si>
-    <t>DLD-D                                         Bahraj</t>
-  </si>
-  <si>
-    <t>OS-C                          Nausheen</t>
-  </si>
-  <si>
-    <t>CN-B                                            Dr Sufian</t>
-  </si>
-  <si>
-    <t>CN-A                                                                Dr Sufian</t>
-  </si>
-  <si>
-    <t>IHRM-GR1                                                        M. Zeeshan</t>
-  </si>
-  <si>
-    <t>IHRM-GR2                                                     M. Zeeshan</t>
-  </si>
-  <si>
-    <t>CP-E                                                 Faiza</t>
-  </si>
-  <si>
-    <t>CP-G                                             Faiza</t>
-  </si>
-  <si>
-    <t>Eng Comp. B2                                                   Ahmed Bux</t>
-  </si>
-  <si>
-    <t>OOAD-GR1                                    Faiza</t>
-  </si>
-  <si>
-    <t>TBW-D                               Sameera</t>
-  </si>
-  <si>
-    <t>CAL I-GR1                  Imran Shah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA-GR1                                    Danish                         </t>
-  </si>
-  <si>
-    <t>NM-GR2            Dr Khusro</t>
-  </si>
-  <si>
-    <t>CAL II-D                  Nadeem</t>
-  </si>
-  <si>
-    <t>NM-GR1                                       Dr Khusro</t>
-  </si>
-  <si>
-    <t>SM-GR2            Dr Fahad</t>
-  </si>
-  <si>
-    <t>SM-GR1                               Dr Fahad</t>
-  </si>
-  <si>
-    <t>LA-GR1                               Dr Fahad</t>
-  </si>
-  <si>
-    <t>Eng Comp. B1                                                   Hafza Yusra</t>
-  </si>
-  <si>
     <t>Prob-B                                                    Asma</t>
   </si>
   <si>
@@ -683,27 +698,12 @@
     <t>CM-GR1                                  Jameel</t>
   </si>
   <si>
-    <t>IRS-F                                            Shahzad</t>
-  </si>
-  <si>
     <t>Psych-GR3                                                    Sumaira</t>
   </si>
   <si>
     <t>Psych-GR4                           Sumaira</t>
   </si>
   <si>
-    <t>Prob-A                                      Osama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pst. C                                                   Kashif </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pst. E                             Kashif </t>
-  </si>
-  <si>
-    <t>Prob-E                                              Osama</t>
-  </si>
-  <si>
     <t>OS-Lab A                                                                                                                        Ms. Summiyah</t>
   </si>
   <si>
@@ -902,12 +902,12 @@
     <t>Pst. B                        Michael</t>
   </si>
   <si>
+    <t>Psych-GR3 Sumaira</t>
+  </si>
+  <si>
     <t xml:space="preserve">CA-GR2                                                Ahsan                        </t>
   </si>
   <si>
-    <t>Psych-GR3 Sumaira</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pst. A                                                        Kashif </t>
   </si>
   <si>
@@ -977,63 +977,66 @@
     <t>IR-GR1                                                             Dr Rafi</t>
   </si>
   <si>
+    <t>DS-A                                     Zeshan</t>
+  </si>
+  <si>
+    <t>DS-B                                     Zeshan</t>
+  </si>
+  <si>
+    <t>DS-C                                  Zeshan</t>
+  </si>
+  <si>
+    <t>CN-E                                                          Faraz</t>
+  </si>
+  <si>
+    <t>TOA-C                                      Shaharbano</t>
+  </si>
+  <si>
+    <t>TOA-G                                     Shaharbano</t>
+  </si>
+  <si>
     <t>ISPM-GR1                                       Ubaid</t>
   </si>
   <si>
     <t>CAL I-GR1                                            Imran Shah</t>
   </si>
   <si>
+    <t>TOA-F                          Subhash</t>
+  </si>
+  <si>
+    <t>TOA-D                                               Subhash</t>
+  </si>
+  <si>
+    <t>TOA-A                                                Shahzad</t>
+  </si>
+  <si>
+    <t>TOA-E                                           Shahzad</t>
+  </si>
+  <si>
     <t>Discrete- GR1                                 Dr Jalal</t>
   </si>
   <si>
-    <t>DS-A                                     Zeshan</t>
-  </si>
-  <si>
-    <t>DS-B                                     Zeshan</t>
-  </si>
-  <si>
-    <t>DS-C                                  Zeshan</t>
-  </si>
-  <si>
-    <t>TOA-A                                                Shahzad</t>
-  </si>
-  <si>
-    <t>CN-E                                                          Faraz</t>
-  </si>
-  <si>
-    <t>TOA-E                                           Shahzad</t>
-  </si>
-  <si>
     <t>OS-A                                              Dr. Hasina</t>
   </si>
   <si>
-    <t>TOA-D                                               Subhash</t>
-  </si>
-  <si>
-    <t>TOA-F                          Subhash</t>
-  </si>
-  <si>
     <t>CV-GR1                               Dr Tahir syed</t>
   </si>
   <si>
-    <t>TOA-C                                      Shaharbano</t>
-  </si>
-  <si>
-    <t>TOA-G                                     Shaharbano</t>
-  </si>
-  <si>
     <t>NM-GR1                              Dr Khusro</t>
   </si>
   <si>
     <t>Prob-G                                   Amjad</t>
   </si>
   <si>
+    <t xml:space="preserve">Pst. C                                          Kashif </t>
+  </si>
+  <si>
+    <t>Prob-D                                      Asma</t>
+  </si>
+  <si>
     <t>Prob-F                                           Asma</t>
   </si>
   <si>
-    <t>Prob-D                                      Asma</t>
-  </si>
-  <si>
     <t>DLD-G                                               Rabia</t>
   </si>
   <si>
@@ -1059,9 +1062,6 @@
   </si>
   <si>
     <t>TBW-F                                              Nazia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pst. C                                          Kashif </t>
   </si>
   <si>
     <t>CN-Lab  G                                                                                                                                   Faizan</t>
@@ -1687,7 +1687,9 @@
       <c r="H6" t="s">
         <v>27</v>
       </c>
-      <c r="I6"/>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -1697,29 +1699,29 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -1730,29 +1732,29 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -1763,27 +1765,27 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -1794,31 +1796,31 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
@@ -1829,29 +1831,29 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
@@ -1862,29 +1864,29 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J12"/>
       <c r="K12"/>
@@ -1895,29 +1897,29 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -1928,26 +1930,24 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14" t="s">
         <v>89</v>
       </c>
+      <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
       <c r="L14"/>
@@ -2106,21 +2106,23 @@
       <c r="A20" t="s">
         <v>120</v>
       </c>
-      <c r="B20"/>
+      <c r="B20" t="s">
+        <v>121</v>
+      </c>
       <c r="C20"/>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E20"/>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
@@ -2131,25 +2133,25 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C21"/>
       <c r="D21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
@@ -2160,24 +2162,24 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E22"/>
       <c r="F22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
@@ -2189,7 +2191,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -2208,21 +2210,21 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -2235,14 +2237,14 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C25"/>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E25"/>
       <c r="F25"/>
@@ -2258,10 +2260,10 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -2279,10 +2281,10 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -2300,18 +2302,18 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F28" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G28"/>
       <c r="H28"/>
@@ -2325,10 +2327,10 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" t="s">
         <v>154</v>
-      </c>
-      <c r="B29" t="s">
-        <v>153</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -2346,16 +2348,16 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
@@ -2369,11 +2371,9 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>157</v>
-      </c>
-      <c r="B31" t="s">
         <v>158</v>
       </c>
+      <c r="B31"/>
       <c r="C31"/>
       <c r="D31" t="s">
         <v>159</v>
@@ -2540,16 +2540,16 @@
         <v>164</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
         <v>165</v>
@@ -2568,16 +2568,16 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
         <v>54</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>167</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
         <v>168</v>
@@ -2599,14 +2599,14 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
         <v>172</v>
@@ -2619,7 +2619,7 @@
         <v>95</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
@@ -2646,10 +2646,10 @@
         <v>177</v>
       </c>
       <c r="H8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
         <v>178</v>
@@ -2689,13 +2689,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
         <v>182</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>186</v>
@@ -2728,10 +2728,10 @@
         <v>187</v>
       </c>
       <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
         <v>83</v>
-      </c>
-      <c r="E11" t="s">
-        <v>82</v>
       </c>
       <c r="F11" t="s">
         <v>188</v>
@@ -2753,13 +2753,13 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
         <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>193</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>198</v>
@@ -2796,7 +2796,7 @@
         <v>199</v>
       </c>
       <c r="D13" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -2817,17 +2817,17 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
         <v>202</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
         <v>203</v>
@@ -2848,7 +2848,7 @@
         <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
         <v>205</v>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="E15"/>
       <c r="F15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
@@ -2907,17 +2907,25 @@
       <c r="A17" t="s">
         <v>103</v>
       </c>
-      <c r="B17"/>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
       <c r="C17"/>
-      <c r="D17"/>
+      <c r="D17" t="s">
+        <v>211</v>
+      </c>
       <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
+      <c r="F17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G17" t="s">
+        <v>213</v>
+      </c>
       <c r="H17" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="I17" t="s">
-        <v>34</v>
+        <v>215</v>
       </c>
       <c r="J17"/>
       <c r="K17"/>
@@ -2932,22 +2940,24 @@
       <c r="B18" t="s">
         <v>108</v>
       </c>
-      <c r="C18"/>
+      <c r="C18" t="s">
+        <v>216</v>
+      </c>
       <c r="D18"/>
       <c r="E18" t="s">
         <v>112</v>
       </c>
       <c r="F18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G18" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="H18" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="I18" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="J18"/>
       <c r="K18"/>
@@ -2960,23 +2970,23 @@
         <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C19" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E19"/>
       <c r="F19" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="G19" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="H19" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
@@ -2990,20 +3000,18 @@
         <v>120</v>
       </c>
       <c r="B20"/>
-      <c r="C20" t="s">
-        <v>220</v>
-      </c>
+      <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="I20" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
@@ -3013,26 +3021,16 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" t="s">
-        <v>115</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
-      <c r="F21" t="s">
-        <v>223</v>
-      </c>
-      <c r="G21" t="s">
-        <v>224</v>
-      </c>
-      <c r="H21" t="s">
-        <v>225</v>
-      </c>
-      <c r="I21" t="s">
-        <v>226</v>
-      </c>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
@@ -3041,7 +3039,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -3059,7 +3057,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -3077,7 +3075,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
         <v>227</v>
@@ -3087,7 +3085,7 @@
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -3099,7 +3097,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
         <v>228</v>
@@ -3127,7 +3125,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B26" t="s">
         <v>233</v>
@@ -3147,7 +3145,7 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B27" t="s">
         <v>234</v>
@@ -3169,7 +3167,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
         <v>236</v>
@@ -3189,7 +3187,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
         <v>236</v>
@@ -3209,7 +3207,7 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
@@ -3231,7 +3229,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -3386,7 +3384,7 @@
         <v>243</v>
       </c>
       <c r="G5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -3396,10 +3394,10 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>244</v>
@@ -3418,19 +3416,19 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>247</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
         <v>248</v>
@@ -3439,16 +3437,16 @@
         <v>249</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
         <v>250</v>
@@ -3468,7 +3466,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
         <v>254</v>
@@ -3493,7 +3491,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
         <v>259</v>
@@ -3518,7 +3516,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>263</v>
@@ -3527,10 +3525,10 @@
         <v>264</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F11" t="s">
         <v>117</v>
@@ -3543,19 +3541,19 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
         <v>266</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
         <v>267</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
         <v>268</v>
@@ -3570,7 +3568,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>271</v>
@@ -3582,7 +3580,7 @@
         <v>272</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F13" t="s">
         <v>273</v>
@@ -3592,12 +3590,12 @@
         <v>274</v>
       </c>
       <c r="I13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
         <v>275</v>
@@ -3618,9 +3616,7 @@
       <c r="H14" t="s">
         <v>280</v>
       </c>
-      <c r="I14" t="s">
-        <v>89</v>
-      </c>
+      <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
@@ -3632,17 +3628,17 @@
         <v>281</v>
       </c>
       <c r="E15" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G15" t="s">
         <v>282</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3663,14 +3659,12 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="H16" t="s">
         <v>286</v>
       </c>
-      <c r="I16" t="s">
-        <v>119</v>
-      </c>
+      <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
@@ -3708,41 +3702,39 @@
       <c r="D18" t="s">
         <v>292</v>
       </c>
-      <c r="E18"/>
+      <c r="E18" t="s">
+        <v>293</v>
+      </c>
       <c r="F18" t="s">
         <v>123</v>
       </c>
       <c r="G18"/>
-      <c r="H18" t="s">
-        <v>158</v>
-      </c>
-      <c r="I18"/>
+      <c r="H18"/>
+      <c r="I18" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C19" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D19" t="s">
         <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>294</v>
-      </c>
-      <c r="F19" t="s">
-        <v>122</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="F19"/>
       <c r="G19"/>
-      <c r="H19" t="s">
-        <v>34</v>
-      </c>
+      <c r="H19"/>
       <c r="I19" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3758,13 +3750,13 @@
         <v>296</v>
       </c>
       <c r="F20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G20" t="s">
         <v>297</v>
       </c>
       <c r="H20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I20" t="s">
         <v>298</v>
@@ -3772,7 +3764,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
@@ -3785,7 +3777,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -3798,7 +3790,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -3811,7 +3803,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
         <v>299</v>
@@ -3828,7 +3820,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
         <v>301</v>
@@ -3845,7 +3837,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B26" t="s">
         <v>303</v>
@@ -3862,7 +3854,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B27" t="s">
         <v>305</v>
@@ -3879,7 +3871,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
         <v>236</v>
@@ -3894,7 +3886,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
         <v>236</v>
@@ -3911,7 +3903,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
@@ -3928,7 +3920,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -3967,7 +3959,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="57" zoomScaleNormal="57" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -3976,7 +3968,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>309</v>
       </c>
@@ -3988,13 +3980,8 @@
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4022,13 +4009,8 @@
       <c r="I2">
         <v>8</v>
       </c>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-    </row>
-    <row r="3" spans="1:14">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4056,13 +4038,8 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4074,13 +4051,8 @@
       <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-    </row>
-    <row r="5" spans="1:14">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4091,7 +4063,7 @@
         <v>311</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
         <v>312</v>
@@ -4099,18 +4071,11 @@
       <c r="F5" t="s">
         <v>313</v>
       </c>
-      <c r="G5" t="s">
-        <v>87</v>
-      </c>
+      <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-    </row>
-    <row r="6" spans="1:14">
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -4128,125 +4093,108 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-    </row>
-    <row r="7" spans="1:14">
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" t="s">
+        <v>319</v>
+      </c>
       <c r="E7"/>
-      <c r="F7"/>
+      <c r="F7" t="s">
+        <v>320</v>
+      </c>
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-    </row>
-    <row r="8" spans="1:14">
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8"/>
-      <c r="C8"/>
+      <c r="C8" t="s">
+        <v>321</v>
+      </c>
       <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
+      <c r="E8" t="s">
+        <v>322</v>
+      </c>
+      <c r="F8" t="s">
+        <v>323</v>
+      </c>
       <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-    </row>
-    <row r="9" spans="1:14">
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="E9" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="F9" t="s">
         <v>203</v>
       </c>
       <c r="G9" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-    </row>
-    <row r="10" spans="1:14">
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
       <c r="C10" t="s">
-        <v>321</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="D10"/>
       <c r="E10" t="s">
-        <v>322</v>
-      </c>
-      <c r="F10" t="s">
-        <v>323</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="F10"/>
       <c r="G10"/>
       <c r="H10"/>
       <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-    </row>
-    <row r="11" spans="1:14">
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C11" t="s">
-        <v>325</v>
-      </c>
-      <c r="D11" t="s">
-        <v>326</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="D11"/>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
         <v>252</v>
@@ -4254,67 +4202,46 @@
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-      <c r="N11"/>
-    </row>
-    <row r="12" spans="1:14">
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>275</v>
+        <v>330</v>
       </c>
       <c r="C12" t="s">
-        <v>327</v>
-      </c>
-      <c r="D12" t="s">
-        <v>328</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="D12"/>
       <c r="E12" t="s">
-        <v>329</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
       <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12"/>
-    </row>
-    <row r="13" spans="1:14">
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
         <v>202</v>
       </c>
-      <c r="D13" t="s">
-        <v>331</v>
-      </c>
-      <c r="E13" t="s">
-        <v>332</v>
-      </c>
+      <c r="D13"/>
+      <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13"/>
       <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-    </row>
-    <row r="14" spans="1:14">
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -4324,13 +4251,8 @@
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="N14"/>
-    </row>
-    <row r="15" spans="1:14">
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -4346,17 +4268,14 @@
         <v>205</v>
       </c>
       <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-    </row>
-    <row r="16" spans="1:14">
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>96</v>
       </c>
-      <c r="B16"/>
+      <c r="B16" t="s">
+        <v>295</v>
+      </c>
       <c r="C16" t="s">
         <v>334</v>
       </c>
@@ -4368,60 +4287,52 @@
         <v>98</v>
       </c>
       <c r="G16"/>
-      <c r="H16"/>
+      <c r="H16" t="s">
+        <v>335</v>
+      </c>
       <c r="I16" t="s">
         <v>99</v>
       </c>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-    </row>
-    <row r="17" spans="1:14">
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>103</v>
       </c>
-      <c r="B17" t="s">
-        <v>335</v>
-      </c>
+      <c r="B17"/>
       <c r="C17" t="s">
         <v>336</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="F17" t="s">
         <v>209</v>
       </c>
-      <c r="G17"/>
+      <c r="G17" t="s">
+        <v>337</v>
+      </c>
       <c r="H17" t="s">
         <v>208</v>
       </c>
       <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-      <c r="M17"/>
-      <c r="N17"/>
-    </row>
-    <row r="18" spans="1:14">
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C18" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G18" t="s">
         <v>112</v>
@@ -4430,101 +4341,75 @@
         <v>206</v>
       </c>
       <c r="I18" t="s">
-        <v>339</v>
-      </c>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-    </row>
-    <row r="19" spans="1:14">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>113</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19"/>
+      <c r="C19" t="s">
+        <v>341</v>
+      </c>
+      <c r="D19" t="s">
+        <v>342</v>
+      </c>
+      <c r="E19" t="s">
+        <v>343</v>
+      </c>
+      <c r="F19" t="s">
+        <v>223</v>
+      </c>
+      <c r="G19" t="s">
         <v>116</v>
       </c>
-      <c r="C19" t="s">
-        <v>340</v>
-      </c>
-      <c r="D19" t="s">
-        <v>341</v>
-      </c>
-      <c r="E19" t="s">
-        <v>342</v>
-      </c>
-      <c r="F19" t="s">
-        <v>218</v>
-      </c>
-      <c r="G19"/>
       <c r="H19" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-    </row>
-    <row r="20" spans="1:14">
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C20" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20" t="s">
-        <v>345</v>
-      </c>
-      <c r="G20"/>
+        <v>346</v>
+      </c>
+      <c r="G20" t="s">
+        <v>124</v>
+      </c>
       <c r="H20" t="s">
         <v>200</v>
       </c>
       <c r="I20" t="s">
-        <v>123</v>
-      </c>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-    </row>
-    <row r="21" spans="1:14">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" t="s">
-        <v>295</v>
-      </c>
-      <c r="C21" t="s">
-        <v>101</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B21"/>
+      <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
-      <c r="H21" t="s">
-        <v>346</v>
-      </c>
-      <c r="I21" t="s">
-        <v>215</v>
-      </c>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="H21"/>
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -4534,15 +4419,10 @@
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-    </row>
-    <row r="23" spans="1:14">
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -4552,15 +4432,10 @@
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="N23"/>
-    </row>
-    <row r="24" spans="1:14">
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
         <v>347</v>
@@ -4574,15 +4449,10 @@
       </c>
       <c r="H24"/>
       <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24"/>
-    </row>
-    <row r="25" spans="1:14">
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
         <v>349</v>
@@ -4596,15 +4466,10 @@
       </c>
       <c r="H25"/>
       <c r="I25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
-      <c r="N25"/>
-    </row>
-    <row r="26" spans="1:14">
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B26" t="s">
         <v>351</v>
@@ -4612,7 +4477,7 @@
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F26"/>
       <c r="G26" t="s">
@@ -4620,15 +4485,10 @@
       </c>
       <c r="H26"/>
       <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-      <c r="N26"/>
-    </row>
-    <row r="27" spans="1:14">
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B27" t="s">
         <v>353</v>
@@ -4640,15 +4500,10 @@
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
-      <c r="J27"/>
-      <c r="K27"/>
-      <c r="L27"/>
-      <c r="M27"/>
-      <c r="N27"/>
-    </row>
-    <row r="28" spans="1:14">
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
         <v>236</v>
@@ -4660,15 +4515,10 @@
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
-      <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-      <c r="N28"/>
-    </row>
-    <row r="29" spans="1:14">
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
         <v>236</v>
@@ -4680,15 +4530,10 @@
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-      <c r="N29"/>
-    </row>
-    <row r="30" spans="1:14">
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
         <v>354</v>
@@ -4702,33 +4547,25 @@
       </c>
       <c r="H30"/>
       <c r="I30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-      <c r="N30"/>
-    </row>
-    <row r="31" spans="1:14">
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
-      <c r="D31"/>
+      <c r="D31" t="s">
+        <v>216</v>
+      </c>
       <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31" t="s">
-        <v>211</v>
-      </c>
-      <c r="I31" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-      <c r="N31"/>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31"/>
+      <c r="I31"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -4881,7 +4718,7 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="E6"/>
       <c r="F6" t="s">
@@ -4895,19 +4732,19 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>361</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
         <v>362</v>
@@ -4920,7 +4757,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -4933,7 +4770,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -4946,7 +4783,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10"/>
       <c r="C10"/>
@@ -4965,7 +4802,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
@@ -4984,7 +4821,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="s">
@@ -5007,7 +4844,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -5020,7 +4857,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
@@ -5034,9 +4871,7 @@
         <v>245</v>
       </c>
       <c r="G14"/>
-      <c r="H14" t="s">
-        <v>89</v>
-      </c>
+      <c r="H14"/>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
@@ -5057,24 +4892,24 @@
         <v>96</v>
       </c>
       <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
         <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
         <v>95</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I16" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -5082,12 +4917,14 @@
         <v>103</v>
       </c>
       <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
         <v>75</v>
       </c>
-      <c r="C17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17"/>
+      <c r="D17" t="s">
+        <v>216</v>
+      </c>
       <c r="E17" t="s">
         <v>205</v>
       </c>
@@ -5096,10 +4933,10 @@
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>211</v>
+        <v>35</v>
       </c>
       <c r="I17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -5110,7 +4947,7 @@
         <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -5119,7 +4956,7 @@
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I18" t="s">
         <v>105</v>
@@ -5132,8 +4969,12 @@
       <c r="B19" t="s">
         <v>284</v>
       </c>
-      <c r="C19"/>
-      <c r="D19"/>
+      <c r="C19" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
       <c r="E19" t="s">
         <v>208</v>
       </c>
@@ -5141,7 +4982,9 @@
         <v>209</v>
       </c>
       <c r="G19"/>
-      <c r="H19"/>
+      <c r="H19" t="s">
+        <v>101</v>
+      </c>
       <c r="I19"/>
     </row>
     <row r="20" spans="1:9">
@@ -5149,35 +4992,35 @@
         <v>120</v>
       </c>
       <c r="B20"/>
-      <c r="C20" t="s">
-        <v>220</v>
-      </c>
+      <c r="C20"/>
       <c r="D20" t="s">
         <v>369</v>
       </c>
       <c r="E20" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="F20" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
         <v>119</v>
       </c>
       <c r="I20" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21"/>
+      <c r="D21" t="s">
+        <v>124</v>
+      </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F21" t="s">
         <v>370</v>
@@ -5186,17 +5029,19 @@
       <c r="H21" t="s">
         <v>200</v>
       </c>
-      <c r="I21"/>
+      <c r="I21" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
         <v>371</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D22" t="s">
         <v>372</v>
@@ -5205,11 +5050,11 @@
         <v>373</v>
       </c>
       <c r="F22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I22" t="s">
         <v>374</v>
@@ -5217,7 +5062,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -5230,7 +5075,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
         <v>375</v>
@@ -5238,20 +5083,20 @@
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
         <v>376</v>
       </c>
       <c r="H24" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
         <v>377</v>
@@ -5270,7 +5115,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B26" t="s">
         <v>379</v>
@@ -5285,7 +5130,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B27" t="s">
         <v>380</v>
@@ -5294,17 +5139,17 @@
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G27"/>
       <c r="H27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
         <v>381</v>
@@ -5319,10 +5164,10 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" t="s">
         <v>154</v>
-      </c>
-      <c r="B29" t="s">
-        <v>153</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -5334,7 +5179,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B30"/>
       <c r="C30"/>
@@ -5351,7 +5196,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>

</xml_diff>

<commit_message>
Update TT to 9th March's v6.0
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -566,6 +566,9 @@
     <t>Dwh-GR2                                                Dr. Zulfiqar</t>
   </si>
   <si>
+    <t>CAL I-GR1                  Imran Shah</t>
+  </si>
+  <si>
     <t>TBW-G                                                 Sameera</t>
   </si>
   <si>
@@ -632,9 +635,6 @@
     <t>TBW-D                               Sameera</t>
   </si>
   <si>
-    <t>CAL I-GR1                  Imran Shah</t>
-  </si>
-  <si>
     <t xml:space="preserve">CA-GR1                                    Danish                         </t>
   </si>
   <si>
@@ -875,259 +875,259 @@
     <t>Prob-D                                                     Asma</t>
   </si>
   <si>
+    <t>OS-B                             Nausheen</t>
+  </si>
+  <si>
+    <t>Prob-B                                                                 Asma</t>
+  </si>
+  <si>
+    <t>CP-B                                                                           Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>CP-F                                             Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>Prob-E                                               Osama</t>
+  </si>
+  <si>
+    <t>Prob-A                                                             Osama</t>
+  </si>
+  <si>
+    <t>CN-F                                                          Faraz</t>
+  </si>
+  <si>
+    <t>Pst. B                        Michael</t>
+  </si>
+  <si>
+    <t>Psych-GR3 Sumaira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA-GR2                                                Ahsan                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pst. A                                                        Kashif </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pst. E                                                        Kashif </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pst. D                                         Kashif </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pst. D                                                    Kashif </t>
+  </si>
+  <si>
+    <t>OS-Lab E                                                                                                                                   Ms. Safia</t>
+  </si>
+  <si>
+    <t>CP-Lab A1+A2                                                                                                                             Tooba &amp; Ammara</t>
+  </si>
+  <si>
+    <t>DS-Lab C                                                                                                            Aziz+Mubashyra</t>
+  </si>
+  <si>
+    <t>OOAD-Lab  GR1                                                                                                                                        Nadeem</t>
+  </si>
+  <si>
+    <t>DS-Lab D                                                                                                                                 Faizan +Irfan</t>
+  </si>
+  <si>
+    <t>ITC-Lab A A1+A2                                                                                                    Rahemeen &amp; Majid</t>
+  </si>
+  <si>
+    <t>OS-Lab  F                                                                                                               Summiyah</t>
+  </si>
+  <si>
+    <t>CP-Lab B1+B2                                                                                                                                 Basit &amp; Maham</t>
+  </si>
+  <si>
+    <t>CN-Lab  E                                                                                                                                      Munim</t>
+  </si>
+  <si>
+    <t>DLD-Lab  C                                                                                                                              Farah</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t>CN-A                                                         Dr Sufian</t>
+  </si>
+  <si>
+    <t>CN-B                                                                    Dr Sufian</t>
+  </si>
+  <si>
+    <t>Dsci-GR2                                                     Dr Zeeshan</t>
+  </si>
+  <si>
+    <t>Dsci-GR1                                      Dr Zeeshan</t>
+  </si>
+  <si>
+    <t>IOT-GR2                                                        Dr. Farooque</t>
+  </si>
+  <si>
+    <t>IOT-GR1                                                          Dr. Farooque</t>
+  </si>
+  <si>
+    <t>NP-GR1                                            Shahbaz</t>
+  </si>
+  <si>
+    <t>IR-GR1                                                             Dr Rafi</t>
+  </si>
+  <si>
+    <t>DS-A                                     Zeshan</t>
+  </si>
+  <si>
+    <t>DS-B                                     Zeshan</t>
+  </si>
+  <si>
+    <t>DS-C                                  Zeshan</t>
+  </si>
+  <si>
+    <t>CN-E                                                          Faraz</t>
+  </si>
+  <si>
+    <t>TOA-C                                      Shaharbano</t>
+  </si>
+  <si>
+    <t>TOA-G                                     Shaharbano</t>
+  </si>
+  <si>
+    <t>ISPM-GR1                                       Ubaid</t>
+  </si>
+  <si>
+    <t>CAL I-GR1                                            Imran Shah</t>
+  </si>
+  <si>
+    <t>TOA-F                          Subhash</t>
+  </si>
+  <si>
+    <t>TOA-D                                               Subhash</t>
+  </si>
+  <si>
+    <t>TOA-A                                                Shahzad</t>
+  </si>
+  <si>
+    <t>TOA-E                                           Shahzad</t>
+  </si>
+  <si>
+    <t>Discrete- GR1                                 Dr Jalal</t>
+  </si>
+  <si>
+    <t>OS-A                                              Dr. Hasina</t>
+  </si>
+  <si>
+    <t>CV-GR1                               Dr Tahir syed</t>
+  </si>
+  <si>
+    <t>NM-GR1                              Dr Khusro</t>
+  </si>
+  <si>
+    <t>Prob-G                                   Amjad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pst. C                                          Kashif </t>
+  </si>
+  <si>
+    <t>Prob-D                                      Asma</t>
+  </si>
+  <si>
+    <t>Prob-F                                           Asma</t>
+  </si>
+  <si>
+    <t>DLD-G                                               Rabia</t>
+  </si>
+  <si>
+    <t>DLD-A                                         Rabia</t>
+  </si>
+  <si>
+    <t>Pst. B                      Michael</t>
+  </si>
+  <si>
+    <t>Prob-C                                        Osama</t>
+  </si>
+  <si>
+    <t>CM-GR1             Jameel</t>
+  </si>
+  <si>
+    <t>Prob-A                                             Osama</t>
+  </si>
+  <si>
+    <t>TBW-C                                                       Nazia</t>
+  </si>
+  <si>
+    <t>TBW-A                                                    Nazia</t>
+  </si>
+  <si>
+    <t>TBW-F                                              Nazia</t>
+  </si>
+  <si>
+    <t>CN-Lab  G                                                                                                                                   Faizan</t>
+  </si>
+  <si>
+    <t>COAL-Lab GR1                                                                                             Zain</t>
+  </si>
+  <si>
+    <t>CP-Lab C1+C2                                                                                                                            Tooba &amp; Irfan</t>
+  </si>
+  <si>
+    <t>CP-Lab E1+E2                                                                                                       Mahrukh &amp; Maham</t>
+  </si>
+  <si>
+    <t>ITC-Lab B B1+B2                                                                                             Rahemeen &amp; Majid</t>
+  </si>
+  <si>
+    <t>DB-Lab GR1                                                                                                    Mubashyra</t>
+  </si>
+  <si>
+    <t>CN-Lab  F                                                                                                                                         Munim</t>
+  </si>
+  <si>
+    <t>DLD-Lab  E                                                                                                                                     Farah</t>
+  </si>
+  <si>
+    <t>DLD-Lab  G                                                                                                                       M. Nadeem</t>
+  </si>
+  <si>
+    <t>FRIDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-G                                                  Dr Rauf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-C                                            Dr Rauf </t>
+  </si>
+  <si>
+    <t>J              UMM           A                                                                                                                                                       P                             R                         A                           Y                           E          R</t>
+  </si>
+  <si>
+    <t>CN-F                                            Faraz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-E                                               Farrukh </t>
+  </si>
+  <si>
+    <t>SE-B                                              Ahsan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-D                                               Farrukh </t>
+  </si>
+  <si>
+    <t>IS -GR2                          Abdul rehman</t>
+  </si>
+  <si>
+    <t>SE-C                                          Rubab</t>
+  </si>
+  <si>
+    <t>SE-E                                                     Rubab</t>
+  </si>
+  <si>
+    <t>SE-A                                       Rubab</t>
+  </si>
+  <si>
+    <t>NM-GR1             Dr Khusro</t>
+  </si>
+  <si>
     <t>LA-GR1                       Dr Fahad</t>
-  </si>
-  <si>
-    <t>OS-B                             Nausheen</t>
-  </si>
-  <si>
-    <t>Prob-B                                                                 Asma</t>
-  </si>
-  <si>
-    <t>CP-B                                                                           Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>CP-F                                             Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>Prob-E                                               Osama</t>
-  </si>
-  <si>
-    <t>Prob-A                                                             Osama</t>
-  </si>
-  <si>
-    <t>CN-F                                                          Faraz</t>
-  </si>
-  <si>
-    <t>Pst. B                        Michael</t>
-  </si>
-  <si>
-    <t>Psych-GR3 Sumaira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA-GR2                                                Ahsan                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pst. A                                                        Kashif </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pst. E                                                        Kashif </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pst. D                                         Kashif </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pst. D                                                    Kashif </t>
-  </si>
-  <si>
-    <t>OS-Lab E                                                                                                                                   Ms. Safia</t>
-  </si>
-  <si>
-    <t>CP-Lab A1+A2                                                                                                                             Tooba &amp; Ammara</t>
-  </si>
-  <si>
-    <t>DS-Lab C                                                                                                            Aziz+Mubashyra</t>
-  </si>
-  <si>
-    <t>OOAD-Lab  GR1                                                                                                                                        Nadeem</t>
-  </si>
-  <si>
-    <t>DS-Lab D                                                                                                                                 Faizan +Irfan</t>
-  </si>
-  <si>
-    <t>ITC-Lab A A1+A2                                                                                                    Rahemeen &amp; Majid</t>
-  </si>
-  <si>
-    <t>OS-Lab  F                                                                                                               Summiyah</t>
-  </si>
-  <si>
-    <t>CP-Lab B1+B2                                                                                                                                 Basit &amp; Maham</t>
-  </si>
-  <si>
-    <t>CN-Lab  E                                                                                                                                      Munim</t>
-  </si>
-  <si>
-    <t>DLD-Lab  C                                                                                                                              Farah</t>
-  </si>
-  <si>
-    <t>THURSDAY</t>
-  </si>
-  <si>
-    <t>CN-A                                                         Dr Sufian</t>
-  </si>
-  <si>
-    <t>CN-B                                                                    Dr Sufian</t>
-  </si>
-  <si>
-    <t>Dsci-GR2                                                     Dr Zeeshan</t>
-  </si>
-  <si>
-    <t>Dsci-GR1                                      Dr Zeeshan</t>
-  </si>
-  <si>
-    <t>IOT-GR2                                                        Dr. Farooque</t>
-  </si>
-  <si>
-    <t>IOT-GR1                                                          Dr. Farooque</t>
-  </si>
-  <si>
-    <t>NP-GR1                                            Shahbaz</t>
-  </si>
-  <si>
-    <t>IR-GR1                                                             Dr Rafi</t>
-  </si>
-  <si>
-    <t>DS-A                                     Zeshan</t>
-  </si>
-  <si>
-    <t>DS-B                                     Zeshan</t>
-  </si>
-  <si>
-    <t>DS-C                                  Zeshan</t>
-  </si>
-  <si>
-    <t>CN-E                                                          Faraz</t>
-  </si>
-  <si>
-    <t>TOA-C                                      Shaharbano</t>
-  </si>
-  <si>
-    <t>TOA-G                                     Shaharbano</t>
-  </si>
-  <si>
-    <t>ISPM-GR1                                       Ubaid</t>
-  </si>
-  <si>
-    <t>CAL I-GR1                                            Imran Shah</t>
-  </si>
-  <si>
-    <t>TOA-F                          Subhash</t>
-  </si>
-  <si>
-    <t>TOA-D                                               Subhash</t>
-  </si>
-  <si>
-    <t>TOA-A                                                Shahzad</t>
-  </si>
-  <si>
-    <t>TOA-E                                           Shahzad</t>
-  </si>
-  <si>
-    <t>Discrete- GR1                                 Dr Jalal</t>
-  </si>
-  <si>
-    <t>OS-A                                              Dr. Hasina</t>
-  </si>
-  <si>
-    <t>CV-GR1                               Dr Tahir syed</t>
-  </si>
-  <si>
-    <t>NM-GR1                              Dr Khusro</t>
-  </si>
-  <si>
-    <t>Prob-G                                   Amjad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pst. C                                          Kashif </t>
-  </si>
-  <si>
-    <t>Prob-D                                      Asma</t>
-  </si>
-  <si>
-    <t>Prob-F                                           Asma</t>
-  </si>
-  <si>
-    <t>DLD-G                                               Rabia</t>
-  </si>
-  <si>
-    <t>DLD-A                                         Rabia</t>
-  </si>
-  <si>
-    <t>Pst. B                      Michael</t>
-  </si>
-  <si>
-    <t>Prob-C                                        Osama</t>
-  </si>
-  <si>
-    <t>CM-GR1             Jameel</t>
-  </si>
-  <si>
-    <t>Prob-A                                             Osama</t>
-  </si>
-  <si>
-    <t>TBW-C                                                       Nazia</t>
-  </si>
-  <si>
-    <t>TBW-A                                                    Nazia</t>
-  </si>
-  <si>
-    <t>TBW-F                                              Nazia</t>
-  </si>
-  <si>
-    <t>CN-Lab  G                                                                                                                                   Faizan</t>
-  </si>
-  <si>
-    <t>COAL-Lab GR1                                                                                             Zain</t>
-  </si>
-  <si>
-    <t>CP-Lab C1+C2                                                                                                                            Tooba &amp; Irfan</t>
-  </si>
-  <si>
-    <t>CP-Lab E1+E2                                                                                                       Mahrukh &amp; Maham</t>
-  </si>
-  <si>
-    <t>ITC-Lab B B1+B2                                                                                             Rahemeen &amp; Majid</t>
-  </si>
-  <si>
-    <t>DB-Lab GR1                                                                                                    Mubashyra</t>
-  </si>
-  <si>
-    <t>CN-Lab  F                                                                                                                                         Munim</t>
-  </si>
-  <si>
-    <t>DLD-Lab  E                                                                                                                                     Farah</t>
-  </si>
-  <si>
-    <t>DLD-Lab  G                                                                                                                       M. Nadeem</t>
-  </si>
-  <si>
-    <t>FRIDAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-G                                                  Dr Rauf </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-C                                            Dr Rauf </t>
-  </si>
-  <si>
-    <t>J              UMM           A                                                                                                                                                       P                             R                         A                           Y                           E          R</t>
-  </si>
-  <si>
-    <t>CN-F                                            Faraz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-E                                               Farrukh </t>
-  </si>
-  <si>
-    <t>SE-B                                              Ahsan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-D                                               Farrukh </t>
-  </si>
-  <si>
-    <t>IS -GR2                          Abdul rehman</t>
-  </si>
-  <si>
-    <t>SE-C                                          Rubab</t>
-  </si>
-  <si>
-    <t>SE-E                                                     Rubab</t>
-  </si>
-  <si>
-    <t>SE-A                                       Rubab</t>
-  </si>
-  <si>
-    <t>NM-GR1             Dr Khusro</t>
   </si>
   <si>
     <t>Pst. B                                            Michael</t>
@@ -2673,12 +2673,14 @@
       <c r="E9" t="s">
         <v>180</v>
       </c>
-      <c r="F9"/>
+      <c r="F9" t="s">
+        <v>181</v>
+      </c>
       <c r="G9" t="s">
         <v>110</v>
       </c>
       <c r="H9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -2698,17 +2700,17 @@
         <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -2722,10 +2724,10 @@
         <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D11" t="s">
         <v>84</v>
@@ -2734,16 +2736,16 @@
         <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
@@ -2756,28 +2758,28 @@
         <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C12" t="s">
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E12" t="s">
         <v>111</v>
       </c>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J12"/>
       <c r="K12"/>
@@ -2790,10 +2792,10 @@
         <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D13" t="s">
         <v>121</v>
@@ -2804,10 +2806,10 @@
         <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -2820,7 +2822,7 @@
         <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
@@ -2829,9 +2831,7 @@
       <c r="E14" t="s">
         <v>89</v>
       </c>
-      <c r="F14" t="s">
-        <v>203</v>
-      </c>
+      <c r="F14"/>
       <c r="G14"/>
       <c r="H14" t="s">
         <v>204</v>
@@ -3498,10 +3498,10 @@
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F10" t="s">
         <v>260</v>
@@ -3648,11 +3648,9 @@
       <c r="B16" t="s">
         <v>283</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16"/>
+      <c r="D16" t="s">
         <v>284</v>
-      </c>
-      <c r="D16" t="s">
-        <v>285</v>
       </c>
       <c r="E16" t="s">
         <v>206</v>
@@ -3662,7 +3660,7 @@
         <v>219</v>
       </c>
       <c r="H16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I16"/>
     </row>
@@ -3671,7 +3669,7 @@
         <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C17" t="s">
         <v>92</v>
@@ -3680,14 +3678,14 @@
         <v>115</v>
       </c>
       <c r="E17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F17"/>
       <c r="G17" t="s">
+        <v>288</v>
+      </c>
+      <c r="H17" t="s">
         <v>289</v>
-      </c>
-      <c r="H17" t="s">
-        <v>290</v>
       </c>
       <c r="I17"/>
     </row>
@@ -3696,14 +3694,14 @@
         <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
+        <v>291</v>
+      </c>
+      <c r="E18" t="s">
         <v>292</v>
-      </c>
-      <c r="E18" t="s">
-        <v>293</v>
       </c>
       <c r="F18" t="s">
         <v>123</v>
@@ -3719,7 +3717,7 @@
         <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C19" t="s">
         <v>211</v>
@@ -3744,22 +3742,22 @@
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20" t="s">
+        <v>294</v>
+      </c>
+      <c r="E20" t="s">
         <v>295</v>
-      </c>
-      <c r="E20" t="s">
-        <v>296</v>
       </c>
       <c r="F20" t="s">
         <v>137</v>
       </c>
       <c r="G20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H20" t="s">
         <v>133</v>
       </c>
       <c r="I20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -3806,14 +3804,16 @@
         <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
-      <c r="E24"/>
+      <c r="E24" t="s">
+        <v>153</v>
+      </c>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -3823,14 +3823,14 @@
         <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -3840,14 +3840,14 @@
         <v>147</v>
       </c>
       <c r="B26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -3857,14 +3857,14 @@
         <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -3896,7 +3896,7 @@
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
@@ -3907,7 +3907,7 @@
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D30"/>
       <c r="E30"/>
@@ -3970,7 +3970,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -4057,19 +4057,19 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5" t="s">
         <v>310</v>
-      </c>
-      <c r="C5" t="s">
-        <v>311</v>
       </c>
       <c r="D5" t="s">
         <v>53</v>
       </c>
       <c r="E5" t="s">
+        <v>311</v>
+      </c>
+      <c r="F5" t="s">
         <v>312</v>
-      </c>
-      <c r="F5" t="s">
-        <v>313</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
@@ -4080,16 +4080,16 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C6" t="s">
         <v>314</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>315</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>316</v>
-      </c>
-      <c r="E6" t="s">
-        <v>317</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="s">
@@ -4106,14 +4106,14 @@
         <v>88</v>
       </c>
       <c r="C7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" t="s">
         <v>318</v>
-      </c>
-      <c r="D7" t="s">
-        <v>319</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
@@ -4125,14 +4125,14 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
+        <v>321</v>
+      </c>
+      <c r="F8" t="s">
         <v>322</v>
-      </c>
-      <c r="F8" t="s">
-        <v>323</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
@@ -4149,16 +4149,16 @@
         <v>84</v>
       </c>
       <c r="D9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E9" t="s">
         <v>324</v>
       </c>
-      <c r="E9" t="s">
-        <v>325</v>
-      </c>
       <c r="F9" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="G9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -4171,11 +4171,11 @@
         <v>275</v>
       </c>
       <c r="C10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -4187,10 +4187,10 @@
         <v>61</v>
       </c>
       <c r="B11" t="s">
+        <v>327</v>
+      </c>
+      <c r="C11" t="s">
         <v>328</v>
-      </c>
-      <c r="C11" t="s">
-        <v>329</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
@@ -4208,17 +4208,17 @@
         <v>69</v>
       </c>
       <c r="B12" t="s">
+        <v>329</v>
+      </c>
+      <c r="C12" t="s">
         <v>330</v>
-      </c>
-      <c r="C12" t="s">
-        <v>331</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
         <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -4261,7 +4261,7 @@
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
@@ -4274,10 +4274,10 @@
         <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I16" t="s">
         <v>99</v>
@@ -4300,7 +4300,7 @@
       </c>
       <c r="B17"/>
       <c r="C17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
@@ -4310,7 +4310,7 @@
         <v>209</v>
       </c>
       <c r="G17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H17" t="s">
         <v>208</v>
@@ -4322,10 +4322,10 @@
         <v>107</v>
       </c>
       <c r="B18" t="s">
+        <v>337</v>
+      </c>
+      <c r="C18" t="s">
         <v>338</v>
-      </c>
-      <c r="C18" t="s">
-        <v>339</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
@@ -4341,7 +4341,7 @@
         <v>206</v>
       </c>
       <c r="I18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -4350,13 +4350,13 @@
       </c>
       <c r="B19"/>
       <c r="C19" t="s">
+        <v>340</v>
+      </c>
+      <c r="D19" t="s">
         <v>341</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>342</v>
-      </c>
-      <c r="E19" t="s">
-        <v>343</v>
       </c>
       <c r="F19" t="s">
         <v>223</v>
@@ -4374,21 +4374,21 @@
         <v>120</v>
       </c>
       <c r="B20" t="s">
+        <v>343</v>
+      </c>
+      <c r="C20" t="s">
         <v>344</v>
-      </c>
-      <c r="C20" t="s">
-        <v>345</v>
       </c>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G20" t="s">
         <v>124</v>
       </c>
       <c r="H20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I20" t="s">
         <v>220</v>
@@ -4438,14 +4438,14 @@
         <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -4455,14 +4455,14 @@
         <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -4472,7 +4472,7 @@
         <v>147</v>
       </c>
       <c r="B26" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -4481,7 +4481,7 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -4491,7 +4491,7 @@
         <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -4536,14 +4536,14 @@
         <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
@@ -4600,7 +4600,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -4693,17 +4693,17 @@
         <v>252</v>
       </c>
       <c r="D5" t="s">
+        <v>356</v>
+      </c>
+      <c r="E5" t="s">
         <v>357</v>
-      </c>
-      <c r="E5" t="s">
-        <v>358</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="s">
+        <v>358</v>
+      </c>
+      <c r="H5" t="s">
         <v>359</v>
-      </c>
-      <c r="H5" t="s">
-        <v>360</v>
       </c>
       <c r="I5"/>
     </row>
@@ -4718,11 +4718,11 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E6"/>
       <c r="F6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G6"/>
       <c r="H6" t="s">
@@ -4741,17 +4741,17 @@
         <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E7" t="s">
         <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I7"/>
     </row>
@@ -4788,10 +4788,10 @@
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -4808,16 +4808,22 @@
       <c r="C11" t="s">
         <v>277</v>
       </c>
-      <c r="D11"/>
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
       <c r="E11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F11" t="s">
         <v>277</v>
       </c>
       <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
+      <c r="H11" t="s">
+        <v>201</v>
+      </c>
+      <c r="I11" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
@@ -4825,20 +4831,20 @@
       </c>
       <c r="B12"/>
       <c r="C12" t="s">
+        <v>364</v>
+      </c>
+      <c r="D12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" t="s">
+        <v>309</v>
+      </c>
+      <c r="F12" t="s">
         <v>365</v>
-      </c>
-      <c r="D12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E12" t="s">
-        <v>310</v>
-      </c>
-      <c r="F12" t="s">
-        <v>366</v>
       </c>
       <c r="G12"/>
       <c r="H12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I12"/>
     </row>
@@ -4929,7 +4935,7 @@
         <v>205</v>
       </c>
       <c r="F17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
@@ -4967,7 +4973,7 @@
         <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>284</v>
+        <v>368</v>
       </c>
       <c r="C19" t="s">
         <v>211</v>
@@ -4985,7 +4991,9 @@
       <c r="H19" t="s">
         <v>101</v>
       </c>
-      <c r="I19"/>
+      <c r="I19" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
@@ -5004,11 +5012,9 @@
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>119</v>
-      </c>
-      <c r="I20" t="s">
-        <v>342</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
@@ -5016,9 +5022,7 @@
       </c>
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21" t="s">
-        <v>124</v>
-      </c>
+      <c r="D21"/>
       <c r="E21" t="s">
         <v>134</v>
       </c>
@@ -5027,11 +5031,9 @@
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>200</v>
-      </c>
-      <c r="I21" t="s">
-        <v>121</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
@@ -5050,7 +5052,7 @@
         <v>373</v>
       </c>
       <c r="F22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G22"/>
       <c r="H22" t="s">

</xml_diff>

<commit_message>
Update TT - 14th March
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -1028,10 +1028,10 @@
     <t xml:space="preserve">Pst. C                                          Kashif </t>
   </si>
   <si>
+    <t>Prob-F                                           Asma</t>
+  </si>
+  <si>
     <t>Prob-D                                      Asma</t>
-  </si>
-  <si>
-    <t>Prob-F                                           Asma</t>
   </si>
   <si>
     <t>DLD-G                                               Rabia</t>
@@ -4071,7 +4071,9 @@
       <c r="F5" t="s">
         <v>312</v>
       </c>
-      <c r="G5"/>
+      <c r="G5" t="s">
+        <v>88</v>
+      </c>
       <c r="H5"/>
       <c r="I5"/>
     </row>
@@ -4102,9 +4104,7 @@
       <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
-        <v>88</v>
-      </c>
+      <c r="B7"/>
       <c r="C7" t="s">
         <v>317</v>
       </c>
@@ -4298,9 +4298,11 @@
       <c r="A17" t="s">
         <v>103</v>
       </c>
-      <c r="B17"/>
+      <c r="B17" t="s">
+        <v>335</v>
+      </c>
       <c r="C17" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
@@ -4309,9 +4311,7 @@
       <c r="F17" t="s">
         <v>209</v>
       </c>
-      <c r="G17" t="s">
-        <v>336</v>
-      </c>
+      <c r="G17"/>
       <c r="H17" t="s">
         <v>208</v>
       </c>
@@ -4348,7 +4348,9 @@
       <c r="A19" t="s">
         <v>113</v>
       </c>
-      <c r="B19"/>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
       <c r="C19" t="s">
         <v>340</v>
       </c>
@@ -4361,9 +4363,7 @@
       <c r="F19" t="s">
         <v>223</v>
       </c>
-      <c r="G19" t="s">
-        <v>116</v>
-      </c>
+      <c r="G19"/>
       <c r="H19" t="s">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
Update TT to v7.0
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -122,7 +122,220 @@
     <t xml:space="preserve">CA-GR3             Ahsan                        </t>
   </si>
   <si>
-    <t>SE-C                    Rubab</t>
+    <t>SE-C                                       Rubab</t>
+  </si>
+  <si>
+    <t>SE-A                        Rubab</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>TOA-F                             Subhash</t>
+  </si>
+  <si>
+    <t>OS-B                        Nausheen</t>
+  </si>
+  <si>
+    <t>DLD-E                      Nouman</t>
+  </si>
+  <si>
+    <t>DLD-F                      Nouman</t>
+  </si>
+  <si>
+    <t>TOA-B                               Subhash</t>
+  </si>
+  <si>
+    <t>TOA-D                                            Subhash</t>
+  </si>
+  <si>
+    <t>DLD-B                      Nouman</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>CP-E                             Faiza</t>
+  </si>
+  <si>
+    <t>CP-G                             Faiza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-D                               Farrukh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-F                               Farrukh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-E                              Farrukh </t>
+  </si>
+  <si>
+    <t>OOAD-GR1                  Faiza</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA-GR1             Danish                         </t>
+  </si>
+  <si>
+    <t>CC-GR1                                          M. Shahzad</t>
+  </si>
+  <si>
+    <t>CC-GR2                                          M. Shahzad</t>
+  </si>
+  <si>
+    <t>OS-E               Tania</t>
+  </si>
+  <si>
+    <t>OS-D                     Tania</t>
+  </si>
+  <si>
+    <t>TOA-A                             Shahzad</t>
+  </si>
+  <si>
+    <t>TOA-E                                Shahzad</t>
+  </si>
+  <si>
+    <t>SE-F                           Javeria</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>ITC-A                             Shahbaz</t>
+  </si>
+  <si>
+    <t>ITC-C                            Shahbaz</t>
+  </si>
+  <si>
+    <t>DLD-D                      Bahraj</t>
+  </si>
+  <si>
+    <t>PIT-GR1                           Khalid</t>
+  </si>
+  <si>
+    <t>PIT-GR2                                                  Khalid</t>
+  </si>
+  <si>
+    <t>EP-GR2                                Wamiq</t>
+  </si>
+  <si>
+    <t>EP-GR1                                 Wamiq</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>ITC-B                            Tania</t>
+  </si>
+  <si>
+    <t>OS-A                            Dr. Hasina</t>
+  </si>
+  <si>
+    <t>Dsci.-GR3                                     Dr. Atif</t>
+  </si>
+  <si>
+    <t>Dsci.-GR4                                     Dr. Atif</t>
+  </si>
+  <si>
+    <t>SE-D                         Javeria</t>
+  </si>
+  <si>
+    <t>IHRM-GR2                               M. Zeeshan</t>
+  </si>
+  <si>
+    <t>IHRM-GR1                                 M. Zeeshan</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>DS-A                         Zeshan</t>
+  </si>
+  <si>
+    <t>Eng Comp. A2                                                   Faiza</t>
+  </si>
+  <si>
+    <t>DS-C                     Zeshan</t>
+  </si>
+  <si>
+    <t>DS-B                           Zeshan</t>
+  </si>
+  <si>
+    <t>Eng Comp. E2                                                   Faiza</t>
+  </si>
+  <si>
+    <t>HCI-GR1                               Bahraj</t>
+  </si>
+  <si>
+    <t>HCI-GR2                               Bahraj</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-C                               Dr Rauf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-G                               Dr Rauf </t>
+  </si>
+  <si>
+    <t>COAL-GR2            Danish</t>
+  </si>
+  <si>
+    <t>COAL-GR1            Danish</t>
+  </si>
+  <si>
+    <t>CR-3 EE</t>
+  </si>
+  <si>
+    <t>CP-B                             Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>CP-D                             Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>BE-GR1                     Javaid Qureshi</t>
+  </si>
+  <si>
+    <t>CP-F                             Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>Eng Comp. C2                                                   Faiza</t>
+  </si>
+  <si>
+    <t>CR-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA-GR2             Ahsan                        </t>
+  </si>
+  <si>
+    <t>CAL II-A                  Fareeha</t>
+  </si>
+  <si>
+    <t>CAL II-C                  Fareeha</t>
+  </si>
+  <si>
+    <t>CAL II-E                  Fareeha</t>
+  </si>
+  <si>
+    <t>IRS-G                                            Shahzad</t>
+  </si>
+  <si>
+    <t>AL-GR1            Shahzad Sheikh</t>
+  </si>
+  <si>
+    <t>CR-7</t>
+  </si>
+  <si>
+    <t>TBW-F                               Nazia</t>
+  </si>
+  <si>
+    <t>TBW-A                               Nazia</t>
+  </si>
+  <si>
+    <t>TBW-C                               Nazia</t>
   </si>
   <si>
     <t>Eng Comp. D1                                                   Hafza Yusra</t>
@@ -131,219 +344,6 @@
     <t>Eng Comp. B1                                                   Hafza Yusra</t>
   </si>
   <si>
-    <t>SE-A                        Rubab</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>TOA-F                             Subhash</t>
-  </si>
-  <si>
-    <t>OS-B                        Nausheen</t>
-  </si>
-  <si>
-    <t>DLD-E                      Nouman</t>
-  </si>
-  <si>
-    <t>DLD-F                      Nouman</t>
-  </si>
-  <si>
-    <t>TOA-B                               Subhash</t>
-  </si>
-  <si>
-    <t>TOA-D                                            Subhash</t>
-  </si>
-  <si>
-    <t>DLD-B                      Nouman</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>CP-E                             Faiza</t>
-  </si>
-  <si>
-    <t>CP-G                             Faiza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-D                               Farrukh </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-F                               Farrukh </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-E                              Farrukh </t>
-  </si>
-  <si>
-    <t>OOAD-GR1                  Faiza</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA-GR1             Danish                         </t>
-  </si>
-  <si>
-    <t>CC-GR1                                          M. Shahzad</t>
-  </si>
-  <si>
-    <t>CC-GR2                                          M. Shahzad</t>
-  </si>
-  <si>
-    <t>OS-E               Tania</t>
-  </si>
-  <si>
-    <t>OS-D                     Tania</t>
-  </si>
-  <si>
-    <t>TOA-A                             Shahzad</t>
-  </si>
-  <si>
-    <t>TOA-E                                Shahzad</t>
-  </si>
-  <si>
-    <t>SE-F                           Javeria</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>ITC-A                             Shahbaz</t>
-  </si>
-  <si>
-    <t>ITC-C                            Shahbaz</t>
-  </si>
-  <si>
-    <t>DLD-D                      Bahraj</t>
-  </si>
-  <si>
-    <t>PIT-GR1                           Khalid</t>
-  </si>
-  <si>
-    <t>PIT-GR2                                                  Khalid</t>
-  </si>
-  <si>
-    <t>EP-GR2                                Wamiq</t>
-  </si>
-  <si>
-    <t>EP-GR1                                 Wamiq</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>ITC-B                            Tania</t>
-  </si>
-  <si>
-    <t>OS-A                            Dr. Hasina</t>
-  </si>
-  <si>
-    <t>Dsci.-GR3                                     Dr. Atif</t>
-  </si>
-  <si>
-    <t>Dsci.-GR4                                     Dr. Atif</t>
-  </si>
-  <si>
-    <t>SE-D                         Javeria</t>
-  </si>
-  <si>
-    <t>IHRM-GR2                               M. Zeeshan</t>
-  </si>
-  <si>
-    <t>IHRM-GR1                                 M. Zeeshan</t>
-  </si>
-  <si>
-    <t>R109</t>
-  </si>
-  <si>
-    <t>DS-A                         Zeshan</t>
-  </si>
-  <si>
-    <t>Eng Comp. A2                                                   Faiza</t>
-  </si>
-  <si>
-    <t>DS-C                     Zeshan</t>
-  </si>
-  <si>
-    <t>DS-B                           Zeshan</t>
-  </si>
-  <si>
-    <t>Eng Comp. E2                                                   Faiza</t>
-  </si>
-  <si>
-    <t>HCI-GR1                               Bahraj</t>
-  </si>
-  <si>
-    <t>HCI-GR2                               Bahraj</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-C                               Dr Rauf </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-G                               Dr Rauf </t>
-  </si>
-  <si>
-    <t>COAL-GR2            Danish</t>
-  </si>
-  <si>
-    <t>COAL-GR1            Danish</t>
-  </si>
-  <si>
-    <t>CR-3 EE</t>
-  </si>
-  <si>
-    <t>CP-B                             Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>CP-D                             Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>BE-GR1                     Javaid Qureshi</t>
-  </si>
-  <si>
-    <t>CP-F                             Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>Eng Comp. C2                                                   Faiza</t>
-  </si>
-  <si>
-    <t>CR-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA-GR2             Ahsan                        </t>
-  </si>
-  <si>
-    <t>CAL II-A                  Fareeha</t>
-  </si>
-  <si>
-    <t>CAL II-C                  Fareeha</t>
-  </si>
-  <si>
-    <t>CAL II-E                  Fareeha</t>
-  </si>
-  <si>
-    <t>IRS-G                                            Shahzad</t>
-  </si>
-  <si>
-    <t>AL-GR1            Shahzad Sheikh</t>
-  </si>
-  <si>
-    <t>CR-7</t>
-  </si>
-  <si>
-    <t>TBW-F                               Nazia</t>
-  </si>
-  <si>
-    <t>TBW-A                               Nazia</t>
-  </si>
-  <si>
-    <t>TBW-C                               Nazia</t>
-  </si>
-  <si>
     <t>CR-10</t>
   </si>
   <si>
@@ -395,6 +395,9 @@
     <t>Psych-GR1 Sumaira</t>
   </si>
   <si>
+    <t>Eng Comp. E1                                                   Ahmed Bux</t>
+  </si>
+  <si>
     <t>Eng Comp. F2                                                   Ahmed Bux</t>
   </si>
   <si>
@@ -416,6 +419,12 @@
     <t>Prob-F                        Asma</t>
   </si>
   <si>
+    <t>Eng Comp. D2                                                   Javed Iqbal</t>
+  </si>
+  <si>
+    <t>Eng Comp. C1                                                   Javed Iqbal</t>
+  </si>
+  <si>
     <t>OB-GR1            Asiya</t>
   </si>
   <si>
@@ -434,9 +443,6 @@
     <t>CAL II-B                  Nadeem</t>
   </si>
   <si>
-    <t>Eng Comp. C1                                                   Javed Iqbal</t>
-  </si>
-  <si>
     <t>LABS</t>
   </si>
   <si>
@@ -500,13 +506,7 @@
     <t>LLC</t>
   </si>
   <si>
-    <t>Eng Comp. D2                                                   Nasir</t>
-  </si>
-  <si>
-    <t>Eng Comp. E1                                                   Nasir</t>
-  </si>
-  <si>
-    <t>ENG-GR1                                                   Nasir</t>
+    <t>ENG-GR1                                                   Nazia</t>
   </si>
   <si>
     <t>TUESDAY</t>
@@ -572,6 +572,9 @@
     <t>TBW-G                                                 Sameera</t>
   </si>
   <si>
+    <t>OOAD-GR1                                    Faiza</t>
+  </si>
+  <si>
     <t>CN-C                                            Shoaib</t>
   </si>
   <si>
@@ -627,9 +630,6 @@
   </si>
   <si>
     <t>Eng Comp. B2                                                   Ahmed Bux</t>
-  </si>
-  <si>
-    <t>OOAD-GR1                                    Faiza</t>
   </si>
   <si>
     <t>TBW-D                               Sameera</t>
@@ -1711,17 +1711,13 @@
       <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>34</v>
-      </c>
-      <c r="H7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" t="s">
-        <v>36</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -1732,29 +1728,29 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
         <v>42</v>
-      </c>
-      <c r="H8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -1765,27 +1761,27 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
         <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" t="s">
         <v>49</v>
-      </c>
-      <c r="H9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" t="s">
-        <v>51</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -1796,31 +1792,31 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
         <v>52</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>53</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>54</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>56</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>57</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>58</v>
-      </c>
-      <c r="H10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" t="s">
-        <v>60</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
@@ -1831,29 +1827,29 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
         <v>61</v>
-      </c>
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" t="s">
-        <v>63</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" t="s">
         <v>64</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>65</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>66</v>
-      </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" t="s">
-        <v>68</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
@@ -1864,29 +1860,29 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
         <v>69</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>70</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>71</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" t="s">
-        <v>73</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" t="s">
         <v>74</v>
-      </c>
-      <c r="H12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" t="s">
-        <v>76</v>
       </c>
       <c r="J12"/>
       <c r="K12"/>
@@ -1897,29 +1893,29 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
         <v>78</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>79</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>80</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>81</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>82</v>
-      </c>
-      <c r="H13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" t="s">
-        <v>84</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -1930,22 +1926,22 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -1957,27 +1953,27 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
         <v>90</v>
-      </c>
-      <c r="B15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" t="s">
-        <v>92</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
@@ -1988,27 +1984,27 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" t="s">
         <v>96</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>97</v>
-      </c>
-      <c r="C16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" t="s">
-        <v>99</v>
       </c>
       <c r="E16"/>
       <c r="F16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -2019,15 +2015,19 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
+      <c r="E17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" t="s">
+        <v>104</v>
+      </c>
       <c r="G17" t="s">
         <v>105</v>
       </c>
@@ -2117,12 +2117,14 @@
       <c r="F20" t="s">
         <v>123</v>
       </c>
-      <c r="G20"/>
+      <c r="G20" t="s">
+        <v>124</v>
+      </c>
       <c r="H20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
@@ -2133,25 +2135,29 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C21"/>
       <c r="D21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F21" t="s">
-        <v>130</v>
-      </c>
-      <c r="G21"/>
-      <c r="H21"/>
+        <v>131</v>
+      </c>
+      <c r="G21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H21" t="s">
+        <v>133</v>
+      </c>
       <c r="I21" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
@@ -2162,25 +2168,23 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E22"/>
       <c r="F22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G22" t="s">
-        <v>136</v>
-      </c>
-      <c r="H22" t="s">
-        <v>137</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2191,7 +2195,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -2210,21 +2214,21 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F24" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -2237,14 +2241,14 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C25"/>
       <c r="D25" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E25"/>
       <c r="F25"/>
@@ -2260,10 +2264,10 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -2281,10 +2285,10 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -2302,18 +2306,18 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F28" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G28"/>
       <c r="H28"/>
@@ -2327,10 +2331,10 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -2348,16 +2352,16 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
@@ -2371,18 +2375,14 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
-      <c r="D31" t="s">
-        <v>159</v>
-      </c>
+      <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
-      <c r="G31" t="s">
-        <v>160</v>
-      </c>
+      <c r="G31"/>
       <c r="H31" t="s">
         <v>161</v>
       </c>
@@ -2540,16 +2540,16 @@
         <v>164</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
         <v>165</v>
@@ -2568,16 +2568,16 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
         <v>167</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
         <v>168</v>
@@ -2603,10 +2603,10 @@
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
         <v>172</v>
@@ -2616,10 +2616,10 @@
         <v>173</v>
       </c>
       <c r="H7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
@@ -2646,10 +2646,10 @@
         <v>177</v>
       </c>
       <c r="H8" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" t="s">
         <v>137</v>
-      </c>
-      <c r="I8" t="s">
-        <v>134</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -2659,13 +2659,13 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
         <v>178</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
         <v>179</v>
@@ -2682,7 +2682,9 @@
       <c r="H9" t="s">
         <v>182</v>
       </c>
-      <c r="I9"/>
+      <c r="I9" t="s">
+        <v>183</v>
+      </c>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
@@ -2691,26 +2693,26 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -2721,31 +2723,31 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
@@ -2755,31 +2757,31 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C12" t="s">
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E12" t="s">
         <v>111</v>
       </c>
       <c r="F12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J12"/>
       <c r="K12"/>
@@ -2789,13 +2791,13 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D13" t="s">
         <v>121</v>
@@ -2806,10 +2808,10 @@
         <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I13" t="s">
-        <v>202</v>
+        <v>124</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -2819,17 +2821,17 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
         <v>203</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -2845,10 +2847,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
         <v>205</v>
@@ -2858,7 +2860,7 @@
       </c>
       <c r="E15"/>
       <c r="F15" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
@@ -2873,23 +2875,23 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16"/>
       <c r="C16" t="s">
         <v>208</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H16" t="s">
         <v>209</v>
@@ -2905,7 +2907,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
         <v>115</v>
@@ -2948,7 +2950,7 @@
         <v>112</v>
       </c>
       <c r="F18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G18" t="s">
         <v>217</v>
@@ -2976,7 +2978,7 @@
         <v>221</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E19"/>
       <c r="F19" t="s">
@@ -2988,7 +2990,9 @@
       <c r="H19" t="s">
         <v>224</v>
       </c>
-      <c r="I19"/>
+      <c r="I19" t="s">
+        <v>161</v>
+      </c>
       <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
@@ -3021,7 +3025,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
@@ -3039,7 +3043,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -3057,7 +3061,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -3075,7 +3079,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
         <v>227</v>
@@ -3085,7 +3089,7 @@
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -3097,7 +3101,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
         <v>228</v>
@@ -3125,7 +3129,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
         <v>233</v>
@@ -3145,7 +3149,7 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
         <v>234</v>
@@ -3167,7 +3171,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
         <v>236</v>
@@ -3187,7 +3191,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
         <v>236</v>
@@ -3207,7 +3211,7 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
@@ -3229,20 +3233,16 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
-      <c r="D31" t="s">
-        <v>160</v>
-      </c>
+      <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
       <c r="H31"/>
-      <c r="I31" t="s">
-        <v>161</v>
-      </c>
+      <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
       <c r="L31"/>
@@ -3384,7 +3384,7 @@
         <v>243</v>
       </c>
       <c r="G5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -3394,10 +3394,10 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
         <v>244</v>
@@ -3422,13 +3422,13 @@
         <v>247</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
         <v>248</v>
@@ -3437,16 +3437,16 @@
         <v>249</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
         <v>250</v>
@@ -3466,7 +3466,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
         <v>254</v>
@@ -3491,17 +3491,17 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
         <v>259</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F10" t="s">
         <v>260</v>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>263</v>
@@ -3525,10 +3525,10 @@
         <v>264</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
         <v>117</v>
@@ -3541,13 +3541,13 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>266</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
         <v>267</v>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
         <v>271</v>
@@ -3580,7 +3580,7 @@
         <v>272</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
         <v>273</v>
@@ -3590,12 +3590,12 @@
         <v>274</v>
       </c>
       <c r="I13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
         <v>275</v>
@@ -3620,7 +3620,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -3628,22 +3628,22 @@
         <v>281</v>
       </c>
       <c r="E15" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
         <v>282</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
         <v>283</v>
@@ -3666,13 +3666,13 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
         <v>286</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
         <v>115</v>
@@ -3680,7 +3680,9 @@
       <c r="E17" t="s">
         <v>287</v>
       </c>
-      <c r="F17"/>
+      <c r="F17" t="s">
+        <v>161</v>
+      </c>
       <c r="G17" t="s">
         <v>288</v>
       </c>
@@ -3709,7 +3711,7 @@
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -3723,7 +3725,7 @@
         <v>211</v>
       </c>
       <c r="D19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
         <v>119</v>
@@ -3732,7 +3734,7 @@
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3748,13 +3750,13 @@
         <v>295</v>
       </c>
       <c r="F20" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G20" t="s">
         <v>296</v>
       </c>
       <c r="H20" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="I20" t="s">
         <v>297</v>
@@ -3762,20 +3764,24 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21"/>
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21"/>
+      <c r="G21" t="s">
+        <v>124</v>
+      </c>
       <c r="H21"/>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -3788,7 +3794,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -3801,7 +3807,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
         <v>298</v>
@@ -3809,7 +3815,7 @@
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
@@ -3820,7 +3826,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
         <v>300</v>
@@ -3837,7 +3843,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
         <v>302</v>
@@ -3854,7 +3860,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
         <v>304</v>
@@ -3871,7 +3877,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
         <v>236</v>
@@ -3886,7 +3892,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
         <v>236</v>
@@ -3903,7 +3909,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
@@ -3920,20 +3926,14 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
-      <c r="D31" t="s">
-        <v>159</v>
-      </c>
+      <c r="D31"/>
       <c r="E31"/>
-      <c r="F31" t="s">
-        <v>161</v>
-      </c>
-      <c r="G31" t="s">
-        <v>160</v>
-      </c>
+      <c r="F31"/>
+      <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
     </row>
@@ -4063,7 +4063,7 @@
         <v>310</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
         <v>311</v>
@@ -4072,7 +4072,7 @@
         <v>312</v>
       </c>
       <c r="G5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -4095,7 +4095,7 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -4121,7 +4121,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
@@ -4140,13 +4140,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
         <v>323</v>
@@ -4165,7 +4165,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
         <v>275</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>327</v>
@@ -4194,7 +4194,7 @@
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
         <v>252</v>
@@ -4205,7 +4205,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>329</v>
@@ -4226,7 +4226,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
@@ -4241,7 +4241,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -4254,7 +4254,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -4271,7 +4271,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
         <v>294</v>
@@ -4281,22 +4281,22 @@
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
         <v>334</v>
       </c>
       <c r="I16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
         <v>335</v>
@@ -4329,10 +4329,10 @@
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F18" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G18" t="s">
         <v>112</v>
@@ -4385,10 +4385,10 @@
         <v>345</v>
       </c>
       <c r="G20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H20" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I20" t="s">
         <v>220</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -4422,7 +4422,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -4435,7 +4435,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
         <v>346</v>
@@ -4452,7 +4452,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
         <v>348</v>
@@ -4469,7 +4469,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
         <v>350</v>
@@ -4488,7 +4488,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
         <v>352</v>
@@ -4503,7 +4503,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
         <v>236</v>
@@ -4518,7 +4518,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
         <v>236</v>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
         <v>353</v>
@@ -4550,7 +4550,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -4559,10 +4559,10 @@
       </c>
       <c r="E31"/>
       <c r="F31" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="G31" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
@@ -4735,7 +4735,7 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -4744,7 +4744,7 @@
         <v>360</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
         <v>361</v>
@@ -4757,7 +4757,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -4770,7 +4770,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -4783,15 +4783,15 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -4802,14 +4802,14 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
         <v>277</v>
       </c>
       <c r="D11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E11" t="s">
         <v>363</v>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I11" t="s">
         <v>121</v>
@@ -4827,14 +4827,14 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="s">
         <v>364</v>
       </c>
       <c r="D12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E12" t="s">
         <v>309</v>
@@ -4850,7 +4850,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -4863,7 +4863,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
@@ -4882,37 +4882,45 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15"/>
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
-      <c r="F15"/>
+      <c r="F15" t="s">
+        <v>161</v>
+      </c>
       <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
+      <c r="H15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I16" t="s">
         <v>220</v>
@@ -4920,13 +4928,13 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D17" t="s">
         <v>216</v>
@@ -4939,34 +4947,28 @@
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="I17" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>107</v>
       </c>
-      <c r="B18" t="s">
-        <v>104</v>
-      </c>
+      <c r="B18"/>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
-      <c r="F18" t="s">
-        <v>106</v>
-      </c>
+      <c r="F18"/>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>128</v>
-      </c>
-      <c r="I18" t="s">
-        <v>105</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
@@ -4979,7 +4981,7 @@
         <v>211</v>
       </c>
       <c r="D19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
         <v>208</v>
@@ -4989,7 +4991,7 @@
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I19" t="s">
         <v>368</v>
@@ -5018,13 +5020,13 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F21" t="s">
         <v>370</v>
@@ -5033,11 +5035,13 @@
       <c r="H21" t="s">
         <v>119</v>
       </c>
-      <c r="I21"/>
+      <c r="I21" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
         <v>371</v>
@@ -5056,7 +5060,7 @@
       </c>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I22" t="s">
         <v>374</v>
@@ -5064,7 +5068,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -5077,7 +5081,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
         <v>375</v>
@@ -5085,20 +5089,20 @@
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
         <v>376</v>
       </c>
       <c r="H24" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
         <v>377</v>
@@ -5117,7 +5121,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
         <v>379</v>
@@ -5132,7 +5136,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
         <v>380</v>
@@ -5141,17 +5145,17 @@
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G27"/>
       <c r="H27" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
         <v>381</v>
@@ -5166,10 +5170,10 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -5181,7 +5185,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B30"/>
       <c r="C30"/>
@@ -5198,19 +5202,15 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
-      <c r="F31" t="s">
-        <v>161</v>
-      </c>
+      <c r="F31"/>
       <c r="G31"/>
-      <c r="H31" t="s">
-        <v>159</v>
-      </c>
+      <c r="H31"/>
       <c r="I31"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow non nu emails, update tt to v1
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -14,14 +14,14 @@
     <sheet name="Friday" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Monday'!$A$1:$I$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Monday'!$A$1:$I$30</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="282">
   <si>
     <t>MONDAY</t>
   </si>
@@ -65,298 +65,298 @@
     <t>DLD-Gr1 Khalid</t>
   </si>
   <si>
-    <t>ITC-C M. Shahzad</t>
-  </si>
-  <si>
-    <t>ITC-E M. Shahzad</t>
-  </si>
-  <si>
-    <t>ITC-A M. Shahzad</t>
+    <t>PF-C M. Shahzad</t>
+  </si>
+  <si>
+    <t>PF-E M. Shahzad</t>
+  </si>
+  <si>
+    <t>PF-A M. Shahzad</t>
   </si>
   <si>
     <t>IS-E Shahbaz</t>
   </si>
   <si>
+    <t>DB-D Anum</t>
+  </si>
+  <si>
+    <t>DB-B Anum</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>IS-G Shahbaz</t>
+  </si>
+  <si>
+    <t>CP-Gr1 Abdul Aziz</t>
+  </si>
+  <si>
+    <t>IS-C Shahbaz</t>
+  </si>
+  <si>
+    <t>CP-Gr2 Abdul Aziz</t>
+  </si>
+  <si>
+    <t>TOA-Gr2 Shaharbano</t>
+  </si>
+  <si>
+    <t>TOA-Gr1 Shaharbano</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>PF-F Tania</t>
+  </si>
+  <si>
+    <t>PF-D Tania</t>
+  </si>
+  <si>
+    <t>PF-H Tania</t>
+  </si>
+  <si>
+    <t>PIT-B Khalid</t>
+  </si>
+  <si>
+    <t>PIT-G Khalid</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>COAL-C Faraz</t>
+  </si>
+  <si>
+    <t>DS-B M.Rafi</t>
+  </si>
+  <si>
+    <t>COAL-D Danish</t>
+  </si>
+  <si>
+    <t>DS-D M.Rafi</t>
+  </si>
+  <si>
+    <t>COAL-F Danish</t>
+  </si>
+  <si>
+    <t>COAL-B Danish</t>
+  </si>
+  <si>
     <t>Algo-C Subhash</t>
   </si>
   <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>IS-G Shahbaz</t>
-  </si>
-  <si>
-    <t>CP-Gr1 Abdul Aziz</t>
-  </si>
-  <si>
-    <t>IS-C Shahbaz</t>
-  </si>
-  <si>
-    <t>CP-Gr2 Abdul Aziz</t>
-  </si>
-  <si>
-    <t>TOA-Gr2 Shaharbano</t>
-  </si>
-  <si>
-    <t>TOA-Gr1 Shaharbano</t>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>HCI-D Dr. Rauf</t>
+  </si>
+  <si>
+    <t>DS-A Nida</t>
+  </si>
+  <si>
+    <t>HCI-F Dr. Rauf</t>
+  </si>
+  <si>
+    <t>DS-G Nida</t>
+  </si>
+  <si>
+    <t>COAL-G Faraz</t>
+  </si>
+  <si>
+    <t>DS-E Nida</t>
+  </si>
+  <si>
+    <t>CN-Gr1 Faraz</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>HCI-E Behraj</t>
+  </si>
+  <si>
+    <t>ICC-Gr1 Dr. Jawwad</t>
+  </si>
+  <si>
+    <t>HCI-A Behraj</t>
+  </si>
+  <si>
+    <t>HCI-C Behraj</t>
+  </si>
+  <si>
+    <t>PF-I Shaoib Rauf</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>COAL-A Nadeem kafi</t>
+  </si>
+  <si>
+    <t>LA-E Javeria</t>
+  </si>
+  <si>
+    <t>COAL-E Nadeem kafi</t>
+  </si>
+  <si>
+    <t>CM-Gr2 Sameera</t>
+  </si>
+  <si>
+    <t>PIT-C Saeeda</t>
+  </si>
+  <si>
+    <t>IS-A Dr. Sufian</t>
+  </si>
+  <si>
+    <t>IS-B Dr. Sufian</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Algo-E Dr. Atif</t>
+  </si>
+  <si>
+    <t>CA-Gr2 Dr. Hasina</t>
+  </si>
+  <si>
+    <t>IS-D Dr. Fahad</t>
+  </si>
+  <si>
+    <t>SE-Gr1 Rubab</t>
+  </si>
+  <si>
+    <t>IS-F Dr. Fahad</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>PIT-F Ali Naqvi</t>
+  </si>
+  <si>
+    <t>DS-C teerath</t>
+  </si>
+  <si>
+    <t>PIT-E Saeeda</t>
+  </si>
+  <si>
+    <t>DS-F teerath</t>
+  </si>
+  <si>
+    <t>PIT-D Ali Naqvi</t>
+  </si>
+  <si>
+    <t>PIT-A Saeeda</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>DS-Gr1 Dr. Zeeshan</t>
+  </si>
+  <si>
+    <t>DS-Gr2 Dr. Zeeshan</t>
+  </si>
+  <si>
+    <t>OOAD-A Javeria</t>
+  </si>
+  <si>
+    <t>FM-Gr2 M. Zeeshan</t>
+  </si>
+  <si>
+    <t>FM-Gr1 M. Zeeshan</t>
+  </si>
+  <si>
+    <t>OOAD-F Javeria</t>
+  </si>
+  <si>
+    <t>OOAD-C Javeria</t>
+  </si>
+  <si>
+    <t>CR-3 EE</t>
+  </si>
+  <si>
+    <t>DB-G Shoaib Rauf</t>
   </si>
   <si>
     <t>DB-E Shoaib Rauf</t>
   </si>
   <si>
-    <t>E3</t>
-  </si>
-  <si>
-    <t>ITC-D Tania</t>
-  </si>
-  <si>
-    <t>ITC-H Tania</t>
-  </si>
-  <si>
-    <t>ITC-F Tania</t>
-  </si>
-  <si>
-    <t>PIT-B Khalid</t>
-  </si>
-  <si>
-    <t>PIT-G Khalid</t>
-  </si>
-  <si>
-    <t>OOAD-C Javeria</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>COAL-C Faraz</t>
-  </si>
-  <si>
-    <t>DS-B M.Rafi</t>
-  </si>
-  <si>
-    <t>COAL-D Danish</t>
-  </si>
-  <si>
-    <t>DS-D M.Rafi</t>
-  </si>
-  <si>
-    <t>COAL-F Danish</t>
-  </si>
-  <si>
-    <t>COAL-B Danish</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>HCI-D Dr. Rauf</t>
-  </si>
-  <si>
-    <t>DS-A Nida</t>
-  </si>
-  <si>
-    <t>HCI-F Dr. Rauf</t>
-  </si>
-  <si>
-    <t>DS-E Nida</t>
-  </si>
-  <si>
-    <t>COAL-G Faraz</t>
-  </si>
-  <si>
-    <t>DS-G Nida</t>
-  </si>
-  <si>
-    <t>CN-Gr1 Faraz</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>HCI-E Behraj</t>
-  </si>
-  <si>
-    <t>ICC-Gr1 Dr. Jawwad</t>
-  </si>
-  <si>
-    <t>HCI-A Behraj</t>
-  </si>
-  <si>
-    <t>HCI-C Behraj</t>
-  </si>
-  <si>
-    <t>Algo-E Dr. Atif</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>COAL-A Nadeem kafi</t>
-  </si>
-  <si>
-    <t>LA-E Javeria</t>
-  </si>
-  <si>
-    <t>COAL-E Nadeem kafi</t>
-  </si>
-  <si>
-    <t>CM-Gr2 Sameera</t>
-  </si>
-  <si>
-    <t>PIT-C Saeeda</t>
-  </si>
-  <si>
-    <t>IS-A Dr. Sufian</t>
-  </si>
-  <si>
-    <t>IS-B Dr. Sufian</t>
-  </si>
-  <si>
-    <t>R12</t>
+    <t>OR-Gr1 Asama</t>
+  </si>
+  <si>
+    <t>AP-H Javaid Qureshi</t>
+  </si>
+  <si>
+    <t>Cal-H Javeria</t>
+  </si>
+  <si>
+    <t>CR-4</t>
+  </si>
+  <si>
+    <t>Algo-A Subhash</t>
+  </si>
+  <si>
+    <t>Eng-B1 Nazia</t>
+  </si>
+  <si>
+    <t>Algo-G Subhash</t>
+  </si>
+  <si>
+    <t>Eng-D1 Nazia</t>
+  </si>
+  <si>
+    <t>CM-Gr1 Nazia</t>
+  </si>
+  <si>
+    <t>AP-A Adeel</t>
+  </si>
+  <si>
+    <t>AP-D Adeel</t>
+  </si>
+  <si>
+    <t>Eng-F1 Nazia</t>
+  </si>
+  <si>
+    <t>CR-6</t>
+  </si>
+  <si>
+    <t>DB-F Anum</t>
   </si>
   <si>
     <t>OOAD-G Rubab</t>
   </si>
   <si>
-    <t>CA-Gr2 Dr. Hasina</t>
-  </si>
-  <si>
-    <t>IS-D Dr. Fahad</t>
-  </si>
-  <si>
-    <t>SE-Gr1 Rubab</t>
-  </si>
-  <si>
-    <t>IS-F Dr. Fahad</t>
-  </si>
-  <si>
-    <t>PIT-A Saeeda</t>
-  </si>
-  <si>
     <t>OOAD-E Rubab</t>
   </si>
   <si>
-    <t>R109</t>
-  </si>
-  <si>
-    <t>PIT-F Ali Naqvi</t>
-  </si>
-  <si>
-    <t>DS-C teerath</t>
-  </si>
-  <si>
-    <t>DS-F teerath</t>
-  </si>
-  <si>
-    <t>PIT-D Ali Naqvi</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>DS-Gr1 Dr. Zeeshan</t>
-  </si>
-  <si>
-    <t>DS-Gr2 Dr. Zeeshan</t>
-  </si>
-  <si>
-    <t>PIT-E Saeeda</t>
-  </si>
-  <si>
-    <t>FM-Gr2 M. Zeeshan</t>
-  </si>
-  <si>
-    <t>FM-Gr1 M. Zeeshan</t>
-  </si>
-  <si>
-    <t>CR-3 EE</t>
-  </si>
-  <si>
-    <t>ITC-I Shaoib Rauf</t>
-  </si>
-  <si>
-    <t>DB-G Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>OR-Gr1 Asama</t>
-  </si>
-  <si>
-    <t>BE-H Javaid Qureshi</t>
-  </si>
-  <si>
-    <t>Cal-H Javeria</t>
-  </si>
-  <si>
-    <t>CR-4</t>
-  </si>
-  <si>
-    <t>Algo-A Subhash</t>
-  </si>
-  <si>
-    <t>Eng-B1 Nazia</t>
-  </si>
-  <si>
-    <t>Algo-G Subhash</t>
-  </si>
-  <si>
-    <t>Eng-D1 Nazia</t>
-  </si>
-  <si>
-    <t>CM-Gr1 Nazia</t>
-  </si>
-  <si>
-    <t>BE-A Adeel</t>
-  </si>
-  <si>
-    <t>BE-D Adeel</t>
-  </si>
-  <si>
-    <t>Eng-F1 Nazia</t>
-  </si>
-  <si>
-    <t>CR-6</t>
-  </si>
-  <si>
-    <t>DB-F Anum</t>
-  </si>
-  <si>
-    <t>OOAD-A Javeria</t>
-  </si>
-  <si>
-    <t>OOAD-F Javeria</t>
-  </si>
-  <si>
     <t>Eng-D2 Ahmed</t>
   </si>
   <si>
     <t>Eng-B2 Ahmed</t>
   </si>
   <si>
-    <t>DB-D Anum</t>
-  </si>
-  <si>
-    <t>DB-B Anum</t>
-  </si>
-  <si>
     <t>Eng-I2 Ahmed</t>
   </si>
   <si>
     <t>CR-7</t>
   </si>
   <si>
-    <t>BE-C Rabia</t>
-  </si>
-  <si>
-    <t>BE-G Rabia</t>
+    <t>AP-C Rabia</t>
+  </si>
+  <si>
+    <t>AP-G Rabia</t>
   </si>
   <si>
     <t>Eng-I1 Hafza</t>
   </si>
   <si>
-    <t>BE-I Rabia</t>
-  </si>
-  <si>
-    <t>BE-E Rabia</t>
+    <t>AP-I Rabia</t>
+  </si>
+  <si>
+    <t>AP-E Rabia</t>
   </si>
   <si>
     <t>Eng-G2 Hafza</t>
@@ -368,24 +368,24 @@
     <t>CR-10</t>
   </si>
   <si>
-    <t>BE-B Javaid Qureshi</t>
+    <t>AP-B Javaid Qureshi</t>
+  </si>
+  <si>
+    <t>IRS-I Dr. Shahzad</t>
+  </si>
+  <si>
+    <t>IRS-B Dr. Shahzad</t>
+  </si>
+  <si>
+    <t>DRE-Gr2 Micheal</t>
+  </si>
+  <si>
+    <t>DRE-Gr1 Micheal</t>
   </si>
   <si>
     <t>IRS-D Dr. Shahzad</t>
   </si>
   <si>
-    <t>IRS-B Dr. Shahzad</t>
-  </si>
-  <si>
-    <t>DRE-Gr2 Micheal</t>
-  </si>
-  <si>
-    <t>DRE-Gr1 Micheal</t>
-  </si>
-  <si>
-    <t>IRS-I Dr. Shahzad</t>
-  </si>
-  <si>
     <t>IRS-F Dr. Shahzad</t>
   </si>
   <si>
@@ -401,24 +401,24 @@
     <t>Eng-Lab C2 Saqib</t>
   </si>
   <si>
+    <t>IRS-C Hassan</t>
+  </si>
+  <si>
+    <t>IRS-A Hassan</t>
+  </si>
+  <si>
     <t>CR-17</t>
   </si>
   <si>
     <t>IRS-G Hassan</t>
   </si>
   <si>
-    <t>BE-F Sonia</t>
+    <t>AP-F Sonia</t>
   </si>
   <si>
     <t>IRS-H Hassan</t>
   </si>
   <si>
-    <t>IRS-C Hassan</t>
-  </si>
-  <si>
-    <t>IRS-A Hassan</t>
-  </si>
-  <si>
     <t>CR-18</t>
   </si>
   <si>
@@ -449,7 +449,7 @@
     <t>ICT-Lab G Munim</t>
   </si>
   <si>
-    <t>ITC-Lab B Abdul Aziz &amp; Mubashara</t>
+    <t>OOAD-Lab E Awais</t>
   </si>
   <si>
     <t>Lab-3</t>
@@ -464,12 +464,15 @@
     <t>Lab-4</t>
   </si>
   <si>
-    <t>OOAD-Lab E Awais</t>
-  </si>
-  <si>
     <t>CP Lab-Gr2 Maham</t>
   </si>
   <si>
+    <t>Lab-6</t>
+  </si>
+  <si>
+    <t>PF-Lab B Abdul Aziz &amp; Mubashara</t>
+  </si>
+  <si>
     <t>EE Lab-8</t>
   </si>
   <si>
@@ -503,51 +506,54 @@
     <t>TUESDAY</t>
   </si>
   <si>
-    <t>ITC-B Dr. Farooque</t>
-  </si>
-  <si>
-    <t>ITC-G Dr. Farooque</t>
+    <t>PF-B Dr. Farooque</t>
+  </si>
+  <si>
+    <t>PF-G Dr. Farooque</t>
+  </si>
+  <si>
+    <t>OS-Gr4 Abdul Rehman</t>
+  </si>
+  <si>
+    <t>IPT-Gr2 Murtaza</t>
+  </si>
+  <si>
+    <t>IPT-Gr1 Murtaza</t>
+  </si>
+  <si>
+    <t>OOAD-D Abdur Rehman</t>
+  </si>
+  <si>
+    <t>OOAD-B Abdur Rehman</t>
+  </si>
+  <si>
+    <t>Discrete-A Shoaib Raza</t>
+  </si>
+  <si>
+    <t>Discrete-C Shoaib Raza</t>
+  </si>
+  <si>
+    <t>Discrete-E Shoaib Raza</t>
+  </si>
+  <si>
+    <t>Discrete-F Dr. Jalaluddin</t>
+  </si>
+  <si>
+    <t>Discrete-B Dr. Jalaluddin</t>
+  </si>
+  <si>
+    <t>Algo-F Zeeshan</t>
+  </si>
+  <si>
+    <t>Algo-B Zeeshan</t>
   </si>
   <si>
     <t>HCI-G Farrukh</t>
   </si>
   <si>
-    <t>OS-Gr4 Abdul Rehman</t>
-  </si>
-  <si>
     <t>HCI-B Farrukh</t>
   </si>
   <si>
-    <t>OOAD-D Abdur Rehman</t>
-  </si>
-  <si>
-    <t>OOAD-B Abdur Rehman</t>
-  </si>
-  <si>
-    <t>IPT-Gr2 Murtaza</t>
-  </si>
-  <si>
-    <t>Discrete-A Shoaib Raza</t>
-  </si>
-  <si>
-    <t>Discrete-C Shoaib Raza</t>
-  </si>
-  <si>
-    <t>Discrete-E Shoaib Raza</t>
-  </si>
-  <si>
-    <t>Discrete-F Dr. Jalaluddin</t>
-  </si>
-  <si>
-    <t>Discrete-B Dr. Jalaluddin</t>
-  </si>
-  <si>
-    <t>Algo-F Zeeshan</t>
-  </si>
-  <si>
-    <t>Algo-B Zeeshan</t>
-  </si>
-  <si>
     <t>FA-Gr1 Ahsan</t>
   </si>
   <si>
@@ -557,33 +563,33 @@
     <t>OS-Gr2 Nousheen</t>
   </si>
   <si>
+    <t>OS-Gr1 Nousheen</t>
+  </si>
+  <si>
+    <t>OS-Gr3 Nousheen</t>
+  </si>
+  <si>
+    <t>ISPM-Gr2 Ubaid</t>
+  </si>
+  <si>
+    <t>LA-F Fareeha</t>
+  </si>
+  <si>
+    <t>LA-D Fareeha</t>
+  </si>
+  <si>
+    <t>Cal-II-Gr1 Fareeha</t>
+  </si>
+  <si>
+    <t>LA-B Fareeha</t>
+  </si>
+  <si>
+    <t>CA-Gr4 Ahsan</t>
+  </si>
+  <si>
     <t>ISPM-Gr1 Ubaid</t>
   </si>
   <si>
-    <t>OS-Gr1 Nousheen</t>
-  </si>
-  <si>
-    <t>OS-Gr3 Nousheen</t>
-  </si>
-  <si>
-    <t>LA-F Fareeha</t>
-  </si>
-  <si>
-    <t>LA-D Fareeha</t>
-  </si>
-  <si>
-    <t>Cal-II-Gr1 Fareeha</t>
-  </si>
-  <si>
-    <t>LA-B Fareeha</t>
-  </si>
-  <si>
-    <t>CA-Gr4 Ahsan</t>
-  </si>
-  <si>
-    <t>IPT-Gr1 Murtaza</t>
-  </si>
-  <si>
     <t>CA-Gr1 Ahsan</t>
   </si>
   <si>
@@ -596,6 +602,9 @@
     <t>MM Gr1 Asiya</t>
   </si>
   <si>
+    <t>MM Gr2 Asiya</t>
+  </si>
+  <si>
     <t>LA-G Dr. Sadaqat</t>
   </si>
   <si>
@@ -656,13 +665,13 @@
     <t>Eng-A2 Javed Iqbal</t>
   </si>
   <si>
-    <t>ITC-Lab A Rahemeen &amp; Faheem</t>
+    <t>PF-Lab A Rahemeen &amp; Faheem</t>
   </si>
   <si>
     <t>ICT-Lab B Munim</t>
   </si>
   <si>
-    <t>ITC-Lab H Farah &amp; Irfan</t>
+    <t>PF-Lab H Farah &amp; Irfan</t>
   </si>
   <si>
     <t>OS Lab- Gr1 Summiyah</t>
@@ -701,12 +710,12 @@
     <t>WEDNESDAY</t>
   </si>
   <si>
+    <t>DB-C Dr. Zulfiqar</t>
+  </si>
+  <si>
     <t>DB-A Dr. Zulfiqar</t>
   </si>
   <si>
-    <t>DB-C Dr. Zulfiqar</t>
-  </si>
-  <si>
     <t>Discrete- E Shoaib Raza</t>
   </si>
   <si>
@@ -716,12 +725,6 @@
     <t>Discrete-G Dr. Nouman</t>
   </si>
   <si>
-    <t>PIT-D TBA</t>
-  </si>
-  <si>
-    <t>PIT-F TBA</t>
-  </si>
-  <si>
     <t>Eng-Lab D1 Kishwar</t>
   </si>
   <si>
@@ -734,13 +737,13 @@
     <t>Cal-D Nadeem</t>
   </si>
   <si>
-    <t>ITC-Lab C Rahemeen &amp; Faheem</t>
+    <t>OOAD-Lab A Tooba</t>
   </si>
   <si>
     <t>ICT-Lab I Munim</t>
   </si>
   <si>
-    <t>ITC-Lab G Abdul Aziz &amp; Mubashara</t>
+    <t>PF-Lab G Abdul Aziz &amp; Mubashara</t>
   </si>
   <si>
     <t>OS Lab- Gr3 Summiyah</t>
@@ -758,6 +761,9 @@
     <t>CN-Gr1 Lab TBA</t>
   </si>
   <si>
+    <t>PF-Lab C Rahemeen &amp; Faheem</t>
+  </si>
+  <si>
     <t>DS Lab-B Maham</t>
   </si>
   <si>
@@ -785,13 +791,16 @@
     <t>Eng-Lab H2 Afreen</t>
   </si>
   <si>
-    <t>ITC-Lab F Farah &amp; Irfan</t>
+    <t>PF-Lab F Farah &amp; Irfan</t>
   </si>
   <si>
     <t>ICT-Lab A Munim</t>
   </si>
   <si>
-    <t>ITC-Lab I Abdul Aziz &amp; Mubashara</t>
+    <t>DB-Lab E Ammara</t>
+  </si>
+  <si>
+    <t>PF-Lab I Abdul Aziz &amp; Mubashara</t>
   </si>
   <si>
     <t>ICT-Lab H Hamza</t>
@@ -839,16 +848,13 @@
     <t>Eng-Lab G2 Hubrah</t>
   </si>
   <si>
-    <t>ITC-Lab E Rahemeen &amp; Faheem</t>
+    <t>PF-Lab E Rahemeen &amp; Faheem</t>
   </si>
   <si>
     <t>B R E A K</t>
   </si>
   <si>
-    <t>ITC-Lab D Farah &amp; Irfan</t>
-  </si>
-  <si>
-    <t>OOAD-Lab A Tooba</t>
+    <t>PF-Lab D Farah &amp; Irfan</t>
   </si>
   <si>
     <t>OS Lab- Gr4 Summiyah</t>
@@ -1200,9 +1206,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" zoomScale="57" zoomScaleNormal="57" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="62" zoomScaleNormal="62" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -1315,36 +1321,36 @@
       <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="H5"/>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" t="s">
         <v>26</v>
       </c>
+      <c r="H6"/>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
@@ -1367,35 +1373,35 @@
       <c r="G7" t="s">
         <v>32</v>
       </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
+      <c r="H7"/>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>38</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8"/>
+      <c r="I8" t="s">
         <v>40</v>
       </c>
-      <c r="H8"/>
-      <c r="I8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
@@ -1494,34 +1500,34 @@
       <c r="G12" t="s">
         <v>68</v>
       </c>
-      <c r="H12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" t="s">
-        <v>70</v>
-      </c>
+      <c r="H12"/>
+      <c r="I12"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
         <v>71</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>72</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>73</v>
       </c>
-      <c r="D13"/>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" t="s">
         <v>74</v>
       </c>
-      <c r="F13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>75</v>
       </c>
-      <c r="H13"/>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
@@ -1543,89 +1549,89 @@
       <c r="F14" t="s">
         <v>81</v>
       </c>
-      <c r="G14"/>
-      <c r="H14"/>
+      <c r="G14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" t="s">
+        <v>83</v>
+      </c>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
         <v>57</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I16" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>102</v>
-      </c>
-      <c r="G17" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" t="s">
         <v>104</v>
       </c>
+      <c r="G17"/>
+      <c r="H17"/>
       <c r="I17" t="s">
         <v>105</v>
       </c>
@@ -1699,33 +1705,31 @@
         <v>125</v>
       </c>
       <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
+      <c r="G20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" t="s">
+        <v>127</v>
+      </c>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C21" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E21"/>
-      <c r="F21" t="s">
-        <v>128</v>
-      </c>
-      <c r="G21" t="s">
-        <v>130</v>
-      </c>
-      <c r="H21" t="s">
-        <v>131</v>
-      </c>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
@@ -1742,10 +1746,10 @@
       <c r="E22" t="s">
         <v>134</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22"/>
+      <c r="G22" t="s">
         <v>135</v>
       </c>
-      <c r="G22"/>
       <c r="H22" t="s">
         <v>136</v>
       </c>
@@ -1806,82 +1810,95 @@
       <c r="A26" t="s">
         <v>146</v>
       </c>
-      <c r="B26" t="s">
-        <v>147</v>
-      </c>
+      <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" t="s">
-        <v>150</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
-      <c r="E28" t="s">
-        <v>154</v>
-      </c>
+      <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F29"/>
-      <c r="G29"/>
+      <c r="G29" t="s">
+        <v>156</v>
+      </c>
       <c r="H29"/>
       <c r="I29"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30"/>
-      <c r="B30"/>
+      <c r="A30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" t="s">
+        <v>158</v>
+      </c>
       <c r="C30"/>
       <c r="D30"/>
-      <c r="E30"/>
+      <c r="E30" t="s">
+        <v>159</v>
+      </c>
       <c r="F30"/>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -1905,18 +1922,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="57" zoomScaleNormal="57" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -1928,8 +1945,14 @@
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1959,8 +1982,14 @@
       </c>
       <c r="J2"/>
       <c r="K2"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1990,8 +2019,14 @@
       </c>
       <c r="J3"/>
       <c r="K3"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2005,8 +2040,14 @@
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2017,54 +2058,66 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F6" t="s">
         <v>67</v>
       </c>
-      <c r="G6"/>
-      <c r="H6" t="s">
-        <v>162</v>
-      </c>
+      <c r="G6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2072,53 +2125,63 @@
         <v>163</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>164</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" t="s">
-        <v>164</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="E7"/>
       <c r="F7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
       <c r="G8" t="s">
-        <v>167</v>
+        <v>52</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -2126,30 +2189,40 @@
         <v>43</v>
       </c>
       <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
         <v>47</v>
       </c>
-      <c r="D9"/>
-      <c r="E9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9"/>
+      <c r="G9" t="s">
+        <v>164</v>
+      </c>
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
         <v>168</v>
@@ -2165,8 +2238,14 @@
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -2177,14 +2256,12 @@
         <v>172</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" t="s">
-        <v>31</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="F11"/>
       <c r="G11" t="s">
         <v>173</v>
       </c>
@@ -2194,250 +2271,312 @@
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>175</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12"/>
+        <v>176</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
       <c r="G12" t="s">
-        <v>115</v>
+        <v>31</v>
       </c>
       <c r="H12" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I12" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="J12"/>
       <c r="K12"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
         <v>71</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>73</v>
-      </c>
-      <c r="C13" t="s">
-        <v>74</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="G13"/>
       <c r="H13" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C14" t="s">
-        <v>177</v>
-      </c>
-      <c r="D14" t="s">
-        <v>178</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="D14"/>
       <c r="E14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G14" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F15" t="s">
-        <v>182</v>
-      </c>
-      <c r="G15"/>
+        <v>184</v>
+      </c>
+      <c r="G15" t="s">
+        <v>130</v>
+      </c>
       <c r="H15" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="I15" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C16" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="D16" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F16" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="I17" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="J17"/>
       <c r="K17"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C18" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F18" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="G18" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H18" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="I18" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="J18"/>
       <c r="K18"/>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H19" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>122</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D20" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E20" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C21"/>
       <c r="D21" t="s">
@@ -2451,40 +2590,52 @@
         <v>134</v>
       </c>
       <c r="H21" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="I21" t="s">
         <v>135</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>132</v>
       </c>
       <c r="B22"/>
       <c r="C22" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E22" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F22"/>
       <c r="G22" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="H22" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>138</v>
       </c>
@@ -2498,124 +2649,187 @@
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>143</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="F25"/>
       <c r="G25" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>146</v>
       </c>
       <c r="B26" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
-      <c r="E27" t="s">
-        <v>219</v>
-      </c>
+      <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" t="s">
-        <v>220</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F28"/>
-      <c r="G28" t="s">
-        <v>222</v>
-      </c>
+      <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
         <v>223</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
-      <c r="E29"/>
+      <c r="E29" t="s">
+        <v>224</v>
+      </c>
       <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29" t="s">
-        <v>224</v>
-      </c>
+      <c r="G29" t="s">
+        <v>225</v>
+      </c>
+      <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" t="s">
+        <v>226</v>
+      </c>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30" t="s">
+        <v>227</v>
+      </c>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -2639,18 +2853,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="60" zoomScaleNormal="60" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2765,16 +2979,26 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>227</v>
-      </c>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
+        <v>176</v>
+      </c>
+      <c r="D5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H5" t="s">
+        <v>230</v>
+      </c>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
@@ -2786,24 +3010,24 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -2819,25 +3043,19 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C7"/>
       <c r="D7"/>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
+      <c r="E7"/>
+      <c r="F7"/>
       <c r="G7" t="s">
         <v>100</v>
       </c>
-      <c r="H7" t="s">
-        <v>99</v>
-      </c>
-      <c r="I7"/>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -2848,23 +3066,15 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8"/>
-      <c r="C8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D8" t="s">
-        <v>162</v>
-      </c>
+      <c r="C8"/>
+      <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
-      <c r="G8" t="s">
-        <v>172</v>
-      </c>
-      <c r="H8" t="s">
-        <v>171</v>
-      </c>
+      <c r="G8"/>
+      <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -2879,14 +3089,14 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" t="s">
         <v>17</v>
@@ -2908,16 +3118,16 @@
         <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
         <v>169</v>
       </c>
       <c r="E10" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G10" t="s">
         <v>168</v>
@@ -2941,14 +3151,14 @@
         <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
         <v>59</v>
@@ -2960,7 +3170,7 @@
         <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
@@ -2975,10 +3185,10 @@
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
@@ -3004,21 +3214,25 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>70</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13" t="s">
-        <v>231</v>
-      </c>
-      <c r="G13"/>
-      <c r="H13"/>
+        <v>74</v>
+      </c>
+      <c r="G13" t="s">
+        <v>172</v>
+      </c>
+      <c r="H13" t="s">
+        <v>171</v>
+      </c>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -3034,7 +3248,7 @@
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D14" t="s">
         <v>163</v>
@@ -3047,7 +3261,7 @@
       </c>
       <c r="G14"/>
       <c r="H14" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -3060,21 +3274,21 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B15"/>
       <c r="C15" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E15"/>
       <c r="F15" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G15" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -3088,7 +3302,7 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -3096,17 +3310,17 @@
         <v>133</v>
       </c>
       <c r="E16" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F16" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -3118,24 +3332,24 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F17" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -3160,7 +3374,7 @@
         <v>124</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s">
         <v>107</v>
@@ -3183,26 +3397,26 @@
         <v>114</v>
       </c>
       <c r="B19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" t="s">
         <v>195</v>
-      </c>
-      <c r="C19" t="s">
-        <v>192</v>
       </c>
       <c r="D19" t="s">
         <v>117</v>
       </c>
       <c r="E19" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F19" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="J19"/>
       <c r="K19"/>
@@ -3217,19 +3431,19 @@
         <v>122</v>
       </c>
       <c r="B20" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F20" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
@@ -3242,29 +3456,29 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21"/>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F21" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G21" t="s">
         <v>57</v>
       </c>
       <c r="H21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I21" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
@@ -3286,14 +3500,14 @@
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F22"/>
       <c r="G22" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H22" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
@@ -3329,16 +3543,16 @@
         <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -3355,16 +3569,16 @@
         <v>143</v>
       </c>
       <c r="B25" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F25"/>
       <c r="G25" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -3381,7 +3595,7 @@
         <v>146</v>
       </c>
       <c r="B26" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -3390,7 +3604,7 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -3404,22 +3618,16 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
-      <c r="E27" t="s">
-        <v>78</v>
-      </c>
-      <c r="F27" t="s">
-        <v>77</v>
-      </c>
-      <c r="G27" t="s">
-        <v>246</v>
-      </c>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -3432,15 +3640,19 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
         <v>247</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
+      <c r="E28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" t="s">
+        <v>77</v>
+      </c>
       <c r="G28" t="s">
         <v>248</v>
       </c>
@@ -3456,7 +3668,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
         <v>249</v>
@@ -3464,13 +3676,11 @@
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
-      <c r="F29" t="s">
+      <c r="F29"/>
+      <c r="G29" t="s">
         <v>250</v>
       </c>
-      <c r="G29"/>
-      <c r="H29" t="s">
-        <v>251</v>
-      </c>
+      <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -3479,6 +3689,32 @@
       <c r="N29"/>
       <c r="O29"/>
       <c r="P29"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" t="s">
+        <v>251</v>
+      </c>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30" t="s">
+        <v>252</v>
+      </c>
+      <c r="G30"/>
+      <c r="H30" t="s">
+        <v>253</v>
+      </c>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -3505,15 +3741,15 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="59" zoomScaleNormal="59" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3618,20 +3854,20 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
         <v>161</v>
-      </c>
-      <c r="C6" t="s">
-        <v>160</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6"/>
       <c r="H6"/>
@@ -3641,43 +3877,45 @@
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7"/>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
       <c r="C7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7"/>
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>188</v>
+      </c>
       <c r="E7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7"/>
+        <v>182</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7" t="s">
+        <v>188</v>
+      </c>
       <c r="H7"/>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" t="s">
-        <v>62</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C8"/>
       <c r="D8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
         <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
       </c>
       <c r="G8"/>
       <c r="H8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I8"/>
     </row>
@@ -3686,23 +3924,23 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D9" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9"/>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9"/>
     </row>
@@ -3711,20 +3949,20 @@
         <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E10" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -3734,20 +3972,20 @@
         <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="E11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="H11" t="s">
         <v>46</v>
@@ -3759,10 +3997,10 @@
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
         <v>65</v>
@@ -3779,7 +4017,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
         <v>173</v>
@@ -3792,13 +4030,13 @@
         <v>43</v>
       </c>
       <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>178</v>
+      </c>
+      <c r="H13" t="s">
         <v>47</v>
-      </c>
-      <c r="G13" t="s">
-        <v>176</v>
-      </c>
-      <c r="H13" t="s">
-        <v>45</v>
       </c>
       <c r="I13"/>
     </row>
@@ -3808,84 +4046,96 @@
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15"/>
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
+        <v>191</v>
+      </c>
       <c r="C15" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" t="s">
         <v>73</v>
       </c>
-      <c r="F15" t="s">
-        <v>74</v>
-      </c>
       <c r="G15" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H15" t="s">
-        <v>187</v>
-      </c>
-      <c r="I15"/>
+        <v>189</v>
+      </c>
+      <c r="I15" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>178</v>
-      </c>
-      <c r="E16"/>
+        <v>82</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
       <c r="F16" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16"/>
+        <v>98</v>
+      </c>
+      <c r="G16" t="s">
+        <v>83</v>
+      </c>
       <c r="H16" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="I16" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17"/>
-      <c r="C17"/>
+        <v>99</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F17" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -3893,21 +4143,21 @@
         <v>106</v>
       </c>
       <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
       <c r="D18" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E18" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="I18" t="s">
         <v>105</v>
@@ -3918,16 +4168,16 @@
         <v>114</v>
       </c>
       <c r="B19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" t="s">
         <v>116</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
       <c r="D19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F19" t="s">
         <v>113</v>
@@ -3944,50 +4194,48 @@
       <c r="A20" t="s">
         <v>122</v>
       </c>
-      <c r="B20" t="s">
-        <v>189</v>
-      </c>
+      <c r="B20"/>
       <c r="C20" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D20" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E20" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F20" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C21" t="s">
         <v>112</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -3995,21 +4243,21 @@
         <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E22" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="I22" t="s">
         <v>109</v>
@@ -4033,16 +4281,16 @@
         <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -4052,16 +4300,16 @@
         <v>143</v>
       </c>
       <c r="B25" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="F25"/>
       <c r="G25" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -4071,55 +4319,55 @@
         <v>146</v>
       </c>
       <c r="B26" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B29"/>
       <c r="C29"/>
@@ -4128,16 +4376,16 @@
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="I29"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B30" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -4171,7 +4419,7 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="64" zoomScaleNormal="64" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -4180,7 +4428,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -4271,36 +4519,30 @@
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E5" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>272</v>
+      </c>
+      <c r="H5" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>269</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
       </c>
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6"/>
       <c r="D6"/>
-      <c r="E6" t="s">
-        <v>104</v>
-      </c>
+      <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
@@ -4311,14 +4553,14 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
@@ -4327,13 +4569,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>174</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D8" t="s">
         <v>171</v>
@@ -4356,18 +4598,20 @@
       <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" t="s">
+        <v>196</v>
+      </c>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="G9"/>
       <c r="H9" t="s">
@@ -4386,7 +4630,7 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E10" t="s">
         <v>168</v>
@@ -4411,15 +4655,15 @@
         <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E11" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I11" t="s">
         <v>59</v>
@@ -4430,30 +4674,32 @@
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12"/>
+        <v>91</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G12"/>
       <c r="H12" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
@@ -4462,15 +4708,11 @@
       <c r="E13" t="s">
         <v>48</v>
       </c>
-      <c r="F13" t="s">
-        <v>189</v>
-      </c>
+      <c r="F13"/>
       <c r="G13"/>
-      <c r="H13" t="s">
-        <v>193</v>
-      </c>
+      <c r="H13"/>
       <c r="I13" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -4486,30 +4728,30 @@
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G14"/>
       <c r="H14" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
@@ -4521,20 +4763,20 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
         <v>105</v>
       </c>
       <c r="E16"/>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
@@ -4546,10 +4788,10 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -4557,14 +4799,14 @@
         <v>124</v>
       </c>
       <c r="F17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="I17" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -4578,10 +4820,10 @@
         <v>108</v>
       </c>
       <c r="D18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E18" t="s">
         <v>195</v>
-      </c>
-      <c r="E18" t="s">
-        <v>192</v>
       </c>
       <c r="F18" t="s">
         <v>111</v>
@@ -4600,23 +4842,23 @@
         <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D19" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E19" t="s">
         <v>121</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -4624,7 +4866,7 @@
         <v>122</v>
       </c>
       <c r="B20" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C20"/>
       <c r="D20" t="s">
@@ -4634,36 +4876,36 @@
         <v>113</v>
       </c>
       <c r="F20" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="I20" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C21" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="I21"/>
     </row>
@@ -4672,10 +4914,10 @@
         <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C22" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D22" t="s">
         <v>137</v>
@@ -4686,7 +4928,7 @@
       </c>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="I22"/>
     </row>
@@ -4708,14 +4950,14 @@
         <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -4725,7 +4967,7 @@
         <v>143</v>
       </c>
       <c r="B25" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
@@ -4739,9 +4981,7 @@
       <c r="A26" t="s">
         <v>146</v>
       </c>
-      <c r="B26" t="s">
-        <v>275</v>
-      </c>
+      <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
@@ -4752,12 +4992,12 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" t="s">
-        <v>276</v>
-      </c>
-      <c r="C27"/>
+        <v>150</v>
+      </c>
+      <c r="B27"/>
+      <c r="C27" t="s">
+        <v>278</v>
+      </c>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
@@ -4767,12 +5007,12 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E28"/>
       <c r="F28"/>
@@ -4782,20 +5022,20 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G29"/>
       <c r="H29" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="I29"/>
     </row>

</xml_diff>

<commit_message>
Update tt to new v2.0
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -605,6 +605,9 @@
     <t>CA-Gr3 Ahsan</t>
   </si>
   <si>
+    <t>FA-Gr2 Ahsan</t>
+  </si>
+  <si>
     <t>FA-Gr1 Ahsan</t>
   </si>
   <si>
@@ -722,9 +725,6 @@
     <t>Eng-Lab H1 &amp; H2 Kishwar</t>
   </si>
   <si>
-    <t>FA-Gr2 Ahsan</t>
-  </si>
-  <si>
     <t>Eng-Lab D1 Kishwar</t>
   </si>
   <si>
@@ -803,21 +803,21 @@
     <t>DB-Lab E Ammara</t>
   </si>
   <si>
+    <t>ICT-Lab A Munim</t>
+  </si>
+  <si>
     <t>DB-Lab F Basit ali</t>
   </si>
   <si>
+    <t>ICT-Lab E Abdul Aziz</t>
+  </si>
+  <si>
     <t>COAL Lab-E Zain</t>
   </si>
   <si>
     <t>ICT-Lab H Hamza</t>
   </si>
   <si>
-    <t>ICT-Lab E Abdul Aziz</t>
-  </si>
-  <si>
-    <t>ICT-Lab A Munim</t>
-  </si>
-  <si>
     <t>OOAD-Lab G Awais</t>
   </si>
   <si>
@@ -845,19 +845,19 @@
     <t>COAL Lab-C Zain</t>
   </si>
   <si>
+    <t>B R E A K</t>
+  </si>
+  <si>
+    <t>PF-Lab E Rahemeen &amp; Faheem</t>
+  </si>
+  <si>
+    <t>OS Lab- Gr4 Summiyah</t>
+  </si>
+  <si>
+    <t>PF-Lab D Farah &amp; Irfan</t>
+  </si>
+  <si>
     <t>CN-Gr1 Lab Faizan</t>
-  </si>
-  <si>
-    <t>B R E A K</t>
-  </si>
-  <si>
-    <t>PF-Lab E Rahemeen &amp; Faheem</t>
-  </si>
-  <si>
-    <t>OS Lab- Gr4 Summiyah</t>
-  </si>
-  <si>
-    <t>PF-Lab D Farah &amp; Irfan</t>
   </si>
   <si>
     <t>OOAD-Lab D Nadeem</t>
@@ -1451,7 +1451,9 @@
         <v>55</v>
       </c>
       <c r="F10"/>
-      <c r="G10"/>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
       <c r="H10" t="s">
         <v>56</v>
       </c>
@@ -2422,7 +2424,7 @@
         <v>194</v>
       </c>
       <c r="I18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J18"/>
       <c r="K18"/>
@@ -2453,24 +2455,24 @@
         <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C20" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
@@ -2481,21 +2483,21 @@
       </c>
       <c r="B21"/>
       <c r="C21" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E21"/>
       <c r="F21" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I21" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
@@ -2508,16 +2510,16 @@
         <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D22" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22" t="s">
         <v>207</v>
       </c>
-      <c r="E22" t="s">
-        <v>206</v>
-      </c>
       <c r="F22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G22"/>
       <c r="H22" t="s">
@@ -2546,7 +2548,7 @@
         <v>143</v>
       </c>
       <c r="H23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I23" t="s">
         <v>145</v>
@@ -2560,20 +2562,20 @@
       </c>
       <c r="B24"/>
       <c r="C24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D24" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I24"/>
       <c r="J24"/>
@@ -2599,16 +2601,16 @@
         <v>147</v>
       </c>
       <c r="B26" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -2620,16 +2622,16 @@
         <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -2641,14 +2643,14 @@
         <v>154</v>
       </c>
       <c r="B28" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
@@ -2660,14 +2662,14 @@
         <v>156</v>
       </c>
       <c r="B29" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
@@ -2679,7 +2681,7 @@
         <v>159</v>
       </c>
       <c r="B30" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -2696,14 +2698,14 @@
         <v>162</v>
       </c>
       <c r="B31" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
@@ -2750,15 +2752,15 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="60" zoomScaleNormal="60" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2864,10 +2866,10 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2974,7 +2976,7 @@
         <v>181</v>
       </c>
       <c r="E10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F10" t="s">
         <v>50</v>
@@ -3095,7 +3097,7 @@
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -3112,10 +3114,10 @@
         <v>52</v>
       </c>
       <c r="E16" t="s">
+        <v>195</v>
+      </c>
+      <c r="F16" t="s">
         <v>194</v>
-      </c>
-      <c r="F16" t="s">
-        <v>233</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
@@ -3129,19 +3131,19 @@
         <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D17" t="s">
         <v>142</v>
       </c>
       <c r="E17" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
@@ -3160,10 +3162,10 @@
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" t="s">
+        <v>206</v>
+      </c>
+      <c r="F18" t="s">
         <v>205</v>
-      </c>
-      <c r="F18" t="s">
-        <v>204</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
@@ -3184,13 +3186,13 @@
       <c r="E19" t="s">
         <v>114</v>
       </c>
-      <c r="F19" t="s">
-        <v>112</v>
-      </c>
+      <c r="F19"/>
       <c r="G19" t="s">
         <v>116</v>
       </c>
-      <c r="H19"/>
+      <c r="H19" t="s">
+        <v>112</v>
+      </c>
       <c r="I19"/>
       <c r="J19"/>
     </row>
@@ -3227,7 +3229,7 @@
         <v>129</v>
       </c>
       <c r="F21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
@@ -3264,10 +3266,10 @@
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23" t="s">
+        <v>201</v>
+      </c>
+      <c r="F23" t="s">
         <v>200</v>
-      </c>
-      <c r="F23" t="s">
-        <v>199</v>
       </c>
       <c r="G23"/>
       <c r="H23" t="s">
@@ -3295,7 +3297,7 @@
         <v>237</v>
       </c>
       <c r="H24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I24"/>
       <c r="J24"/>
@@ -3569,10 +3571,10 @@
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" t="s">
         <v>230</v>
-      </c>
-      <c r="D5" t="s">
-        <v>229</v>
       </c>
       <c r="E5"/>
       <c r="F5" t="s">
@@ -3630,9 +3632,7 @@
       <c r="F7" t="s">
         <v>76</v>
       </c>
-      <c r="G7" t="s">
-        <v>56</v>
-      </c>
+      <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
     </row>
@@ -3767,18 +3767,22 @@
       <c r="C13" t="s">
         <v>40</v>
       </c>
-      <c r="D13"/>
+      <c r="D13" t="s">
+        <v>175</v>
+      </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>176</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13"/>
-      <c r="H13" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13"/>
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
@@ -3836,13 +3840,15 @@
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="G16"/>
-      <c r="H16"/>
+      <c r="H16" t="s">
+        <v>86</v>
+      </c>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
@@ -3850,14 +3856,14 @@
         <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -3882,24 +3888,24 @@
         <v>121</v>
       </c>
       <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18" t="s">
+      <c r="H18" t="s">
         <v>119</v>
       </c>
+      <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -3907,7 +3913,7 @@
         <v>255</v>
       </c>
       <c r="I19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3915,7 +3921,7 @@
         <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C20" t="s">
         <v>237</v>
@@ -3923,16 +3929,20 @@
       <c r="D20" t="s">
         <v>236</v>
       </c>
-      <c r="E20"/>
-      <c r="F20"/>
+      <c r="E20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" t="s">
+        <v>107</v>
+      </c>
       <c r="G20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H20" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I20" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -3966,13 +3976,13 @@
         <v>138</v>
       </c>
       <c r="C22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D22" t="s">
         <v>207</v>
       </c>
-      <c r="D22" t="s">
-        <v>206</v>
-      </c>
       <c r="E22" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F22" t="s">
         <v>134</v>
@@ -4067,7 +4077,9 @@
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27"/>
+      <c r="H27" t="s">
+        <v>260</v>
+      </c>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
@@ -4075,14 +4087,16 @@
         <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
-      <c r="H28"/>
+      <c r="H28" t="s">
+        <v>262</v>
+      </c>
       <c r="I28"/>
     </row>
     <row r="29" spans="1:9">
@@ -4090,7 +4104,7 @@
         <v>154</v>
       </c>
       <c r="B29" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -4105,18 +4119,14 @@
         <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C30"/>
-      <c r="D30" t="s">
-        <v>263</v>
-      </c>
+      <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
-      <c r="H30" t="s">
-        <v>264</v>
-      </c>
+      <c r="H30"/>
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9">
@@ -4321,18 +4331,18 @@
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
       <c r="C6" t="s">
         <v>73</v>
       </c>
-      <c r="D6" t="s">
-        <v>72</v>
-      </c>
+      <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I6" t="s">
         <v>255</v>
@@ -4343,17 +4353,13 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C7" t="s">
-        <v>230</v>
-      </c>
-      <c r="D7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E7" t="s">
-        <v>175</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="s">
@@ -4406,7 +4412,7 @@
         <v>179</v>
       </c>
       <c r="D10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E10"/>
       <c r="F10" t="s">
@@ -4447,18 +4453,12 @@
       <c r="A12" t="s">
         <v>65</v>
       </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
+      <c r="B12"/>
       <c r="C12" t="s">
         <v>66</v>
       </c>
-      <c r="D12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
+      <c r="D12"/>
+      <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12" t="s">
@@ -4472,13 +4472,13 @@
       <c r="A13" t="s">
         <v>71</v>
       </c>
-      <c r="B13"/>
+      <c r="B13" t="s">
+        <v>183</v>
+      </c>
       <c r="C13" t="s">
-        <v>183</v>
-      </c>
-      <c r="D13" t="s">
         <v>182</v>
       </c>
+      <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
@@ -4520,20 +4520,20 @@
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E16" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F16" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I16" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -4578,7 +4578,7 @@
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I18"/>
     </row>
@@ -4587,19 +4587,19 @@
         <v>104</v>
       </c>
       <c r="B19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" t="s">
         <v>214</v>
-      </c>
-      <c r="C19" t="s">
-        <v>213</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I19" t="s">
         <v>114</v>
@@ -4635,7 +4635,7 @@
         <v>117</v>
       </c>
       <c r="B21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C21" t="s">
         <v>109</v>
@@ -4681,22 +4681,22 @@
         <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C23" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G23"/>
       <c r="H23" t="s">
         <v>235</v>
       </c>
       <c r="I23" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -4710,7 +4710,7 @@
         <v>236</v>
       </c>
       <c r="D24" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E24"/>
       <c r="F24"/>
@@ -4745,15 +4745,11 @@
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
-      <c r="F26" t="s">
+      <c r="F26"/>
+      <c r="G26" t="s">
         <v>274</v>
       </c>
-      <c r="G26" t="s">
-        <v>275</v>
-      </c>
-      <c r="H26" t="s">
-        <v>274</v>
-      </c>
+      <c r="H26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
@@ -4761,7 +4757,7 @@
         <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -4778,7 +4774,7 @@
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E28"/>
       <c r="F28"/>
@@ -4791,7 +4787,7 @@
         <v>156</v>
       </c>
       <c r="B29" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -4806,7 +4802,9 @@
         <v>159</v>
       </c>
       <c r="B30"/>
-      <c r="C30"/>
+      <c r="C30" t="s">
+        <v>278</v>
+      </c>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>

</xml_diff>

<commit_message>
Add All Sections badfix, update TT to v3.0
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -341,9 +341,6 @@
     <t>Eng-I1 Hafza</t>
   </si>
   <si>
-    <t>Eng-G2 Hafza</t>
-  </si>
-  <si>
     <t>DS-F teerath</t>
   </si>
   <si>
@@ -539,6 +536,9 @@
     <t>PF-G Dr. Farooque</t>
   </si>
   <si>
+    <t>Eng-G2 Afsheen</t>
+  </si>
+  <si>
     <t>IPT-Gr2 Murtaza</t>
   </si>
   <si>
@@ -797,7 +797,7 @@
     <t>New Building Auditorium</t>
   </si>
   <si>
-    <t>ICT-Lab</t>
+    <t>ICT-Lab All Sections</t>
   </si>
   <si>
     <t>DB-Lab E Ammara</t>
@@ -1649,155 +1649,153 @@
         <v>105</v>
       </c>
       <c r="C19"/>
-      <c r="D19" t="s">
+      <c r="D19"/>
+      <c r="E19" t="s">
         <v>106</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>107</v>
-      </c>
-      <c r="F19" t="s">
-        <v>108</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" t="s">
         <v>109</v>
-      </c>
-      <c r="I19" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
         <v>111</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>112</v>
-      </c>
-      <c r="C20" t="s">
-        <v>113</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" t="s">
         <v>114</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>115</v>
-      </c>
-      <c r="G20" t="s">
-        <v>116</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" t="s">
         <v>117</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>118</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>119</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>120</v>
       </c>
-      <c r="E21" t="s">
-        <v>121</v>
-      </c>
       <c r="F21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" t="s">
         <v>122</v>
-      </c>
-      <c r="I21" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22"/>
       <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
         <v>125</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>126</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>127</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>128</v>
-      </c>
-      <c r="G22" t="s">
-        <v>129</v>
       </c>
       <c r="H22"/>
       <c r="I22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" t="s">
         <v>131</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>132</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>133</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>134</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>135</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>136</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>137</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>138</v>
-      </c>
-      <c r="I23" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" t="s">
         <v>140</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>141</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>141</v>
+      </c>
+      <c r="E24" t="s">
         <v>142</v>
-      </c>
-      <c r="D24" t="s">
-        <v>142</v>
-      </c>
-      <c r="E24" t="s">
-        <v>143</v>
       </c>
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I24" t="s">
         <v>144</v>
-      </c>
-      <c r="I24" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -1810,16 +1808,16 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" t="s">
         <v>147</v>
-      </c>
-      <c r="B26" t="s">
-        <v>148</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G26"/>
       <c r="H26"/>
@@ -1827,29 +1825,29 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" t="s">
         <v>150</v>
-      </c>
-      <c r="B27" t="s">
-        <v>151</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" t="s">
         <v>154</v>
-      </c>
-      <c r="B28" t="s">
-        <v>155</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -1861,33 +1859,33 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" t="s">
         <v>159</v>
-      </c>
-      <c r="B30" t="s">
-        <v>160</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
@@ -1895,24 +1893,24 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" t="s">
         <v>162</v>
-      </c>
-      <c r="B31" t="s">
-        <v>163</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B32"/>
       <c r="C32"/>
@@ -1967,7 +1965,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2093,7 +2091,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -2108,10 +2106,10 @@
         <v>23</v>
       </c>
       <c r="G6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" t="s">
         <v>168</v>
-      </c>
-      <c r="H6" t="s">
-        <v>169</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -2128,16 +2126,20 @@
         <v>37</v>
       </c>
       <c r="D7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" t="s">
         <v>170</v>
-      </c>
-      <c r="E7" t="s">
-        <v>171</v>
       </c>
       <c r="F7" t="s">
         <v>42</v>
       </c>
-      <c r="G7"/>
-      <c r="H7"/>
+      <c r="G7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H7" t="s">
+        <v>171</v>
+      </c>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -2303,7 +2305,7 @@
         <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
         <v>184</v>
@@ -2335,7 +2337,7 @@
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F15" t="s">
         <v>55</v>
@@ -2358,7 +2360,7 @@
         <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
@@ -2368,7 +2370,7 @@
         <v>86</v>
       </c>
       <c r="G16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H16" t="s">
         <v>90</v>
@@ -2384,21 +2386,21 @@
         <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
         <v>190</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -2452,7 +2454,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
         <v>196</v>
@@ -2479,7 +2481,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21"/>
       <c r="C21" t="s">
@@ -2504,7 +2506,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
         <v>103</v>
@@ -2523,7 +2525,7 @@
       </c>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I22" t="s">
         <v>100</v>
@@ -2533,32 +2535,32 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23"/>
+        <v>130</v>
+      </c>
+      <c r="B23" t="s">
+        <v>144</v>
+      </c>
       <c r="C23"/>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F23"/>
       <c r="G23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H23" t="s">
         <v>210</v>
       </c>
-      <c r="I23" t="s">
-        <v>145</v>
-      </c>
+      <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B24"/>
       <c r="C24" t="s">
@@ -2583,7 +2585,7 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -2598,7 +2600,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B26" t="s">
         <v>216</v>
@@ -2619,7 +2621,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B27" t="s">
         <v>219</v>
@@ -2640,7 +2642,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
         <v>222</v>
@@ -2659,7 +2661,7 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
         <v>224</v>
@@ -2678,7 +2680,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
         <v>226</v>
@@ -2695,7 +2697,7 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B31" t="s">
         <v>227</v>
@@ -2714,7 +2716,7 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B32"/>
       <c r="C32"/>
@@ -2752,8 +2754,8 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="60" zoomScaleNormal="60" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2879,10 +2881,10 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" t="s">
         <v>170</v>
-      </c>
-      <c r="C6" t="s">
-        <v>171</v>
       </c>
       <c r="D6" t="s">
         <v>174</v>
@@ -2909,7 +2911,9 @@
         <v>59</v>
       </c>
       <c r="D7"/>
-      <c r="E7"/>
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
       <c r="F7"/>
       <c r="G7" t="s">
         <v>47</v>
@@ -3066,10 +3070,10 @@
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G14"/>
       <c r="H14" t="s">
@@ -3137,7 +3141,7 @@
         <v>198</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E17" t="s">
         <v>199</v>
@@ -3177,40 +3181,40 @@
         <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19"/>
       <c r="G19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
@@ -3218,15 +3222,15 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F21" t="s">
         <v>209</v>
@@ -3238,17 +3242,17 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
         <v>234</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E22" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>
@@ -3258,7 +3262,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
         <v>235</v>
@@ -3280,13 +3284,13 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" t="s">
         <v>140</v>
       </c>
-      <c r="B24" t="s">
-        <v>141</v>
-      </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="s">
@@ -3304,7 +3308,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -3318,7 +3322,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B26" t="s">
         <v>238</v>
@@ -3338,7 +3342,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B27" t="s">
         <v>241</v>
@@ -3358,7 +3362,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
         <v>244</v>
@@ -3378,7 +3382,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
         <v>246</v>
@@ -3396,7 +3400,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
         <v>248</v>
@@ -3418,7 +3422,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B31"/>
       <c r="C31" t="s">
@@ -3436,7 +3440,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B32" t="s">
         <v>252</v>
@@ -3576,13 +3580,13 @@
       <c r="D5" t="s">
         <v>230</v>
       </c>
-      <c r="E5"/>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
       <c r="F5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" t="s">
-        <v>69</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
     </row>
@@ -3591,10 +3595,10 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D6" t="s">
         <v>190</v>
@@ -3715,16 +3719,16 @@
       <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
+      <c r="D11"/>
       <c r="E11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11"/>
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
       <c r="H11" t="s">
         <v>103</v>
       </c>
@@ -3735,10 +3739,10 @@
         <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
         <v>67</v>
@@ -3876,20 +3880,20 @@
       </c>
       <c r="B18"/>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I18"/>
     </row>
@@ -3918,7 +3922,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
         <v>209</v>
@@ -3930,10 +3934,10 @@
         <v>236</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G20" t="s">
         <v>209</v>
@@ -3947,7 +3951,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
         <v>95</v>
@@ -3970,10 +3974,10 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
         <v>208</v>
@@ -3984,57 +3988,55 @@
       <c r="E22" t="s">
         <v>208</v>
       </c>
-      <c r="F22" t="s">
-        <v>134</v>
-      </c>
+      <c r="F22"/>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>132</v>
-      </c>
-      <c r="I22" t="s">
-        <v>137</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="I22"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23"/>
-      <c r="C23" t="s">
-        <v>106</v>
-      </c>
+      <c r="C23"/>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G23"/>
       <c r="H23" t="s">
         <v>105</v>
       </c>
       <c r="I23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C24"/>
       <c r="D24" t="s">
-        <v>139</v>
-      </c>
-      <c r="E24"/>
-      <c r="F24"/>
+        <v>138</v>
+      </c>
+      <c r="E24" t="s">
+        <v>136</v>
+      </c>
+      <c r="F24" t="s">
+        <v>133</v>
+      </c>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -4054,7 +4056,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26"/>
       <c r="C26"/>
@@ -4067,7 +4069,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B27" t="s">
         <v>259</v>
@@ -4084,7 +4086,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
         <v>261</v>
@@ -4101,7 +4103,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
         <v>263</v>
@@ -4116,7 +4118,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B30" t="s">
         <v>264</v>
@@ -4131,7 +4133,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
         <v>265</v>
@@ -4146,7 +4148,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B32" t="s">
         <v>266</v>
@@ -4161,7 +4163,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -4307,14 +4309,14 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F5" t="s">
         <v>70</v>
@@ -4420,10 +4422,10 @@
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4462,7 +4464,7 @@
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I12" t="s">
         <v>68</v>
@@ -4548,10 +4550,10 @@
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
@@ -4602,47 +4604,45 @@
         <v>206</v>
       </c>
       <c r="I19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
         <v>111</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>112</v>
-      </c>
-      <c r="C20" t="s">
-        <v>113</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" t="s">
         <v>115</v>
-      </c>
-      <c r="I20" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
         <v>198</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" t="s">
-        <v>106</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D21"/>
       <c r="E21" t="s">
         <v>256</v>
       </c>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I21" t="s">
         <v>105</v>
@@ -4659,14 +4659,14 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
@@ -4678,7 +4678,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
         <v>210</v>
@@ -4701,10 +4701,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" t="s">
         <v>236</v>
@@ -4716,15 +4716,15 @@
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -4737,7 +4737,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B26" t="s">
         <v>273</v>
@@ -4754,7 +4754,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B27" t="s">
         <v>275</v>
@@ -4769,7 +4769,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
@@ -4784,7 +4784,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
         <v>277</v>
@@ -4799,7 +4799,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
@@ -4814,7 +4814,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -4829,7 +4829,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B32" t="s">
         <v>280</v>

</xml_diff>

<commit_message>
tt update to v4.0
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -215,25 +215,25 @@
     <t>IS-E Shahbaz</t>
   </si>
   <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Algo-E Dr. Atif</t>
+  </si>
+  <si>
+    <t>CA-Gr2 Dr. Hasina</t>
+  </si>
+  <si>
+    <t>CM-Gr2 Sameera</t>
+  </si>
+  <si>
+    <t>TOA-Gr2 Shaharbano</t>
+  </si>
+  <si>
+    <t>TOA-Gr1 Shaharbano</t>
+  </si>
+  <si>
     <t>PIT-C Saeeda</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>Algo-E Dr. Atif</t>
-  </si>
-  <si>
-    <t>CA-Gr2 Dr. Hasina</t>
-  </si>
-  <si>
-    <t>CM-Gr2 Sameera</t>
-  </si>
-  <si>
-    <t>TOA-Gr2 Shaharbano</t>
-  </si>
-  <si>
-    <t>TOA-Gr1 Shaharbano</t>
   </si>
   <si>
     <t>R109</t>
@@ -1482,31 +1482,31 @@
       <c r="H11" t="s">
         <v>63</v>
       </c>
-      <c r="I11" t="s">
-        <v>64</v>
-      </c>
+      <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
         <v>65</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" t="s">
         <v>68</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>69</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>70</v>
       </c>
-      <c r="H12"/>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9">
@@ -2240,21 +2240,19 @@
         <v>73</v>
       </c>
       <c r="H11"/>
-      <c r="I11" t="s">
-        <v>72</v>
-      </c>
+      <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
         <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
         <v>41</v>
@@ -2284,14 +2282,10 @@
         <v>17</v>
       </c>
       <c r="D13"/>
-      <c r="E13" t="s">
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13" t="s">
         <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" t="s">
-        <v>45</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="s">
@@ -2304,9 +2298,7 @@
       <c r="A14" t="s">
         <v>77</v>
       </c>
-      <c r="B14" t="s">
-        <v>106</v>
-      </c>
+      <c r="B14"/>
       <c r="C14" t="s">
         <v>184</v>
       </c>
@@ -2335,7 +2327,9 @@
         <v>188</v>
       </c>
       <c r="C15"/>
-      <c r="D15"/>
+      <c r="D15" t="s">
+        <v>106</v>
+      </c>
       <c r="E15" t="s">
         <v>107</v>
       </c>
@@ -2395,9 +2389,11 @@
       <c r="E17" t="s">
         <v>117</v>
       </c>
-      <c r="F17"/>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="H17" t="s">
         <v>122</v>
@@ -2446,7 +2442,7 @@
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
@@ -3005,7 +3001,7 @@
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
@@ -3014,10 +3010,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
@@ -3627,15 +3623,11 @@
       <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s">
-        <v>75</v>
-      </c>
+      <c r="D7"/>
       <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" t="s">
-        <v>76</v>
-      </c>
+      <c r="F7"/>
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -3657,7 +3649,9 @@
       <c r="F8" t="s">
         <v>39</v>
       </c>
-      <c r="G8"/>
+      <c r="G8" t="s">
+        <v>76</v>
+      </c>
       <c r="H8"/>
       <c r="I8"/>
     </row>
@@ -3724,10 +3718,10 @@
         <v>167</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
         <v>103</v>
@@ -3736,7 +3730,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
         <v>166</v>
@@ -3745,10 +3739,10 @@
         <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
         <v>191</v>
@@ -3860,18 +3854,22 @@
         <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C17" t="s">
-        <v>214</v>
-      </c>
-      <c r="D17"/>
+        <v>203</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
       <c r="E17" t="s">
-        <v>215</v>
+        <v>72</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17"/>
+      <c r="H17" t="s">
+        <v>255</v>
+      </c>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
@@ -3901,21 +3899,15 @@
       <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B19" t="s">
-        <v>202</v>
-      </c>
-      <c r="C19" t="s">
-        <v>203</v>
-      </c>
+      <c r="B19"/>
+      <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
-      <c r="H19" t="s">
-        <v>255</v>
-      </c>
+      <c r="H19"/>
       <c r="I19" t="s">
         <v>198</v>
       </c>
@@ -3999,11 +3991,15 @@
       <c r="A23" t="s">
         <v>130</v>
       </c>
-      <c r="B23"/>
-      <c r="C23"/>
+      <c r="B23" t="s">
+        <v>211</v>
+      </c>
+      <c r="C23" t="s">
+        <v>214</v>
+      </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>215</v>
       </c>
       <c r="F23" t="s">
         <v>125</v>
@@ -4168,7 +4164,9 @@
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
-      <c r="E33"/>
+      <c r="E33" t="s">
+        <v>210</v>
+      </c>
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33"/>
@@ -4319,13 +4317,13 @@
         <v>167</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" t="s">
         <v>270</v>
       </c>
       <c r="H5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I5"/>
     </row>
@@ -4453,11 +4451,11 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -4467,7 +4465,7 @@
         <v>122</v>
       </c>
       <c r="I12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -4595,7 +4593,9 @@
         <v>214</v>
       </c>
       <c r="D19"/>
-      <c r="E19"/>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
       <c r="F19" t="s">
         <v>205</v>
       </c>

</xml_diff>

<commit_message>
partial working EE, updated to v6
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -140,7 +140,7 @@
     <t>OOAD-E Rubab</t>
   </si>
   <si>
-    <t>DS-D M.Rafi</t>
+    <t>DS-D &amp; DS- F M.Rafi</t>
   </si>
   <si>
     <t>HCI-D Dr. Rauf</t>
@@ -287,6 +287,9 @@
     <t>DS-G Nida</t>
   </si>
   <si>
+    <t>DS-C Nida</t>
+  </si>
+  <si>
     <t>DS-A Nida</t>
   </si>
   <si>
@@ -344,12 +347,6 @@
     <t>AP-F Sonia</t>
   </si>
   <si>
-    <t>DS-F teerath</t>
-  </si>
-  <si>
-    <t>DS-C teerath</t>
-  </si>
-  <si>
     <t>Eng-F2 Hafza</t>
   </si>
   <si>
@@ -545,6 +542,9 @@
     <t>OS-Gr4 Abdul Rehman</t>
   </si>
   <si>
+    <t>OS-Gr2 Nousheen</t>
+  </si>
+  <si>
     <t>HCI-G Farrukh</t>
   </si>
   <si>
@@ -572,25 +572,25 @@
     <t>Discrete-F Dr. Jalaluddin</t>
   </si>
   <si>
+    <t>OS-Gr1 Nousheen</t>
+  </si>
+  <si>
+    <t>OS-Gr3 Nousheen</t>
+  </si>
+  <si>
     <t>ISPM-Gr2 Ubaid</t>
   </si>
   <si>
     <t>ISPM-Gr1 Ubaid</t>
   </si>
   <si>
-    <t>OS-Gr1 Nousheen</t>
-  </si>
-  <si>
-    <t>OS-Gr3 Nousheen</t>
+    <t>DS-D &amp; DS-F M.Rafi</t>
   </si>
   <si>
     <t>Eng-Lab B1 &amp; B2 Hubrah</t>
   </si>
   <si>
     <t>Eng-Lab E1 &amp; E2 Hubrah</t>
-  </si>
-  <si>
-    <t>OS-Gr2 Nousheen</t>
   </si>
   <si>
     <t>CA-Gr4 Ahsan</t>
@@ -1516,10 +1516,10 @@
       <c r="B13" t="s">
         <v>72</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13"/>
+      <c r="D13" t="s">
         <v>73</v>
       </c>
-      <c r="D13"/>
       <c r="E13" t="s">
         <v>74</v>
       </c>
@@ -1577,225 +1577,223 @@
       <c r="B16" t="s">
         <v>86</v>
       </c>
-      <c r="C16"/>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H18"/>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D19"/>
-      <c r="E19" t="s">
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19" t="s">
         <v>107</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>108</v>
       </c>
-      <c r="G19" t="s">
-        <v>106</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>109</v>
-      </c>
-      <c r="I19" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
         <v>111</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>112</v>
-      </c>
-      <c r="C20" t="s">
-        <v>113</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" t="s">
         <v>114</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>115</v>
-      </c>
-      <c r="G20" t="s">
-        <v>116</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" t="s">
         <v>117</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>118</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>119</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>120</v>
       </c>
-      <c r="E21" t="s">
-        <v>121</v>
-      </c>
       <c r="F21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" t="s">
         <v>122</v>
-      </c>
-      <c r="I21" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22"/>
       <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
         <v>125</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>126</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>127</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>128</v>
-      </c>
-      <c r="G22" t="s">
-        <v>129</v>
       </c>
       <c r="H22"/>
       <c r="I22"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
         <v>130</v>
-      </c>
-      <c r="B23" t="s">
-        <v>131</v>
       </c>
       <c r="C23"/>
       <c r="D23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" t="s">
         <v>132</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>133</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>134</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>135</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>136</v>
-      </c>
-      <c r="I23" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
         <v>138</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>139</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" t="s">
         <v>140</v>
-      </c>
-      <c r="D24" t="s">
-        <v>140</v>
-      </c>
-      <c r="E24" t="s">
-        <v>141</v>
       </c>
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24" t="s">
+        <v>141</v>
+      </c>
+      <c r="I24" t="s">
         <v>142</v>
-      </c>
-      <c r="I24" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -1808,16 +1806,16 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" t="s">
         <v>145</v>
-      </c>
-      <c r="B26" t="s">
-        <v>146</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G26"/>
       <c r="H26"/>
@@ -1825,29 +1823,29 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" t="s">
         <v>148</v>
-      </c>
-      <c r="B27" t="s">
-        <v>149</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" t="s">
         <v>152</v>
-      </c>
-      <c r="B28" t="s">
-        <v>153</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -1859,33 +1857,33 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" t="s">
         <v>157</v>
-      </c>
-      <c r="B30" t="s">
-        <v>158</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
@@ -1893,24 +1891,24 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" t="s">
         <v>160</v>
-      </c>
-      <c r="B31" t="s">
-        <v>161</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B32"/>
       <c r="C32"/>
@@ -1965,7 +1963,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2091,7 +2089,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -2106,10 +2104,10 @@
         <v>23</v>
       </c>
       <c r="G6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H6" t="s">
         <v>166</v>
-      </c>
-      <c r="H6" t="s">
-        <v>167</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -2124,19 +2122,19 @@
         <v>37</v>
       </c>
       <c r="D7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" t="s">
         <v>168</v>
-      </c>
-      <c r="E7" t="s">
-        <v>169</v>
       </c>
       <c r="F7" t="s">
         <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -2148,19 +2146,15 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" t="s">
         <v>171</v>
       </c>
-      <c r="D8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" t="s">
-        <v>39</v>
-      </c>
+      <c r="E8"/>
+      <c r="F8"/>
       <c r="G8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H8" t="s">
         <v>38</v>
@@ -2174,9 +2168,11 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" t="s">
         <v>173</v>
       </c>
-      <c r="C9"/>
       <c r="D9" t="s">
         <v>174</v>
       </c>
@@ -2267,7 +2263,9 @@
         <v>182</v>
       </c>
       <c r="H12"/>
-      <c r="I12"/>
+      <c r="I12" t="s">
+        <v>86</v>
+      </c>
       <c r="J12"/>
       <c r="K12"/>
     </row>
@@ -2282,8 +2280,12 @@
         <v>17</v>
       </c>
       <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
+      <c r="E13" t="s">
+        <v>183</v>
+      </c>
+      <c r="F13" t="s">
+        <v>184</v>
+      </c>
       <c r="G13" t="s">
         <v>18</v>
       </c>
@@ -2300,19 +2302,19 @@
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D14" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G14" t="s">
         <v>185</v>
-      </c>
-      <c r="F14" t="s">
-        <v>186</v>
-      </c>
-      <c r="G14" t="s">
-        <v>183</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
@@ -2324,15 +2326,11 @@
         <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C15"/>
-      <c r="D15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" t="s">
-        <v>108</v>
-      </c>
+      <c r="D15"/>
+      <c r="E15"/>
       <c r="F15" t="s">
         <v>55</v>
       </c>
@@ -2340,7 +2338,7 @@
         <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -2354,38 +2352,36 @@
         <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
         <v>88</v>
-      </c>
-      <c r="F16" t="s">
-        <v>86</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" t="s">
         <v>90</v>
-      </c>
-      <c r="I16" t="s">
-        <v>89</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" t="s">
-        <v>189</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C17"/>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F17" t="s">
         <v>44</v>
@@ -2394,7 +2390,7 @@
         <v>45</v>
       </c>
       <c r="H17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -2402,7 +2398,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
         <v>190</v>
@@ -2427,7 +2423,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
@@ -2448,7 +2444,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
         <v>195</v>
@@ -2475,7 +2471,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21"/>
       <c r="C21" t="s">
@@ -2500,10 +2496,10 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
         <v>206</v>
@@ -2519,31 +2515,31 @@
       </c>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J22"/>
       <c r="K22"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C23"/>
       <c r="D23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F23"/>
       <c r="G23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H23" t="s">
         <v>209</v>
@@ -2554,7 +2550,7 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B24"/>
       <c r="C24" t="s">
@@ -2579,7 +2575,7 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -2594,7 +2590,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B26" t="s">
         <v>215</v>
@@ -2615,7 +2611,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
         <v>218</v>
@@ -2636,7 +2632,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
         <v>221</v>
@@ -2655,7 +2651,7 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
         <v>223</v>
@@ -2674,7 +2670,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
         <v>225</v>
@@ -2691,7 +2687,7 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31" t="s">
         <v>226</v>
@@ -2710,7 +2706,7 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B32"/>
       <c r="C32"/>
@@ -2875,13 +2871,13 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" t="s">
         <v>168</v>
       </c>
-      <c r="C6" t="s">
-        <v>169</v>
-      </c>
       <c r="D6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
@@ -2906,7 +2902,7 @@
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="s">
@@ -3022,11 +3018,11 @@
         <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J12"/>
     </row>
@@ -3059,22 +3055,22 @@
         <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G14"/>
       <c r="H14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J14"/>
     </row>
@@ -3083,15 +3079,15 @@
         <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" t="s">
         <v>102</v>
-      </c>
-      <c r="F15" t="s">
-        <v>101</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
@@ -3126,7 +3122,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
         <v>195</v>
@@ -3135,7 +3131,7 @@
         <v>197</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E17" t="s">
         <v>198</v>
@@ -3145,16 +3141,16 @@
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B18"/>
       <c r="C18"/>
@@ -3172,43 +3168,43 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19"/>
       <c r="G19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
@@ -3216,7 +3212,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
@@ -3224,13 +3220,13 @@
         <v>233</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F21" t="s">
         <v>208</v>
       </c>
       <c r="G21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
@@ -3238,17 +3234,17 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
         <v>234</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>
@@ -3258,7 +3254,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
         <v>235</v>
@@ -3280,13 +3276,13 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
         <v>138</v>
       </c>
-      <c r="B24" t="s">
-        <v>139</v>
-      </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="s">
@@ -3304,7 +3300,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -3318,7 +3314,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B26" t="s">
         <v>238</v>
@@ -3338,7 +3334,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
         <v>241</v>
@@ -3358,7 +3354,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
         <v>244</v>
@@ -3378,7 +3374,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
         <v>246</v>
@@ -3396,7 +3392,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
         <v>248</v>
@@ -3418,7 +3414,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31"/>
       <c r="C31" t="s">
@@ -3436,7 +3432,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B32" t="s">
         <v>252</v>
@@ -3591,13 +3587,13 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -3607,10 +3603,10 @@
       </c>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3646,9 +3642,7 @@
       <c r="E8" t="s">
         <v>36</v>
       </c>
-      <c r="F8" t="s">
-        <v>39</v>
-      </c>
+      <c r="F8"/>
       <c r="G8" t="s">
         <v>76</v>
       </c>
@@ -3669,17 +3663,17 @@
         <v>177</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G9"/>
       <c r="H9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3708,14 +3702,14 @@
         <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F11" t="s">
         <v>69</v>
@@ -3724,7 +3718,7 @@
         <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I11"/>
     </row>
@@ -3733,10 +3727,10 @@
         <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
         <v>66</v>
@@ -3793,16 +3787,16 @@
         <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E14" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F14" t="s">
-        <v>63</v>
+        <v>187</v>
       </c>
       <c r="G14" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H14" t="s">
         <v>58</v>
@@ -3818,14 +3812,16 @@
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
         <v>171</v>
-      </c>
-      <c r="F15"/>
-      <c r="G15" t="s">
-        <v>172</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -3835,13 +3831,15 @@
         <v>85</v>
       </c>
       <c r="B16"/>
-      <c r="C16"/>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
       <c r="D16"/>
       <c r="E16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
         <v>88</v>
-      </c>
-      <c r="F16" t="s">
-        <v>87</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
@@ -3851,7 +3849,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
         <v>201</v>
@@ -3874,43 +3872,43 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19"/>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
         <v>233</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I19" t="s">
         <v>197</v>
@@ -3918,7 +3916,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
         <v>208</v>
@@ -3929,12 +3927,8 @@
       <c r="D20" t="s">
         <v>236</v>
       </c>
-      <c r="E20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" t="s">
-        <v>107</v>
-      </c>
+      <c r="E20"/>
+      <c r="F20"/>
       <c r="G20" t="s">
         <v>208</v>
       </c>
@@ -3947,33 +3941,33 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
         <v>256</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" t="s">
         <v>207</v>
@@ -3987,13 +3981,13 @@
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I22"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
         <v>210</v>
@@ -4008,31 +4002,31 @@
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C24"/>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -4052,7 +4046,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B26"/>
       <c r="C26"/>
@@ -4065,7 +4059,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B27" t="s">
         <v>259</v>
@@ -4082,7 +4076,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
         <v>261</v>
@@ -4099,7 +4093,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B29" t="s">
         <v>263</v>
@@ -4114,7 +4108,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B30" t="s">
         <v>264</v>
@@ -4129,7 +4123,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B31" t="s">
         <v>265</v>
@@ -4144,7 +4138,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B32" t="s">
         <v>266</v>
@@ -4159,7 +4153,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -4307,14 +4301,14 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F5" t="s">
         <v>69</v>
@@ -4420,10 +4414,10 @@
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4443,10 +4437,10 @@
       </c>
       <c r="G11"/>
       <c r="H11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" t="s">
         <v>102</v>
-      </c>
-      <c r="I11" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -4462,7 +4456,7 @@
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I12" t="s">
         <v>67</v>
@@ -4538,32 +4532,32 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
         <v>233</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" t="s">
         <v>96</v>
-      </c>
-      <c r="I17" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -4584,7 +4578,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
         <v>214</v>
@@ -4594,7 +4588,7 @@
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F19" t="s">
         <v>204</v>
@@ -4604,43 +4598,43 @@
         <v>205</v>
       </c>
       <c r="I19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
         <v>111</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>112</v>
-      </c>
-      <c r="C20" t="s">
-        <v>113</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" t="s">
         <v>115</v>
-      </c>
-      <c r="I20" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
         <v>197</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
@@ -4651,22 +4645,22 @@
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I21" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
@@ -4678,7 +4672,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
         <v>209</v>
@@ -4701,10 +4695,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24" t="s">
         <v>236</v>
@@ -4716,15 +4710,15 @@
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -4737,7 +4731,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B26" t="s">
         <v>273</v>
@@ -4754,7 +4748,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
         <v>275</v>
@@ -4769,7 +4763,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
@@ -4784,7 +4778,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
         <v>277</v>
@@ -4799,7 +4793,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
@@ -4814,7 +4808,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -4829,7 +4823,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B32" t="s">
         <v>280</v>

</xml_diff>

<commit_message>
replace GR with Gr in fix.php
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -83,7 +83,7 @@
     <t>E2</t>
   </si>
   <si>
-    <t>DS-GR1 Abdul Aziz</t>
+    <t>DS-Gr1 Abdul Aziz</t>
   </si>
   <si>
     <t>OS-E Tania</t>
@@ -137,10 +137,10 @@
     <t>TOA-E Shaharbano</t>
   </si>
   <si>
-    <t>DS-GR3 Anum</t>
-  </si>
-  <si>
-    <t>DS-GR2 Anum</t>
+    <t>DS-Gr3 Anum</t>
+  </si>
+  <si>
+    <t>DS-Gr2 Anum</t>
   </si>
   <si>
     <t>E5</t>
@@ -161,13 +161,13 @@
     <t>E6</t>
   </si>
   <si>
-    <t>CG GR2 Javeria</t>
+    <t>CG Gr2 Javeria</t>
   </si>
   <si>
     <t>CG- Gr1 Javeria</t>
   </si>
   <si>
-    <t>HCI-GR1 Bahraj</t>
+    <t>HCI-Gr1 Bahraj</t>
   </si>
   <si>
     <t>DLD-E Behraj</t>
@@ -182,7 +182,7 @@
     <t>OOP-B Zain</t>
   </si>
   <si>
-    <t>Dsci GR1 Dr. Atif</t>
+    <t>Dsci Gr1 Dr. Atif</t>
   </si>
   <si>
     <t>OR Gr1 Aasma</t>
@@ -212,10 +212,10 @@
     <t>SE-F Dr. Nauman Ghazi</t>
   </si>
   <si>
-    <t>BLN GR1 Dr. Sufian</t>
-  </si>
-  <si>
-    <t>BLN GR2 Dr. Sufian</t>
+    <t>BLN Gr1 Dr. Sufian</t>
+  </si>
+  <si>
+    <t>BLN Gr2 Dr. Sufian</t>
   </si>
   <si>
     <t>R109</t>
@@ -242,16 +242,16 @@
     <t>S1</t>
   </si>
   <si>
-    <t>DP GR1 Abdul Rahman</t>
-  </si>
-  <si>
-    <t>DP GR2 Abdul Rahman</t>
+    <t>DP Gr1 Abdul Rahman</t>
+  </si>
+  <si>
+    <t>DP Gr2 Abdul Rahman</t>
   </si>
   <si>
     <t>ME Gr1 Michael</t>
   </si>
   <si>
-    <t>DP GR3 Abdul Rahman</t>
+    <t>DP Gr3 Abdul Rahman</t>
   </si>
   <si>
     <t>S2</t>
@@ -263,10 +263,10 @@
     <t>Prob-E Javeria Iftikhar</t>
   </si>
   <si>
-    <t>CAL-GR2 Javeria Iftikhar</t>
-  </si>
-  <si>
-    <t>CAL-GR1 Javeria Iftikhar</t>
+    <t>CAL-Gr2 Javeria Iftikhar</t>
+  </si>
+  <si>
+    <t>CAL-Gr1 Javeria Iftikhar</t>
   </si>
   <si>
     <t>OS-F Nousheen</t>
@@ -308,7 +308,7 @@
     <t>Prob-D Osama</t>
   </si>
   <si>
-    <t>DS-GR4 Nida</t>
+    <t>DS-Gr4 Nida</t>
   </si>
   <si>
     <t>CPS-F Javed Iqbal</t>
@@ -332,13 +332,13 @@
     <t>AL Gr1 Dr. Shahzad</t>
   </si>
   <si>
-    <t>CG GR3 Javeria</t>
+    <t>CG Gr3 Javeria</t>
   </si>
   <si>
     <t>DLD-B Rabia</t>
   </si>
   <si>
-    <t>Al GR1 Dr. Shahzad</t>
+    <t>Al Gr1 Dr. Shahzad</t>
   </si>
   <si>
     <t>CR-10</t>
@@ -440,7 +440,7 @@
     <t>Dsci Gr2 Dr. Zeeshan</t>
   </si>
   <si>
-    <t>OOAD-GR1 Tooba</t>
+    <t>OOAD-Gr1 Tooba</t>
   </si>
   <si>
     <t>CN Lab-A Munim</t>
@@ -470,7 +470,7 @@
     <t>EE Lab-8</t>
   </si>
   <si>
-    <t>DS Lab- GR2 Irfan</t>
+    <t>DS Lab- Gr2 Irfan</t>
   </si>
   <si>
     <t>OS Lab-E Abdullah</t>
@@ -512,13 +512,13 @@
     <t>TUESDAY</t>
   </si>
   <si>
-    <t>Dwh GR1 Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>Dwh GR2 Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>DB-GR1 Anum</t>
+    <t>Dwh Gr1 Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>Dwh Gr2 Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>DB-Gr1 Anum</t>
   </si>
   <si>
     <t>AI-B Dr. Rauf</t>
@@ -539,22 +539,22 @@
     <t>Pst.-G Amanullah</t>
   </si>
   <si>
-    <t>OOAD-GR1 Rubab</t>
+    <t>OOAD-Gr1 Rubab</t>
   </si>
   <si>
     <t>TBW-D Sameera</t>
   </si>
   <si>
-    <t>ALGO-GR1 Zeshan Khan</t>
+    <t>ALGO-Gr1 Zeshan Khan</t>
   </si>
   <si>
     <t>DLD-H Javed Qureshi</t>
   </si>
   <si>
-    <t>WP GR3 Dr. Farooque</t>
-  </si>
-  <si>
-    <t>WP GR4 Dr. Farooque</t>
+    <t>WP Gr3 Dr. Farooque</t>
+  </si>
+  <si>
+    <t>WP Gr4 Dr. Farooque</t>
   </si>
   <si>
     <t>AI-F Saeeda</t>
@@ -566,22 +566,22 @@
     <t>AI-E Saeeda</t>
   </si>
   <si>
-    <t>IPT GR1 Murtaza</t>
-  </si>
-  <si>
-    <t>IPT GR2 Murtaza</t>
+    <t>IPT Gr1 Murtaza</t>
+  </si>
+  <si>
+    <t>IPT Gr2 Murtaza</t>
   </si>
   <si>
     <t>NM Gr2 Mr. Shahbaz</t>
   </si>
   <si>
-    <t>ISPM GR1 Ubaid</t>
-  </si>
-  <si>
-    <t>WP GR1 Salman</t>
-  </si>
-  <si>
-    <t>WP GR2 Salman</t>
+    <t>ISPM Gr1 Ubaid</t>
+  </si>
+  <si>
+    <t>WP Gr1 Salman</t>
+  </si>
+  <si>
+    <t>WP Gr2 Salman</t>
   </si>
   <si>
     <t>Prob-A Nadeem Khan</t>
@@ -638,7 +638,7 @@
     <t>OOP-Lab B Basit</t>
   </si>
   <si>
-    <t>DS Lab- GR1 Abdul Aziz</t>
+    <t>DS Lab- Gr1 Abdul Aziz</t>
   </si>
   <si>
     <t>DLD-Lab A1 Mubashyra</t>
@@ -650,7 +650,7 @@
     <t>OS Lab-A Safia</t>
   </si>
   <si>
-    <t>COAL Lab- GR2 Summiyah</t>
+    <t>COAL Lab- Gr2 Summiyah</t>
   </si>
   <si>
     <t>DLD-Lab B2 Hamza</t>
@@ -677,10 +677,10 @@
     <t>CN-D Nadeem Kafi</t>
   </si>
   <si>
-    <t>CA-GR3 Dr. Noman Durrani</t>
-  </si>
-  <si>
-    <t>CA-GR1 Dr. Noman Durrani</t>
+    <t>CA-Gr3 Dr. Noman Durrani</t>
+  </si>
+  <si>
+    <t>CA-Gr1 Dr. Noman Durrani</t>
   </si>
   <si>
     <t>DLD-A Khalid</t>
@@ -689,16 +689,16 @@
     <t>DLD-C Khalid</t>
   </si>
   <si>
-    <t>PIT-GR1 Khalid</t>
-  </si>
-  <si>
-    <t>CA-GR2 Dr. Asif</t>
-  </si>
-  <si>
-    <t>CA-GR4 Dr. Asif</t>
-  </si>
-  <si>
-    <t>IS-GR1 TBA</t>
+    <t>PIT-Gr1 Khalid</t>
+  </si>
+  <si>
+    <t>CA-Gr2 Dr. Asif</t>
+  </si>
+  <si>
+    <t>CA-Gr4 Dr. Asif</t>
+  </si>
+  <si>
+    <t>IS-Gr1 TBA</t>
   </si>
   <si>
     <t>AI-A Nida</t>
@@ -713,7 +713,7 @@
     <t>Pst.-A Kashif</t>
   </si>
   <si>
-    <t>AP-GR1 Javed Qureshi</t>
+    <t>AP-Gr1 Javed Qureshi</t>
   </si>
   <si>
     <t>Prob-E Javeria</t>
@@ -728,10 +728,10 @@
     <t>OS Lab-D Summiyah</t>
   </si>
   <si>
-    <t>DS Lab- GR3 Irfan</t>
-  </si>
-  <si>
-    <t>DS Lab- GR4 Safia</t>
+    <t>DS Lab- Gr3 Irfan</t>
+  </si>
+  <si>
+    <t>DS Lab- Gr4 Safia</t>
   </si>
   <si>
     <t>OS Lab-F Abdullah</t>
@@ -767,10 +767,10 @@
     <t>THURSDAY</t>
   </si>
   <si>
-    <t>Discrete-GR1 Dr. Jalal</t>
-  </si>
-  <si>
-    <t>LA-GR1 Fareeha</t>
+    <t>Discrete-Gr1 Dr. Jalal</t>
+  </si>
+  <si>
+    <t>LA-Gr1 Fareeha</t>
   </si>
   <si>
     <t>Pst.-C Kashif</t>
@@ -788,7 +788,7 @@
     <t>CPS-Lab H2 Kishwar</t>
   </si>
   <si>
-    <t>DB Lab-GR1 Irfan</t>
+    <t>DB Lab-Gr1 Irfan</t>
   </si>
   <si>
     <t>CN Lab-E Awais</t>
@@ -827,7 +827,7 @@
     <t>J UMMA PRAYER</t>
   </si>
   <si>
-    <t>COAL Lab- GR1 Summiyah</t>
+    <t>COAL Lab- Gr1 Summiyah</t>
   </si>
   <si>
     <t>B R E A K</t>

</xml_diff>

<commit_message>
update tt to v2.0
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="274">
   <si>
     <t>MONDAY</t>
   </si>
@@ -71,9 +71,6 @@
     <t>SE-A Farrukh</t>
   </si>
   <si>
-    <t>SE-B Farrukh</t>
-  </si>
-  <si>
     <t>CN-C Dr. Fahad</t>
   </si>
   <si>
@@ -110,7 +107,7 @@
     <t>OOP-A Mahrukh</t>
   </si>
   <si>
-    <t>CC- Gr1 Shahzad</t>
+    <t>TOA-F Shahzad</t>
   </si>
   <si>
     <t>OOP-E Mahrukh</t>
@@ -290,9 +287,6 @@
     <t>TOA-C Zeshan</t>
   </si>
   <si>
-    <t>TOA-F Zeshan</t>
-  </si>
-  <si>
     <t>CR-5</t>
   </si>
   <si>
@@ -443,19 +437,19 @@
     <t>OOAD-Gr1 Tooba</t>
   </si>
   <si>
-    <t>CN Lab-A Munim</t>
+    <t>CN-Lab A Munim</t>
   </si>
   <si>
     <t>Lab-3</t>
   </si>
   <si>
-    <t>CN Lab-D Faizan</t>
+    <t>CN-Lab D Faizan</t>
   </si>
   <si>
     <t>Lab-4</t>
   </si>
   <si>
-    <t>CN Lab-G Awais</t>
+    <t>CN-Lab G1+G2 Awais &amp; Faizan</t>
   </si>
   <si>
     <t>Lab-6</t>
@@ -482,18 +476,15 @@
     <t>OS Lab-G Safia</t>
   </si>
   <si>
+    <t>EE MPI Lab</t>
+  </si>
+  <si>
+    <t>DLD-Lab G1 Farah</t>
+  </si>
+  <si>
     <t>DLD-Lab C2 Maham</t>
   </si>
   <si>
-    <t>EE MPI Lab</t>
-  </si>
-  <si>
-    <t>DLD-Lab G1 Farah</t>
-  </si>
-  <si>
-    <t>RESERVED EE</t>
-  </si>
-  <si>
     <t>LLC</t>
   </si>
   <si>
@@ -512,6 +503,9 @@
     <t>TUESDAY</t>
   </si>
   <si>
+    <t>OOAD-Gr1 Rubab</t>
+  </si>
+  <si>
     <t>Dwh Gr1 Dr. Zulfiqar</t>
   </si>
   <si>
@@ -521,6 +515,12 @@
     <t>DB-Gr1 Anum</t>
   </si>
   <si>
+    <t>SE-B Rubab</t>
+  </si>
+  <si>
+    <t>ALGO-Gr1 Zeshan Khan</t>
+  </si>
+  <si>
     <t>AI-B Dr. Rauf</t>
   </si>
   <si>
@@ -539,13 +539,13 @@
     <t>Pst.-G Amanullah</t>
   </si>
   <si>
-    <t>OOAD-Gr1 Rubab</t>
-  </si>
-  <si>
     <t>TBW-D Sameera</t>
   </si>
   <si>
-    <t>ALGO-Gr1 Zeshan Khan</t>
+    <t>AI-C Saeeda</t>
+  </si>
+  <si>
+    <t>AI-E Saeeda</t>
   </si>
   <si>
     <t>DLD-H Javed Qureshi</t>
@@ -560,12 +560,6 @@
     <t>AI-F Saeeda</t>
   </si>
   <si>
-    <t>AI-C Saeeda</t>
-  </si>
-  <si>
-    <t>AI-E Saeeda</t>
-  </si>
-  <si>
     <t>IPT Gr1 Murtaza</t>
   </si>
   <si>
@@ -644,13 +638,13 @@
     <t>DLD-Lab A1 Mubashyra</t>
   </si>
   <si>
-    <t>PF-Lab A Abdul Aziz &amp; Tooba</t>
+    <t>PF-Lab A Abdul Aziz &amp; Sadia</t>
   </si>
   <si>
     <t>OS Lab-A Safia</t>
   </si>
   <si>
-    <t>COAL Lab- Gr2 Summiyah</t>
+    <t>COAL-Lab Gr2 Tooba</t>
   </si>
   <si>
     <t>DLD-Lab B2 Hamza</t>
@@ -737,16 +731,16 @@
     <t>OS Lab-F Abdullah</t>
   </si>
   <si>
-    <t>CN Lab-B Munim</t>
-  </si>
-  <si>
-    <t>PF-Lab B Faizan &amp; Rahemeen</t>
+    <t>CN-Lab B Munim</t>
+  </si>
+  <si>
+    <t>PF-Lab B Sadia &amp; Rahemeen</t>
   </si>
   <si>
     <t>DLD-Lab H1 Abdul Khaliq</t>
   </si>
   <si>
-    <t>CN Lab-C Awais</t>
+    <t>CN-Lab C Awais</t>
   </si>
   <si>
     <t>OOP-Lab C Basit</t>
@@ -791,10 +785,10 @@
     <t>DB Lab-Gr1 Irfan</t>
   </si>
   <si>
-    <t>CN Lab-E Awais</t>
-  </si>
-  <si>
-    <t>CN Lab-F Munim</t>
+    <t>CN-Lab E Awais</t>
+  </si>
+  <si>
+    <t>CN-Lab F1+F2 Faizan &amp; Munim</t>
   </si>
   <si>
     <t>OOP-Lab E Farah</t>
@@ -809,6 +803,9 @@
     <t>OOP-Lab F Fahim</t>
   </si>
   <si>
+    <t>ICT-Lab Gr1 Summiyah</t>
+  </si>
+  <si>
     <t>OS Lab-C Abdullah</t>
   </si>
   <si>
@@ -827,7 +824,7 @@
     <t>J UMMA PRAYER</t>
   </si>
   <si>
-    <t>COAL Lab- Gr1 Summiyah</t>
+    <t>COAL Lab- Gr1 Tooba</t>
   </si>
   <si>
     <t>B R E A K</t>
@@ -842,7 +839,7 @@
     <t>DLD-Lab F2 Hamza</t>
   </si>
   <si>
-    <t>PF-Lab D Faizan &amp; Rahemeen</t>
+    <t>PF-Lab D Sadia &amp; Rahemeen</t>
   </si>
   <si>
     <t>DLD-Lab F1 Nadeem</t>
@@ -1188,8 +1185,8 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="71" zoomScaleNormal="71" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="14.42578125" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1292,239 +1289,237 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5"/>
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
       </c>
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
         <v>32</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
       </c>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
       </c>
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
         <v>38</v>
-      </c>
-      <c r="H8" t="s">
-        <v>39</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9"/>
       <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
         <v>43</v>
-      </c>
-      <c r="G9" t="s">
-        <v>44</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
         <v>49</v>
-      </c>
-      <c r="H10" t="s">
-        <v>50</v>
       </c>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
-      </c>
-      <c r="B11" t="s">
-        <v>52</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
         <v>53</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>54</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>55</v>
-      </c>
-      <c r="G11" t="s">
-        <v>56</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>58</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>61</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>62</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>63</v>
-      </c>
-      <c r="H12" t="s">
-        <v>64</v>
       </c>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
         <v>65</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>66</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>67</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>68</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>69</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>70</v>
-      </c>
-      <c r="G13" t="s">
-        <v>71</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
         <v>72</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>73</v>
-      </c>
-      <c r="C14" t="s">
-        <v>74</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" t="s">
         <v>75</v>
-      </c>
-      <c r="F14" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" t="s">
-        <v>76</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -1537,222 +1532,220 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
         <v>78</v>
-      </c>
-      <c r="B16" t="s">
-        <v>79</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" t="s">
         <v>80</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>81</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>82</v>
-      </c>
-      <c r="H16" t="s">
-        <v>83</v>
       </c>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
         <v>84</v>
-      </c>
-      <c r="B17" t="s">
-        <v>85</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" t="s">
         <v>86</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>87</v>
       </c>
-      <c r="G17" t="s">
-        <v>88</v>
-      </c>
-      <c r="H17" t="s">
-        <v>89</v>
-      </c>
+      <c r="H17"/>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
         <v>90</v>
-      </c>
-      <c r="B18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" t="s">
-        <v>92</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" t="s">
         <v>93</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>94</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>95</v>
-      </c>
-      <c r="H18" t="s">
-        <v>96</v>
-      </c>
-      <c r="I18" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
         <v>98</v>
-      </c>
-      <c r="B19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" t="s">
-        <v>100</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" t="s">
         <v>101</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>102</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
         <v>103</v>
-      </c>
-      <c r="H19" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
         <v>106</v>
-      </c>
-      <c r="B20" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" t="s">
-        <v>108</v>
       </c>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" t="s">
         <v>113</v>
       </c>
-      <c r="F21" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" t="s">
-        <v>115</v>
-      </c>
       <c r="H21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="s">
         <v>116</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>117</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>118</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22" t="s">
         <v>119</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>120</v>
       </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>121</v>
-      </c>
-      <c r="G22" t="s">
-        <v>122</v>
-      </c>
-      <c r="H22" t="s">
-        <v>123</v>
       </c>
       <c r="I22"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" t="s">
         <v>124</v>
-      </c>
-      <c r="B23" t="s">
-        <v>125</v>
-      </c>
-      <c r="C23" t="s">
-        <v>126</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G23"/>
       <c r="H23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C24"/>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -1765,28 +1758,28 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" t="s">
         <v>136</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>137</v>
-      </c>
-      <c r="C26" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" t="s">
-        <v>139</v>
       </c>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B27"/>
       <c r="C27"/>
@@ -1794,14 +1787,14 @@
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
@@ -1809,97 +1802,95 @@
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
-      <c r="G31" t="s">
-        <v>153</v>
-      </c>
+      <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C33"/>
       <c r="D33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H33" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I33"/>
     </row>
@@ -1939,15 +1930,15 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="71" zoomScaleNormal="71" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2034,83 +2025,87 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
         <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
       </c>
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6"/>
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
       <c r="C6"/>
       <c r="D6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F6" t="s">
         <v>163</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>164</v>
       </c>
-      <c r="F6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>160</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7"/>
-      <c r="I7"/>
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I7" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C8"/>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
         <v>166</v>
@@ -2119,42 +2114,44 @@
         <v>167</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9"/>
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>168</v>
@@ -2167,7 +2164,7 @@
         <v>170</v>
       </c>
       <c r="H10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I10" t="s">
         <v>171</v>
@@ -2175,66 +2172,64 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11"/>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" t="s">
         <v>51</v>
       </c>
-      <c r="B11" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" t="s">
         <v>173</v>
       </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>89</v>
-      </c>
-      <c r="G11" t="s">
-        <v>88</v>
-      </c>
       <c r="H11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I11" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
         <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" t="s">
-        <v>58</v>
       </c>
       <c r="E12"/>
       <c r="F12" t="s">
         <v>175</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
         <v>176</v>
@@ -2248,133 +2243,129 @@
       <c r="F13" t="s">
         <v>176</v>
       </c>
-      <c r="G13" t="s">
-        <v>179</v>
-      </c>
+      <c r="G13"/>
       <c r="H13" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" t="s">
-        <v>180</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
         <v>72</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G14" t="s">
+        <v>182</v>
+      </c>
+      <c r="H14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" t="s">
         <v>73</v>
-      </c>
-      <c r="C14" t="s">
-        <v>181</v>
-      </c>
-      <c r="D14" t="s">
-        <v>182</v>
-      </c>
-      <c r="E14" t="s">
-        <v>183</v>
-      </c>
-      <c r="F14" t="s">
-        <v>181</v>
-      </c>
-      <c r="G14" t="s">
-        <v>184</v>
-      </c>
-      <c r="H14" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>183</v>
+      </c>
+      <c r="G15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="s">
-        <v>185</v>
-      </c>
-      <c r="D15" t="s">
-        <v>186</v>
-      </c>
-      <c r="E15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" t="s">
-        <v>185</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
       <c r="H15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
         <v>49</v>
       </c>
-      <c r="D16" t="s">
-        <v>50</v>
-      </c>
       <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" t="s">
         <v>80</v>
       </c>
-      <c r="F16" t="s">
-        <v>81</v>
-      </c>
       <c r="G16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" t="s">
+        <v>186</v>
+      </c>
+      <c r="E17" t="s">
         <v>86</v>
-      </c>
-      <c r="C17" t="s">
-        <v>187</v>
-      </c>
-      <c r="D17" t="s">
-        <v>188</v>
-      </c>
-      <c r="E17" t="s">
-        <v>87</v>
       </c>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18"/>
       <c r="C18"/>
@@ -2387,155 +2378,155 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F20" t="s">
         <v>171</v>
       </c>
       <c r="G20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F21"/>
       <c r="G21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B22"/>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B23"/>
       <c r="C23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H24" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -2548,47 +2539,47 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F28"/>
       <c r="G28"/>
@@ -2597,30 +2588,30 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F30"/>
       <c r="G30"/>
@@ -2629,44 +2620,44 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -2674,7 +2665,7 @@
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I33"/>
     </row>
@@ -2711,7 +2702,7 @@
   <sheetData>
     <row r="1" spans="1:30">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2880,16 +2871,16 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
         <v>178</v>
@@ -2897,7 +2888,7 @@
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
@@ -2923,7 +2914,7 @@
     </row>
     <row r="6" spans="1:30">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -2932,22 +2923,22 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" t="s">
         <v>86</v>
       </c>
-      <c r="G6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" t="s">
-        <v>87</v>
-      </c>
       <c r="I6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J6"/>
       <c r="K6"/>
@@ -2973,28 +2964,28 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -3021,7 +3012,7 @@
     </row>
     <row r="8" spans="1:30">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -3055,27 +3046,27 @@
     </row>
     <row r="9" spans="1:30">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E9"/>
       <c r="F9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -3101,10 +3092,10 @@
     </row>
     <row r="10" spans="1:30">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
@@ -3143,23 +3134,25 @@
     </row>
     <row r="11" spans="1:30">
       <c r="A11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11"/>
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -3187,31 +3180,29 @@
     </row>
     <row r="12" spans="1:30">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
+      <c r="E12"/>
       <c r="F12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G12" t="s">
         <v>15</v>
       </c>
       <c r="H12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" t="s">
         <v>82</v>
-      </c>
-      <c r="I12" t="s">
-        <v>83</v>
       </c>
       <c r="J12"/>
       <c r="K12"/>
@@ -3237,31 +3228,31 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="s">
+        <v>224</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>186</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" t="s">
         <v>187</v>
-      </c>
-      <c r="C13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" t="s">
-        <v>226</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" t="s">
-        <v>188</v>
-      </c>
-      <c r="G13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" t="s">
-        <v>189</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -3287,25 +3278,25 @@
     </row>
     <row r="14" spans="1:30">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H14" t="s">
         <v>171</v>
@@ -3335,26 +3326,26 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I15" t="s">
         <v>175</v>
@@ -3383,7 +3374,7 @@
     </row>
     <row r="16" spans="1:30">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -3417,29 +3408,29 @@
     </row>
     <row r="17" spans="1:30">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J17"/>
       <c r="K17"/>
@@ -3465,7 +3456,7 @@
     </row>
     <row r="18" spans="1:30">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18"/>
       <c r="C18"/>
@@ -3499,16 +3490,16 @@
     </row>
     <row r="19" spans="1:30">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
@@ -3539,7 +3530,7 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B20"/>
       <c r="C20"/>
@@ -3573,29 +3564,29 @@
     </row>
     <row r="21" spans="1:30">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21"/>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
@@ -3621,26 +3612,26 @@
     </row>
     <row r="22" spans="1:30">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
@@ -3667,7 +3658,7 @@
     </row>
     <row r="23" spans="1:30">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -3701,23 +3692,23 @@
     </row>
     <row r="24" spans="1:30">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J24"/>
       <c r="K24"/>
@@ -3743,7 +3734,7 @@
     </row>
     <row r="25" spans="1:30">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -3777,17 +3768,17 @@
     </row>
     <row r="26" spans="1:30">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -3815,17 +3806,17 @@
     </row>
     <row r="27" spans="1:30">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B27" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -3853,17 +3844,17 @@
     </row>
     <row r="28" spans="1:30">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
@@ -3891,10 +3882,10 @@
     </row>
     <row r="29" spans="1:30">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -3927,17 +3918,17 @@
     </row>
     <row r="30" spans="1:30">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
@@ -3965,17 +3956,17 @@
     </row>
     <row r="31" spans="1:30">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B31" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
@@ -4003,17 +3994,17 @@
     </row>
     <row r="32" spans="1:30">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
@@ -4041,10 +4032,10 @@
     </row>
     <row r="33" spans="1:30">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -4100,15 +4091,15 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="71" zoomScaleNormal="71" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -4223,20 +4214,20 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
         <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
       </c>
       <c r="H5" t="s">
         <v>166</v>
@@ -4254,16 +4245,16 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -4272,13 +4263,13 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" t="s">
         <v>73</v>
       </c>
-      <c r="H6" t="s">
-        <v>74</v>
-      </c>
       <c r="I6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J6"/>
       <c r="K6"/>
@@ -4290,29 +4281,27 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C7"/>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -4324,28 +4313,28 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
       <c r="G8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -4358,25 +4347,25 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -4390,22 +4379,26 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10"/>
-      <c r="C10"/>
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
       <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
         <v>63</v>
-      </c>
-      <c r="E10" t="s">
-        <v>64</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -4418,26 +4411,26 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
-      </c>
-      <c r="B11" t="s">
-        <v>52</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -4450,22 +4443,22 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>58</v>
-      </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -4480,23 +4473,23 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -4510,24 +4503,24 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -4540,23 +4533,23 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
@@ -4568,25 +4561,25 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E16"/>
       <c r="F16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -4598,27 +4591,27 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" t="s">
         <v>35</v>
       </c>
-      <c r="E17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" t="s">
-        <v>36</v>
-      </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I17" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J17"/>
       <c r="K17"/>
@@ -4630,26 +4623,26 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18"/>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I18"/>
       <c r="J18"/>
@@ -4662,7 +4655,7 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
@@ -4682,7 +4675,7 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B20"/>
       <c r="C20"/>
@@ -4702,7 +4695,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
@@ -4722,7 +4715,7 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -4742,28 +4735,28 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I23"/>
       <c r="J23"/>
@@ -4776,24 +4769,24 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C24"/>
       <c r="D24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E24"/>
       <c r="F24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G24" t="s">
+        <v>250</v>
+      </c>
+      <c r="H24" t="s">
         <v>252</v>
-      </c>
-      <c r="H24" t="s">
-        <v>254</v>
       </c>
       <c r="I24"/>
       <c r="J24"/>
@@ -4806,7 +4799,7 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -4826,19 +4819,19 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -4852,7 +4845,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B27"/>
       <c r="C27"/>
@@ -4860,7 +4853,7 @@
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -4874,7 +4867,7 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
@@ -4882,7 +4875,7 @@
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
@@ -4896,17 +4889,17 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
@@ -4920,7 +4913,7 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B30"/>
       <c r="C30"/>
@@ -4928,7 +4921,7 @@
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
@@ -4942,15 +4935,17 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" t="s">
-        <v>151</v>
-      </c>
-      <c r="B31"/>
+        <v>149</v>
+      </c>
+      <c r="B31" t="s">
+        <v>260</v>
+      </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
@@ -4964,10 +4959,10 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
@@ -4986,10 +4981,10 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -4997,7 +4992,7 @@
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I33"/>
       <c r="J33"/>
@@ -5033,15 +5028,15 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="71" zoomScaleNormal="71" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -5135,45 +5130,47 @@
         <v>176</v>
       </c>
       <c r="E5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F5" t="s">
         <v>177</v>
       </c>
       <c r="G5" t="s">
-        <v>267</v>
-      </c>
-      <c r="H5"/>
-      <c r="I5"/>
+        <v>266</v>
+      </c>
+      <c r="H5" t="s">
+        <v>178</v>
+      </c>
+      <c r="I5" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E6" t="s">
-        <v>174</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E6"/>
       <c r="F6" t="s">
         <v>175</v>
       </c>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7"/>
       <c r="C7"/>
@@ -5186,49 +5183,49 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8" t="s">
         <v>224</v>
-      </c>
-      <c r="D8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E8" t="s">
-        <v>180</v>
-      </c>
-      <c r="F8" t="s">
-        <v>226</v>
       </c>
       <c r="G8"/>
       <c r="H8" t="s">
-        <v>178</v>
-      </c>
-      <c r="I8" t="s">
-        <v>41</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="I8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D9"/>
-      <c r="E9"/>
+        <v>216</v>
+      </c>
+      <c r="D9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" t="s">
+        <v>160</v>
+      </c>
       <c r="F9" t="s">
         <v>167</v>
       </c>
       <c r="G9"/>
       <c r="H9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I9" t="s">
         <v>166</v>
@@ -5236,7 +5233,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
@@ -5255,87 +5252,87 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G12"/>
       <c r="H12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
       <c r="I13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E14"/>
       <c r="F14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
@@ -5343,18 +5340,18 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15"/>
       <c r="C15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E15"/>
       <c r="F15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
@@ -5362,18 +5359,18 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
@@ -5381,18 +5378,18 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
@@ -5400,108 +5397,108 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C21"/>
       <c r="D21" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G22"/>
       <c r="H22"/>
@@ -5509,18 +5506,18 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" t="s">
         <v>91</v>
-      </c>
-      <c r="F23" t="s">
-        <v>93</v>
       </c>
       <c r="G23"/>
       <c r="H23"/>
@@ -5528,7 +5525,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -5541,7 +5538,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -5554,31 +5551,31 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -5590,10 +5587,10 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -5605,7 +5602,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B29"/>
       <c r="C29"/>
@@ -5618,10 +5615,10 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -5633,10 +5630,10 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
@@ -5648,10 +5645,10 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
@@ -5663,7 +5660,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>

</xml_diff>

<commit_message>
update tt to v3
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -80,6 +80,9 @@
     <t>E2</t>
   </si>
   <si>
+    <t>OS-E Tania</t>
+  </si>
+  <si>
     <t>OOP-F Abdul Aziz</t>
   </si>
   <si>
@@ -104,9 +107,6 @@
     <t>DS-Gr1 Anum</t>
   </si>
   <si>
-    <t>OS-E Tania</t>
-  </si>
-  <si>
     <t>OR Gr1 Aasma</t>
   </si>
   <si>
@@ -182,66 +182,72 @@
     <t>OOP-C Mahrukh</t>
   </si>
   <si>
+    <t>CPS-E Faiza</t>
+  </si>
+  <si>
+    <t>CPS-D Faiza</t>
+  </si>
+  <si>
+    <t>DLD-H Javed Qureshi</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>OOP-B Zain</t>
+  </si>
+  <si>
+    <t>HCI-Gr1 Behraj</t>
+  </si>
+  <si>
+    <t>Dsci Gr3 Dr. Atif</t>
+  </si>
+  <si>
+    <t>SE-E Ahsan</t>
+  </si>
+  <si>
+    <t>OOP-G Basit</t>
+  </si>
+  <si>
+    <t>SE-B Rubab</t>
+  </si>
+  <si>
+    <t>DP Gr3 Abdul Rahman</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>OS-A Dr. Hasina</t>
+  </si>
+  <si>
+    <t>CN-F Dr. Jawwad</t>
+  </si>
+  <si>
+    <t>OS-C Dr. Hasina</t>
+  </si>
+  <si>
+    <t>PF-D Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>TOA-D Shahzad</t>
+  </si>
+  <si>
+    <t>TOA-B Shahzad</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>DP Gr2 Abdul Rahman</t>
+  </si>
+  <si>
+    <t>DP Gr1 Abdul Rahman</t>
+  </si>
+  <si>
     <t>OS-G Tania</t>
   </si>
   <si>
-    <t>DLD-H Javed Qureshi</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>OOP-B Zain</t>
-  </si>
-  <si>
-    <t>HCI-Gr1 Behraj</t>
-  </si>
-  <si>
-    <t>Dsci Gr3 Dr. Atif</t>
-  </si>
-  <si>
-    <t>SE-E Ahsan</t>
-  </si>
-  <si>
-    <t>OOP-G Basit</t>
-  </si>
-  <si>
-    <t>SE-B Rubab</t>
-  </si>
-  <si>
-    <t>DP Gr3 Abdul Rahman</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>OS-A Dr. Hasina</t>
-  </si>
-  <si>
-    <t>CN-F Dr. Jawwad</t>
-  </si>
-  <si>
-    <t>OS-C Dr. Hasina</t>
-  </si>
-  <si>
-    <t>PF-D Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>TOA-D Shahzad</t>
-  </si>
-  <si>
-    <t>TOA-B Shahzad</t>
-  </si>
-  <si>
-    <t>R109</t>
-  </si>
-  <si>
-    <t>DP Gr2 Abdul Rahman</t>
-  </si>
-  <si>
-    <t>DP Gr1 Abdul Rahman</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -281,507 +287,501 @@
     <t>CR-3 EE</t>
   </si>
   <si>
+    <t>CAL-Gr2 Javeria Iftikhar</t>
+  </si>
+  <si>
+    <t>CAL-Gr1 Javeria Iftikhar</t>
+  </si>
+  <si>
+    <t>CR-4</t>
+  </si>
+  <si>
+    <t>Prob-A Nadeem Khan</t>
+  </si>
+  <si>
+    <t>DE-A Fareeha</t>
+  </si>
+  <si>
+    <t>DE-C Fareeha</t>
+  </si>
+  <si>
+    <t>Prob-C Nadeem Khan</t>
+  </si>
+  <si>
+    <t>Prob-F Nadeem Khan</t>
+  </si>
+  <si>
+    <t>Prob-G Osama</t>
+  </si>
+  <si>
+    <t>CR-5</t>
+  </si>
+  <si>
+    <t>DE-E Amber</t>
+  </si>
+  <si>
+    <t>DE-H Amber</t>
+  </si>
+  <si>
+    <t>TBW-C Nazia</t>
+  </si>
+  <si>
+    <t>DE-G Amber</t>
+  </si>
+  <si>
+    <t>TBW-A Nazia</t>
+  </si>
+  <si>
+    <t>TBW-E Nazia</t>
+  </si>
+  <si>
+    <t>CR-7</t>
+  </si>
+  <si>
+    <t>Al Gr1 Dr. Shahzad</t>
+  </si>
+  <si>
+    <t>AL Gr2 Dr. Shahzad</t>
+  </si>
+  <si>
+    <t>AL Gr1 Dr. Shahzad</t>
+  </si>
+  <si>
+    <t>HRM-A Ahsan</t>
+  </si>
+  <si>
+    <t>HRM-C Ahsan</t>
+  </si>
+  <si>
+    <t>CR-10</t>
+  </si>
+  <si>
+    <t>HRM-CSG M. Zeeshan</t>
+  </si>
+  <si>
+    <t>HRM-F M. Zeeshan</t>
+  </si>
+  <si>
+    <t>NM Gr4 Dr. Khusro</t>
+  </si>
+  <si>
+    <t>HRM-D M. Zeeshan</t>
+  </si>
+  <si>
+    <t>HRM-B M. Zeeshan</t>
+  </si>
+  <si>
+    <t>CR-11</t>
+  </si>
+  <si>
+    <t>Pst.-F Kashif</t>
+  </si>
+  <si>
+    <t>Pst.-A Kashif</t>
+  </si>
+  <si>
+    <t>NM Gr1 Mr. Shahbaz</t>
+  </si>
+  <si>
+    <t>NM Gr3 Mr. Shahbaz</t>
+  </si>
+  <si>
+    <t>Pst.-H Kashif</t>
+  </si>
+  <si>
+    <t>Pst.-C Kashif</t>
+  </si>
+  <si>
+    <t>ME Gr2 Michael</t>
+  </si>
+  <si>
+    <t>CR-16</t>
+  </si>
+  <si>
+    <t>DE-D Jamil</t>
+  </si>
+  <si>
+    <t>DE-F Jamil</t>
+  </si>
+  <si>
+    <t>Cal-II Gr1 Jamil</t>
+  </si>
+  <si>
+    <t>CPS-A Hafza</t>
+  </si>
+  <si>
+    <t>DE-B Jamil</t>
+  </si>
+  <si>
+    <t>CPS-B Javed Iqbal</t>
+  </si>
+  <si>
+    <t>CR-17</t>
+  </si>
+  <si>
+    <t>Psych Gr3 Sumaira</t>
+  </si>
+  <si>
+    <t>Psych Gr1 Sumaira</t>
+  </si>
+  <si>
+    <t>Psych Gr2 Sumaira</t>
+  </si>
+  <si>
+    <t>CR-18</t>
+  </si>
+  <si>
+    <t>CPS-Lab C1 Hubrah</t>
+  </si>
+  <si>
+    <t>CPS-Lab B1 Javed Iqbal</t>
+  </si>
+  <si>
+    <t>Prob-D Osama</t>
+  </si>
+  <si>
+    <t>Prob-B Osama</t>
+  </si>
+  <si>
+    <t>CPS-Lab A1 Hubrah</t>
+  </si>
+  <si>
+    <t>LABS</t>
+  </si>
+  <si>
+    <t>Lab-1</t>
+  </si>
+  <si>
+    <t>Dsci Gr1 Dr. Zeeshan</t>
+  </si>
+  <si>
+    <t>Dsci Gr2 Dr. Zeeshan</t>
+  </si>
+  <si>
+    <t>CN-Lab G1+G2 Awais &amp; Faizan</t>
+  </si>
+  <si>
+    <t>OOAD-Gr1 Maham</t>
+  </si>
+  <si>
+    <t>Lab-3</t>
+  </si>
+  <si>
+    <t>IS-Gr1 Shahbaz</t>
+  </si>
+  <si>
+    <t>CG- Gr1 Javeria</t>
+  </si>
+  <si>
+    <t>CG Gr2 Javeria</t>
+  </si>
+  <si>
+    <t>CG Gr3 Javeria</t>
+  </si>
+  <si>
+    <t>Lab-4</t>
+  </si>
+  <si>
+    <t>Lab-6</t>
+  </si>
+  <si>
+    <t>DLD-Lab G2 Abdul Khaliq</t>
+  </si>
+  <si>
+    <t>DLD-Lab F1 Nadeem</t>
+  </si>
+  <si>
+    <t>EE Lab-9</t>
+  </si>
+  <si>
+    <t>DS Lab- Gr2 Irfan</t>
+  </si>
+  <si>
+    <t>OS Lab-E Abdullah</t>
+  </si>
+  <si>
+    <t>EE Lab 10</t>
+  </si>
+  <si>
+    <t>OS Lab-G Safia</t>
+  </si>
+  <si>
+    <t>EE MPI Lab</t>
+  </si>
+  <si>
+    <t>DLD-Lab G1 Farah</t>
+  </si>
+  <si>
+    <t>DLD-Lab F2 Hamza</t>
+  </si>
+  <si>
+    <t>LLC</t>
+  </si>
+  <si>
+    <t>CPS-Lab C2 Kishwar</t>
+  </si>
+  <si>
+    <t>CPS-Lab B2 Hafza</t>
+  </si>
+  <si>
+    <t>CPS-Lab A2 Kishwar</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>AI-B Dr. Rauf</t>
+  </si>
+  <si>
+    <t>AI-G Dr. Rauf</t>
+  </si>
+  <si>
+    <t>AI-C Saeeda</t>
+  </si>
+  <si>
+    <t>IOT- Gr1 Dr. Farooque</t>
+  </si>
+  <si>
+    <t>IPT Gr2 Murtaza</t>
+  </si>
+  <si>
+    <t>IPT Gr1 Murtaza</t>
+  </si>
+  <si>
+    <t>PF-B Dr. Farooque</t>
+  </si>
+  <si>
+    <t>AI-E Saeeda</t>
+  </si>
+  <si>
+    <t>AI-F Saeeda</t>
+  </si>
+  <si>
+    <t>Dwh Gr1 Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>Dwh Gr2 Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>ALGO-Gr1 Zeshan Khan</t>
+  </si>
+  <si>
+    <t>CN-A Shoaib Raza</t>
+  </si>
+  <si>
+    <t>CN-B Shoaib Raza</t>
+  </si>
+  <si>
+    <t>TOA-C Zeshan</t>
+  </si>
+  <si>
+    <t>CPS-G Javed Iqbal</t>
+  </si>
+  <si>
+    <t>OOAD-Gr1 Rubab</t>
+  </si>
+  <si>
+    <t>Dsci Gr1 Dr. Atif</t>
+  </si>
+  <si>
+    <t>Pst.-G Amanullah</t>
+  </si>
+  <si>
+    <t>Pst.-E Amanullah</t>
+  </si>
+  <si>
+    <t>ISPM Gr1 Ubaid</t>
+  </si>
+  <si>
+    <t>WP Gr2 Salman</t>
+  </si>
+  <si>
+    <t>WP Gr1 Salman</t>
+  </si>
+  <si>
+    <t>OR Gr2 Aasma</t>
+  </si>
+  <si>
+    <t>TBW-G Nazia</t>
+  </si>
+  <si>
+    <t>LA-Gr1 Fareeha</t>
+  </si>
+  <si>
+    <t>DLD-B Rabia</t>
+  </si>
+  <si>
+    <t>TBW-D Sameera</t>
+  </si>
+  <si>
+    <t>DLD-D Rabia</t>
+  </si>
+  <si>
+    <t>DLD-F Rabia</t>
+  </si>
+  <si>
+    <t>NM Gr2 Mr. Shahbaz</t>
+  </si>
+  <si>
+    <t>Prob-E Javeria</t>
+  </si>
+  <si>
+    <t>CPS-Lab D2 Kishwar</t>
+  </si>
+  <si>
+    <t>CPS-Lab H2 Kishwar</t>
+  </si>
+  <si>
+    <t>COAL-Lab Gr3 Tooba</t>
+  </si>
+  <si>
+    <t>OOP-Lab A Zain</t>
+  </si>
+  <si>
+    <t>OS Lab-A Safia</t>
+  </si>
+  <si>
+    <t>OOP-Lab B Basit</t>
+  </si>
+  <si>
+    <t>OS Lab-B Summiyah</t>
+  </si>
+  <si>
+    <t>CN-Lab A Munim</t>
+  </si>
+  <si>
+    <t>DLD-Lab A1 Mubashyra</t>
+  </si>
+  <si>
+    <t>PF-Lab A Abdul Aziz &amp; Sadia</t>
+  </si>
+  <si>
+    <t>OOP-Lab F Fahim</t>
+  </si>
+  <si>
+    <t>CN-Lab E1+E2 Faizan &amp; Awais</t>
+  </si>
+  <si>
+    <t>DS Lab- Gr1 Irfan</t>
+  </si>
+  <si>
+    <t>DLD-Lab D2 Hamza</t>
+  </si>
+  <si>
+    <t>DLD-Lab A2 Maham</t>
+  </si>
+  <si>
+    <t>DLD-Lab D1 Nadeem</t>
+  </si>
+  <si>
+    <t>CPS-Lab D1 Javed Iqbal</t>
+  </si>
+  <si>
+    <t>CPS-Lab H1 Hubrah</t>
+  </si>
+  <si>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
+    <t>ALGO-Gr2 Zeshan Khan</t>
+  </si>
+  <si>
+    <t>CV- Gr1 Dr. Tahir Syed</t>
+  </si>
+  <si>
+    <t>CV- Gr2 Dr. Tahir Syed</t>
+  </si>
+  <si>
+    <t>COAL Gr1 Danish</t>
+  </si>
+  <si>
+    <t>COAL Gr2 Danish</t>
+  </si>
+  <si>
+    <t>COAL Gr3 Danish</t>
+  </si>
+  <si>
+    <t>CA-Gr4 Dr. Asif</t>
+  </si>
+  <si>
+    <t>DLD-A Khalid</t>
+  </si>
+  <si>
+    <t>DLD-C Khalid</t>
+  </si>
+  <si>
+    <t>PIT-Gr1 Khalid</t>
+  </si>
+  <si>
+    <t>CA-Gr3 Dr. Noman Durrani</t>
+  </si>
+  <si>
+    <t>CA-Gr1 Dr. Noman Durrani</t>
+  </si>
+  <si>
+    <t>CN-G Nadeem Kafi</t>
+  </si>
+  <si>
+    <t>CN-D Nadeem Kafi</t>
+  </si>
+  <si>
+    <t>CPS-H Urooj</t>
+  </si>
+  <si>
+    <t>CPS-F Urooj</t>
+  </si>
+  <si>
+    <t>CPS-C Hafza</t>
+  </si>
+  <si>
+    <t>CPS-Lab F1 Hubrah</t>
+  </si>
+  <si>
+    <t>OOP-Lab D Fahim</t>
+  </si>
+  <si>
+    <t>OS Lab-D Summiyah</t>
+  </si>
+  <si>
+    <t>DS Lab- Gr3 Safia</t>
+  </si>
+  <si>
+    <t>COAL Lab- Gr1 Tooba</t>
+  </si>
+  <si>
+    <t>OS Lab-F Abdullah</t>
+  </si>
+  <si>
+    <t>PF-Lab B Sadia &amp; Rahemeen</t>
+  </si>
+  <si>
+    <t>DLD-Lab E2 Abdul Khaliq</t>
+  </si>
+  <si>
+    <t>OOP-Lab C Basit</t>
+  </si>
+  <si>
+    <t>DLD-Lab B2 Hamza</t>
+  </si>
+  <si>
+    <t>DLD-Lab E1 Mubashyra</t>
+  </si>
+  <si>
+    <t>DLD-Lab B1 Nadeem</t>
+  </si>
+  <si>
+    <t>CPS-Lab F2 Kishwar</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t>Discrete-Gr1 Dr. Jalal</t>
+  </si>
+  <si>
     <t>Prob-E Javeria Iftikhar</t>
   </si>
   <si>
-    <t>CAL-Gr2 Javeria Iftikhar</t>
-  </si>
-  <si>
-    <t>CAL-Gr1 Javeria Iftikhar</t>
-  </si>
-  <si>
-    <t>CR-4</t>
-  </si>
-  <si>
-    <t>Prob-A Nadeem Khan</t>
-  </si>
-  <si>
-    <t>DE-A Fareeha</t>
-  </si>
-  <si>
-    <t>DE-C Fareeha</t>
-  </si>
-  <si>
-    <t>Prob-C Nadeem Khan</t>
-  </si>
-  <si>
-    <t>Prob-F Nadeem Khan</t>
-  </si>
-  <si>
-    <t>Prob-G Osama</t>
-  </si>
-  <si>
-    <t>CR-5</t>
-  </si>
-  <si>
-    <t>DE-E Amber</t>
-  </si>
-  <si>
-    <t>DE-H Amber</t>
-  </si>
-  <si>
-    <t>TBW-C Nazia</t>
-  </si>
-  <si>
-    <t>DE-G Amber</t>
-  </si>
-  <si>
-    <t>TBW-A Nazia</t>
-  </si>
-  <si>
-    <t>TBW-E Nazia</t>
-  </si>
-  <si>
-    <t>CR-7</t>
-  </si>
-  <si>
-    <t>Al Gr1 Dr. Shahzad</t>
-  </si>
-  <si>
-    <t>AL Gr2 Dr. Shahzad</t>
-  </si>
-  <si>
-    <t>AL Gr1 Dr. Shahzad</t>
-  </si>
-  <si>
-    <t>HRM-A Ahsan</t>
-  </si>
-  <si>
-    <t>HRM-C Ahsan</t>
-  </si>
-  <si>
-    <t>CR-10</t>
-  </si>
-  <si>
-    <t>HRM-CSG M. Zeeshan</t>
-  </si>
-  <si>
-    <t>HRM-F M. Zeeshan</t>
-  </si>
-  <si>
-    <t>NM Gr4 Dr. Khusro</t>
-  </si>
-  <si>
-    <t>HRM-D M. Zeeshan</t>
-  </si>
-  <si>
-    <t>HRM-B M. Zeeshan</t>
-  </si>
-  <si>
-    <t>CR-11</t>
-  </si>
-  <si>
-    <t>Pst.-F Kashif</t>
-  </si>
-  <si>
-    <t>Pst.-A Kashif</t>
-  </si>
-  <si>
-    <t>NM Gr1 Mr. Shahbaz</t>
-  </si>
-  <si>
-    <t>NM Gr3 Mr. Shahbaz</t>
-  </si>
-  <si>
-    <t>Pst.-H Kashif</t>
-  </si>
-  <si>
-    <t>Pst.-C Kashif</t>
-  </si>
-  <si>
-    <t>ME Gr2 Michael</t>
-  </si>
-  <si>
-    <t>CR-16</t>
-  </si>
-  <si>
-    <t>DE-D Jamil</t>
-  </si>
-  <si>
-    <t>DE-F Jamil</t>
-  </si>
-  <si>
-    <t>Cal-II Gr1 Jamil</t>
-  </si>
-  <si>
-    <t>CPS-A Hafza</t>
-  </si>
-  <si>
-    <t>DE-B Jamil</t>
-  </si>
-  <si>
-    <t>CPS-B Javed Iqbal</t>
-  </si>
-  <si>
-    <t>CR-17</t>
-  </si>
-  <si>
-    <t>Psych Gr3 Sumaira</t>
-  </si>
-  <si>
-    <t>Psych Gr1 Sumaira</t>
-  </si>
-  <si>
-    <t>CPS-D Faiza</t>
-  </si>
-  <si>
-    <t>CPS-E Faiza</t>
-  </si>
-  <si>
-    <t>Psych Gr2 Sumaira</t>
-  </si>
-  <si>
-    <t>CR-18</t>
-  </si>
-  <si>
-    <t>CPS-Lab C1 Hubrah</t>
-  </si>
-  <si>
-    <t>CPS-Lab B1 Javed Iqbal</t>
-  </si>
-  <si>
-    <t>Prob-D Osama</t>
-  </si>
-  <si>
-    <t>Prob-B Osama</t>
-  </si>
-  <si>
-    <t>CPS-Lab A1 Hubrah</t>
-  </si>
-  <si>
-    <t>LABS</t>
-  </si>
-  <si>
-    <t>Lab-1</t>
-  </si>
-  <si>
-    <t>Dsci Gr1 Dr. Zeeshan</t>
-  </si>
-  <si>
-    <t>Dsci Gr2 Dr. Zeeshan</t>
-  </si>
-  <si>
-    <t>CN-Lab G1+G2 Awais &amp; Faizan</t>
-  </si>
-  <si>
-    <t>OOAD-Gr1 Maham</t>
-  </si>
-  <si>
-    <t>Lab-3</t>
-  </si>
-  <si>
-    <t>IS-Gr1 Shahbaz</t>
-  </si>
-  <si>
-    <t>CG- Gr1 Javeria</t>
-  </si>
-  <si>
-    <t>CG Gr2 Javeria</t>
-  </si>
-  <si>
-    <t>CG Gr3 Javeria</t>
-  </si>
-  <si>
-    <t>Lab-4</t>
-  </si>
-  <si>
-    <t>Lab-6</t>
-  </si>
-  <si>
-    <t>DLD-Lab G2 Abdul Khaliq</t>
-  </si>
-  <si>
-    <t>DLD-Lab F1 Nadeem</t>
-  </si>
-  <si>
-    <t>EE Lab-9</t>
-  </si>
-  <si>
-    <t>DS Lab- Gr2 Irfan</t>
-  </si>
-  <si>
-    <t>OS Lab-E Abdullah</t>
-  </si>
-  <si>
-    <t>EE Lab 10</t>
-  </si>
-  <si>
-    <t>OS Lab-G Safia</t>
-  </si>
-  <si>
-    <t>EE MPI Lab</t>
-  </si>
-  <si>
-    <t>DLD-Lab G1 Farah</t>
-  </si>
-  <si>
-    <t>DLD-Lab F2 Hamza</t>
-  </si>
-  <si>
-    <t>LLC</t>
-  </si>
-  <si>
-    <t>CPS-Lab C2 Kishwar</t>
-  </si>
-  <si>
-    <t>CPS-Lab B2 Hafza</t>
-  </si>
-  <si>
-    <t>CPS-Lab A2 Kishwar</t>
-  </si>
-  <si>
-    <t>TUESDAY</t>
-  </si>
-  <si>
-    <t>AI-B Dr. Rauf</t>
-  </si>
-  <si>
-    <t>AI-G Dr. Rauf</t>
-  </si>
-  <si>
-    <t>AI-C Saeeda</t>
-  </si>
-  <si>
-    <t>IOT- Gr1 Dr. Farooque</t>
-  </si>
-  <si>
-    <t>IPT Gr2 Murtaza</t>
-  </si>
-  <si>
-    <t>IPT Gr1 Murtaza</t>
-  </si>
-  <si>
-    <t>PF-B Dr. Farooque</t>
-  </si>
-  <si>
-    <t>AI-E Saeeda</t>
-  </si>
-  <si>
-    <t>AI-F Saeeda</t>
-  </si>
-  <si>
-    <t>Dwh Gr1 Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>Dwh Gr2 Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>ALGO-Gr1 Zeshan Khan</t>
-  </si>
-  <si>
-    <t>CN-A Shoaib Raza</t>
-  </si>
-  <si>
-    <t>CN-B Shoaib Raza</t>
-  </si>
-  <si>
-    <t>TOA-C Zeshan</t>
-  </si>
-  <si>
-    <t>CPS-G Javed Iqbal</t>
-  </si>
-  <si>
-    <t>OOAD-Gr1 Rubab</t>
-  </si>
-  <si>
-    <t>Dsci Gr1 Dr. Atif</t>
-  </si>
-  <si>
-    <t>Pst.-G Amanullah</t>
-  </si>
-  <si>
-    <t>Pst.-E Amanullah</t>
-  </si>
-  <si>
-    <t>ISPM Gr1 Ubaid</t>
-  </si>
-  <si>
-    <t>WP Gr2 Salman</t>
-  </si>
-  <si>
-    <t>WP Gr1 Salman</t>
-  </si>
-  <si>
-    <t>OR Gr2 Aasma</t>
-  </si>
-  <si>
-    <t>TBW-G Nazia</t>
-  </si>
-  <si>
-    <t>LA-Gr1 Fareeha</t>
-  </si>
-  <si>
-    <t>DLD-B Rabia</t>
-  </si>
-  <si>
-    <t>TBW-D Sameera</t>
-  </si>
-  <si>
-    <t>DLD-D Rabia</t>
-  </si>
-  <si>
-    <t>DLD-F Rabia</t>
-  </si>
-  <si>
-    <t>NM Gr2 Mr. Shahbaz</t>
-  </si>
-  <si>
-    <t>Prob-E Javeria</t>
-  </si>
-  <si>
-    <t>CPS-Lab D2 Kishwar</t>
-  </si>
-  <si>
-    <t>CPS-Lab H2 Kishwar</t>
-  </si>
-  <si>
-    <t>COAL-Lab Gr3 Tooba</t>
-  </si>
-  <si>
-    <t>OOP-Lab A Zain</t>
-  </si>
-  <si>
-    <t>OS Lab-A Safia</t>
-  </si>
-  <si>
-    <t>OOP-Lab B Basit</t>
-  </si>
-  <si>
-    <t>OS Lab-B Summiyah</t>
-  </si>
-  <si>
-    <t>CN-Lab A Munim</t>
-  </si>
-  <si>
-    <t>DLD-Lab A1 Mubashyra</t>
-  </si>
-  <si>
-    <t>PF-Lab A Abdul Aziz &amp; Sadia</t>
-  </si>
-  <si>
-    <t>OOP-Lab F Fahim</t>
-  </si>
-  <si>
-    <t>CN-Lab E1+E2 Faizan &amp; Awais</t>
-  </si>
-  <si>
-    <t>DS Lab- Gr1 Irfan</t>
-  </si>
-  <si>
-    <t>DLD-Lab D2 Hamza</t>
-  </si>
-  <si>
-    <t>DLD-Lab A2 Maham</t>
-  </si>
-  <si>
-    <t>DLD-Lab D1 Nadeem</t>
-  </si>
-  <si>
-    <t>CPS-Lab D1 Javed Iqbal</t>
-  </si>
-  <si>
-    <t>CPS-Lab H1 Hubrah</t>
-  </si>
-  <si>
-    <t>WEDNESDAY</t>
-  </si>
-  <si>
-    <t>ALGO-Gr2 Zeshan Khan</t>
-  </si>
-  <si>
-    <t>CV- Gr1 Dr. Tahir Syed</t>
-  </si>
-  <si>
-    <t>CV- Gr2 Dr. Tahir Syed</t>
-  </si>
-  <si>
-    <t>COAL Gr1 Danish</t>
-  </si>
-  <si>
-    <t>COAL Gr2 Danish</t>
-  </si>
-  <si>
-    <t>COAL Gr3 Danish</t>
-  </si>
-  <si>
-    <t>CA-Gr4 Dr. Asif</t>
-  </si>
-  <si>
-    <t>DLD-A Khalid</t>
-  </si>
-  <si>
-    <t>DLD-C Khalid</t>
-  </si>
-  <si>
-    <t>PIT-Gr1 Khalid</t>
-  </si>
-  <si>
-    <t>CA-Gr3 Dr. Noman Durrani</t>
-  </si>
-  <si>
-    <t>CA-Gr1 Dr. Noman Durrani</t>
-  </si>
-  <si>
-    <t>CN-G Nadeem Kafi</t>
-  </si>
-  <si>
-    <t>CN-D Nadeem Kafi</t>
-  </si>
-  <si>
-    <t>CPS-H Urooj</t>
-  </si>
-  <si>
-    <t>CPS-F Urooj</t>
-  </si>
-  <si>
-    <t>CPS-C Hafza</t>
-  </si>
-  <si>
-    <t>CPS-Lab F1 Hubrah</t>
-  </si>
-  <si>
-    <t>OOP-Lab D Fahim</t>
-  </si>
-  <si>
-    <t>OS Lab-D Summiyah</t>
-  </si>
-  <si>
-    <t>DS Lab- Gr3 Safia</t>
-  </si>
-  <si>
-    <t>COAL Lab- Gr1 Tooba</t>
-  </si>
-  <si>
-    <t>OS Lab-F Abdullah</t>
-  </si>
-  <si>
-    <t>PF-Lab B Sadia &amp; Rahemeen</t>
-  </si>
-  <si>
-    <t>DLD-Lab E2 Abdul Khaliq</t>
-  </si>
-  <si>
-    <t>OOP-Lab C Basit</t>
-  </si>
-  <si>
-    <t>DLD-Lab B2 Hamza</t>
-  </si>
-  <si>
-    <t>DLD-Lab E1 Mubashyra</t>
-  </si>
-  <si>
-    <t>DLD-Lab B1 Nadeem</t>
-  </si>
-  <si>
-    <t>CPS-Lab F2 Kishwar</t>
-  </si>
-  <si>
-    <t>THURSDAY</t>
-  </si>
-  <si>
-    <t>Discrete-Gr1 Dr. Jalal</t>
-  </si>
-  <si>
     <t>Pst.-B Abid</t>
   </si>
   <si>
@@ -818,40 +818,40 @@
     <t>ICT-Lab Gr1 Summiyah</t>
   </si>
   <si>
+    <t>OS Lab-C Abdullah</t>
+  </si>
+  <si>
+    <t>DLD-Lab H2 Maham</t>
+  </si>
+  <si>
+    <t>CPS-Lab G2 Kishwar</t>
+  </si>
+  <si>
+    <t>CPS-Lab E1 Hubrah</t>
+  </si>
+  <si>
+    <t>FRIDAY</t>
+  </si>
+  <si>
+    <t>J UMMA PRAYER</t>
+  </si>
+  <si>
+    <t>CN-Lab B Munim</t>
+  </si>
+  <si>
+    <t>DB Lab-Gr2 Abdul Aziz</t>
+  </si>
+  <si>
+    <t>B R E A K</t>
+  </si>
+  <si>
+    <t>CN-Lab C Awais</t>
+  </si>
+  <si>
+    <t>COAL-Lab Gr2 Tooba</t>
+  </si>
+  <si>
     <t>OOP-Lab E Farah</t>
-  </si>
-  <si>
-    <t>OS Lab-C Abdullah</t>
-  </si>
-  <si>
-    <t>DLD-Lab H2 Maham</t>
-  </si>
-  <si>
-    <t>CPS-Lab G2 Kishwar</t>
-  </si>
-  <si>
-    <t>CPS-Lab E1 Hubrah</t>
-  </si>
-  <si>
-    <t>FRIDAY</t>
-  </si>
-  <si>
-    <t>J UMMA PRAYER</t>
-  </si>
-  <si>
-    <t>CN-Lab B Munim</t>
-  </si>
-  <si>
-    <t>DB Lab-Gr2 Abdul Aziz</t>
-  </si>
-  <si>
-    <t>B R E A K</t>
-  </si>
-  <si>
-    <t>CN-Lab C Awais</t>
-  </si>
-  <si>
-    <t>COAL-Lab Gr2 Tooba</t>
   </si>
   <si>
     <t>DLD-Lab C1 Mubashyra</t>
@@ -1320,38 +1320,38 @@
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
         <v>27</v>
       </c>
+      <c r="D7"/>
       <c r="E7" t="s">
         <v>28</v>
       </c>
@@ -1438,146 +1438,148 @@
       <c r="E10" t="s">
         <v>52</v>
       </c>
-      <c r="F10"/>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" t="s">
         <v>62</v>
-      </c>
-      <c r="I11" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13"/>
+        <v>73</v>
+      </c>
+      <c r="G13" t="s">
+        <v>74</v>
+      </c>
       <c r="H13"/>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
@@ -1585,201 +1587,199 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H18"/>
-      <c r="I18"/>
+      <c r="I18" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G20" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H20"/>
       <c r="I20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F21" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G21" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
-      </c>
-      <c r="G23" t="s">
         <v>133</v>
       </c>
-      <c r="H23" t="s">
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23" t="s">
         <v>134</v>
-      </c>
-      <c r="I23" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" t="s">
         <v>136</v>
-      </c>
-      <c r="B24" t="s">
-        <v>137</v>
       </c>
       <c r="C24"/>
       <c r="D24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E24"/>
       <c r="F24" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" t="s">
         <v>139</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>140</v>
-      </c>
-      <c r="H24" t="s">
-        <v>141</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -1792,49 +1792,49 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" t="s">
         <v>143</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>144</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>145</v>
-      </c>
-      <c r="D26" t="s">
-        <v>146</v>
       </c>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" t="s">
         <v>148</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>149</v>
-      </c>
-      <c r="C27" t="s">
-        <v>150</v>
       </c>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G27"/>
       <c r="H27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
@@ -1847,44 +1847,44 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" t="s">
         <v>154</v>
-      </c>
-      <c r="B29" t="s">
-        <v>155</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" t="s">
         <v>157</v>
-      </c>
-      <c r="B30" t="s">
-        <v>158</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" t="s">
         <v>160</v>
-      </c>
-      <c r="B31" t="s">
-        <v>161</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
@@ -1896,37 +1896,37 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32" t="s">
         <v>162</v>
-      </c>
-      <c r="B32" t="s">
-        <v>163</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" t="s">
         <v>165</v>
-      </c>
-      <c r="B33" t="s">
-        <v>166</v>
       </c>
       <c r="C33"/>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I33"/>
     </row>
@@ -1974,7 +1974,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2061,23 +2061,23 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" t="s">
         <v>170</v>
       </c>
-      <c r="C5" t="s">
-        <v>171</v>
-      </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I5" t="s">
         <v>37</v>
@@ -2088,19 +2088,19 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" t="s">
         <v>173</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>174</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>175</v>
       </c>
-      <c r="E6" t="s">
-        <v>176</v>
-      </c>
       <c r="F6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G6"/>
       <c r="H6"/>
@@ -2108,19 +2108,19 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
         <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -2134,22 +2134,22 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
         <v>177</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
@@ -2164,10 +2164,10 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" t="s">
         <v>179</v>
-      </c>
-      <c r="D9" t="s">
-        <v>180</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
@@ -2176,13 +2176,13 @@
         <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H9" t="s">
         <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2190,72 +2190,72 @@
         <v>48</v>
       </c>
       <c r="B10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" t="s">
         <v>181</v>
       </c>
-      <c r="C10" t="s">
-        <v>181</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>182</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>183</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>184</v>
-      </c>
-      <c r="G10" t="s">
-        <v>185</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" t="s">
         <v>119</v>
-      </c>
-      <c r="H11" t="s">
-        <v>118</v>
       </c>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
         <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="s">
@@ -2264,7 +2264,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -2275,36 +2275,36 @@
         <v>34</v>
       </c>
       <c r="F13" t="s">
+        <v>187</v>
+      </c>
+      <c r="G13" t="s">
         <v>188</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>189</v>
       </c>
-      <c r="H13" t="s">
-        <v>190</v>
-      </c>
       <c r="I13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
       </c>
       <c r="C14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" t="s">
         <v>191</v>
-      </c>
-      <c r="D14" t="s">
-        <v>192</v>
       </c>
       <c r="E14" t="s">
         <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G14" t="s">
         <v>52</v>
@@ -2314,99 +2314,99 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" t="s">
         <v>92</v>
-      </c>
-      <c r="E18" t="s">
-        <v>122</v>
-      </c>
-      <c r="F18" t="s">
-        <v>91</v>
       </c>
       <c r="G18" t="s">
         <v>29</v>
@@ -2415,12 +2415,12 @@
         <v>28</v>
       </c>
       <c r="I18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
@@ -2433,130 +2433,130 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" t="s">
         <v>98</v>
       </c>
-      <c r="F20" t="s">
-        <v>97</v>
-      </c>
       <c r="G20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" t="s">
         <v>106</v>
-      </c>
-      <c r="H20" t="s">
-        <v>105</v>
       </c>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" t="s">
         <v>196</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>197</v>
-      </c>
-      <c r="D21" t="s">
-        <v>198</v>
       </c>
       <c r="E21" t="s">
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G21" t="s">
         <v>43</v>
       </c>
       <c r="H21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H22"/>
       <c r="I22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G23" t="s">
+        <v>133</v>
+      </c>
+      <c r="H23" t="s">
         <v>132</v>
       </c>
-      <c r="H23" t="s">
-        <v>131</v>
-      </c>
       <c r="I23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -2569,131 +2569,131 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B26"/>
       <c r="C26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F28"/>
       <c r="G28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -2701,7 +2701,7 @@
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I33"/>
     </row>
@@ -2738,7 +2738,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2869,19 +2869,19 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2900,25 +2900,25 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F6" t="s">
+        <v>222</v>
+      </c>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" t="s">
         <v>72</v>
-      </c>
-      <c r="C6" t="s">
-        <v>222</v>
-      </c>
-      <c r="D6" t="s">
-        <v>178</v>
-      </c>
-      <c r="E6" t="s">
-        <v>223</v>
-      </c>
-      <c r="F6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" t="s">
-        <v>71</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -2934,28 +2934,28 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
         <v>144</v>
       </c>
-      <c r="C7" t="s">
-        <v>145</v>
-      </c>
       <c r="D7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
       </c>
       <c r="F7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H7" t="s">
         <v>176</v>
-      </c>
-      <c r="G7" t="s">
-        <v>172</v>
-      </c>
-      <c r="H7" t="s">
-        <v>177</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -2974,26 +2974,26 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" t="s">
         <v>225</v>
-      </c>
-      <c r="E8" t="s">
-        <v>184</v>
-      </c>
-      <c r="F8" t="s">
-        <v>226</v>
       </c>
       <c r="G8" t="s">
         <v>31</v>
       </c>
       <c r="H8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -3014,13 +3014,13 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F9"/>
       <c r="G9"/>
@@ -3042,16 +3042,16 @@
         <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" t="s">
         <v>182</v>
-      </c>
-      <c r="E10" t="s">
-        <v>183</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -3070,27 +3070,27 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" t="s">
         <v>228</v>
-      </c>
-      <c r="E11" t="s">
-        <v>229</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H11"/>
       <c r="I11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
@@ -3105,26 +3105,26 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F12" t="s">
         <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I12" t="s">
         <v>47</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -3165,31 +3165,31 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" t="s">
+        <v>232</v>
+      </c>
+      <c r="E14" t="s">
+        <v>233</v>
+      </c>
+      <c r="F14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G14" t="s">
         <v>151</v>
       </c>
-      <c r="C14" t="s">
-        <v>150</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="H14" t="s">
         <v>233</v>
       </c>
-      <c r="E14" t="s">
-        <v>234</v>
-      </c>
-      <c r="F14" t="s">
-        <v>186</v>
-      </c>
-      <c r="G14" t="s">
-        <v>152</v>
-      </c>
-      <c r="H14" t="s">
-        <v>234</v>
-      </c>
       <c r="I14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J14"/>
       <c r="K14"/>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -3227,28 +3227,28 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
+        <v>234</v>
+      </c>
+      <c r="D16" t="s">
         <v>235</v>
-      </c>
-      <c r="D16" t="s">
-        <v>236</v>
       </c>
       <c r="E16" t="s">
         <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
@@ -3264,10 +3264,10 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -3275,13 +3275,13 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G17" t="s">
         <v>29</v>
       </c>
       <c r="H17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -3297,31 +3297,31 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J18"/>
       <c r="K18"/>
@@ -3336,29 +3336,29 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F19"/>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J19"/>
       <c r="K19"/>
@@ -3373,29 +3373,29 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
@@ -3433,25 +3433,25 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F22"/>
       <c r="G22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H22"/>
       <c r="I22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J22"/>
       <c r="K22"/>
@@ -3466,27 +3466,25 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B23"/>
       <c r="C23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
-      </c>
-      <c r="G23" t="s">
-        <v>134</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="G23"/>
       <c r="H23" t="s">
-        <v>133</v>
+        <v>54</v>
       </c>
       <c r="I23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J23"/>
       <c r="K23"/>
@@ -3501,23 +3499,23 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J24"/>
       <c r="K24"/>
@@ -3532,7 +3530,7 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -3555,17 +3553,17 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -3582,17 +3580,17 @@
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -3609,10 +3607,10 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -3634,10 +3632,10 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -3659,10 +3657,10 @@
     </row>
     <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -3684,17 +3682,17 @@
     </row>
     <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
@@ -3711,17 +3709,17 @@
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
@@ -3738,10 +3736,10 @@
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -3794,7 +3792,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3881,20 +3879,20 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
         <v>231</v>
-      </c>
-      <c r="C5" t="s">
-        <v>232</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -3904,10 +3902,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D6" t="s">
         <v>36</v>
@@ -3926,25 +3924,25 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H7"/>
       <c r="I7" t="s">
@@ -3956,17 +3954,17 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
@@ -3977,21 +3975,21 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" t="s">
         <v>170</v>
-      </c>
-      <c r="C9" t="s">
-        <v>171</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I9"/>
     </row>
@@ -4000,69 +3998,69 @@
         <v>48</v>
       </c>
       <c r="B10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" t="s">
+        <v>228</v>
+      </c>
+      <c r="E10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" t="s">
         <v>151</v>
-      </c>
-      <c r="C10" t="s">
-        <v>228</v>
-      </c>
-      <c r="D10" t="s">
-        <v>229</v>
-      </c>
-      <c r="E10" t="s">
-        <v>150</v>
-      </c>
-      <c r="F10" t="s">
-        <v>152</v>
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
         <v>69</v>
       </c>
-      <c r="C12" t="s">
-        <v>68</v>
-      </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -4070,7 +4068,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>49</v>
@@ -4080,45 +4078,45 @@
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
+        <v>224</v>
+      </c>
+      <c r="F13" t="s">
         <v>225</v>
-      </c>
-      <c r="F13" t="s">
-        <v>226</v>
       </c>
       <c r="G13" t="s">
         <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
         <v>73</v>
-      </c>
-      <c r="B14" t="s">
-        <v>72</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
@@ -4127,42 +4125,44 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E15" t="s">
         <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E16"/>
       <c r="F16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H16"/>
-      <c r="I16"/>
+      <c r="I16" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -4171,78 +4171,76 @@
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
-      <c r="I17" t="s">
-        <v>195</v>
-      </c>
+      <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" t="s">
         <v>94</v>
-      </c>
-      <c r="E18" t="s">
-        <v>93</v>
       </c>
       <c r="F18" t="s">
         <v>51</v>
       </c>
       <c r="G18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H18"/>
-      <c r="I18" t="s">
-        <v>201</v>
-      </c>
+      <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H19"/>
-      <c r="I19" t="s">
-        <v>194</v>
-      </c>
+      <c r="I19"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F20"/>
-      <c r="G20"/>
+      <c r="G20" t="s">
+        <v>252</v>
+      </c>
       <c r="H20"/>
-      <c r="I20"/>
+      <c r="I20" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B21"/>
       <c r="C21"/>
@@ -4255,7 +4253,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -4268,7 +4266,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B23"/>
       <c r="C23" t="s">
@@ -4287,7 +4285,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
         <v>255</v>
@@ -4295,7 +4293,7 @@
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F24"/>
       <c r="G24"/>
@@ -4306,7 +4304,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -4319,7 +4317,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B26" t="s">
         <v>257</v>
@@ -4327,7 +4325,7 @@
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F26"/>
       <c r="G26" t="s">
@@ -4338,7 +4336,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27"/>
       <c r="C27"/>
@@ -4353,7 +4351,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
@@ -4368,7 +4366,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
         <v>261</v>
@@ -4385,7 +4383,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
         <v>263</v>
@@ -4402,16 +4400,14 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>160</v>
-      </c>
-      <c r="B31" t="s">
-        <v>265</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
@@ -4419,10 +4415,10 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
@@ -4434,10 +4430,10 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -4445,7 +4441,7 @@
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I33"/>
     </row>
@@ -4482,7 +4478,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -4578,7 +4574,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -4588,10 +4584,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
@@ -4606,26 +4602,26 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" t="s">
+        <v>230</v>
+      </c>
+      <c r="F7" t="s">
         <v>231</v>
-      </c>
-      <c r="F7" t="s">
-        <v>232</v>
       </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I7"/>
     </row>
@@ -4634,24 +4630,24 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G8"/>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4659,10 +4655,10 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
@@ -4678,16 +4674,16 @@
         <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>
       </c>
       <c r="D10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" t="s">
         <v>182</v>
-      </c>
-      <c r="E10" t="s">
-        <v>183</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -4696,28 +4692,28 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12"/>
       <c r="C12"/>
@@ -4730,7 +4726,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -4743,66 +4739,66 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E14"/>
       <c r="F14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G14"/>
       <c r="H14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E15"/>
       <c r="F15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
         <v>88</v>
-      </c>
-      <c r="F16" t="s">
-        <v>87</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
@@ -4810,33 +4806,33 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B17"/>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C18" t="s">
         <v>254</v>
@@ -4844,7 +4840,9 @@
       <c r="D18" t="s">
         <v>253</v>
       </c>
-      <c r="E18"/>
+      <c r="E18" t="s">
+        <v>139</v>
+      </c>
       <c r="F18" t="s">
         <v>254</v>
       </c>
@@ -4854,99 +4852,103 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>134</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>115</v>
-      </c>
-      <c r="B21"/>
-      <c r="C21"/>
+        <v>116</v>
+      </c>
+      <c r="B21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" t="s">
+        <v>138</v>
+      </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -4959,7 +4961,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -4972,7 +4974,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -4985,50 +4987,50 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G26" t="s">
         <v>273</v>
       </c>
-      <c r="G26" t="s">
-        <v>274</v>
-      </c>
       <c r="H26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -5040,7 +5042,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29"/>
       <c r="C29"/>
@@ -5053,7 +5055,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
         <v>277</v>
@@ -5068,7 +5070,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31" t="s">
         <v>278</v>
@@ -5083,7 +5085,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B32" t="s">
         <v>279</v>
@@ -5098,7 +5100,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>

</xml_diff>

<commit_message>
update tt to v4.0
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -179,45 +179,45 @@
     <t>AP-Gr1 Javed Qureshi</t>
   </si>
   <si>
+    <t>SE-E Ahsan</t>
+  </si>
+  <si>
+    <t>CPS-E Faiza</t>
+  </si>
+  <si>
+    <t>CPS-D Faiza</t>
+  </si>
+  <si>
+    <t>DLD-H Javed Qureshi</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>OOP-B Zain</t>
+  </si>
+  <si>
+    <t>Dsci Gr3 Dr. Atif</t>
+  </si>
+  <si>
     <t>OOP-C Mahrukh</t>
   </si>
   <si>
-    <t>CPS-E Faiza</t>
-  </si>
-  <si>
-    <t>CPS-D Faiza</t>
-  </si>
-  <si>
-    <t>DLD-H Javed Qureshi</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>OOP-B Zain</t>
+    <t>OOP-G Basit</t>
+  </si>
+  <si>
+    <t>SE-B Rubab</t>
+  </si>
+  <si>
+    <t>DP Gr3 Abdul Rahman</t>
+  </si>
+  <si>
+    <t>R12</t>
   </si>
   <si>
     <t>HCI-Gr1 Behraj</t>
   </si>
   <si>
-    <t>Dsci Gr3 Dr. Atif</t>
-  </si>
-  <si>
-    <t>SE-E Ahsan</t>
-  </si>
-  <si>
-    <t>OOP-G Basit</t>
-  </si>
-  <si>
-    <t>SE-B Rubab</t>
-  </si>
-  <si>
-    <t>DP Gr3 Abdul Rahman</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
     <t>OS-A Dr. Hasina</t>
   </si>
   <si>
@@ -266,6 +266,9 @@
     <t>CN-E Dr. Fahad</t>
   </si>
   <si>
+    <t>SE-C Ahsan</t>
+  </si>
+  <si>
     <t>SE-G Ahsan</t>
   </si>
   <si>
@@ -281,9 +284,6 @@
     <t>ME Gr1 Michael</t>
   </si>
   <si>
-    <t>SE-C Ahsan</t>
-  </si>
-  <si>
     <t>CR-3 EE</t>
   </si>
   <si>
@@ -338,69 +338,72 @@
     <t>CR-7</t>
   </si>
   <si>
+    <t>AL Gr2 Dr. Shahzad</t>
+  </si>
+  <si>
+    <t>AL Gr1 Dr. Shahzad</t>
+  </si>
+  <si>
+    <t>HRM-A Ahsan</t>
+  </si>
+  <si>
+    <t>HRM-C Ahsan</t>
+  </si>
+  <si>
+    <t>CR-10</t>
+  </si>
+  <si>
+    <t>Prob-B Osama</t>
+  </si>
+  <si>
+    <t>HRM-CSG M. Zeeshan</t>
+  </si>
+  <si>
+    <t>HRM-F M. Zeeshan</t>
+  </si>
+  <si>
+    <t>NM Gr4 Dr. Khusro</t>
+  </si>
+  <si>
+    <t>HRM-D M. Zeeshan</t>
+  </si>
+  <si>
+    <t>HRM-B M. Zeeshan</t>
+  </si>
+  <si>
+    <t>CR-11</t>
+  </si>
+  <si>
+    <t>Pst.-F Kashif</t>
+  </si>
+  <si>
+    <t>Pst.-A Kashif</t>
+  </si>
+  <si>
+    <t>NM Gr1 Mr. Shahbaz</t>
+  </si>
+  <si>
+    <t>NM Gr3 Mr. Shahbaz</t>
+  </si>
+  <si>
+    <t>Pst.-H Kashif</t>
+  </si>
+  <si>
+    <t>Pst.-C Kashif</t>
+  </si>
+  <si>
+    <t>ME Gr2 Michael</t>
+  </si>
+  <si>
+    <t>CR-16</t>
+  </si>
+  <si>
+    <t>DE-D Jamil</t>
+  </si>
+  <si>
     <t>Al Gr1 Dr. Shahzad</t>
   </si>
   <si>
-    <t>AL Gr2 Dr. Shahzad</t>
-  </si>
-  <si>
-    <t>AL Gr1 Dr. Shahzad</t>
-  </si>
-  <si>
-    <t>HRM-A Ahsan</t>
-  </si>
-  <si>
-    <t>HRM-C Ahsan</t>
-  </si>
-  <si>
-    <t>CR-10</t>
-  </si>
-  <si>
-    <t>HRM-CSG M. Zeeshan</t>
-  </si>
-  <si>
-    <t>HRM-F M. Zeeshan</t>
-  </si>
-  <si>
-    <t>NM Gr4 Dr. Khusro</t>
-  </si>
-  <si>
-    <t>HRM-D M. Zeeshan</t>
-  </si>
-  <si>
-    <t>HRM-B M. Zeeshan</t>
-  </si>
-  <si>
-    <t>CR-11</t>
-  </si>
-  <si>
-    <t>Pst.-F Kashif</t>
-  </si>
-  <si>
-    <t>Pst.-A Kashif</t>
-  </si>
-  <si>
-    <t>NM Gr1 Mr. Shahbaz</t>
-  </si>
-  <si>
-    <t>NM Gr3 Mr. Shahbaz</t>
-  </si>
-  <si>
-    <t>Pst.-H Kashif</t>
-  </si>
-  <si>
-    <t>Pst.-C Kashif</t>
-  </si>
-  <si>
-    <t>ME Gr2 Michael</t>
-  </si>
-  <si>
-    <t>CR-16</t>
-  </si>
-  <si>
-    <t>DE-D Jamil</t>
-  </si>
-  <si>
     <t>DE-F Jamil</t>
   </si>
   <si>
@@ -440,9 +443,6 @@
     <t>Prob-D Osama</t>
   </si>
   <si>
-    <t>Prob-B Osama</t>
-  </si>
-  <si>
     <t>CPS-Lab A1 Hubrah</t>
   </si>
   <si>
@@ -467,21 +467,21 @@
     <t>Lab-3</t>
   </si>
   <si>
+    <t>CG- Gr1 Javeria</t>
+  </si>
+  <si>
+    <t>CG Gr2 Javeria</t>
+  </si>
+  <si>
+    <t>CG Gr3 Javeria</t>
+  </si>
+  <si>
+    <t>Lab-4</t>
+  </si>
+  <si>
     <t>IS-Gr1 Shahbaz</t>
   </si>
   <si>
-    <t>CG- Gr1 Javeria</t>
-  </si>
-  <si>
-    <t>CG Gr2 Javeria</t>
-  </si>
-  <si>
-    <t>CG Gr3 Javeria</t>
-  </si>
-  <si>
-    <t>Lab-4</t>
-  </si>
-  <si>
     <t>Lab-6</t>
   </si>
   <si>
@@ -563,6 +563,9 @@
     <t>Dwh Gr2 Dr. Zulfiqar</t>
   </si>
   <si>
+    <t>ALGO-Gr2 Zeshan Khan</t>
+  </si>
+  <si>
     <t>ALGO-Gr1 Zeshan Khan</t>
   </si>
   <si>
@@ -683,9 +686,6 @@
     <t>WEDNESDAY</t>
   </si>
   <si>
-    <t>ALGO-Gr2 Zeshan Khan</t>
-  </si>
-  <si>
     <t>CV- Gr1 Dr. Tahir Syed</t>
   </si>
   <si>
@@ -779,13 +779,13 @@
     <t>Discrete-Gr1 Dr. Jalal</t>
   </si>
   <si>
+    <t>Pst.-B Abid</t>
+  </si>
+  <si>
+    <t>Pst.-D Abid</t>
+  </si>
+  <si>
     <t>Prob-E Javeria Iftikhar</t>
-  </si>
-  <si>
-    <t>Pst.-B Abid</t>
-  </si>
-  <si>
-    <t>Pst.-D Abid</t>
   </si>
   <si>
     <t>CPS-Lab G1 Hubrah</t>
@@ -1456,33 +1456,33 @@
       <c r="B11" t="s">
         <v>57</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11"/>
+      <c r="D11" t="s">
         <v>58</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>59</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>60</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>61</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>62</v>
       </c>
-      <c r="H11" t="s">
-        <v>63</v>
-      </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
         <v>64</v>
       </c>
-      <c r="B12"/>
       <c r="C12" t="s">
         <v>65</v>
       </c>
@@ -1542,30 +1542,30 @@
         <v>80</v>
       </c>
       <c r="G14"/>
-      <c r="H14"/>
+      <c r="H14" t="s">
+        <v>81</v>
+      </c>
       <c r="I14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G15"/>
-      <c r="H15" t="s">
-        <v>86</v>
-      </c>
+      <c r="H15"/>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
@@ -1641,30 +1641,30 @@
       <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B19" t="s">
-        <v>105</v>
-      </c>
+      <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" t="s">
         <v>106</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>107</v>
-      </c>
-      <c r="G19" t="s">
-        <v>108</v>
       </c>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" t="s">
         <v>110</v>
       </c>
-      <c r="B20"/>
       <c r="C20" t="s">
         <v>111</v>
       </c>
@@ -1717,60 +1717,62 @@
       <c r="B22" t="s">
         <v>125</v>
       </c>
-      <c r="C22"/>
+      <c r="C22" t="s">
+        <v>126</v>
+      </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C24"/>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E24"/>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G24" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="H24" t="s">
         <v>140</v>
@@ -1815,29 +1817,29 @@
       <c r="A27" t="s">
         <v>147</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27"/>
+      <c r="C27" t="s">
         <v>148</v>
-      </c>
-      <c r="C27" t="s">
-        <v>149</v>
       </c>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G27"/>
       <c r="H27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28"/>
+      <c r="C28" t="s">
         <v>152</v>
       </c>
-      <c r="B28"/>
-      <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
@@ -2111,7 +2113,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
         <v>69</v>
@@ -2181,9 +2183,7 @@
       <c r="H9" t="s">
         <v>16</v>
       </c>
-      <c r="I9" t="s">
-        <v>70</v>
-      </c>
+      <c r="I9"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
@@ -2193,19 +2193,19 @@
         <v>180</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -2215,19 +2215,19 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
         <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
         <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G11" t="s">
         <v>120</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
@@ -2255,7 +2255,7 @@
         <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="s">
@@ -2275,16 +2275,16 @@
         <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G13" t="s">
+        <v>189</v>
+      </c>
+      <c r="H13" t="s">
+        <v>190</v>
+      </c>
+      <c r="I13" t="s">
         <v>188</v>
-      </c>
-      <c r="H13" t="s">
-        <v>189</v>
-      </c>
-      <c r="I13" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2295,29 +2295,29 @@
         <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D14" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E14" t="s">
         <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -2334,7 +2334,7 @@
         <v>117</v>
       </c>
       <c r="I15" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2342,19 +2342,19 @@
         <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E16" t="s">
         <v>102</v>
       </c>
       <c r="F16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s">
         <v>113</v>
@@ -2363,7 +2363,7 @@
         <v>100</v>
       </c>
       <c r="I16" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2382,10 +2382,10 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" t="s">
         <v>85</v>
-      </c>
-      <c r="H17" t="s">
-        <v>84</v>
       </c>
       <c r="I17"/>
     </row>
@@ -2405,9 +2405,7 @@
       <c r="E18" t="s">
         <v>123</v>
       </c>
-      <c r="F18" t="s">
-        <v>92</v>
-      </c>
+      <c r="F18"/>
       <c r="G18" t="s">
         <v>29</v>
       </c>
@@ -2415,7 +2413,7 @@
         <v>28</v>
       </c>
       <c r="I18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2433,10 +2431,10 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -2447,10 +2445,10 @@
         <v>98</v>
       </c>
       <c r="G20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I20"/>
     </row>
@@ -2459,19 +2457,19 @@
         <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C21" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E21" t="s">
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G21" t="s">
         <v>43</v>
@@ -2480,7 +2478,7 @@
         <v>101</v>
       </c>
       <c r="I21" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2488,10 +2486,10 @@
         <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D22"/>
       <c r="E22"/>
@@ -2499,19 +2497,19 @@
         <v>125</v>
       </c>
       <c r="G22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H22"/>
       <c r="I22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
@@ -2522,10 +2520,10 @@
         <v>89</v>
       </c>
       <c r="G23" t="s">
+        <v>134</v>
+      </c>
+      <c r="H23" t="s">
         <v>133</v>
-      </c>
-      <c r="H23" t="s">
-        <v>132</v>
       </c>
       <c r="I23" t="s">
         <v>96</v>
@@ -2533,24 +2531,22 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>134</v>
-      </c>
-      <c r="F24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24"/>
+      <c r="G24" t="s">
         <v>139</v>
       </c>
-      <c r="G24" t="s">
-        <v>138</v>
-      </c>
       <c r="H24" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I24"/>
     </row>
@@ -2573,13 +2569,13 @@
       </c>
       <c r="B26"/>
       <c r="C26" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -2589,33 +2585,33 @@
         <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F28"/>
       <c r="G28" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
@@ -2625,14 +2621,14 @@
         <v>153</v>
       </c>
       <c r="B29" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
@@ -2642,14 +2638,14 @@
         <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
@@ -2659,14 +2655,14 @@
         <v>159</v>
       </c>
       <c r="B31" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
@@ -2676,14 +2672,14 @@
         <v>161</v>
       </c>
       <c r="B32" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
@@ -2693,7 +2689,7 @@
         <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -2701,7 +2697,7 @@
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I33"/>
     </row>
@@ -2730,15 +2726,15 @@
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="64" zoomScaleNormal="64" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2875,13 +2871,13 @@
         <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="H5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2915,7 +2911,7 @@
         <v>222</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
         <v>72</v>
@@ -2981,7 +2977,7 @@
         <v>224</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F8" t="s">
         <v>225</v>
@@ -2990,10 +2986,10 @@
         <v>31</v>
       </c>
       <c r="H8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -3014,7 +3010,7 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
@@ -3048,10 +3044,10 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -3105,7 +3101,7 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
         <v>179</v>
@@ -3113,7 +3109,9 @@
       <c r="C12" t="s">
         <v>178</v>
       </c>
-      <c r="D12"/>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
       <c r="E12" t="s">
         <v>230</v>
       </c>
@@ -3168,10 +3166,10 @@
         <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D14" t="s">
         <v>232</v>
@@ -3180,16 +3178,16 @@
         <v>233</v>
       </c>
       <c r="F14" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H14" t="s">
         <v>233</v>
       </c>
       <c r="I14" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J14"/>
       <c r="K14"/>
@@ -3204,7 +3202,7 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -3267,7 +3265,7 @@
         <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -3275,7 +3273,7 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G17" t="s">
         <v>29</v>
@@ -3300,28 +3298,28 @@
         <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E18" t="s">
         <v>119</v>
       </c>
       <c r="F18" t="s">
+        <v>189</v>
+      </c>
+      <c r="G18" t="s">
         <v>188</v>
       </c>
-      <c r="G18" t="s">
-        <v>187</v>
-      </c>
       <c r="H18" t="s">
+        <v>199</v>
+      </c>
+      <c r="I18" t="s">
         <v>198</v>
-      </c>
-      <c r="I18" t="s">
-        <v>197</v>
       </c>
       <c r="J18"/>
       <c r="K18"/>
@@ -3339,16 +3337,16 @@
         <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C19" t="s">
         <v>111</v>
       </c>
       <c r="D19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" t="s">
         <v>108</v>
-      </c>
-      <c r="E19" t="s">
-        <v>109</v>
       </c>
       <c r="F19"/>
       <c r="G19" t="s">
@@ -3358,7 +3356,7 @@
         <v>115</v>
       </c>
       <c r="I19" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J19"/>
       <c r="K19"/>
@@ -3373,7 +3371,7 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
@@ -3383,10 +3381,10 @@
         <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
         <v>113</v>
@@ -3440,10 +3438,10 @@
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F22"/>
       <c r="G22" t="s">
@@ -3451,7 +3449,7 @@
       </c>
       <c r="H22"/>
       <c r="I22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J22"/>
       <c r="K22"/>
@@ -3466,25 +3464,25 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B23"/>
       <c r="C23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G23"/>
       <c r="H23" t="s">
         <v>54</v>
       </c>
       <c r="I23" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="J23"/>
       <c r="K23"/>
@@ -3499,7 +3497,7 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
         <v>237</v>
@@ -3507,10 +3505,10 @@
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" t="s">
         <v>106</v>
-      </c>
-      <c r="F24" t="s">
-        <v>107</v>
       </c>
       <c r="G24"/>
       <c r="H24"/>
@@ -3607,7 +3605,7 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
         <v>242</v>
@@ -3998,7 +3996,7 @@
         <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s">
         <v>227</v>
@@ -4007,10 +4005,10 @@
         <v>228</v>
       </c>
       <c r="E10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
@@ -4032,7 +4030,7 @@
         <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
@@ -4045,7 +4043,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
         <v>70</v>
@@ -4057,7 +4055,7 @@
         <v>67</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
         <v>65</v>
@@ -4074,7 +4072,7 @@
         <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
@@ -4106,7 +4104,7 @@
         <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" t="s">
         <v>72</v>
@@ -4116,7 +4114,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
@@ -4125,7 +4123,7 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E15" t="s">
         <v>42</v>
@@ -4134,7 +4132,7 @@
         <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -4148,16 +4146,18 @@
       <c r="D16" t="s">
         <v>96</v>
       </c>
-      <c r="E16"/>
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
       <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="s">
         <v>139</v>
-      </c>
-      <c r="G16" t="s">
-        <v>138</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -4203,21 +4203,29 @@
       <c r="B19" t="s">
         <v>100</v>
       </c>
-      <c r="C19"/>
+      <c r="C19" t="s">
+        <v>252</v>
+      </c>
       <c r="D19" t="s">
         <v>102</v>
       </c>
-      <c r="E19"/>
-      <c r="F19"/>
+      <c r="E19" t="s">
+        <v>253</v>
+      </c>
+      <c r="F19" t="s">
+        <v>252</v>
+      </c>
       <c r="G19" t="s">
         <v>103</v>
       </c>
       <c r="H19"/>
-      <c r="I19"/>
+      <c r="I19" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
         <v>112</v>
@@ -4231,11 +4239,11 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="H20"/>
       <c r="I20" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -4266,26 +4274,20 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B23"/>
-      <c r="C23" t="s">
-        <v>253</v>
-      </c>
+      <c r="C23"/>
       <c r="D23"/>
-      <c r="E23" t="s">
-        <v>254</v>
-      </c>
-      <c r="F23" t="s">
-        <v>253</v>
-      </c>
+      <c r="E23"/>
+      <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
         <v>255</v>
@@ -4351,7 +4353,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
@@ -4605,13 +4607,13 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="E7" t="s">
         <v>230</v>
@@ -4621,7 +4623,7 @@
       </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I7"/>
     </row>
@@ -4637,7 +4639,7 @@
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
         <v>171</v>
@@ -4674,16 +4676,16 @@
         <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -4713,7 +4715,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12"/>
       <c r="C12"/>
@@ -4762,20 +4764,20 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
         <v>227</v>
       </c>
       <c r="C15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" t="s">
         <v>191</v>
-      </c>
-      <c r="D15" t="s">
-        <v>190</v>
       </c>
       <c r="E15"/>
       <c r="F15" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
@@ -4790,7 +4792,7 @@
         <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -4824,7 +4826,7 @@
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -4832,19 +4834,19 @@
         <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D18" t="s">
+        <v>252</v>
+      </c>
+      <c r="E18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" t="s">
         <v>253</v>
-      </c>
-      <c r="E18" t="s">
-        <v>139</v>
-      </c>
-      <c r="F18" t="s">
-        <v>254</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
@@ -4855,7 +4857,7 @@
         <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C19" t="s">
         <v>114</v>
@@ -4879,22 +4881,22 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I20"/>
     </row>
@@ -4906,21 +4908,21 @@
         <v>96</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" t="s">
         <v>108</v>
-      </c>
-      <c r="I21" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -4948,7 +4950,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -4961,7 +4963,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -5027,7 +5029,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
         <v>276</v>

</xml_diff>

<commit_message>
update timetable to v4
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -32,28 +32,28 @@
     <t>Venues/time</t>
   </si>
   <si>
-    <t>08-8:55</t>
-  </si>
-  <si>
-    <t>09-09:55</t>
-  </si>
-  <si>
-    <t>10-10:55</t>
-  </si>
-  <si>
-    <t>11-11:55</t>
-  </si>
-  <si>
-    <t>12-12:55</t>
-  </si>
-  <si>
-    <t>1-1:55</t>
-  </si>
-  <si>
-    <t>2-2:55</t>
-  </si>
-  <si>
-    <t>3-3:55</t>
+    <t>08-8:45</t>
+  </si>
+  <si>
+    <t>08:45-09:30</t>
+  </si>
+  <si>
+    <t>09:30-10:15</t>
+  </si>
+  <si>
+    <t>10:15-11:00</t>
+  </si>
+  <si>
+    <t>11:00-11:45</t>
+  </si>
+  <si>
+    <t>11:45-12:30</t>
+  </si>
+  <si>
+    <t>12:30-1:15</t>
+  </si>
+  <si>
+    <t>1:15-2:00</t>
   </si>
   <si>
     <t>CLASSROOMS</t>
@@ -656,7 +656,7 @@
     <t>DLD-Lab A1 Mubashyra</t>
   </si>
   <si>
-    <t>PF-Lab A Abdul Aziz &amp; Sadia</t>
+    <t>PF-Lab A Abdul Aziz &amp; Aqsa</t>
   </si>
   <si>
     <t>OOP-Lab F Fahim</t>
@@ -752,7 +752,7 @@
     <t>OS Lab-F Abdullah</t>
   </si>
   <si>
-    <t>PF-Lab B Sadia &amp; Rahemeen</t>
+    <t>PF-Lab B Aqsa &amp; Rahemeen</t>
   </si>
   <si>
     <t>DLD-Lab E2 Abdul Khaliq</t>
@@ -833,7 +833,7 @@
     <t>FRIDAY</t>
   </si>
   <si>
-    <t>J UMMA PRAYER</t>
+    <t>J U M M A P R A Y E R</t>
   </si>
   <si>
     <t>CN-Lab B Munim</t>
@@ -857,7 +857,7 @@
     <t>DLD-Lab C1 Mubashyra</t>
   </si>
   <si>
-    <t>PF-Lab D Sadia &amp; Rahemeen</t>
+    <t>PF-Lab D Aqsa &amp; Rahemeen</t>
   </si>
   <si>
     <t>DLD-Lab C2 Maham</t>
@@ -2726,8 +2726,8 @@
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="64" zoomScaleNormal="64" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4575,11 +4575,11 @@
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
-      <c r="G5" t="s">
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5" t="s">
         <v>270</v>
       </c>
-      <c r="H5"/>
-      <c r="I5"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
@@ -4621,10 +4621,10 @@
       <c r="F7" t="s">
         <v>231</v>
       </c>
-      <c r="G7"/>
-      <c r="H7" t="s">
+      <c r="G7" t="s">
         <v>181</v>
       </c>
+      <c r="H7"/>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
@@ -4644,13 +4644,13 @@
       <c r="F8" t="s">
         <v>171</v>
       </c>
-      <c r="G8"/>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
       <c r="H8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" t="s">
         <v>24</v>
       </c>
+      <c r="I8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
@@ -4666,10 +4666,10 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9" t="s">
+      <c r="H9" t="s">
         <v>43</v>
       </c>
+      <c r="I9"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
@@ -4707,10 +4707,10 @@
         <v>78</v>
       </c>
       <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11" t="s">
+      <c r="G11" t="s">
         <v>225</v>
       </c>
+      <c r="H11"/>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
@@ -4754,13 +4754,13 @@
       <c r="F14" t="s">
         <v>174</v>
       </c>
-      <c r="G14"/>
+      <c r="G14" t="s">
+        <v>235</v>
+      </c>
       <c r="H14" t="s">
-        <v>235</v>
-      </c>
-      <c r="I14" t="s">
         <v>234</v>
       </c>
+      <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
@@ -4779,13 +4779,13 @@
       <c r="F15" t="s">
         <v>192</v>
       </c>
-      <c r="G15"/>
+      <c r="G15" t="s">
+        <v>229</v>
+      </c>
       <c r="H15" t="s">
-        <v>229</v>
-      </c>
-      <c r="I15" t="s">
         <v>228</v>
       </c>
+      <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
@@ -4824,10 +4824,10 @@
         <v>93</v>
       </c>
       <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17" t="s">
+      <c r="H17" t="s">
         <v>195</v>
       </c>
+      <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
@@ -4871,13 +4871,13 @@
       <c r="F19" t="s">
         <v>112</v>
       </c>
-      <c r="G19"/>
+      <c r="G19" t="s">
+        <v>236</v>
+      </c>
       <c r="H19" t="s">
-        <v>236</v>
-      </c>
-      <c r="I19" t="s">
         <v>115</v>
       </c>
+      <c r="I19"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
@@ -4894,10 +4894,10 @@
       <c r="F20" t="s">
         <v>129</v>
       </c>
-      <c r="G20"/>
-      <c r="H20" t="s">
+      <c r="G20" t="s">
         <v>198</v>
       </c>
+      <c r="H20"/>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
@@ -4917,13 +4917,13 @@
       <c r="F21" t="s">
         <v>131</v>
       </c>
-      <c r="G21"/>
+      <c r="G21" t="s">
+        <v>107</v>
+      </c>
       <c r="H21" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21" t="s">
         <v>108</v>
       </c>
+      <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
@@ -4940,13 +4940,13 @@
       <c r="F22" t="s">
         <v>99</v>
       </c>
-      <c r="G22"/>
+      <c r="G22" t="s">
+        <v>101</v>
+      </c>
       <c r="H22" t="s">
-        <v>101</v>
-      </c>
-      <c r="I22" t="s">
         <v>98</v>
       </c>
+      <c r="I22"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
@@ -5000,13 +5000,11 @@
       <c r="F26" t="s">
         <v>272</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26" t="s">
         <v>273</v>
       </c>
-      <c r="H26" t="s">
-        <v>272</v>
-      </c>
-      <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
@@ -5022,9 +5020,7 @@
       </c>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27" t="s">
-        <v>275</v>
-      </c>
+      <c r="H27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">

</xml_diff>

<commit_message>
update tt to spring 2020 v2.0
</commit_message>
<xml_diff>
--- a/include/BSCS-modified.xlsx
+++ b/include/BSCS-modified.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="286">
   <si>
     <t>MONDAY</t>
   </si>
@@ -92,6 +92,9 @@
     <t>OOP-G Basit</t>
   </si>
   <si>
+    <t>OOP-C Danish</t>
+  </si>
+  <si>
     <t>OOP SE-B Basit</t>
   </si>
   <si>
@@ -107,666 +110,663 @@
     <t>OOP-F Zain</t>
   </si>
   <si>
-    <t>OOP-C Danish</t>
+    <t>OOP-E Dr. Abdul Aziz</t>
+  </si>
+  <si>
+    <t>OOP SE-A Dr. Abdul Aziz</t>
+  </si>
+  <si>
+    <t>HCI-Gr1 Behraj</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>IR Gr1 Dr. Rafi</t>
+  </si>
+  <si>
+    <t>IR Gr2 Dr. Rafi</t>
+  </si>
+  <si>
+    <t>DDR Gr1 Abdul Rahman</t>
+  </si>
+  <si>
+    <t>DDR Gr2 Abdul Rahman</t>
+  </si>
+  <si>
+    <t>BLN Gr1 Dr. Sufian</t>
+  </si>
+  <si>
+    <t>Dwh Gr3 Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>DDR Gr3 Abdul Rahman</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>Dsci. Gr1 Dr. Noman</t>
+  </si>
+  <si>
+    <t>Dsci. Gr2 Dr. Noman</t>
+  </si>
+  <si>
+    <t>OOP-B Danish</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>ISS-Gr1 Shahbaz Siddiqui</t>
+  </si>
+  <si>
+    <t>Dsci-Gr1 Dr. Atif</t>
+  </si>
+  <si>
+    <t>Discrete SE-B Shoaib Raza</t>
+  </si>
+  <si>
+    <t>Discrete Gr1 Shoaib Raza</t>
+  </si>
+  <si>
+    <t>DS-Gr4 Nadeem Kafi</t>
+  </si>
+  <si>
+    <t>Discrete SE-A Shoaib Raza</t>
+  </si>
+  <si>
+    <t>RM Gr1 Shoaib Raza</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>OS-Gr1 Nousheen</t>
+  </si>
+  <si>
+    <t>OS-Gr5 Nousheen</t>
+  </si>
+  <si>
+    <t>COAL Gr1 Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>CN-F Dr. Ghufran</t>
+  </si>
+  <si>
+    <t>CN-D Dr. Ghufran</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>DS-Gr1 Nida pervaiz</t>
+  </si>
+  <si>
+    <t>OS-Gr3 Dr. Hasina</t>
+  </si>
+  <si>
+    <t>AI-E Dr. Fahad Sherwani</t>
+  </si>
+  <si>
+    <t>OS-Gr4 Dr. Hasina</t>
+  </si>
+  <si>
+    <t>AI-B Dr. Fahad Sherwani</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>Dwh Gr2 Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>Dwh Gr1 Dr. Zulfiqar</t>
+  </si>
+  <si>
+    <t>Pst.-D Amanullah</t>
+  </si>
+  <si>
+    <t>Pst.-B Amanullah</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>BLN Gr1 Dr. Jawwad</t>
+  </si>
+  <si>
+    <t>SE-B Romasha</t>
+  </si>
+  <si>
+    <t>SE-E Romasha</t>
   </si>
   <si>
     <t>OOP-D Zain</t>
   </si>
   <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>IR Gr1 Dr. Rafi</t>
-  </si>
-  <si>
-    <t>IR Gr2 Dr. Rafi</t>
-  </si>
-  <si>
-    <t>DDR Gr1 Abdul Rahman</t>
-  </si>
-  <si>
-    <t>OOP-E Dr. Abdul Aziz</t>
-  </si>
-  <si>
-    <t>OOP SE-A Dr. Abdul Aziz</t>
-  </si>
-  <si>
-    <t>DDR Gr2 Abdul Rahman</t>
-  </si>
-  <si>
-    <t>DDR Gr3 Abdul Rahman</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>Dsci. Gr1 Dr. Noman</t>
-  </si>
-  <si>
-    <t>Dsci. Gr2 Dr. Noman</t>
-  </si>
-  <si>
-    <t>IOT Gr2 Dr. Fahad Samad</t>
+    <t>SE-F Romasha</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>CR-3 EE</t>
+  </si>
+  <si>
+    <t>ME Gr2 Michael</t>
+  </si>
+  <si>
+    <t>ME Gr3 Michael</t>
+  </si>
+  <si>
+    <t>ME Gr1 Michael</t>
+  </si>
+  <si>
+    <t>CA Gr1 Asim</t>
+  </si>
+  <si>
+    <t>CR-4</t>
+  </si>
+  <si>
+    <t>DS-Gr2 Anum</t>
+  </si>
+  <si>
+    <t>DS-Gr5 Anum</t>
+  </si>
+  <si>
+    <t>CPS-H Faiza</t>
+  </si>
+  <si>
+    <t>Psych Gr1 Saba</t>
+  </si>
+  <si>
+    <t>PROB-D Osama</t>
+  </si>
+  <si>
+    <t>CR-5</t>
+  </si>
+  <si>
+    <t>PROB-H Nadeem Khan</t>
+  </si>
+  <si>
+    <t>NC-A Nadeem Khan</t>
+  </si>
+  <si>
+    <t>TBW-D Sameera</t>
+  </si>
+  <si>
+    <t>AI-F Nida Pervaiz</t>
+  </si>
+  <si>
+    <t>AI-D Nida Pervaiz</t>
+  </si>
+  <si>
+    <t>TBW-B Sameera</t>
+  </si>
+  <si>
+    <t>NC-C Nadeem Khan</t>
+  </si>
+  <si>
+    <t>CR-7</t>
+  </si>
+  <si>
+    <t>FA Gr1 Ahsan</t>
+  </si>
+  <si>
+    <t>CPS Lab SE-A Saba</t>
+  </si>
+  <si>
+    <t>TBW-E Javeria Ali</t>
+  </si>
+  <si>
+    <t>CPS Lab SE-B Saba</t>
+  </si>
+  <si>
+    <t>CR-8</t>
+  </si>
+  <si>
+    <t>Ethics Gr1 Dr. Shahzad</t>
+  </si>
+  <si>
+    <t>IRS SE-B Dr. Shahzad</t>
+  </si>
+  <si>
+    <t>Psych Gr2 Saba</t>
+  </si>
+  <si>
+    <t>Pst.-C Kashif</t>
+  </si>
+  <si>
+    <t>Pst.-H Kashif</t>
+  </si>
+  <si>
+    <t>CPS-G Hafza</t>
+  </si>
+  <si>
+    <t>EP-Gr1 Dr. Nazia Nazeer</t>
+  </si>
+  <si>
+    <t>CR-10</t>
+  </si>
+  <si>
+    <t>NC-G M.Shahbaz</t>
+  </si>
+  <si>
+    <t>NC-B M.Shahbaz</t>
+  </si>
+  <si>
+    <t>LA-Gr1 Dr. Sadaqaat</t>
+  </si>
+  <si>
+    <t>CPS-J Hafza</t>
+  </si>
+  <si>
+    <t>Cal-Gr1 Dr. Sadaaqat</t>
+  </si>
+  <si>
+    <t>NC-D M.Shahbaz</t>
+  </si>
+  <si>
+    <t>EP-Gr2 Asiya</t>
+  </si>
+  <si>
+    <t>CR-11</t>
+  </si>
+  <si>
+    <t>Pst.-J Kashif</t>
+  </si>
+  <si>
+    <t>Pst.-F Kashif</t>
+  </si>
+  <si>
+    <t>HRM Gr2 M. Zeeshan</t>
+  </si>
+  <si>
+    <t>HRM Gr3 M. Zeeshan</t>
+  </si>
+  <si>
+    <t>Socio Gr1 Sumaira</t>
+  </si>
+  <si>
+    <t>HRM Gr1 M. Zeeshan</t>
+  </si>
+  <si>
+    <t>EP-Gr3 Ahsan</t>
+  </si>
+  <si>
+    <t>CR-16</t>
+  </si>
+  <si>
+    <t>Socio Gr2 Sumaira</t>
+  </si>
+  <si>
+    <t>OOP-J Danish</t>
+  </si>
+  <si>
+    <t>Socio Gr3 Sumaira</t>
+  </si>
+  <si>
+    <t>DE-J Amber</t>
+  </si>
+  <si>
+    <t>DE-A Amber</t>
+  </si>
+  <si>
+    <t>SIT-Gr1 Dr. Saad</t>
+  </si>
+  <si>
+    <t>CR-17</t>
+  </si>
+  <si>
+    <t>Pst.-G Ibrahim</t>
+  </si>
+  <si>
+    <t>Pst.-E Ibrahim</t>
+  </si>
+  <si>
+    <t>DE-E Amber</t>
+  </si>
+  <si>
+    <t>DE-F Javeria</t>
+  </si>
+  <si>
+    <t>DE-B Javeria</t>
+  </si>
+  <si>
+    <t>DE-H Javeria</t>
+  </si>
+  <si>
+    <t>CR-18</t>
+  </si>
+  <si>
+    <t>DE-C Fareeha</t>
+  </si>
+  <si>
+    <t>DE-G Fareeha</t>
+  </si>
+  <si>
+    <t>DE-D Fareeha</t>
+  </si>
+  <si>
+    <t>IRS SE-A Dr. Shahzad</t>
+  </si>
+  <si>
+    <t>CR-20</t>
+  </si>
+  <si>
+    <t>LABS</t>
+  </si>
+  <si>
+    <t>Lab-1</t>
+  </si>
+  <si>
+    <t>CN Lab-A Rabia</t>
+  </si>
+  <si>
+    <t>DS Lab-Gr1 Anum</t>
+  </si>
+  <si>
+    <t>Lab-3</t>
+  </si>
+  <si>
+    <t>CN Lab-C Kariz</t>
+  </si>
+  <si>
+    <t>OS Lab-Gr1 Rahemeen</t>
+  </si>
+  <si>
+    <t>Lab-4</t>
+  </si>
+  <si>
+    <t>NP Gr1 Shahbaz Siddiqui</t>
+  </si>
+  <si>
+    <t>COAL Lab Gr2 Atiya</t>
+  </si>
+  <si>
+    <t>EE Lab-6</t>
+  </si>
+  <si>
+    <t>DLD Lab-A2 Musawar</t>
+  </si>
+  <si>
+    <t>DLD Lab-G1 Mubashyra</t>
+  </si>
+  <si>
+    <t>EE Lab-9</t>
+  </si>
+  <si>
+    <t>EE Lab 10</t>
+  </si>
+  <si>
+    <t>LLC</t>
+  </si>
+  <si>
+    <t>CPS- Lab B1 Hubrah</t>
+  </si>
+  <si>
+    <t>EE MPI Lab</t>
+  </si>
+  <si>
+    <t>DLD Lab-A1 M. Nadeem</t>
+  </si>
+  <si>
+    <t>DLD Lab-G2 Hamza</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>PF-A Atiya</t>
+  </si>
+  <si>
+    <t>DLD-B Musawar</t>
+  </si>
+  <si>
+    <t>COAL Gr2 Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>DLD-H Musawar</t>
+  </si>
+  <si>
+    <t>CN-B Abdullah</t>
+  </si>
+  <si>
+    <t>CN-E Abdullah</t>
+  </si>
+  <si>
+    <t>SE-A Farrukh</t>
+  </si>
+  <si>
+    <t>SE-D Farrukh</t>
+  </si>
+  <si>
+    <t>CN-A Dr. Hassan</t>
+  </si>
+  <si>
+    <t>CN-C Dr. Hassan</t>
+  </si>
+  <si>
+    <t>OOAD Gr1 Ubaid</t>
+  </si>
+  <si>
+    <t>TOA-B Shaharbano</t>
+  </si>
+  <si>
+    <t>SE-C Rubab</t>
+  </si>
+  <si>
+    <t>ISE SE-B Rubab</t>
+  </si>
+  <si>
+    <t>ISE SE-A Rubab</t>
+  </si>
+  <si>
+    <t>AI-A Saeeda</t>
+  </si>
+  <si>
+    <t>AI-C Saeeda</t>
+  </si>
+  <si>
+    <t>TOA-F Shahzad</t>
+  </si>
+  <si>
+    <t>TOA-H Shahzad</t>
+  </si>
+  <si>
+    <t>DLD-G Behraj</t>
+  </si>
+  <si>
+    <t>TOA-E Bakhtawar</t>
+  </si>
+  <si>
+    <t>TOA-C Bakhtawar</t>
+  </si>
+  <si>
+    <t>TOA-A Bakhtawar</t>
+  </si>
+  <si>
+    <t>TOA-D Shaharbano</t>
+  </si>
+  <si>
+    <t>TOA-G Shaharbano</t>
+  </si>
+  <si>
+    <t>DLD-A Behraj</t>
+  </si>
+  <si>
+    <t>WP Gr2 Abdul Rahman</t>
+  </si>
+  <si>
+    <t>CPS-D Atifa</t>
+  </si>
+  <si>
+    <t>AP Gr1 Javaid Qureshi</t>
+  </si>
+  <si>
+    <t>CPS SE-B Javed Iqbal</t>
+  </si>
+  <si>
+    <t>CPS SE-A Javed Iqbal</t>
+  </si>
+  <si>
+    <t>PROB-A Fareeha</t>
+  </si>
+  <si>
+    <t>PROB-F Osama</t>
+  </si>
+  <si>
+    <t>TBW-C Javeria Ali</t>
+  </si>
+  <si>
+    <t>TBW-A Javeria Ali</t>
+  </si>
+  <si>
+    <t>CPS-A Nazia Imam</t>
+  </si>
+  <si>
+    <t>CPS- Lab C2 Kishwar</t>
+  </si>
+  <si>
+    <t>NC-H Jamil</t>
+  </si>
+  <si>
+    <t>NC-F Jamil</t>
+  </si>
+  <si>
+    <t>NC-E Jamil</t>
+  </si>
+  <si>
+    <t>DLD-D Bilal</t>
+  </si>
+  <si>
+    <t>DLD-F Bilal</t>
+  </si>
+  <si>
+    <t>PROB-G Asma</t>
+  </si>
+  <si>
+    <t>PROB-E Asma</t>
+  </si>
+  <si>
+    <t>DLD-C Rabia</t>
+  </si>
+  <si>
+    <t>TBW-F Sameera</t>
+  </si>
+  <si>
+    <t>DLD-J Rabia</t>
+  </si>
+  <si>
+    <t>DLD-E Rabia</t>
+  </si>
+  <si>
+    <t>CPS- Lab G1 Nazia Imam</t>
+  </si>
+  <si>
+    <t>COAL Lab Gr1 Shoaib Rauf</t>
+  </si>
+  <si>
+    <t>PF Lab-A Aqsa</t>
+  </si>
+  <si>
+    <t>CN Lab-D Rabia</t>
+  </si>
+  <si>
+    <t>OOP Lab-A Nida Munawar</t>
+  </si>
+  <si>
+    <t>OOP Lab-B Irfan</t>
+  </si>
+  <si>
+    <t>DLD Lab-D2 Fahim Ahmed</t>
+  </si>
+  <si>
+    <t>DLD Lab-B2 Fahim Ahmed</t>
+  </si>
+  <si>
+    <t>OS Lab-Gr2 Safia</t>
+  </si>
+  <si>
+    <t>DS Lab-Gr2 Ammara</t>
+  </si>
+  <si>
+    <t>CPS- Lab E1 Hubrah</t>
+  </si>
+  <si>
+    <t>CPS- Lab G2 Atifa</t>
+  </si>
+  <si>
+    <t>DLD Lab-D1 Hamza</t>
+  </si>
+  <si>
+    <t>DLD Lab-C1 M. Nadeem</t>
+  </si>
+  <si>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
+    <t>CPS-B Atifa</t>
+  </si>
+  <si>
+    <t>CPS-F Atifa</t>
+  </si>
+  <si>
+    <t>DS-Gr3 Basit</t>
+  </si>
+  <si>
+    <t>PIT-Gr1 Saeeda</t>
   </si>
   <si>
     <t>IOT Gr1 Dr. Fahad Samad</t>
   </si>
   <si>
-    <t>OOP-B Danish</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>ISS-Gr1 Shahbaz Siddiqui</t>
-  </si>
-  <si>
-    <t>Dsci-Gr1 Dr. Atif</t>
-  </si>
-  <si>
-    <t>Discrete SE-B Shoaib Raza</t>
-  </si>
-  <si>
-    <t>Discrete Gr1 Shoaib Raza</t>
-  </si>
-  <si>
-    <t>Discrete SE-A Shoaib Raza</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>OS-Gr1 Nousheen</t>
-  </si>
-  <si>
-    <t>OS-Gr5 Nousheen</t>
-  </si>
-  <si>
-    <t>COAL Gr1 Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>CN-D Dr. Ghufran</t>
-  </si>
-  <si>
-    <t>CN-F Dr. Ghufran</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>DS-Gr1 Nida pervaiz</t>
-  </si>
-  <si>
-    <t>OS-Gr3 Dr. Hasina</t>
-  </si>
-  <si>
-    <t>AI-E Dr. Fahad Sherwani</t>
-  </si>
-  <si>
-    <t>OS-Gr4 Dr. Hasina</t>
-  </si>
-  <si>
-    <t>AI-B Dr. Fahad Sherwani</t>
-  </si>
-  <si>
-    <t>R109</t>
-  </si>
-  <si>
-    <t>Dwh Gr2 Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>Dwh Gr1 Dr. Zulfiqar</t>
-  </si>
-  <si>
-    <t>Pst.-D Amanullah</t>
-  </si>
-  <si>
-    <t>DS-Gr4 Nadeem Kafi</t>
-  </si>
-  <si>
-    <t>Pst.-B Amanullah</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>BLN Gr1 Dr. Jawwad</t>
-  </si>
-  <si>
-    <t>SE-B Romasha</t>
-  </si>
-  <si>
-    <t>SE-E Romasha</t>
-  </si>
-  <si>
-    <t>SE-F Romasha</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>FA Gr1 Ahsan</t>
-  </si>
-  <si>
-    <t>BLN Gr1 Dr. Sufian</t>
-  </si>
-  <si>
-    <t>BLN Gr2 Dr. Sufian</t>
-  </si>
-  <si>
-    <t>CR-3 EE</t>
-  </si>
-  <si>
-    <t>ME Gr2 Michael</t>
-  </si>
-  <si>
-    <t>ME Gr3 Michael</t>
-  </si>
-  <si>
-    <t>ME Gr1 Michael</t>
-  </si>
-  <si>
-    <t>CA Gr1 Asim</t>
-  </si>
-  <si>
-    <t>CR-4</t>
-  </si>
-  <si>
-    <t>DS-Gr2 Anum</t>
-  </si>
-  <si>
-    <t>DS-Gr5 Anum</t>
-  </si>
-  <si>
-    <t>CPS-H Faiza</t>
-  </si>
-  <si>
-    <t>NP Gr1 Shahbaz Siddiqui</t>
-  </si>
-  <si>
-    <t>CR-5</t>
-  </si>
-  <si>
-    <t>PROB-H Nadeem Khan</t>
-  </si>
-  <si>
-    <t>NC-A Nadeem Khan</t>
-  </si>
-  <si>
-    <t>TBW-D Sameera</t>
-  </si>
-  <si>
-    <t>AI-F Nida Pervaiz</t>
-  </si>
-  <si>
-    <t>AI-D Nida Pervaiz</t>
-  </si>
-  <si>
-    <t>TBW-B Sameera</t>
-  </si>
-  <si>
-    <t>NC-C Nadeem Khan</t>
-  </si>
-  <si>
-    <t>CR-7</t>
-  </si>
-  <si>
-    <t>Pst.-A Hassan</t>
-  </si>
-  <si>
-    <t>CPS Lab SE-A Saba</t>
-  </si>
-  <si>
-    <t>TBW-E Javeria Ali</t>
-  </si>
-  <si>
-    <t>CPS Lab SE-B Saba</t>
-  </si>
-  <si>
-    <t>CR-8</t>
-  </si>
-  <si>
-    <t>Ethics Gr1 Dr. Shahzad</t>
-  </si>
-  <si>
-    <t>IRS SE-B Dr. Shahzad</t>
-  </si>
-  <si>
-    <t>Psych Gr2 Saba</t>
-  </si>
-  <si>
-    <t>Psych Gr1 Saba</t>
-  </si>
-  <si>
-    <t>Pst.-C Kashif</t>
-  </si>
-  <si>
-    <t>Pst.-H Kashif</t>
-  </si>
-  <si>
-    <t>CPS-G Hafza</t>
-  </si>
-  <si>
-    <t>EP-Gr1 Dr. Nazia Nazeer</t>
-  </si>
-  <si>
-    <t>CR-10</t>
-  </si>
-  <si>
-    <t>NC-G M.Shahbaz</t>
-  </si>
-  <si>
-    <t>NC-B M.Shahbaz</t>
-  </si>
-  <si>
-    <t>LA-Gr1 Dr. Sadaqaat</t>
-  </si>
-  <si>
-    <t>CPS-J Hafza</t>
-  </si>
-  <si>
-    <t>Cal-Gr1 Dr. Sadaaqat</t>
-  </si>
-  <si>
-    <t>NC-D M.Shahbaz</t>
-  </si>
-  <si>
-    <t>EP-Gr2 Asiya</t>
-  </si>
-  <si>
-    <t>CR-11</t>
-  </si>
-  <si>
-    <t>Pst.-J Kashif</t>
-  </si>
-  <si>
-    <t>Pst.-F Kashif</t>
-  </si>
-  <si>
-    <t>HRM Gr2 M. Zeeshan</t>
-  </si>
-  <si>
-    <t>HRM Gr3 M. Zeeshan</t>
-  </si>
-  <si>
-    <t>HRM Gr1 M. Zeeshan</t>
-  </si>
-  <si>
-    <t>EP-Gr3 Ahsan</t>
-  </si>
-  <si>
-    <t>CR-16</t>
-  </si>
-  <si>
-    <t>Socio Gr2 Sumaira</t>
-  </si>
-  <si>
-    <t>OOP-J Danish</t>
-  </si>
-  <si>
-    <t>Socio Gr3 Sumaira</t>
-  </si>
-  <si>
-    <t>Socio Gr1 Sumaira</t>
-  </si>
-  <si>
-    <t>DE-J Amber</t>
-  </si>
-  <si>
-    <t>DE-A Amber</t>
-  </si>
-  <si>
-    <t>SIT-Gr1 Dr. Saad</t>
-  </si>
-  <si>
-    <t>CR-17</t>
-  </si>
-  <si>
-    <t>Pst.-G Ibrahim</t>
-  </si>
-  <si>
-    <t>Pst.-E Ibrahim</t>
-  </si>
-  <si>
-    <t>DE-E Amber</t>
-  </si>
-  <si>
-    <t>DE-F Javeria</t>
-  </si>
-  <si>
-    <t>DE-B Javeria</t>
-  </si>
-  <si>
-    <t>DE-H Javeria</t>
-  </si>
-  <si>
-    <t>CR-18</t>
-  </si>
-  <si>
-    <t>DE-C Fareeha</t>
-  </si>
-  <si>
-    <t>DE-G Fareeha</t>
-  </si>
-  <si>
-    <t>DE-D Fareeha</t>
-  </si>
-  <si>
-    <t>CR-20</t>
-  </si>
-  <si>
-    <t>LABS</t>
-  </si>
-  <si>
-    <t>Lab-1</t>
-  </si>
-  <si>
-    <t>CN Lab-A Rabia</t>
-  </si>
-  <si>
-    <t>DS Lab-Gr1 Anum</t>
-  </si>
-  <si>
-    <t>Lab-3</t>
-  </si>
-  <si>
-    <t>CN Lab-C Abdullah</t>
-  </si>
-  <si>
-    <t>OS Lab-Gr1 Rahemeen</t>
-  </si>
-  <si>
-    <t>Lab-4</t>
-  </si>
-  <si>
-    <t>COAL Lab Gr2 Atiya</t>
-  </si>
-  <si>
-    <t>EE Lab-6</t>
-  </si>
-  <si>
-    <t>DLD Lab-A2 Musawar</t>
-  </si>
-  <si>
-    <t>DLD Lab-G1 Mubashyra</t>
-  </si>
-  <si>
-    <t>EE Lab-9</t>
-  </si>
-  <si>
-    <t>EE Lab 10</t>
-  </si>
-  <si>
-    <t>LLC</t>
-  </si>
-  <si>
-    <t>CPS- Lab B1 Hubrah</t>
-  </si>
-  <si>
-    <t>EE MPI Lab</t>
-  </si>
-  <si>
-    <t>DLD Lab-A1 M. Nadeem</t>
-  </si>
-  <si>
-    <t>DLD Lab-G2 Hamza</t>
-  </si>
-  <si>
-    <t>TUESDAY</t>
-  </si>
-  <si>
-    <t>PF-A Atiya</t>
-  </si>
-  <si>
-    <t>DLD-B Musawar</t>
-  </si>
-  <si>
-    <t>COAL Gr2 Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>DLD-H Musawar</t>
-  </si>
-  <si>
-    <t>CN-B Abdullah</t>
-  </si>
-  <si>
-    <t>CN-E Abdullah</t>
-  </si>
-  <si>
-    <t>SE-A Farrukh</t>
-  </si>
-  <si>
-    <t>SE-D Farrukh</t>
-  </si>
-  <si>
-    <t>CN-A Dr. Hassan</t>
-  </si>
-  <si>
-    <t>CN-C Dr. Hassan</t>
-  </si>
-  <si>
-    <t>OOAD Gr1 Ubaid</t>
-  </si>
-  <si>
-    <t>RM Gr1 Shoaib Raza</t>
-  </si>
-  <si>
-    <t>TOA-B Shaharbano</t>
-  </si>
-  <si>
-    <t>Bio-Gr1 Dr. Rauf</t>
-  </si>
-  <si>
-    <t>SE-C Rubab</t>
-  </si>
-  <si>
-    <t>ISE SE-B Rubab</t>
-  </si>
-  <si>
     <t>BA-Gr1 Dr. Rauf</t>
   </si>
   <si>
-    <t>ISE SE-A Rubab</t>
-  </si>
-  <si>
-    <t>AI-A Saeeda</t>
-  </si>
-  <si>
-    <t>AI-C Saeeda</t>
-  </si>
-  <si>
-    <t>TOA-F Shahzad</t>
-  </si>
-  <si>
-    <t>TOA-H Shahzad</t>
-  </si>
-  <si>
-    <t>PIT-Gr1 Saeeda</t>
-  </si>
-  <si>
-    <t>TOA-E Bakhtawar</t>
-  </si>
-  <si>
-    <t>TOA-C Bakhtawar</t>
-  </si>
-  <si>
-    <t>TOA-A Bakhtawar</t>
-  </si>
-  <si>
-    <t>TOA-D Shaharbano</t>
-  </si>
-  <si>
-    <t>TOA-G Shaharbano</t>
-  </si>
-  <si>
-    <t>HCI-Gr1 Behraj</t>
-  </si>
-  <si>
-    <t>DLD-A Behraj</t>
-  </si>
-  <si>
-    <t>CPS SE-B Javed Iqbal</t>
-  </si>
-  <si>
-    <t>DLD-G Behraj</t>
-  </si>
-  <si>
-    <t>CPS-D Atifa</t>
-  </si>
-  <si>
-    <t>AP Gr1 Javaid Qureshi</t>
-  </si>
-  <si>
-    <t>CPS SE-A Javed Iqbal</t>
-  </si>
-  <si>
-    <t>PROB-A Fareeha</t>
-  </si>
-  <si>
-    <t>PROB-F Osama</t>
-  </si>
-  <si>
-    <t>PROB-D Osama</t>
-  </si>
-  <si>
-    <t>TBW-C Javeria Ali</t>
-  </si>
-  <si>
-    <t>TBW-A Javeria Ali</t>
-  </si>
-  <si>
-    <t>IRS SE-A Dr. Shahzad</t>
-  </si>
-  <si>
-    <t>CPS-A Nazia Imam</t>
-  </si>
-  <si>
-    <t>CPS- Lab C2 Kishwar</t>
-  </si>
-  <si>
-    <t>NC-H Jamil</t>
-  </si>
-  <si>
-    <t>NC-F Jamil</t>
-  </si>
-  <si>
-    <t>NC-E Jamil</t>
-  </si>
-  <si>
-    <t>DLD-D Bilal</t>
-  </si>
-  <si>
-    <t>DLD-F Bilal</t>
-  </si>
-  <si>
-    <t>PROB-G Asma</t>
-  </si>
-  <si>
-    <t>PROB-E Asma</t>
-  </si>
-  <si>
-    <t>DLD-C Rabia</t>
-  </si>
-  <si>
-    <t>TBW-F Sameera</t>
-  </si>
-  <si>
-    <t>DLD-J Rabia</t>
-  </si>
-  <si>
-    <t>DLD-E Rabia</t>
-  </si>
-  <si>
-    <t>CPS- Lab G1 Nazia Imam</t>
-  </si>
-  <si>
-    <t>COAL Lab Gr1 Shoaib Rauf</t>
-  </si>
-  <si>
-    <t>PF Lab-A Aqsa</t>
-  </si>
-  <si>
-    <t>CN Lab-D Rabia</t>
-  </si>
-  <si>
-    <t>OOP Lab-A Nida Munawar</t>
-  </si>
-  <si>
-    <t>OOP Lab-B Irfan</t>
-  </si>
-  <si>
-    <t>DLD Lab-D2 Fahim Ahmed</t>
-  </si>
-  <si>
-    <t>DLD Lab-B2 Fahim Ahmed</t>
-  </si>
-  <si>
-    <t>OS Lab-Gr2 Safia</t>
-  </si>
-  <si>
-    <t>DS Lab-Gr2 Ammara</t>
-  </si>
-  <si>
-    <t>CPS- Lab E1 Hubrah</t>
-  </si>
-  <si>
-    <t>CPS- Lab G2 Atifa</t>
-  </si>
-  <si>
-    <t>DLD Lab-D1 Hamza</t>
-  </si>
-  <si>
-    <t>DLD Lab-C1 M. Nadeem</t>
-  </si>
-  <si>
-    <t>WEDNESDAY</t>
-  </si>
-  <si>
-    <t>CPS-B Atifa</t>
-  </si>
-  <si>
-    <t>CPS-F Atifa</t>
-  </si>
-  <si>
-    <t>DS-Gr3 Basit</t>
+    <t>PROB-B Osama</t>
+  </si>
+  <si>
+    <t>PROB-C Asma</t>
+  </si>
+  <si>
+    <t>CPS-E Nazia Imam</t>
+  </si>
+  <si>
+    <t>CPS-C Nazia Imam</t>
+  </si>
+  <si>
+    <t>CPS- Lab A1 Hafza</t>
+  </si>
+  <si>
+    <t>CPS- Lab A2 Javed Iqbal</t>
+  </si>
+  <si>
+    <t>Pst.-A Aliya</t>
+  </si>
+  <si>
+    <t>CPS- Lab B2 Kishwar</t>
+  </si>
+  <si>
+    <t>OOP Lab SE-A Irfan</t>
+  </si>
+  <si>
+    <t>PF Lab-D Safia</t>
+  </si>
+  <si>
+    <t>OOP Lab SE-B M. Fahim</t>
+  </si>
+  <si>
+    <t>OOP Lab-H M. Fahim</t>
+  </si>
+  <si>
+    <t>PF Lab Gr1 Aqsa</t>
   </si>
   <si>
     <t>BLN-Gr1 Dr. Jawwad</t>
   </si>
   <si>
-    <t>PROB-C Asma</t>
-  </si>
-  <si>
-    <t>CPS-E Nazia Imam</t>
-  </si>
-  <si>
-    <t>CPS-C Nazia Imam</t>
-  </si>
-  <si>
-    <t>PROB-B Osama</t>
-  </si>
-  <si>
-    <t>CPS- Lab A1 Hafza</t>
-  </si>
-  <si>
-    <t>CPS- Lab A2 Javed Iqbal</t>
-  </si>
-  <si>
-    <t>CPS- Lab B2 Kishwar</t>
-  </si>
-  <si>
-    <t>OOP Lab SE-A Irfan</t>
-  </si>
-  <si>
-    <t>OOP Lab SE-B M. Fahim</t>
-  </si>
-  <si>
-    <t>OOP Lab-H M. Fahim</t>
-  </si>
-  <si>
-    <t>PF Lab Gr1 Aqsa</t>
-  </si>
-  <si>
     <t>OOP Lab-J Nida Munawar</t>
   </si>
   <si>
@@ -803,12 +803,12 @@
     <t>THURSDAY</t>
   </si>
   <si>
+    <t>DLP-Gr1 Dr. Tahir Syed</t>
+  </si>
+  <si>
     <t>Dsci-Gr3 Zeshan Khan</t>
   </si>
   <si>
-    <t>DLP-Gr1 Dr. Tahir Syed</t>
-  </si>
-  <si>
     <t>CPS- Lab F1 Hubrah</t>
   </si>
   <si>
@@ -827,28 +827,31 @@
     <t>OS Lab-Gr5 Rahemeen</t>
   </si>
   <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>DLD Lab-E1 M. Nadeem</t>
+  </si>
+  <si>
+    <t>OOAD Lab Gr1 Irfan</t>
+  </si>
+  <si>
     <t>OS Lab-Gr4 Safia</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
-    <t>DLD Lab-E1 M. Nadeem</t>
-  </si>
-  <si>
-    <t>OOAD Lab Gr1 Irfan</t>
-  </si>
-  <si>
     <t>CPS- Lab E2 Kishwar</t>
   </si>
   <si>
     <t>DLD Lab-F2 Mubashyra</t>
   </si>
   <si>
+    <t>FRIDAY</t>
+  </si>
+  <si>
     <t>J U M M A P R A Y E R</t>
   </si>
   <si>
-    <t>PF Lab-B Kariz</t>
+    <t>PF Lab-B1 &amp; B2 Safia &amp; Kariz</t>
   </si>
   <si>
     <t>OS Lab-Gr3 Rahemeen</t>
@@ -869,7 +872,7 @@
     <t>DB Lab Gr1 Tania</t>
   </si>
   <si>
-    <t>PF Lab-C Safia</t>
+    <t>PF Lab-C Abdullah</t>
   </si>
   <si>
     <t>OOP Lab-F Irfan</t>
@@ -1346,81 +1349,81 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="E6"/>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7"/>
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
       <c r="H7"/>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D9"/>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>42</v>
-      </c>
+      <c r="E9"/>
+      <c r="F9"/>
       <c r="G9" t="s">
         <v>43</v>
       </c>
@@ -1440,173 +1443,173 @@
       <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="E10"/>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10"/>
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E11"/>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G11"/>
-      <c r="H11"/>
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
         <v>61</v>
-      </c>
-      <c r="G12" t="s">
-        <v>59</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" t="s">
-        <v>66</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E13"/>
       <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" t="s">
         <v>67</v>
-      </c>
-      <c r="G13" t="s">
-        <v>65</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14"/>
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
-      <c r="E15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" t="s">
-        <v>76</v>
-      </c>
+      <c r="E15"/>
+      <c r="F15"/>
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
         <v>77</v>
-      </c>
-      <c r="B16" t="s">
-        <v>78</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" t="s">
         <v>79</v>
       </c>
-      <c r="E16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16"/>
       <c r="G16"/>
       <c r="H16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
         <v>82</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>84</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17"/>
+      <c r="F17" t="s">
         <v>85</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17"/>
+      <c r="H17" t="s">
         <v>86</v>
       </c>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
@@ -1670,69 +1673,69 @@
       <c r="D20" t="s">
         <v>103</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20"/>
+      <c r="F20" t="s">
         <v>104</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>105</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>106</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>107</v>
-      </c>
-      <c r="I20" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" t="s">
         <v>109</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>110</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>111</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>112</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>113</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>114</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" t="s">
         <v>115</v>
-      </c>
-      <c r="H21" t="s">
-        <v>114</v>
-      </c>
-      <c r="I21" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" t="s">
         <v>117</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>118</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>119</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>120</v>
       </c>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22" t="s">
+      <c r="F22" t="s">
         <v>121</v>
       </c>
+      <c r="G22"/>
       <c r="H22" t="s">
         <v>122</v>
       </c>
@@ -1753,65 +1756,65 @@
       <c r="D23" t="s">
         <v>127</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23"/>
+      <c r="F23" t="s">
         <v>128</v>
-      </c>
-      <c r="F23" t="s">
-        <v>129</v>
       </c>
       <c r="G23"/>
       <c r="H23" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" t="s">
         <v>130</v>
-      </c>
-      <c r="I23" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" t="s">
         <v>132</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>133</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>134</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" t="s">
         <v>135</v>
-      </c>
-      <c r="E24" t="s">
-        <v>133</v>
-      </c>
-      <c r="F24" t="s">
-        <v>136</v>
       </c>
       <c r="G24"/>
       <c r="H24" t="s">
+        <v>136</v>
+      </c>
+      <c r="I24" t="s">
         <v>137</v>
-      </c>
-      <c r="I24" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25"/>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G25"/>
       <c r="H25" t="s">
+        <v>141</v>
+      </c>
+      <c r="I25" t="s">
         <v>142</v>
       </c>
-      <c r="I25"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
@@ -1881,33 +1884,35 @@
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
-      <c r="F30"/>
+      <c r="F30" t="s">
+        <v>152</v>
+      </c>
       <c r="G30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B31"/>
       <c r="C31" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B32"/>
       <c r="C32"/>
@@ -1920,7 +1925,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -1933,11 +1938,11 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34"/>
       <c r="C34" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D34"/>
       <c r="E34"/>
@@ -1948,17 +1953,17 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B35"/>
       <c r="C35" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D35"/>
       <c r="E35"/>
       <c r="F35"/>
       <c r="G35" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H35"/>
       <c r="I35"/>
@@ -1996,7 +2001,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2083,7 +2088,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -2092,7 +2097,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -2101,10 +2106,10 @@
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2115,97 +2120,91 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
         <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" t="s">
         <v>170</v>
       </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>171</v>
-      </c>
-      <c r="I7"/>
+        <v>59</v>
+      </c>
+      <c r="I7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" t="s">
-        <v>76</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D8"/>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" t="s">
-        <v>92</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="I8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9"/>
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
       <c r="C9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E9" t="s">
-        <v>174</v>
-      </c>
-      <c r="F9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9"/>
+        <v>175</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
       <c r="H9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I9"/>
     </row>
@@ -2213,9 +2212,11 @@
       <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
         <v>47</v>
@@ -2223,24 +2224,26 @@
       <c r="E10" t="s">
         <v>48</v>
       </c>
-      <c r="F10"/>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
       <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10"/>
-      <c r="I10" t="s">
-        <v>175</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
@@ -2253,136 +2256,134 @@
         <v>22</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12"/>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
         <v>56</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>177</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>60</v>
       </c>
-      <c r="D12"/>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>178</v>
       </c>
-      <c r="F12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="H12"/>
+      <c r="I12" t="s">
         <v>179</v>
-      </c>
-      <c r="H12" t="s">
-        <v>180</v>
-      </c>
-      <c r="I12" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" t="s">
+        <v>181</v>
+      </c>
+      <c r="D13" t="s">
         <v>182</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>183</v>
-      </c>
-      <c r="D13" t="s">
-        <v>184</v>
-      </c>
-      <c r="E13" t="s">
-        <v>185</v>
       </c>
       <c r="F13" t="s">
         <v>18</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F14" t="s">
         <v>187</v>
       </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
         <v>188</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I14" t="s">
         <v>189</v>
-      </c>
-      <c r="G14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" t="s">
-        <v>190</v>
-      </c>
-      <c r="I14" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" t="s">
-        <v>192</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B15"/>
       <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="D15"/>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
       <c r="E15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F15" t="s">
-        <v>194</v>
-      </c>
-      <c r="G15" t="s">
-        <v>45</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G15"/>
       <c r="H15" t="s">
-        <v>195</v>
-      </c>
-      <c r="I15"/>
+        <v>39</v>
+      </c>
+      <c r="I15" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>193</v>
+      </c>
+      <c r="F16" t="s">
         <v>67</v>
-      </c>
-      <c r="E16" t="s">
-        <v>197</v>
-      </c>
-      <c r="F16" t="s">
-        <v>65</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
@@ -2390,7 +2391,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
         <v>194</v>
@@ -2399,18 +2400,16 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E17"/>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>199</v>
-      </c>
-      <c r="H17" t="s">
-        <v>198</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="H17"/>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
@@ -2418,18 +2417,22 @@
         <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
-      <c r="F18"/>
+      <c r="F18" t="s">
+        <v>194</v>
+      </c>
       <c r="G18" t="s">
-        <v>201</v>
-      </c>
-      <c r="H18"/>
+        <v>86</v>
+      </c>
+      <c r="H18" t="s">
+        <v>195</v>
+      </c>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
@@ -2437,26 +2440,26 @@
         <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
         <v>98</v>
       </c>
       <c r="E19"/>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H19" t="s">
         <v>102</v>
       </c>
       <c r="I19" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2464,62 +2467,62 @@
         <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>204</v>
+        <v>142</v>
       </c>
       <c r="C20"/>
       <c r="D20" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G21" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" t="s">
         <v>117</v>
       </c>
-      <c r="B22" t="s">
-        <v>118</v>
-      </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F22" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2527,60 +2530,66 @@
         <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C23" t="s">
-        <v>213</v>
-      </c>
-      <c r="D23"/>
+        <v>208</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
+      </c>
       <c r="E23"/>
-      <c r="F23"/>
+      <c r="F23" t="s">
+        <v>119</v>
+      </c>
       <c r="G23" t="s">
-        <v>212</v>
-      </c>
-      <c r="H23"/>
+        <v>207</v>
+      </c>
+      <c r="H23" t="s">
+        <v>122</v>
+      </c>
       <c r="I23" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C24" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D24" t="s">
         <v>93</v>
       </c>
       <c r="E24" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H24"/>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25"/>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -2616,14 +2625,14 @@
         <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
@@ -2633,7 +2642,7 @@
         <v>148</v>
       </c>
       <c r="B29" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -2642,7 +2651,7 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
@@ -2657,35 +2666,33 @@
       <c r="E30" t="s">
         <v>46</v>
       </c>
-      <c r="F30" t="s">
-        <v>86</v>
-      </c>
+      <c r="F30"/>
       <c r="G30" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B31" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B32"/>
       <c r="C32"/>
@@ -2693,14 +2700,14 @@
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -2708,41 +2715,41 @@
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H33"/>
       <c r="I33"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
       <c r="F34"/>
       <c r="G34" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H34"/>
       <c r="I34"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B35" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
       <c r="F35"/>
       <c r="G35" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H35"/>
       <c r="I35"/>
@@ -2780,7 +2787,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2867,23 +2874,23 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" t="s">
         <v>187</v>
-      </c>
-      <c r="C5" t="s">
-        <v>189</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G5" t="s">
         <v>176</v>
       </c>
       <c r="H5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I5"/>
     </row>
@@ -2891,55 +2898,49 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6"/>
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6" t="s">
         <v>169</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" t="s">
         <v>170</v>
-      </c>
-      <c r="D6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" t="s">
-        <v>168</v>
-      </c>
-      <c r="H6" t="s">
-        <v>169</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>92</v>
@@ -2948,39 +2949,39 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E8"/>
       <c r="F8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9"/>
-      <c r="H9"/>
+        <v>82</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H9" t="s">
+        <v>181</v>
+      </c>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9">
@@ -2988,63 +2989,59 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C11" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D11" t="s">
-        <v>235</v>
-      </c>
-      <c r="E11" t="s">
-        <v>86</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D12"/>
-      <c r="E12" t="s">
-        <v>236</v>
-      </c>
+      <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12"/>
@@ -3052,44 +3049,44 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D13" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
-      <c r="G13" t="s">
-        <v>182</v>
-      </c>
-      <c r="H13" t="s">
-        <v>183</v>
-      </c>
+      <c r="G13"/>
+      <c r="H13"/>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>180</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D14" t="s">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
-        <v>177</v>
-      </c>
-      <c r="E14"/>
-      <c r="F14"/>
+      <c r="E14" t="s">
+        <v>231</v>
+      </c>
+      <c r="F14" t="s">
+        <v>232</v>
+      </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H14" t="s">
         <v>36</v>
@@ -3098,59 +3095,59 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15"/>
+        <v>233</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15" t="s">
+        <v>233</v>
+      </c>
       <c r="F15"/>
       <c r="G15" t="s">
         <v>98</v>
       </c>
       <c r="H15" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="I15" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" t="s">
         <v>110</v>
       </c>
-      <c r="C16" t="s">
-        <v>115</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="G16" t="s">
         <v>140</v>
-      </c>
-      <c r="E16" t="s">
-        <v>142</v>
-      </c>
-      <c r="F16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" t="s">
-        <v>141</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
         <v>89</v>
@@ -3164,27 +3161,29 @@
         <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H17"/>
-      <c r="I17"/>
+      <c r="I17" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G18" t="s">
         <v>90</v>
@@ -3199,20 +3198,20 @@
         <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F19"/>
       <c r="G19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3220,52 +3219,50 @@
         <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C20" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G20" t="s">
-        <v>204</v>
+        <v>142</v>
       </c>
       <c r="H20" t="s">
         <v>102</v>
       </c>
       <c r="I20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>214</v>
-      </c>
-      <c r="C21" t="s">
-        <v>122</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="C21"/>
       <c r="D21" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E21" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="G21" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" t="s">
         <v>120</v>
-      </c>
-      <c r="H21" t="s">
-        <v>121</v>
       </c>
       <c r="I21" t="s">
         <v>123</v>
@@ -3273,25 +3270,25 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E22"/>
       <c r="F22" t="s">
-        <v>201</v>
+        <v>86</v>
       </c>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="I22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -3299,56 +3296,56 @@
         <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C23" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F23"/>
       <c r="G23" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H23"/>
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" t="s">
+        <v>136</v>
+      </c>
+      <c r="F24" t="s">
         <v>137</v>
       </c>
-      <c r="F24" t="s">
-        <v>138</v>
-      </c>
       <c r="G24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>240</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -3384,13 +3381,15 @@
         <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
-      <c r="G28"/>
+      <c r="G28" t="s">
+        <v>243</v>
+      </c>
       <c r="H28"/>
       <c r="I28"/>
     </row>
@@ -3399,14 +3398,14 @@
         <v>148</v>
       </c>
       <c r="B29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
@@ -3416,11 +3415,13 @@
         <v>151</v>
       </c>
       <c r="B30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
-      <c r="E30"/>
+      <c r="E30" t="s">
+        <v>247</v>
+      </c>
       <c r="F30"/>
       <c r="G30" t="s">
         <v>248</v>
@@ -3430,7 +3431,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B31" t="s">
         <v>249</v>
@@ -3447,7 +3448,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B32" t="s">
         <v>251</v>
@@ -3464,7 +3465,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
         <v>253</v>
@@ -3481,7 +3482,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34" t="s">
         <v>255</v>
@@ -3498,7 +3499,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B35" t="s">
         <v>257</v>
@@ -3638,7 +3639,7 @@
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -3647,14 +3648,14 @@
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H5"/>
       <c r="I5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="J5"/>
     </row>
@@ -3665,98 +3666,96 @@
       <c r="B6"/>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>260</v>
+        <v>184</v>
       </c>
       <c r="G6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H6" t="s">
-        <v>192</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="H6"/>
       <c r="I6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7"/>
-      <c r="C7"/>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
       <c r="D7" t="s">
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>195</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F7"/>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>261</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>232</v>
       </c>
       <c r="F8" t="s">
-        <v>261</v>
+        <v>66</v>
       </c>
       <c r="G8"/>
       <c r="H8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J8"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F9" t="s">
         <v>176</v>
       </c>
       <c r="G9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -3766,91 +3765,93 @@
       <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
       <c r="C10"/>
       <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
         <v>49</v>
-      </c>
-      <c r="E10" t="s">
-        <v>66</v>
       </c>
       <c r="F10" t="s">
         <v>48</v>
       </c>
-      <c r="G10"/>
+      <c r="G10" t="s">
+        <v>191</v>
+      </c>
       <c r="H10" t="s">
         <v>47</v>
       </c>
-      <c r="I10" t="s">
-        <v>175</v>
-      </c>
+      <c r="I10"/>
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>186</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B11"/>
       <c r="C11"/>
       <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
       <c r="F11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>180</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B12"/>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12"/>
+        <v>260</v>
+      </c>
+      <c r="G12" t="s">
+        <v>233</v>
+      </c>
       <c r="H12" t="s">
-        <v>177</v>
+        <v>232</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>126</v>
       </c>
-      <c r="F13"/>
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
       <c r="G13" t="s">
         <v>43</v>
       </c>
@@ -3860,78 +3861,80 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14"/>
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G14"/>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>170</v>
       </c>
       <c r="H15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J15"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
         <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G16" t="s">
         <v>94</v>
@@ -3944,22 +3947,24 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17"/>
+        <v>240</v>
+      </c>
+      <c r="C17" t="s">
+        <v>240</v>
+      </c>
       <c r="D17" t="s">
-        <v>183</v>
-      </c>
-      <c r="E17"/>
+        <v>181</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
       <c r="F17" t="s">
-        <v>182</v>
-      </c>
-      <c r="G17" t="s">
-        <v>45</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
@@ -3975,15 +3980,15 @@
         <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18" t="s">
-        <v>204</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>261</v>
+      </c>
+      <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -3993,17 +3998,13 @@
         <v>95</v>
       </c>
       <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19" t="s">
         <v>79</v>
       </c>
-      <c r="C19" t="s">
-        <v>240</v>
-      </c>
-      <c r="D19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" t="s">
-        <v>201</v>
-      </c>
+      <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
@@ -4015,17 +4016,19 @@
         <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
         <v>133</v>
       </c>
-      <c r="D20"/>
-      <c r="E20" t="s">
-        <v>134</v>
-      </c>
       <c r="F20" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>
@@ -4034,20 +4037,22 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
         <v>103</v>
       </c>
-      <c r="C21"/>
+      <c r="C21" t="s">
+        <v>122</v>
+      </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F21" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G21" t="s">
         <v>262</v>
@@ -4058,17 +4063,17 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
         <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F22"/>
       <c r="G22" t="s">
@@ -4086,13 +4091,13 @@
         <v>127</v>
       </c>
       <c r="C23" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D23" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E23" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F23"/>
       <c r="G23" t="s">
@@ -4104,7 +4109,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -4118,7 +4123,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -4163,9 +4168,7 @@
         <v>145</v>
       </c>
       <c r="B28"/>
-      <c r="C28" t="s">
-        <v>175</v>
-      </c>
+      <c r="C28"/>
       <c r="D28" t="s">
         <v>265</v>
       </c>
@@ -4183,13 +4186,13 @@
         <v>148</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E29"/>
       <c r="F29"/>
@@ -4205,22 +4208,24 @@
         <v>151</v>
       </c>
       <c r="B30"/>
-      <c r="C30"/>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
-      <c r="G30" t="s">
-        <v>268</v>
-      </c>
-      <c r="H30"/>
+      <c r="G30"/>
+      <c r="H30" t="s">
+        <v>191</v>
+      </c>
       <c r="I30"/>
       <c r="J30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -4228,7 +4233,7 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
@@ -4236,7 +4241,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B32"/>
       <c r="C32"/>
@@ -4244,7 +4249,7 @@
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
@@ -4252,21 +4257,23 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
       <c r="F33"/>
-      <c r="G33"/>
+      <c r="G33" t="s">
+        <v>271</v>
+      </c>
       <c r="H33"/>
       <c r="I33"/>
       <c r="J33"/>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34"/>
       <c r="C34"/>
@@ -4282,7 +4289,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B35"/>
       <c r="C35"/>
@@ -4328,7 +4335,9 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1"/>
+      <c r="A1" t="s">
+        <v>274</v>
+      </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
@@ -4419,7 +4428,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -4439,7 +4448,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7"/>
       <c r="C7"/>
@@ -4452,7 +4461,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -4465,7 +4474,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -4491,7 +4500,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
@@ -4504,28 +4513,30 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E12"/>
+        <v>260</v>
+      </c>
+      <c r="E12" t="s">
+        <v>260</v>
+      </c>
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12"/>
       <c r="I12" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -4538,121 +4549,117 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B14"/>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" t="s">
-        <v>36</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="F14"/>
       <c r="G14"/>
       <c r="H14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" t="s">
-        <v>110</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15"/>
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16"/>
+        <v>111</v>
+      </c>
+      <c r="D16" t="s">
+        <v>114</v>
+      </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G16"/>
-      <c r="H16"/>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>231</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17" t="s">
-        <v>115</v>
-      </c>
+      <c r="H17" t="s">
+        <v>235</v>
+      </c>
+      <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" t="s">
         <v>140</v>
-      </c>
-      <c r="F18" t="s">
-        <v>141</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -4660,97 +4667,93 @@
         <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C19" t="s">
         <v>123</v>
       </c>
       <c r="D19" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" t="s">
+        <v>207</v>
+      </c>
+      <c r="F19" t="s">
         <v>237</v>
-      </c>
-      <c r="E19" t="s">
-        <v>212</v>
-      </c>
-      <c r="F19" t="s">
-        <v>239</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>238</v>
-      </c>
-      <c r="I19" t="s">
-        <v>213</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="I19"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="E20" t="s">
-        <v>200</v>
-      </c>
-      <c r="F20"/>
+        <v>197</v>
+      </c>
+      <c r="F20" t="s">
+        <v>109</v>
+      </c>
       <c r="G20"/>
-      <c r="H20" t="s">
-        <v>210</v>
-      </c>
-      <c r="I20" t="s">
-        <v>211</v>
-      </c>
+      <c r="H20"/>
+      <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
         <v>103</v>
       </c>
-      <c r="D21"/>
+      <c r="D21" t="s">
+        <v>205</v>
+      </c>
       <c r="E21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21"/>
+        <v>106</v>
+      </c>
+      <c r="I21" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C22" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D22"/>
-      <c r="E22" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" t="s">
-        <v>121</v>
-      </c>
+      <c r="E22"/>
+      <c r="F22"/>
       <c r="G22"/>
       <c r="H22" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I22" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -4758,7 +4761,7 @@
         <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
         <v>127</v>
@@ -4774,38 +4777,38 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24"/>
       <c r="C24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F25"/>
       <c r="G25"/>
@@ -4843,19 +4846,19 @@
         <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F28"/>
       <c r="G28" t="s">
+        <v>278</v>
+      </c>
+      <c r="H28" t="s">
         <v>277</v>
-      </c>
-      <c r="H28" t="s">
-        <v>276</v>
       </c>
       <c r="I28"/>
     </row>
@@ -4864,17 +4867,17 @@
         <v>148</v>
       </c>
       <c r="B29" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I29"/>
     </row>
@@ -4883,26 +4886,26 @@
         <v>151</v>
       </c>
       <c r="B30" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F30"/>
       <c r="G30"/>
       <c r="H30" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B31" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
@@ -4914,10 +4917,10 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B32" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
@@ -4929,10 +4932,10 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -4944,7 +4947,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34"/>
       <c r="C34"/>
@@ -4957,7 +4960,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B35"/>
       <c r="C35"/>

</xml_diff>